<commit_message>
TODO: West Field - Add NPCS, South Field - Add sidequests, Forest - Finish scripting encounter with Canson, add loot, add side enemies
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Undead" sheetId="1" r:id="rId1"/>
+    <sheet name="Goblin" sheetId="2" r:id="rId2"/>
+    <sheet name="VillianCanson" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="22">
   <si>
     <t>Skeletons are the most basic undead, they have low magical attributes, agility, and luck.</t>
   </si>
@@ -67,6 +69,30 @@
   <si>
     <t>The Skeleton Soldier is a common undead, its armor and weapons are usually rusted.</t>
   </si>
+  <si>
+    <t>Goblins are a type of demihuman with short lifespans. They have a baselevel of 1</t>
+  </si>
+  <si>
+    <t>Goblin Scout</t>
+  </si>
+  <si>
+    <t>Goblin</t>
+  </si>
+  <si>
+    <t>Goblin Shaman</t>
+  </si>
+  <si>
+    <t>If they aren't add: 33 def, 30 attack</t>
+  </si>
+  <si>
+    <t>Goblin Scouts use crude iron daggers, studded leather armor, and studded leather helmets</t>
+  </si>
+  <si>
+    <t>Iron daggers should be weaker than iron sword -&gt; 25 attack 5 agility, 10 def, 8 mdf</t>
+  </si>
+  <si>
+    <t>First Encounter. Has tech 2 gear. 40 MAT from staff, 3/10 from engraved robe, 3/2 from studded leather helmet</t>
+  </si>
 </sst>
 </file>
 
@@ -89,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -97,18 +123,440 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="53">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -150,8 +598,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2861DD08-92F9-4821-84C5-84F68B225D94}" name="Table1" displayName="Table1" ref="A4:J6" totalsRowShown="0">
-  <autoFilter ref="A4:J6" xr:uid="{634C2810-B5E1-4DB3-A486-F7F8D8DC6C73}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2861DD08-92F9-4821-84C5-84F68B225D94}" name="Table1" displayName="Table1" ref="A4:J5" totalsRowShown="0">
+  <autoFilter ref="A4:J5" xr:uid="{634C2810-B5E1-4DB3-A486-F7F8D8DC6C73}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{117C7306-80A7-4222-9DFB-71039A554839}" name="Name"/>
     <tableColumn id="2" xr3:uid="{18C02B4B-873F-49A2-AD1E-C8DCBB95D8A6}" name="HP"/>
@@ -162,7 +610,7 @@
     <tableColumn id="7" xr3:uid="{F9852B29-E77D-4E17-A56E-5F0C649FA862}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{9A914BFF-1060-46E4-B8F9-412BD9293C3D}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2F83B650-811D-4FEE-92D5-03D4DC4376E5}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="8">
+    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="52">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -175,29 +623,220 @@
   <autoFilter ref="A8:I13" xr:uid="{67385006-CBB9-4472-99D4-7881E042769D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FD96F8F7-CCAB-44FA-B525-A5081670706A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="51">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="50">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="6">
+    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="49">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="5">
+    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="48">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="47">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="3">
+    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="46">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="45">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="4">
+    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="44">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{7268DD6D-84F4-43D7-A05F-EB56AE11DFF7}" name="Table131611" displayName="Table131611" ref="K8:S13" totalsRowShown="0">
+  <autoFilter ref="K8:S13" xr:uid="{AB7E938D-7ACC-4BFB-A6B9-682B8B29CEF2}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{66EB8EF1-BCF4-44F7-B8A6-3C3B425F8FF5}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="22">
+      <calculatedColumnFormula>Table131611[[#This Row],[Level]]*56.25+200</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="26">
+      <calculatedColumnFormula>Table131611[[#This Row],[Level]]*10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="21">
+      <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25+ 15+30</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="20">
+      <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25 + 15+33</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="25">
+      <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="24">
+      <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="19">
+      <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="23">
+      <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DE335D90-A9BD-40A2-B9C7-73CA6E6CAB11}" name="Table15" displayName="Table15" ref="A4:J7" totalsRowShown="0">
+  <autoFilter ref="A4:J7" xr:uid="{CE759384-ADAA-40BA-B9E0-40CE462A16EC}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{DAE2EC63-1D40-4ED3-8C7B-1C8C0375CA6B}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{0BF5F099-BE0D-4349-90FC-65863CB0E17C}" name="HP"/>
+    <tableColumn id="3" xr3:uid="{CCC1BCC5-CFE4-4B8A-8323-673868BD95EF}" name="MP"/>
+    <tableColumn id="4" xr3:uid="{FE1FBFE1-8412-412B-A359-6E322B02EF8B}" name="ATK"/>
+    <tableColumn id="5" xr3:uid="{8DA4C046-05AD-4DAC-A5E6-0889B4BA4F65}" name="DEF"/>
+    <tableColumn id="6" xr3:uid="{90827F4E-7CAE-4259-B6F9-E364498748A0}" name="MAT"/>
+    <tableColumn id="7" xr3:uid="{22216E02-260E-4471-8BB1-4E6E1250BAC9}" name="MDF"/>
+    <tableColumn id="8" xr3:uid="{DC2670AC-8DF2-47F7-A3F6-EE7896309BC9}" name="AGI"/>
+    <tableColumn id="9" xr3:uid="{749652E2-F6CF-428C-B67C-FD0B1EFCCBBF}" name="LUK"/>
+    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="43">
+      <calculatedColumnFormula>SUM(Table15[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{11E951F1-5D13-41C6-A7E5-8F4298DA5463}" name="Table13167" displayName="Table13167" ref="A11:I16" totalsRowShown="0">
+  <autoFilter ref="A11:I16" xr:uid="{A1CF627F-8D28-44AD-9A35-411103976FCA}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{F14CC326-DE44-48D8-856F-8DCDCFC89CAD}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="42">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="41">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="39">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="40">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="38">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="37">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="36">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="35">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{60D4A7A8-82BF-4B58-A912-589523D22F05}" name="Table131679" displayName="Table131679" ref="K11:S17" totalsRowShown="0">
+  <autoFilter ref="K11:S17" xr:uid="{EAF9FB6A-F011-40E3-AB2F-E53826722AFB}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{DF3E0800-6EE4-4E1B-BA6F-0194351D6E7C}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="27">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*56.25+100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="34">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="31">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="30">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="33">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="29">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="28">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="32">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BACB03CE-1DAD-4E5F-8D00-25D6D07FC945}" name="Table131620" displayName="Table131620" ref="A3:I9" totalsRowShown="0">
+  <autoFilter ref="A3:I9" xr:uid="{A90D1C2A-DBF9-4EEF-ACC2-3DC17C207301}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{BD3505AC-AE6D-4947-A74E-A6C2D68658F1}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="18">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="17">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*15+100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="16">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="15">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="11">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="12">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="14">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="13">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="0" tableBorderDxfId="10">
+  <autoFilter ref="L3:T4" xr:uid="{5D2C3EA8-1297-4C77-AF32-84E50F8232C5}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="8">
+      <calculatedColumnFormula>Table19[Level]*50 + 100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="7">
+      <calculatedColumnFormula>Table19[[#This Row],[Level]]*15+100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="6">
+      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="5">
+      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1 + 15 + 6</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="4">
+      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="3">
+      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 12</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="2">
+      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="1">
+      <calculatedColumnFormula>Table19[Level] + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -501,10 +1140,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F7AABB-3532-4A29-877B-ED130C7A9042}">
-  <dimension ref="A2:J13"/>
+  <dimension ref="A2:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,12 +1152,12 @@
     <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -550,7 +1189,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -583,16 +1222,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="1">
-        <f>SUM(Table1[[#This Row],[HP]:[LUK]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -620,8 +1261,35 @@
       <c r="I8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" t="s">
+        <v>4</v>
+      </c>
+      <c r="O8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P8" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>7</v>
+      </c>
+      <c r="R8" t="s">
+        <v>8</v>
+      </c>
+      <c r="S8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -657,8 +1325,43 @@
         <f>Table1316[[#This Row],[Level]]*1</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <f>Table131611[[#This Row],[Level]]*56.25+200</f>
+        <v>256.25</v>
+      </c>
+      <c r="M9">
+        <f>Table131611[[#This Row],[Level]]*10</f>
+        <v>10</v>
+      </c>
+      <c r="N9">
+        <f>Table131611[[#This Row],[Level]]*1.25+ 15+30</f>
+        <v>46.25</v>
+      </c>
+      <c r="O9">
+        <f>Table131611[[#This Row],[Level]]*1.25 + 15+33</f>
+        <v>49.25</v>
+      </c>
+      <c r="P9">
+        <f>Table131611[[#This Row],[Level]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <f>Table131611[[#This Row],[Level]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <f>Table131611[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+      <c r="S9">
+        <f>Table131611[[#This Row],[Level]]*1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -694,8 +1397,43 @@
         <f>Table1316[[#This Row],[Level]]*1</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>10</v>
+      </c>
+      <c r="L10">
+        <f>Table131611[[#This Row],[Level]]*56.25+200</f>
+        <v>762.5</v>
+      </c>
+      <c r="M10">
+        <f>Table131611[[#This Row],[Level]]*10</f>
+        <v>100</v>
+      </c>
+      <c r="N10">
+        <f>Table131611[[#This Row],[Level]]*1.25+ 15+30</f>
+        <v>57.5</v>
+      </c>
+      <c r="O10">
+        <f>Table131611[[#This Row],[Level]]*1.25 + 15+33</f>
+        <v>60.5</v>
+      </c>
+      <c r="P10">
+        <f>Table131611[[#This Row],[Level]]*1</f>
+        <v>10</v>
+      </c>
+      <c r="Q10">
+        <f>Table131611[[#This Row],[Level]]*1</f>
+        <v>10</v>
+      </c>
+      <c r="R10">
+        <f>Table131611[[#This Row],[Level]]*1 + 15</f>
+        <v>25</v>
+      </c>
+      <c r="S10">
+        <f>Table131611[[#This Row],[Level]]*1</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>25</v>
       </c>
@@ -731,8 +1469,43 @@
         <f>Table1316[[#This Row],[Level]]*1</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>25</v>
+      </c>
+      <c r="L11">
+        <f>Table131611[[#This Row],[Level]]*56.25+200</f>
+        <v>1606.25</v>
+      </c>
+      <c r="M11">
+        <f>Table131611[[#This Row],[Level]]*10</f>
+        <v>250</v>
+      </c>
+      <c r="N11">
+        <f>Table131611[[#This Row],[Level]]*1.25+ 15+30</f>
+        <v>76.25</v>
+      </c>
+      <c r="O11">
+        <f>Table131611[[#This Row],[Level]]*1.25 + 15+33</f>
+        <v>79.25</v>
+      </c>
+      <c r="P11">
+        <f>Table131611[[#This Row],[Level]]*1</f>
+        <v>25</v>
+      </c>
+      <c r="Q11">
+        <f>Table131611[[#This Row],[Level]]*1</f>
+        <v>25</v>
+      </c>
+      <c r="R11">
+        <f>Table131611[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="S11">
+        <f>Table131611[[#This Row],[Level]]*1</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>35</v>
       </c>
@@ -768,8 +1541,43 @@
         <f>Table1316[[#This Row],[Level]]*1</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>35</v>
+      </c>
+      <c r="L12">
+        <f>Table131611[[#This Row],[Level]]*56.25+200</f>
+        <v>2168.75</v>
+      </c>
+      <c r="M12">
+        <f>Table131611[[#This Row],[Level]]*10</f>
+        <v>350</v>
+      </c>
+      <c r="N12">
+        <f>Table131611[[#This Row],[Level]]*1.25+ 15+30</f>
+        <v>88.75</v>
+      </c>
+      <c r="O12">
+        <f>Table131611[[#This Row],[Level]]*1.25 + 15+33</f>
+        <v>91.75</v>
+      </c>
+      <c r="P12">
+        <f>Table131611[[#This Row],[Level]]*1</f>
+        <v>35</v>
+      </c>
+      <c r="Q12">
+        <f>Table131611[[#This Row],[Level]]*1</f>
+        <v>35</v>
+      </c>
+      <c r="R12">
+        <f>Table131611[[#This Row],[Level]]*1 + 15</f>
+        <v>50</v>
+      </c>
+      <c r="S12">
+        <f>Table131611[[#This Row],[Level]]*1</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>99</v>
       </c>
@@ -804,6 +1612,1007 @@
       <c r="I13">
         <f>Table1316[[#This Row],[Level]]*1</f>
         <v>99</v>
+      </c>
+      <c r="K13">
+        <v>99</v>
+      </c>
+      <c r="L13">
+        <f>Table131611[[#This Row],[Level]]*56.25+200</f>
+        <v>5768.75</v>
+      </c>
+      <c r="M13">
+        <f>Table131611[[#This Row],[Level]]*10</f>
+        <v>990</v>
+      </c>
+      <c r="N13">
+        <f>Table131611[[#This Row],[Level]]*1.25+ 15+30</f>
+        <v>168.75</v>
+      </c>
+      <c r="O13">
+        <f>Table131611[[#This Row],[Level]]*1.25 + 15+33</f>
+        <v>171.75</v>
+      </c>
+      <c r="P13">
+        <f>Table131611[[#This Row],[Level]]*1</f>
+        <v>99</v>
+      </c>
+      <c r="Q13">
+        <f>Table131611[[#This Row],[Level]]*1</f>
+        <v>99</v>
+      </c>
+      <c r="R13">
+        <f>Table131611[[#This Row],[Level]]*1 + 15</f>
+        <v>114</v>
+      </c>
+      <c r="S13">
+        <f>Table131611[[#This Row],[Level]]*1</f>
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4195E475-9F10-4DD8-82F0-E47D9A595A6E}">
+  <dimension ref="A2:S17"/>
+  <sheetViews>
+    <sheetView topLeftCell="J7" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <f>SUM(Table15[[#This Row],[HP]:[LUK]])</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1">
+        <f>SUM(Table15[[#This Row],[HP]:[LUK]])</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1">
+        <f>SUM(Table15[[#This Row],[HP]:[LUK]])</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" t="s">
+        <v>2</v>
+      </c>
+      <c r="M11" t="s">
+        <v>3</v>
+      </c>
+      <c r="N11" t="s">
+        <v>4</v>
+      </c>
+      <c r="O11" t="s">
+        <v>5</v>
+      </c>
+      <c r="P11" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>7</v>
+      </c>
+      <c r="R11" t="s">
+        <v>8</v>
+      </c>
+      <c r="S11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <f>Table13167[[#This Row],[Level]]*56.25-100</f>
+        <v>-43.75</v>
+      </c>
+      <c r="C12">
+        <f>Table13167[[#This Row],[Level]]*10</f>
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <f>Table13167[[#This Row],[Level]]*1.375+ 15</f>
+        <v>16.375</v>
+      </c>
+      <c r="E12">
+        <f>Table13167[[#This Row],[Level]]*1.25 + 15</f>
+        <v>16.25</v>
+      </c>
+      <c r="F12">
+        <f>Table13167[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+      <c r="G12">
+        <f>Table13167[[#This Row],[Level]]*1.25+ 15</f>
+        <v>16.25</v>
+      </c>
+      <c r="H12">
+        <f>Table13167[[#This Row],[Level]]*1.5 + 15</f>
+        <v>16.5</v>
+      </c>
+      <c r="I12">
+        <f>Table13167[[#This Row],[Level]]*1.125 + 15</f>
+        <v>16.125</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <f>Table131679[[#This Row],[Level]]*56.25+100</f>
+        <v>156.25</v>
+      </c>
+      <c r="M12">
+        <f>Table131679[[#This Row],[Level]]*10</f>
+        <v>10</v>
+      </c>
+      <c r="N12">
+        <f>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</f>
+        <v>41.375</v>
+      </c>
+      <c r="O12">
+        <f>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</f>
+        <v>26.25</v>
+      </c>
+      <c r="P12">
+        <f>Table131679[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+      <c r="Q12">
+        <f>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</f>
+        <v>24.25</v>
+      </c>
+      <c r="R12">
+        <f>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</f>
+        <v>21.5</v>
+      </c>
+      <c r="S12">
+        <f>Table131679[[#This Row],[Level]]*1.125 + 15</f>
+        <v>16.125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <f>Table13167[[#This Row],[Level]]*56.25-100</f>
+        <v>462.5</v>
+      </c>
+      <c r="C13">
+        <f>Table13167[[#This Row],[Level]]*10</f>
+        <v>100</v>
+      </c>
+      <c r="D13">
+        <f>Table13167[[#This Row],[Level]]*1.375+ 15</f>
+        <v>28.75</v>
+      </c>
+      <c r="E13">
+        <f>Table13167[[#This Row],[Level]]*1.25 + 15</f>
+        <v>27.5</v>
+      </c>
+      <c r="F13">
+        <f>Table13167[[#This Row],[Level]]*1 + 15</f>
+        <v>25</v>
+      </c>
+      <c r="G13">
+        <f>Table13167[[#This Row],[Level]]*1.25+ 15</f>
+        <v>27.5</v>
+      </c>
+      <c r="H13">
+        <f>Table13167[[#This Row],[Level]]*1.5 + 15</f>
+        <v>30</v>
+      </c>
+      <c r="I13">
+        <f>Table13167[[#This Row],[Level]]*1.125 + 15</f>
+        <v>26.25</v>
+      </c>
+      <c r="K13">
+        <v>10</v>
+      </c>
+      <c r="L13">
+        <f>Table131679[[#This Row],[Level]]*56.25+100</f>
+        <v>662.5</v>
+      </c>
+      <c r="M13">
+        <f>Table131679[[#This Row],[Level]]*10</f>
+        <v>100</v>
+      </c>
+      <c r="N13">
+        <f>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</f>
+        <v>53.75</v>
+      </c>
+      <c r="O13">
+        <f>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</f>
+        <v>37.5</v>
+      </c>
+      <c r="P13">
+        <f>Table131679[[#This Row],[Level]]*1 + 15</f>
+        <v>25</v>
+      </c>
+      <c r="Q13">
+        <f>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</f>
+        <v>35.5</v>
+      </c>
+      <c r="R13">
+        <f>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</f>
+        <v>35</v>
+      </c>
+      <c r="S13">
+        <f>Table131679[[#This Row],[Level]]*1.125 + 15</f>
+        <v>26.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <f>Table13167[[#This Row],[Level]]*56.25-100</f>
+        <v>1306.25</v>
+      </c>
+      <c r="C14">
+        <f>Table13167[[#This Row],[Level]]*10</f>
+        <v>250</v>
+      </c>
+      <c r="D14">
+        <f>Table13167[[#This Row],[Level]]*1.375+ 15</f>
+        <v>49.375</v>
+      </c>
+      <c r="E14">
+        <f>Table13167[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+      <c r="F14">
+        <f>Table13167[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="G14">
+        <f>Table13167[[#This Row],[Level]]*1.25+ 15</f>
+        <v>46.25</v>
+      </c>
+      <c r="H14">
+        <f>Table13167[[#This Row],[Level]]*1.5 + 15</f>
+        <v>52.5</v>
+      </c>
+      <c r="I14">
+        <f>Table13167[[#This Row],[Level]]*1.125 + 15</f>
+        <v>43.125</v>
+      </c>
+      <c r="K14">
+        <v>25</v>
+      </c>
+      <c r="L14">
+        <f>Table131679[[#This Row],[Level]]*56.25+100</f>
+        <v>1506.25</v>
+      </c>
+      <c r="M14">
+        <f>Table131679[[#This Row],[Level]]*10</f>
+        <v>250</v>
+      </c>
+      <c r="N14">
+        <f>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</f>
+        <v>74.375</v>
+      </c>
+      <c r="O14">
+        <f>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</f>
+        <v>56.25</v>
+      </c>
+      <c r="P14">
+        <f>Table131679[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="Q14">
+        <f>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</f>
+        <v>54.25</v>
+      </c>
+      <c r="R14">
+        <f>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</f>
+        <v>57.5</v>
+      </c>
+      <c r="S14">
+        <f>Table131679[[#This Row],[Level]]*1.125 + 15</f>
+        <v>43.125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>35</v>
+      </c>
+      <c r="B15">
+        <f>Table13167[[#This Row],[Level]]*56.25-100</f>
+        <v>1868.75</v>
+      </c>
+      <c r="C15">
+        <f>Table13167[[#This Row],[Level]]*10</f>
+        <v>350</v>
+      </c>
+      <c r="D15">
+        <f>Table13167[[#This Row],[Level]]*1.375+ 15</f>
+        <v>63.125</v>
+      </c>
+      <c r="E15">
+        <f>Table13167[[#This Row],[Level]]*1.25 + 15</f>
+        <v>58.75</v>
+      </c>
+      <c r="F15">
+        <f>Table13167[[#This Row],[Level]]*1 + 15</f>
+        <v>50</v>
+      </c>
+      <c r="G15">
+        <f>Table13167[[#This Row],[Level]]*1.25+ 15</f>
+        <v>58.75</v>
+      </c>
+      <c r="H15">
+        <f>Table13167[[#This Row],[Level]]*1.5 + 15</f>
+        <v>67.5</v>
+      </c>
+      <c r="I15">
+        <f>Table13167[[#This Row],[Level]]*1.125 + 15</f>
+        <v>54.375</v>
+      </c>
+      <c r="K15">
+        <v>35</v>
+      </c>
+      <c r="L15">
+        <f>Table131679[[#This Row],[Level]]*56.25+100</f>
+        <v>2068.75</v>
+      </c>
+      <c r="M15">
+        <f>Table131679[[#This Row],[Level]]*10</f>
+        <v>350</v>
+      </c>
+      <c r="N15">
+        <f>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</f>
+        <v>88.125</v>
+      </c>
+      <c r="O15">
+        <f>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</f>
+        <v>68.75</v>
+      </c>
+      <c r="P15">
+        <f>Table131679[[#This Row],[Level]]*1 + 15</f>
+        <v>50</v>
+      </c>
+      <c r="Q15">
+        <f>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</f>
+        <v>66.75</v>
+      </c>
+      <c r="R15">
+        <f>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</f>
+        <v>72.5</v>
+      </c>
+      <c r="S15">
+        <f>Table131679[[#This Row],[Level]]*1.125 + 15</f>
+        <v>54.375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>99</v>
+      </c>
+      <c r="B16">
+        <f>Table13167[[#This Row],[Level]]*56.25-100</f>
+        <v>5468.75</v>
+      </c>
+      <c r="C16">
+        <f>Table13167[[#This Row],[Level]]*10</f>
+        <v>990</v>
+      </c>
+      <c r="D16">
+        <f>Table13167[[#This Row],[Level]]*1.375+ 15</f>
+        <v>151.125</v>
+      </c>
+      <c r="E16">
+        <f>Table13167[[#This Row],[Level]]*1.25 + 15</f>
+        <v>138.75</v>
+      </c>
+      <c r="F16">
+        <f>Table13167[[#This Row],[Level]]*1 + 15</f>
+        <v>114</v>
+      </c>
+      <c r="G16">
+        <f>Table13167[[#This Row],[Level]]*1.25+ 15</f>
+        <v>138.75</v>
+      </c>
+      <c r="H16">
+        <f>Table13167[[#This Row],[Level]]*1.5 + 15</f>
+        <v>163.5</v>
+      </c>
+      <c r="I16">
+        <f>Table13167[[#This Row],[Level]]*1.125 + 15</f>
+        <v>126.375</v>
+      </c>
+      <c r="K16">
+        <v>99</v>
+      </c>
+      <c r="L16">
+        <f>Table131679[[#This Row],[Level]]*56.25+100</f>
+        <v>5668.75</v>
+      </c>
+      <c r="M16">
+        <f>Table131679[[#This Row],[Level]]*10</f>
+        <v>990</v>
+      </c>
+      <c r="N16">
+        <f>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</f>
+        <v>176.125</v>
+      </c>
+      <c r="O16">
+        <f>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</f>
+        <v>148.75</v>
+      </c>
+      <c r="P16">
+        <f>Table131679[[#This Row],[Level]]*1 + 15</f>
+        <v>114</v>
+      </c>
+      <c r="Q16">
+        <f>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</f>
+        <v>146.75</v>
+      </c>
+      <c r="R16">
+        <f>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</f>
+        <v>168.5</v>
+      </c>
+      <c r="S16">
+        <f>Table131679[[#This Row],[Level]]*1.125 + 15</f>
+        <v>126.375</v>
+      </c>
+    </row>
+    <row r="17" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <v>3</v>
+      </c>
+      <c r="L17" s="1">
+        <f>Table131679[[#This Row],[Level]]*56.25+100</f>
+        <v>268.75</v>
+      </c>
+      <c r="M17" s="1">
+        <f>Table131679[[#This Row],[Level]]*10</f>
+        <v>30</v>
+      </c>
+      <c r="N17" s="1">
+        <f>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</f>
+        <v>44.125</v>
+      </c>
+      <c r="O17" s="1">
+        <f>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</f>
+        <v>28.75</v>
+      </c>
+      <c r="P17" s="1">
+        <f>Table131679[[#This Row],[Level]]*1 + 15</f>
+        <v>18</v>
+      </c>
+      <c r="Q17" s="1">
+        <f>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</f>
+        <v>26.75</v>
+      </c>
+      <c r="R17" s="1">
+        <f>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</f>
+        <v>24.5</v>
+      </c>
+      <c r="S17" s="1">
+        <f>Table131679[[#This Row],[Level]]*1.125 + 15</f>
+        <v>18.375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED846686-A238-4174-849F-9F6770BD1F9B}">
+  <dimension ref="A1:T9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="I1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R3" t="s">
+        <v>7</v>
+      </c>
+      <c r="S3" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
+        <v>150</v>
+      </c>
+      <c r="C4">
+        <f>Table131620[[#This Row],[Level]]*15+100</f>
+        <v>115</v>
+      </c>
+      <c r="D4">
+        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>16.5</v>
+      </c>
+      <c r="G4">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>16.5</v>
+      </c>
+      <c r="H4">
+        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
+        <v>16.25</v>
+      </c>
+      <c r="I4">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+      <c r="L4" s="2">
+        <v>20</v>
+      </c>
+      <c r="M4" s="3">
+        <f>Table19[Level]*50 + 100</f>
+        <v>1100</v>
+      </c>
+      <c r="N4" s="3">
+        <f>Table19[[#This Row],[Level]]*15+100</f>
+        <v>400</v>
+      </c>
+      <c r="O4" s="3">
+        <f>Table19[[#This Row],[Level]]*1+ 15</f>
+        <v>35</v>
+      </c>
+      <c r="P4" s="3">
+        <f>Table19[[#This Row],[Level]]*1 + 15 + 6</f>
+        <v>41</v>
+      </c>
+      <c r="Q4" s="3">
+        <f>Table19[[#This Row],[Level]]*1.5 + 15 + 40</f>
+        <v>85</v>
+      </c>
+      <c r="R4" s="3">
+        <f>Table19[[#This Row],[Level]]*1.5 + 15 + 12</f>
+        <v>57</v>
+      </c>
+      <c r="S4" s="3">
+        <f>Table19[[#This Row],[Level]]*1.25 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="T4" s="4">
+        <f>Table19[Level] + 15</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
+        <v>850</v>
+      </c>
+      <c r="C5">
+        <f>Table131620[[#This Row],[Level]]*15+100</f>
+        <v>325</v>
+      </c>
+      <c r="D5">
+        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>37.5</v>
+      </c>
+      <c r="G5">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>37.5</v>
+      </c>
+      <c r="H5">
+        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
+        <v>33.75</v>
+      </c>
+      <c r="I5">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
+        <v>1350</v>
+      </c>
+      <c r="C6">
+        <f>Table131620[[#This Row],[Level]]*15+100</f>
+        <v>475</v>
+      </c>
+      <c r="D6">
+        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+        <v>40</v>
+      </c>
+      <c r="E6">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>52.5</v>
+      </c>
+      <c r="G6">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>52.5</v>
+      </c>
+      <c r="H6">
+        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+      <c r="I6">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>35</v>
+      </c>
+      <c r="B7">
+        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
+        <v>1850</v>
+      </c>
+      <c r="C7">
+        <f>Table131620[[#This Row],[Level]]*15+100</f>
+        <v>625</v>
+      </c>
+      <c r="D7">
+        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+        <v>50</v>
+      </c>
+      <c r="E7">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>67.5</v>
+      </c>
+      <c r="G7">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>67.5</v>
+      </c>
+      <c r="H7">
+        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
+        <v>58.75</v>
+      </c>
+      <c r="I7">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>99</v>
+      </c>
+      <c r="B8">
+        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
+        <v>5050</v>
+      </c>
+      <c r="C8">
+        <f>Table131620[[#This Row],[Level]]*15+100</f>
+        <v>1585</v>
+      </c>
+      <c r="D8">
+        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+        <v>114</v>
+      </c>
+      <c r="E8">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>114</v>
+      </c>
+      <c r="F8">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>163.5</v>
+      </c>
+      <c r="G8">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>163.5</v>
+      </c>
+      <c r="H8">
+        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
+        <v>138.75</v>
+      </c>
+      <c r="I8">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1">
+        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
+        <v>1100</v>
+      </c>
+      <c r="C9" s="1">
+        <f>Table131620[[#This Row],[Level]]*15+100</f>
+        <v>400</v>
+      </c>
+      <c r="D9" s="1">
+        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+        <v>35</v>
+      </c>
+      <c r="E9" s="1">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>35</v>
+      </c>
+      <c r="F9" s="1">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>45</v>
+      </c>
+      <c r="G9" s="1">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>45</v>
+      </c>
+      <c r="H9" s="1">
+        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="I9" s="1">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>35</v>
+      </c>
+      <c r="K9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished forest, working on goblin forest side, west field side
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
   </bookViews>
   <sheets>
-    <sheet name="Undead" sheetId="1" r:id="rId1"/>
-    <sheet name="Goblin" sheetId="2" r:id="rId2"/>
+    <sheet name="Skeleton Soldier" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
     <sheet name="VillianCanson" sheetId="4" r:id="rId3"/>
+    <sheet name="Goblin" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="25">
   <si>
     <t>Skeletons are the most basic undead, they have low magical attributes, agility, and luck.</t>
   </si>
@@ -92,6 +93,15 @@
   </si>
   <si>
     <t>First Encounter. Has tech 2 gear. 40 MAT from staff, 3/10 from engraved robe, 3/2 from studded leather helmet</t>
+  </si>
+  <si>
+    <t>Zombie</t>
+  </si>
+  <si>
+    <t>They usually swarm in huge numbers though, and their touch corrupts defence</t>
+  </si>
+  <si>
+    <t>Zombies are the type of undead made from decomposing corpses. Only uses weapons, can't use armor. Often made from peasants, using shovels</t>
   </si>
 </sst>
 </file>
@@ -168,24 +178,33 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="53">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+  <dxfs count="62">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -459,6 +478,24 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -610,8 +647,42 @@
     <tableColumn id="7" xr3:uid="{F9852B29-E77D-4E17-A56E-5F0C649FA862}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{9A914BFF-1060-46E4-B8F9-412BD9293C3D}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2F83B650-811D-4FEE-92D5-03D4DC4376E5}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="52">
+    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="61">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{60D4A7A8-82BF-4B58-A912-589523D22F05}" name="Table131679" displayName="Table131679" ref="K11:S17" totalsRowShown="0">
+  <autoFilter ref="K11:S17" xr:uid="{EAF9FB6A-F011-40E3-AB2F-E53826722AFB}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{DF3E0800-6EE4-4E1B-BA6F-0194351D6E7C}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="35">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*56.25+100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="34">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="33">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="32">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="31">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="30">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="29">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="28">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -623,28 +694,28 @@
   <autoFilter ref="A8:I13" xr:uid="{67385006-CBB9-4472-99D4-7881E042769D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FD96F8F7-CCAB-44FA-B525-A5081670706A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="51">
+    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="60">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="50">
+    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="59">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="49">
+    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="58">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="48">
+    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="57">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="47">
+    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="56">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="46">
+    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="55">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="45">
+    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="54">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="44">
+    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="53">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -657,28 +728,28 @@
   <autoFilter ref="K8:S13" xr:uid="{AB7E938D-7ACC-4BFB-A6B9-682B8B29CEF2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{66EB8EF1-BCF4-44F7-B8A6-3C3B425F8FF5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="22">
+    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="52">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*56.25+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="26">
+    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="51">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="21">
+    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="50">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25+ 15+30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="20">
+    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="49">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25 + 15+33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="25">
+    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="48">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="24">
+    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="47">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="19">
+    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="46">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="23">
+    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="45">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -687,6 +758,129 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{671A73B1-117F-4F40-B5B7-178F8355834B}" name="Table16" displayName="Table16" ref="A5:J6" totalsRowShown="0">
+  <autoFilter ref="A5:J6" xr:uid="{6C0AACD2-FA3F-4094-92F8-D2B9E23D5ABC}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{58197158-FD57-4F30-A650-67B2263D3800}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{F44FE952-D7BA-4DB1-836A-DD3B50D3F9E3}" name="HP"/>
+    <tableColumn id="3" xr3:uid="{579A554D-FD3C-4BB1-9D51-8697075641A3}" name="MP"/>
+    <tableColumn id="4" xr3:uid="{13D9B90B-E0BA-4850-A6F0-8F28FD71DDCB}" name="ATK"/>
+    <tableColumn id="5" xr3:uid="{0217E9E2-E13B-40B7-9079-429225374577}" name="DEF"/>
+    <tableColumn id="6" xr3:uid="{72ED865C-9977-41E9-BA4A-7DFB0D0A6048}" name="MAT"/>
+    <tableColumn id="7" xr3:uid="{3A2FD57C-060A-462E-8BB9-B06F717E9D20}" name="MDF"/>
+    <tableColumn id="8" xr3:uid="{ED9393EA-F7F9-4661-8D0B-0D9246DDABF8}" name="AGI"/>
+    <tableColumn id="9" xr3:uid="{6F56342F-5442-42CD-8B6C-D98B6D6C0C56}" name="LUK"/>
+    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="8">
+      <calculatedColumnFormula>SUM(Table16[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0489A86C-0040-4142-8D05-11877F6AC5E6}" name="Table131610" displayName="Table131610" ref="A8:I13" totalsRowShown="0">
+  <autoFilter ref="A8:I13" xr:uid="{7BE337CC-37BD-4688-B60D-A66F4420668B}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{71340E4C-6101-4C59-8ED7-689E2AD5A962}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="3">
+      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*63-100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="7">
+      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="2">
+      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="1">
+      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="6">
+      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="5">
+      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="0">
+      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="4">
+      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BACB03CE-1DAD-4E5F-8D00-25D6D07FC945}" name="Table131620" displayName="Table131620" ref="A3:I9" totalsRowShown="0">
+  <autoFilter ref="A3:I9" xr:uid="{A90D1C2A-DBF9-4EEF-ACC2-3DC17C207301}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{BD3505AC-AE6D-4947-A74E-A6C2D68658F1}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="27">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="26">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*15+100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="25">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="24">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="23">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="22">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="21">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="20">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="19" tableBorderDxfId="18">
+  <autoFilter ref="L3:T4" xr:uid="{5D2C3EA8-1297-4C77-AF32-84E50F8232C5}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="16">
+      <calculatedColumnFormula>Table19[Level]*50 + 100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="15">
+      <calculatedColumnFormula>Table19[[#This Row],[Level]]*15+100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="14">
+      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="13">
+      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1 + 15 + 6</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="12">
+      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="11">
+      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 12</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="10">
+      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="9">
+      <calculatedColumnFormula>Table19[Level] + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DE335D90-A9BD-40A2-B9C7-73CA6E6CAB11}" name="Table15" displayName="Table15" ref="A4:J7" totalsRowShown="0">
   <autoFilter ref="A4:J7" xr:uid="{CE759384-ADAA-40BA-B9E0-40CE462A16EC}"/>
   <tableColumns count="10">
@@ -699,7 +893,7 @@
     <tableColumn id="7" xr3:uid="{22216E02-260E-4471-8BB1-4E6E1250BAC9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{DC2670AC-8DF2-47F7-A3F6-EE7896309BC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{749652E2-F6CF-428C-B67C-FD0B1EFCCBBF}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="43">
+    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="44">
       <calculatedColumnFormula>SUM(Table15[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -707,136 +901,34 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{11E951F1-5D13-41C6-A7E5-8F4298DA5463}" name="Table13167" displayName="Table13167" ref="A11:I16" totalsRowShown="0">
   <autoFilter ref="A11:I16" xr:uid="{A1CF627F-8D28-44AD-9A35-411103976FCA}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F14CC326-DE44-48D8-856F-8DCDCFC89CAD}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="42">
+    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="43">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="41">
+    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="42">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="39">
+    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="41">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="40">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="38">
+    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="39">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="37">
+    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="38">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="36">
+    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="37">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="35">
+    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="36">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{60D4A7A8-82BF-4B58-A912-589523D22F05}" name="Table131679" displayName="Table131679" ref="K11:S17" totalsRowShown="0">
-  <autoFilter ref="K11:S17" xr:uid="{EAF9FB6A-F011-40E3-AB2F-E53826722AFB}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{DF3E0800-6EE4-4E1B-BA6F-0194351D6E7C}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="27">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*56.25+100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="34">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*10</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="31">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="30">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="33">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="29">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="28">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="32">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BACB03CE-1DAD-4E5F-8D00-25D6D07FC945}" name="Table131620" displayName="Table131620" ref="A3:I9" totalsRowShown="0">
-  <autoFilter ref="A3:I9" xr:uid="{A90D1C2A-DBF9-4EEF-ACC2-3DC17C207301}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{BD3505AC-AE6D-4947-A74E-A6C2D68658F1}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="18">
-      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="17">
-      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*15+100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="16">
-      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="15">
-      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="11">
-      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="12">
-      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="14">
-      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="13">
-      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="0" tableBorderDxfId="10">
-  <autoFilter ref="L3:T4" xr:uid="{5D2C3EA8-1297-4C77-AF32-84E50F8232C5}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="8">
-      <calculatedColumnFormula>Table19[Level]*50 + 100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="7">
-      <calculatedColumnFormula>Table19[[#This Row],[Level]]*15+100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="6">
-      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="5">
-      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1 + 15 + 6</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="4">
-      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="3">
-      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 12</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="2">
-      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="1">
-      <calculatedColumnFormula>Table19[Level] + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1143,7 +1235,7 @@
   <dimension ref="A2:S13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:J5"/>
+      <selection activeCell="A8" sqref="A8:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1660,6 +1752,660 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FEB1284-A899-416A-A581-E0E1F5719020}">
+  <dimension ref="A2:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <f>SUM(Table16[[#This Row],[HP]:[LUK]])</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <f>Table131610[[#This Row],[Level]]*63-100</f>
+        <v>-37</v>
+      </c>
+      <c r="C9">
+        <f>Table131610[[#This Row],[Level]]*10</f>
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <f>Table131610[[#This Row],[Level]]*1.375+ 15</f>
+        <v>16.375</v>
+      </c>
+      <c r="E9">
+        <f>Table131610[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+      <c r="F9">
+        <f>Table131610[[#This Row],[Level]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f>Table131610[[#This Row],[Level]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <f>Table131610[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+      <c r="I9">
+        <f>Table131610[[#This Row],[Level]]*1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <f>Table131610[[#This Row],[Level]]*63-100</f>
+        <v>530</v>
+      </c>
+      <c r="C10">
+        <f>Table131610[[#This Row],[Level]]*10</f>
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <f>Table131610[[#This Row],[Level]]*1.375+ 15</f>
+        <v>28.75</v>
+      </c>
+      <c r="E10">
+        <f>Table131610[[#This Row],[Level]]*1 + 15</f>
+        <v>25</v>
+      </c>
+      <c r="F10">
+        <f>Table131610[[#This Row],[Level]]*1</f>
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <f>Table131610[[#This Row],[Level]]*1</f>
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <f>Table131610[[#This Row],[Level]]*1 + 15</f>
+        <v>25</v>
+      </c>
+      <c r="I10">
+        <f>Table131610[[#This Row],[Level]]*1</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <f>Table131610[[#This Row],[Level]]*63-100</f>
+        <v>1475</v>
+      </c>
+      <c r="C11">
+        <f>Table131610[[#This Row],[Level]]*10</f>
+        <v>250</v>
+      </c>
+      <c r="D11">
+        <f>Table131610[[#This Row],[Level]]*1.375+ 15</f>
+        <v>49.375</v>
+      </c>
+      <c r="E11">
+        <f>Table131610[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="F11">
+        <f>Table131610[[#This Row],[Level]]*1</f>
+        <v>25</v>
+      </c>
+      <c r="G11">
+        <f>Table131610[[#This Row],[Level]]*1</f>
+        <v>25</v>
+      </c>
+      <c r="H11">
+        <f>Table131610[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="I11">
+        <f>Table131610[[#This Row],[Level]]*1</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <f>Table131610[[#This Row],[Level]]*63-100</f>
+        <v>2105</v>
+      </c>
+      <c r="C12">
+        <f>Table131610[[#This Row],[Level]]*10</f>
+        <v>350</v>
+      </c>
+      <c r="D12">
+        <f>Table131610[[#This Row],[Level]]*1.375+ 15</f>
+        <v>63.125</v>
+      </c>
+      <c r="E12">
+        <f>Table131610[[#This Row],[Level]]*1 + 15</f>
+        <v>50</v>
+      </c>
+      <c r="F12">
+        <f>Table131610[[#This Row],[Level]]*1</f>
+        <v>35</v>
+      </c>
+      <c r="G12">
+        <f>Table131610[[#This Row],[Level]]*1</f>
+        <v>35</v>
+      </c>
+      <c r="H12">
+        <f>Table131610[[#This Row],[Level]]*1 + 15</f>
+        <v>50</v>
+      </c>
+      <c r="I12">
+        <f>Table131610[[#This Row],[Level]]*1</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>99</v>
+      </c>
+      <c r="B13">
+        <f>Table131610[[#This Row],[Level]]*63-100</f>
+        <v>6137</v>
+      </c>
+      <c r="C13">
+        <f>Table131610[[#This Row],[Level]]*10</f>
+        <v>990</v>
+      </c>
+      <c r="D13">
+        <f>Table131610[[#This Row],[Level]]*1.375+ 15</f>
+        <v>151.125</v>
+      </c>
+      <c r="E13">
+        <f>Table131610[[#This Row],[Level]]*1 + 15</f>
+        <v>114</v>
+      </c>
+      <c r="F13">
+        <f>Table131610[[#This Row],[Level]]*1</f>
+        <v>99</v>
+      </c>
+      <c r="G13">
+        <f>Table131610[[#This Row],[Level]]*1</f>
+        <v>99</v>
+      </c>
+      <c r="H13">
+        <f>Table131610[[#This Row],[Level]]*1 + 15</f>
+        <v>114</v>
+      </c>
+      <c r="I13">
+        <f>Table131610[[#This Row],[Level]]*1</f>
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED846686-A238-4174-849F-9F6770BD1F9B}">
+  <dimension ref="A1:T9"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="I1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R3" t="s">
+        <v>7</v>
+      </c>
+      <c r="S3" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
+        <v>150</v>
+      </c>
+      <c r="C4">
+        <f>Table131620[[#This Row],[Level]]*15+100</f>
+        <v>115</v>
+      </c>
+      <c r="D4">
+        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>16.5</v>
+      </c>
+      <c r="G4">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>16.5</v>
+      </c>
+      <c r="H4">
+        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
+        <v>16.25</v>
+      </c>
+      <c r="I4">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+      <c r="L4" s="2">
+        <v>20</v>
+      </c>
+      <c r="M4" s="3">
+        <f>Table19[Level]*50 + 100</f>
+        <v>1100</v>
+      </c>
+      <c r="N4" s="3">
+        <f>Table19[[#This Row],[Level]]*15+100</f>
+        <v>400</v>
+      </c>
+      <c r="O4" s="3">
+        <f>Table19[[#This Row],[Level]]*1+ 15</f>
+        <v>35</v>
+      </c>
+      <c r="P4" s="3">
+        <f>Table19[[#This Row],[Level]]*1 + 15 + 6</f>
+        <v>41</v>
+      </c>
+      <c r="Q4" s="3">
+        <f>Table19[[#This Row],[Level]]*1.5 + 15 + 40</f>
+        <v>85</v>
+      </c>
+      <c r="R4" s="3">
+        <f>Table19[[#This Row],[Level]]*1.5 + 15 + 12</f>
+        <v>57</v>
+      </c>
+      <c r="S4" s="3">
+        <f>Table19[[#This Row],[Level]]*1.25 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="T4" s="4">
+        <f>Table19[Level] + 15</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
+        <v>850</v>
+      </c>
+      <c r="C5">
+        <f>Table131620[[#This Row],[Level]]*15+100</f>
+        <v>325</v>
+      </c>
+      <c r="D5">
+        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>37.5</v>
+      </c>
+      <c r="G5">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>37.5</v>
+      </c>
+      <c r="H5">
+        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
+        <v>33.75</v>
+      </c>
+      <c r="I5">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
+        <v>1350</v>
+      </c>
+      <c r="C6">
+        <f>Table131620[[#This Row],[Level]]*15+100</f>
+        <v>475</v>
+      </c>
+      <c r="D6">
+        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+        <v>40</v>
+      </c>
+      <c r="E6">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>52.5</v>
+      </c>
+      <c r="G6">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>52.5</v>
+      </c>
+      <c r="H6">
+        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+      <c r="I6">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>35</v>
+      </c>
+      <c r="B7">
+        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
+        <v>1850</v>
+      </c>
+      <c r="C7">
+        <f>Table131620[[#This Row],[Level]]*15+100</f>
+        <v>625</v>
+      </c>
+      <c r="D7">
+        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+        <v>50</v>
+      </c>
+      <c r="E7">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>67.5</v>
+      </c>
+      <c r="G7">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>67.5</v>
+      </c>
+      <c r="H7">
+        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
+        <v>58.75</v>
+      </c>
+      <c r="I7">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>99</v>
+      </c>
+      <c r="B8">
+        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
+        <v>5050</v>
+      </c>
+      <c r="C8">
+        <f>Table131620[[#This Row],[Level]]*15+100</f>
+        <v>1585</v>
+      </c>
+      <c r="D8">
+        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+        <v>114</v>
+      </c>
+      <c r="E8">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>114</v>
+      </c>
+      <c r="F8">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>163.5</v>
+      </c>
+      <c r="G8">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>163.5</v>
+      </c>
+      <c r="H8">
+        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
+        <v>138.75</v>
+      </c>
+      <c r="I8">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1">
+        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
+        <v>1100</v>
+      </c>
+      <c r="C9" s="1">
+        <f>Table131620[[#This Row],[Level]]*15+100</f>
+        <v>400</v>
+      </c>
+      <c r="D9" s="1">
+        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+        <v>35</v>
+      </c>
+      <c r="E9" s="1">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>35</v>
+      </c>
+      <c r="F9" s="1">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>45</v>
+      </c>
+      <c r="G9" s="1">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>45</v>
+      </c>
+      <c r="H9" s="1">
+        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="I9" s="1">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>35</v>
+      </c>
+      <c r="K9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4195E475-9F10-4DD8-82F0-E47D9A595A6E}">
   <dimension ref="A2:S17"/>
   <sheetViews>
@@ -2276,350 +3022,4 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED846686-A238-4174-849F-9F6770BD1F9B}">
-  <dimension ref="A1:T9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>5</v>
-      </c>
-      <c r="I1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O3" t="s">
-        <v>4</v>
-      </c>
-      <c r="P3" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R3" t="s">
-        <v>7</v>
-      </c>
-      <c r="S3" t="s">
-        <v>8</v>
-      </c>
-      <c r="T3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
-        <v>150</v>
-      </c>
-      <c r="C4">
-        <f>Table131620[[#This Row],[Level]]*15+100</f>
-        <v>115</v>
-      </c>
-      <c r="D4">
-        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
-        <v>16</v>
-      </c>
-      <c r="E4">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>16</v>
-      </c>
-      <c r="F4">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
-        <v>16.5</v>
-      </c>
-      <c r="G4">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
-        <v>16.5</v>
-      </c>
-      <c r="H4">
-        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
-        <v>16.25</v>
-      </c>
-      <c r="I4">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>16</v>
-      </c>
-      <c r="L4" s="2">
-        <v>20</v>
-      </c>
-      <c r="M4" s="3">
-        <f>Table19[Level]*50 + 100</f>
-        <v>1100</v>
-      </c>
-      <c r="N4" s="3">
-        <f>Table19[[#This Row],[Level]]*15+100</f>
-        <v>400</v>
-      </c>
-      <c r="O4" s="3">
-        <f>Table19[[#This Row],[Level]]*1+ 15</f>
-        <v>35</v>
-      </c>
-      <c r="P4" s="3">
-        <f>Table19[[#This Row],[Level]]*1 + 15 + 6</f>
-        <v>41</v>
-      </c>
-      <c r="Q4" s="3">
-        <f>Table19[[#This Row],[Level]]*1.5 + 15 + 40</f>
-        <v>85</v>
-      </c>
-      <c r="R4" s="3">
-        <f>Table19[[#This Row],[Level]]*1.5 + 15 + 12</f>
-        <v>57</v>
-      </c>
-      <c r="S4" s="3">
-        <f>Table19[[#This Row],[Level]]*1.25 + 15</f>
-        <v>40</v>
-      </c>
-      <c r="T4" s="4">
-        <f>Table19[Level] + 15</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
-        <v>850</v>
-      </c>
-      <c r="C5">
-        <f>Table131620[[#This Row],[Level]]*15+100</f>
-        <v>325</v>
-      </c>
-      <c r="D5">
-        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
-        <v>30</v>
-      </c>
-      <c r="E5">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>30</v>
-      </c>
-      <c r="F5">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
-        <v>37.5</v>
-      </c>
-      <c r="G5">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
-        <v>37.5</v>
-      </c>
-      <c r="H5">
-        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
-        <v>33.75</v>
-      </c>
-      <c r="I5">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>25</v>
-      </c>
-      <c r="B6">
-        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
-        <v>1350</v>
-      </c>
-      <c r="C6">
-        <f>Table131620[[#This Row],[Level]]*15+100</f>
-        <v>475</v>
-      </c>
-      <c r="D6">
-        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
-        <v>40</v>
-      </c>
-      <c r="E6">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>40</v>
-      </c>
-      <c r="F6">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
-        <v>52.5</v>
-      </c>
-      <c r="G6">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
-        <v>52.5</v>
-      </c>
-      <c r="H6">
-        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
-        <v>46.25</v>
-      </c>
-      <c r="I6">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>35</v>
-      </c>
-      <c r="B7">
-        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
-        <v>1850</v>
-      </c>
-      <c r="C7">
-        <f>Table131620[[#This Row],[Level]]*15+100</f>
-        <v>625</v>
-      </c>
-      <c r="D7">
-        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
-        <v>50</v>
-      </c>
-      <c r="E7">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>50</v>
-      </c>
-      <c r="F7">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
-        <v>67.5</v>
-      </c>
-      <c r="G7">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
-        <v>67.5</v>
-      </c>
-      <c r="H7">
-        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
-        <v>58.75</v>
-      </c>
-      <c r="I7">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>99</v>
-      </c>
-      <c r="B8">
-        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
-        <v>5050</v>
-      </c>
-      <c r="C8">
-        <f>Table131620[[#This Row],[Level]]*15+100</f>
-        <v>1585</v>
-      </c>
-      <c r="D8">
-        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
-        <v>114</v>
-      </c>
-      <c r="E8">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>114</v>
-      </c>
-      <c r="F8">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
-        <v>163.5</v>
-      </c>
-      <c r="G8">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
-        <v>163.5</v>
-      </c>
-      <c r="H8">
-        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
-        <v>138.75</v>
-      </c>
-      <c r="I8">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>20</v>
-      </c>
-      <c r="B9" s="1">
-        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
-        <v>1100</v>
-      </c>
-      <c r="C9" s="1">
-        <f>Table131620[[#This Row],[Level]]*15+100</f>
-        <v>400</v>
-      </c>
-      <c r="D9" s="1">
-        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
-        <v>35</v>
-      </c>
-      <c r="E9" s="1">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>35</v>
-      </c>
-      <c r="F9" s="1">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
-        <v>45</v>
-      </c>
-      <c r="G9" s="1">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
-        <v>45</v>
-      </c>
-      <c r="H9" s="1">
-        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
-        <v>40</v>
-      </c>
-      <c r="I9" s="1">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>35</v>
-      </c>
-      <c r="K9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Mostly finished side quest zone
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -9,13 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="2" activeTab="4" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Skeleton Soldier" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
-    <sheet name="VillianCanson" sheetId="4" r:id="rId3"/>
-    <sheet name="Goblin" sheetId="2" r:id="rId4"/>
+    <sheet name="Zombie" sheetId="5" r:id="rId2"/>
+    <sheet name="SpiritPuppet" sheetId="6" r:id="rId3"/>
+    <sheet name="Acolyte" sheetId="7" r:id="rId4"/>
+    <sheet name="Death Knight" sheetId="8" r:id="rId5"/>
+    <sheet name="VillianCanson" sheetId="4" r:id="rId6"/>
+    <sheet name="Goblin" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="35">
   <si>
     <t>Skeletons are the most basic undead, they have low magical attributes, agility, and luck.</t>
   </si>
@@ -102,6 +105,36 @@
   </si>
   <si>
     <t>Zombies are the type of undead made from decomposing corpses. Only uses weapons, can't use armor. Often made from peasants, using shovels</t>
+  </si>
+  <si>
+    <t>These puppets originally were used by Aseran priests as representations of the harvest God</t>
+  </si>
+  <si>
+    <t>Ever since the Empire conquered Asera, the religion was banned and these puppets became rare</t>
+  </si>
+  <si>
+    <t>Somehow, Canson's acolytes have infused these with mana to create constructs that advent the Hell Gods</t>
+  </si>
+  <si>
+    <t>Spirit Puppet</t>
+  </si>
+  <si>
+    <t>Acolytes is a term that refers to an apprentice. It has connotations with necromancy due to lesser hellgod priests appearing with necromancers</t>
+  </si>
+  <si>
+    <t>This acolyte is actually a mage</t>
+  </si>
+  <si>
+    <t>First Encounter. Has tech 2 gear armor and tech 1 staff 28 MAT from staff, 3/10 from engraved robe, 3/2 from studded leather helmet</t>
+  </si>
+  <si>
+    <t>Death Knight</t>
+  </si>
+  <si>
+    <t>Death Knights are top tier undead. Equipped with heavy armor and weapons as well as a powerful base</t>
+  </si>
+  <si>
+    <t>Sidequest: Tech 2 Gear. Iron Spear: 30, Body: 11/11, Helm: 6/2, Heavy Shield: 9/3</t>
   </si>
 </sst>
 </file>
@@ -178,19 +211,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="62">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="99">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -613,6 +634,385 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -647,7 +1047,7 @@
     <tableColumn id="7" xr3:uid="{F9852B29-E77D-4E17-A56E-5F0C649FA862}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{9A914BFF-1060-46E4-B8F9-412BD9293C3D}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2F83B650-811D-4FEE-92D5-03D4DC4376E5}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="61">
+    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="98">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -656,32 +1056,198 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{6BEAD6DA-F1CC-4DB1-9830-FAC45EABEE4E}" name="Table16821" displayName="Table16821" ref="A4:J5" totalsRowShown="0">
+  <autoFilter ref="A4:J5" xr:uid="{0874E50B-9ED5-4CBB-94CE-FE34DD543476}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{D24DE64F-AD99-44F1-A563-00A2EC86C8A5}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{FA1ADA16-085A-4D07-AC3D-BD752AD74C02}" name="HP"/>
+    <tableColumn id="3" xr3:uid="{7603371D-40BD-4E83-877D-566EDA75BB06}" name="MP"/>
+    <tableColumn id="4" xr3:uid="{CAE8D85C-6716-4520-ABE5-F9AEF2B25E8E}" name="ATK"/>
+    <tableColumn id="5" xr3:uid="{245407F3-8672-4D23-8668-D1E8EF177882}" name="DEF"/>
+    <tableColumn id="6" xr3:uid="{CF958570-2481-49F8-81D3-7C212DEE19E7}" name="MAT"/>
+    <tableColumn id="7" xr3:uid="{AEFF5C29-BE6A-4CF8-A2BB-F6B076077DA9}" name="MDF"/>
+    <tableColumn id="8" xr3:uid="{4DE9B01E-67F2-4136-ADC3-60389FB67DCC}" name="AGI"/>
+    <tableColumn id="9" xr3:uid="{F5A82F03-513C-46D4-9F91-470F0060526B}" name="LUK"/>
+    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="16">
+      <calculatedColumnFormula>SUM(Table16821[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="15" tableBorderDxfId="14">
+  <autoFilter ref="A15:I16" xr:uid="{434CBBE2-2F8D-4EEB-895C-68FC850EF1FD}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="12">
+      <calculatedColumnFormula>Table1922[Level]*75 + 500</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="11">
+      <calculatedColumnFormula>Table1922[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BACB03CE-1DAD-4E5F-8D00-25D6D07FC945}" name="Table131620" displayName="Table131620" ref="A3:I9" totalsRowShown="0">
+  <autoFilter ref="A3:I9" xr:uid="{A90D1C2A-DBF9-4EEF-ACC2-3DC17C207301}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{BD3505AC-AE6D-4947-A74E-A6C2D68658F1}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="73">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="72">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*15+100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="71">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="70">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="69">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="68">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="67">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="66">
+      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="65" tableBorderDxfId="64">
+  <autoFilter ref="L3:T4" xr:uid="{5D2C3EA8-1297-4C77-AF32-84E50F8232C5}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="62">
+      <calculatedColumnFormula>Table19[Level]*50 + 100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="61">
+      <calculatedColumnFormula>Table19[[#This Row],[Level]]*15+100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="60">
+      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="59">
+      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1 + 15 + 6</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="58">
+      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="57">
+      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 12</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="56">
+      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="55">
+      <calculatedColumnFormula>Table19[Level] + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DE335D90-A9BD-40A2-B9C7-73CA6E6CAB11}" name="Table15" displayName="Table15" ref="A4:J7" totalsRowShown="0">
+  <autoFilter ref="A4:J7" xr:uid="{CE759384-ADAA-40BA-B9E0-40CE462A16EC}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{DAE2EC63-1D40-4ED3-8C7B-1C8C0375CA6B}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{0BF5F099-BE0D-4349-90FC-65863CB0E17C}" name="HP"/>
+    <tableColumn id="3" xr3:uid="{CCC1BCC5-CFE4-4B8A-8323-673868BD95EF}" name="MP"/>
+    <tableColumn id="4" xr3:uid="{FE1FBFE1-8412-412B-A359-6E322B02EF8B}" name="ATK"/>
+    <tableColumn id="5" xr3:uid="{8DA4C046-05AD-4DAC-A5E6-0889B4BA4F65}" name="DEF"/>
+    <tableColumn id="6" xr3:uid="{90827F4E-7CAE-4259-B6F9-E364498748A0}" name="MAT"/>
+    <tableColumn id="7" xr3:uid="{22216E02-260E-4471-8BB1-4E6E1250BAC9}" name="MDF"/>
+    <tableColumn id="8" xr3:uid="{DC2670AC-8DF2-47F7-A3F6-EE7896309BC9}" name="AGI"/>
+    <tableColumn id="9" xr3:uid="{749652E2-F6CF-428C-B67C-FD0B1EFCCBBF}" name="LUK"/>
+    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="54">
+      <calculatedColumnFormula>SUM(Table15[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{11E951F1-5D13-41C6-A7E5-8F4298DA5463}" name="Table13167" displayName="Table13167" ref="A11:I16" totalsRowShown="0">
+  <autoFilter ref="A11:I16" xr:uid="{A1CF627F-8D28-44AD-9A35-411103976FCA}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{F14CC326-DE44-48D8-856F-8DCDCFC89CAD}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="53">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="52">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="51">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="50">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="49">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="48">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="47">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="46">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{60D4A7A8-82BF-4B58-A912-589523D22F05}" name="Table131679" displayName="Table131679" ref="K11:S17" totalsRowShown="0">
   <autoFilter ref="K11:S17" xr:uid="{EAF9FB6A-F011-40E3-AB2F-E53826722AFB}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DF3E0800-6EE4-4E1B-BA6F-0194351D6E7C}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="35">
+    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="45">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*56.25+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="34">
+    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="44">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="33">
+    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="43">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="32">
+    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="42">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="31">
+    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="41">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="30">
+    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="40">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="29">
+    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="39">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="28">
+    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="38">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -694,28 +1260,28 @@
   <autoFilter ref="A8:I13" xr:uid="{67385006-CBB9-4472-99D4-7881E042769D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FD96F8F7-CCAB-44FA-B525-A5081670706A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="60">
+    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="97">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="59">
+    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="96">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="58">
+    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="95">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="57">
+    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="94">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="56">
+    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="93">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="55">
+    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="92">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="54">
+    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="91">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="53">
+    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="90">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -728,28 +1294,28 @@
   <autoFilter ref="K8:S13" xr:uid="{AB7E938D-7ACC-4BFB-A6B9-682B8B29CEF2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{66EB8EF1-BCF4-44F7-B8A6-3C3B425F8FF5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="52">
+    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="89">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*56.25+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="51">
+    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="88">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="50">
+    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="87">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25+ 15+30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="49">
+    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="86">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25 + 15+33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="48">
+    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="85">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="47">
+    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="84">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="46">
+    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="83">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="45">
+    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="82">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -770,7 +1336,7 @@
     <tableColumn id="7" xr3:uid="{3A2FD57C-060A-462E-8BB9-B06F717E9D20}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{ED9393EA-F7F9-4661-8D0B-0D9246DDABF8}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{6F56342F-5442-42CD-8B6C-D98B6D6C0C56}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="8">
+    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="81">
       <calculatedColumnFormula>SUM(Table16[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -783,28 +1349,28 @@
   <autoFilter ref="A8:I13" xr:uid="{7BE337CC-37BD-4688-B60D-A66F4420668B}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{71340E4C-6101-4C59-8ED7-689E2AD5A962}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="3">
+    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="35">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*63-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="80">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="2">
+    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="79">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="78">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="6">
+    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="77">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="5">
+    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="76">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="75">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="4">
+    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="74">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -813,33 +1379,20 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BACB03CE-1DAD-4E5F-8D00-25D6D07FC945}" name="Table131620" displayName="Table131620" ref="A3:I9" totalsRowShown="0">
-  <autoFilter ref="A3:I9" xr:uid="{A90D1C2A-DBF9-4EEF-ACC2-3DC17C207301}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{BD3505AC-AE6D-4947-A74E-A6C2D68658F1}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="27">
-      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="26">
-      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*15+100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="25">
-      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="24">
-      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="23">
-      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="22">
-      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="21">
-      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="20">
-      <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{0A2DAD7E-8DB8-432C-AD24-4A1116190AFC}" name="Table168" displayName="Table168" ref="A6:J7" totalsRowShown="0">
+  <autoFilter ref="A6:J7" xr:uid="{3F070465-048B-4A60-A5D6-289DD81841E3}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{46422AF1-99B7-4965-8F6A-D256072E575C}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{0A71C80C-CA2E-4E72-9D93-350B3DA84447}" name="HP"/>
+    <tableColumn id="3" xr3:uid="{DF6C3EB9-3A52-40CE-AC4E-B7F04A1EBB64}" name="MP"/>
+    <tableColumn id="4" xr3:uid="{F31DDD26-7F37-4DBC-8236-79185692625B}" name="ATK"/>
+    <tableColumn id="5" xr3:uid="{34BB612C-EF90-4001-865D-C0BBE9DDE35C}" name="DEF"/>
+    <tableColumn id="6" xr3:uid="{3C2ED426-96C6-4371-9F06-FA42D5AE2877}" name="MAT"/>
+    <tableColumn id="7" xr3:uid="{4899BF24-9D2A-4CC0-AE35-4F49604AAC5A}" name="MDF"/>
+    <tableColumn id="8" xr3:uid="{CB1CC6BA-1D38-4B74-9BC6-7057FB9773EE}" name="AGI"/>
+    <tableColumn id="9" xr3:uid="{C47FADF6-C526-4188-9187-383757CE17C1}" name="LUK"/>
+    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="37">
+      <calculatedColumnFormula>SUM(Table168[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -847,33 +1400,33 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="19" tableBorderDxfId="18">
-  <autoFilter ref="L3:T4" xr:uid="{5D2C3EA8-1297-4C77-AF32-84E50F8232C5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{E50ECAD0-74A3-4ED4-B8F9-3CED6CCBE3D4}" name="Table13161013" displayName="Table13161013" ref="A9:I14" totalsRowShown="0">
+  <autoFilter ref="A9:I14" xr:uid="{06A56D17-07E5-4650-8EE9-7EA8F94D4020}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="16">
-      <calculatedColumnFormula>Table19[Level]*50 + 100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="15">
-      <calculatedColumnFormula>Table19[[#This Row],[Level]]*15+100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="14">
-      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="13">
-      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1 + 15 + 6</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="12">
-      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="11">
-      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 12</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="10">
-      <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="9">
-      <calculatedColumnFormula>Table19[Level] + 15</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{A2BE27C9-9DAE-49F5-9A70-C6CF7428BF31}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="34">
+      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="33">
+      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*10+20</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="32">
+      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="36">
+      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="31">
+      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.375+15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="30">
+      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="29">
+      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="28">
+      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -881,20 +1434,33 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DE335D90-A9BD-40A2-B9C7-73CA6E6CAB11}" name="Table15" displayName="Table15" ref="A4:J7" totalsRowShown="0">
-  <autoFilter ref="A4:J7" xr:uid="{CE759384-ADAA-40BA-B9E0-40CE462A16EC}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{DAE2EC63-1D40-4ED3-8C7B-1C8C0375CA6B}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{0BF5F099-BE0D-4349-90FC-65863CB0E17C}" name="HP"/>
-    <tableColumn id="3" xr3:uid="{CCC1BCC5-CFE4-4B8A-8323-673868BD95EF}" name="MP"/>
-    <tableColumn id="4" xr3:uid="{FE1FBFE1-8412-412B-A359-6E322B02EF8B}" name="ATK"/>
-    <tableColumn id="5" xr3:uid="{8DA4C046-05AD-4DAC-A5E6-0889B4BA4F65}" name="DEF"/>
-    <tableColumn id="6" xr3:uid="{90827F4E-7CAE-4259-B6F9-E364498748A0}" name="MAT"/>
-    <tableColumn id="7" xr3:uid="{22216E02-260E-4471-8BB1-4E6E1250BAC9}" name="MDF"/>
-    <tableColumn id="8" xr3:uid="{DC2670AC-8DF2-47F7-A3F6-EE7896309BC9}" name="AGI"/>
-    <tableColumn id="9" xr3:uid="{749652E2-F6CF-428C-B67C-FD0B1EFCCBBF}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="44">
-      <calculatedColumnFormula>SUM(Table15[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{537551B7-B0FC-43E4-9401-043CCFC4A3B0}" name="Table13162015" displayName="Table13162015" ref="A4:I10" totalsRowShown="0">
+  <autoFilter ref="A4:I10" xr:uid="{A1EAC62C-C07D-464E-91B1-4A34E6604BA2}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{430FD3D4-914C-4309-B2E6-6F01B5CAED94}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="27">
+      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="26">
+      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*15+100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="25">
+      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="24">
+      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="23">
+      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="22">
+      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="21">
+      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="20">
+      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -902,33 +1468,33 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{11E951F1-5D13-41C6-A7E5-8F4298DA5463}" name="Table13167" displayName="Table13167" ref="A11:I16" totalsRowShown="0">
-  <autoFilter ref="A11:I16" xr:uid="{A1CF627F-8D28-44AD-9A35-411103976FCA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{F3CEF94F-0A77-45F7-9EF0-B6E7B4DA3B1F}" name="Table131618" displayName="Table131618" ref="A7:I12" totalsRowShown="0">
+  <autoFilter ref="A7:I12" xr:uid="{9BE7336F-352A-4FAE-B0E4-61965FC814C7}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{F14CC326-DE44-48D8-856F-8DCDCFC89CAD}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="43">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="42">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*10</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="41">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="40">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="39">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="38">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="37">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="36">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{B8DA50BB-4379-43D1-879B-CDBE6D82C13A}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="19">
+      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="18">
+      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*10+20</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="4">
+      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="3">
+      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="17">
+      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="2">
+      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="1">
+      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="0">
+      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1235,7 +1801,7 @@
   <dimension ref="A2:S13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:I13"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1755,8 +2321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FEB1284-A899-416A-A581-E0E1F5719020}">
   <dimension ref="A2:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2060,340 +2626,307 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED846686-A238-4174-849F-9F6770BD1F9B}">
-  <dimension ref="A1:T9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9807F697-48C3-4A93-87DF-719DC89F6DFD}">
+  <dimension ref="A2:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F1">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
         <v>5</v>
       </c>
-      <c r="G1">
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
         <v>5</v>
       </c>
-      <c r="I1">
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <f>SUM(Table168[[#This Row],[HP]:[LUK]])</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O3" t="s">
-        <v>4</v>
-      </c>
-      <c r="P3" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R3" t="s">
-        <v>7</v>
-      </c>
-      <c r="S3" t="s">
-        <v>8</v>
-      </c>
-      <c r="T3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
-        <v>150</v>
-      </c>
-      <c r="C4">
-        <f>Table131620[[#This Row],[Level]]*15+100</f>
-        <v>115</v>
-      </c>
-      <c r="D4">
-        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+      <c r="B10">
+        <f>Table13161013[[#This Row],[Level]]*56.25-100</f>
+        <v>-43.75</v>
+      </c>
+      <c r="C10">
+        <f>Table13161013[[#This Row],[Level]]*10+20</f>
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <f>Table13161013[[#This Row],[Level]]*1+ 15</f>
         <v>16</v>
       </c>
-      <c r="E4">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+      <c r="E10">
+        <f>Table13161013[[#This Row],[Level]]*1 + 15</f>
         <v>16</v>
       </c>
-      <c r="F4">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+      <c r="F10">
+        <f>Table13161013[[#This Row],[Level]]*1.375+15</f>
+        <v>16.375</v>
+      </c>
+      <c r="G10">
+        <f>Table13161013[[#This Row],[Level]]*1.5+15</f>
         <v>16.5</v>
       </c>
-      <c r="G4">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+      <c r="H10">
+        <f>Table13161013[[#This Row],[Level]]*1.125 + 15</f>
+        <v>16.125</v>
+      </c>
+      <c r="I10">
+        <f>Table13161013[[#This Row],[Level]]*1.5+15</f>
         <v>16.5</v>
       </c>
-      <c r="H4">
-        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
-        <v>16.25</v>
-      </c>
-      <c r="I4">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>16</v>
-      </c>
-      <c r="L4" s="2">
-        <v>20</v>
-      </c>
-      <c r="M4" s="3">
-        <f>Table19[Level]*50 + 100</f>
-        <v>1100</v>
-      </c>
-      <c r="N4" s="3">
-        <f>Table19[[#This Row],[Level]]*15+100</f>
-        <v>400</v>
-      </c>
-      <c r="O4" s="3">
-        <f>Table19[[#This Row],[Level]]*1+ 15</f>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f>Table13161013[[#This Row],[Level]]*56.25-100</f>
+        <v>462.5</v>
+      </c>
+      <c r="C11">
+        <f>Table13161013[[#This Row],[Level]]*10+20</f>
+        <v>120</v>
+      </c>
+      <c r="D11">
+        <f>Table13161013[[#This Row],[Level]]*1+ 15</f>
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <f>Table13161013[[#This Row],[Level]]*1 + 15</f>
+        <v>25</v>
+      </c>
+      <c r="F11">
+        <f>Table13161013[[#This Row],[Level]]*1.375+15</f>
+        <v>28.75</v>
+      </c>
+      <c r="G11">
+        <f>Table13161013[[#This Row],[Level]]*1.5+15</f>
+        <v>30</v>
+      </c>
+      <c r="H11">
+        <f>Table13161013[[#This Row],[Level]]*1.125 + 15</f>
+        <v>26.25</v>
+      </c>
+      <c r="I11">
+        <f>Table13161013[[#This Row],[Level]]*1.5+15</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <f>Table13161013[[#This Row],[Level]]*56.25-100</f>
+        <v>1306.25</v>
+      </c>
+      <c r="C12">
+        <f>Table13161013[[#This Row],[Level]]*10+20</f>
+        <v>270</v>
+      </c>
+      <c r="D12">
+        <f>Table13161013[[#This Row],[Level]]*1+ 15</f>
+        <v>40</v>
+      </c>
+      <c r="E12">
+        <f>Table13161013[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="F12">
+        <f>Table13161013[[#This Row],[Level]]*1.375+15</f>
+        <v>49.375</v>
+      </c>
+      <c r="G12">
+        <f>Table13161013[[#This Row],[Level]]*1.5+15</f>
+        <v>52.5</v>
+      </c>
+      <c r="H12">
+        <f>Table13161013[[#This Row],[Level]]*1.125 + 15</f>
+        <v>43.125</v>
+      </c>
+      <c r="I12">
+        <f>Table13161013[[#This Row],[Level]]*1.5+15</f>
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>35</v>
       </c>
-      <c r="P4" s="3">
-        <f>Table19[[#This Row],[Level]]*1 + 15 + 6</f>
-        <v>41</v>
-      </c>
-      <c r="Q4" s="3">
-        <f>Table19[[#This Row],[Level]]*1.5 + 15 + 40</f>
-        <v>85</v>
-      </c>
-      <c r="R4" s="3">
-        <f>Table19[[#This Row],[Level]]*1.5 + 15 + 12</f>
-        <v>57</v>
-      </c>
-      <c r="S4" s="3">
-        <f>Table19[[#This Row],[Level]]*1.25 + 15</f>
-        <v>40</v>
-      </c>
-      <c r="T4" s="4">
-        <f>Table19[Level] + 15</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
-        <v>850</v>
-      </c>
-      <c r="C5">
-        <f>Table131620[[#This Row],[Level]]*15+100</f>
-        <v>325</v>
-      </c>
-      <c r="D5">
-        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
-        <v>30</v>
-      </c>
-      <c r="E5">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>30</v>
-      </c>
-      <c r="F5">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
-        <v>37.5</v>
-      </c>
-      <c r="G5">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
-        <v>37.5</v>
-      </c>
-      <c r="H5">
-        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
-        <v>33.75</v>
-      </c>
-      <c r="I5">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>25</v>
-      </c>
-      <c r="B6">
-        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
-        <v>1350</v>
-      </c>
-      <c r="C6">
-        <f>Table131620[[#This Row],[Level]]*15+100</f>
-        <v>475</v>
-      </c>
-      <c r="D6">
-        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
-        <v>40</v>
-      </c>
-      <c r="E6">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>40</v>
-      </c>
-      <c r="F6">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
-        <v>52.5</v>
-      </c>
-      <c r="G6">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
-        <v>52.5</v>
-      </c>
-      <c r="H6">
-        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
-        <v>46.25</v>
-      </c>
-      <c r="I6">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>35</v>
-      </c>
-      <c r="B7">
-        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
-        <v>1850</v>
-      </c>
-      <c r="C7">
-        <f>Table131620[[#This Row],[Level]]*15+100</f>
-        <v>625</v>
-      </c>
-      <c r="D7">
-        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+      <c r="B13">
+        <f>Table13161013[[#This Row],[Level]]*56.25-100</f>
+        <v>1868.75</v>
+      </c>
+      <c r="C13">
+        <f>Table13161013[[#This Row],[Level]]*10+20</f>
+        <v>370</v>
+      </c>
+      <c r="D13">
+        <f>Table13161013[[#This Row],[Level]]*1+ 15</f>
         <v>50</v>
       </c>
-      <c r="E7">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+      <c r="E13">
+        <f>Table13161013[[#This Row],[Level]]*1 + 15</f>
         <v>50</v>
       </c>
-      <c r="F7">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+      <c r="F13">
+        <f>Table13161013[[#This Row],[Level]]*1.375+15</f>
+        <v>63.125</v>
+      </c>
+      <c r="G13">
+        <f>Table13161013[[#This Row],[Level]]*1.5+15</f>
         <v>67.5</v>
       </c>
-      <c r="G7">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+      <c r="H13">
+        <f>Table13161013[[#This Row],[Level]]*1.125 + 15</f>
+        <v>54.375</v>
+      </c>
+      <c r="I13">
+        <f>Table13161013[[#This Row],[Level]]*1.5+15</f>
         <v>67.5</v>
       </c>
-      <c r="H7">
-        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
-        <v>58.75</v>
-      </c>
-      <c r="I7">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>99</v>
       </c>
-      <c r="B8">
-        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
-        <v>5050</v>
-      </c>
-      <c r="C8">
-        <f>Table131620[[#This Row],[Level]]*15+100</f>
-        <v>1585</v>
-      </c>
-      <c r="D8">
-        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+      <c r="B14">
+        <f>Table13161013[[#This Row],[Level]]*56.25-100</f>
+        <v>5468.75</v>
+      </c>
+      <c r="C14">
+        <f>Table13161013[[#This Row],[Level]]*10+20</f>
+        <v>1010</v>
+      </c>
+      <c r="D14">
+        <f>Table13161013[[#This Row],[Level]]*1+ 15</f>
         <v>114</v>
       </c>
-      <c r="E8">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+      <c r="E14">
+        <f>Table13161013[[#This Row],[Level]]*1 + 15</f>
         <v>114</v>
       </c>
-      <c r="F8">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+      <c r="F14">
+        <f>Table13161013[[#This Row],[Level]]*1.375+15</f>
+        <v>151.125</v>
+      </c>
+      <c r="G14">
+        <f>Table13161013[[#This Row],[Level]]*1.5+15</f>
         <v>163.5</v>
       </c>
-      <c r="G8">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+      <c r="H14">
+        <f>Table13161013[[#This Row],[Level]]*1.125 + 15</f>
+        <v>126.375</v>
+      </c>
+      <c r="I14">
+        <f>Table13161013[[#This Row],[Level]]*1.5+15</f>
         <v>163.5</v>
-      </c>
-      <c r="H8">
-        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
-        <v>138.75</v>
-      </c>
-      <c r="I8">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>20</v>
-      </c>
-      <c r="B9" s="1">
-        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
-        <v>1100</v>
-      </c>
-      <c r="C9" s="1">
-        <f>Table131620[[#This Row],[Level]]*15+100</f>
-        <v>400</v>
-      </c>
-      <c r="D9" s="1">
-        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
-        <v>35</v>
-      </c>
-      <c r="E9" s="1">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>35</v>
-      </c>
-      <c r="F9" s="1">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
-        <v>45</v>
-      </c>
-      <c r="G9" s="1">
-        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
-        <v>45</v>
-      </c>
-      <c r="H9" s="1">
-        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
-        <v>40</v>
-      </c>
-      <c r="I9" s="1">
-        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
-        <v>35</v>
-      </c>
-      <c r="K9" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -2406,6 +2939,1005 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA7AE8E-3CBD-43D4-8334-3506A3BDF6FA}">
+  <dimension ref="A2:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <f>Table13162015[[#This Row],[Level]]*50 + 100</f>
+        <v>150</v>
+      </c>
+      <c r="C5">
+        <f>Table13162015[[#This Row],[Level]]*15+100</f>
+        <v>115</v>
+      </c>
+      <c r="D5">
+        <f>Table13162015[[#This Row],[Level]]*1+ 15</f>
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <f>Table13162015[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
+        <v>16.5</v>
+      </c>
+      <c r="G5">
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
+        <v>16.5</v>
+      </c>
+      <c r="H5">
+        <f>Table13162015[[#This Row],[Level]]*1.25 + 15</f>
+        <v>16.25</v>
+      </c>
+      <c r="I5">
+        <f>Table13162015[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <f>Table13162015[[#This Row],[Level]]*50 + 100</f>
+        <v>850</v>
+      </c>
+      <c r="C6">
+        <f>Table13162015[[#This Row],[Level]]*15+100</f>
+        <v>325</v>
+      </c>
+      <c r="D6">
+        <f>Table13162015[[#This Row],[Level]]*1+ 15</f>
+        <v>30</v>
+      </c>
+      <c r="E6">
+        <f>Table13162015[[#This Row],[Level]]*1 + 15</f>
+        <v>30</v>
+      </c>
+      <c r="F6">
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
+        <v>37.5</v>
+      </c>
+      <c r="G6">
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
+        <v>37.5</v>
+      </c>
+      <c r="H6">
+        <f>Table13162015[[#This Row],[Level]]*1.25 + 15</f>
+        <v>33.75</v>
+      </c>
+      <c r="I6">
+        <f>Table13162015[[#This Row],[Level]]*1 + 15</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <f>Table13162015[[#This Row],[Level]]*50 + 100</f>
+        <v>1350</v>
+      </c>
+      <c r="C7">
+        <f>Table13162015[[#This Row],[Level]]*15+100</f>
+        <v>475</v>
+      </c>
+      <c r="D7">
+        <f>Table13162015[[#This Row],[Level]]*1+ 15</f>
+        <v>40</v>
+      </c>
+      <c r="E7">
+        <f>Table13162015[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="F7">
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
+        <v>52.5</v>
+      </c>
+      <c r="G7">
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
+        <v>52.5</v>
+      </c>
+      <c r="H7">
+        <f>Table13162015[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+      <c r="I7">
+        <f>Table13162015[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <f>Table13162015[[#This Row],[Level]]*50 + 100</f>
+        <v>1850</v>
+      </c>
+      <c r="C8">
+        <f>Table13162015[[#This Row],[Level]]*15+100</f>
+        <v>625</v>
+      </c>
+      <c r="D8">
+        <f>Table13162015[[#This Row],[Level]]*1+ 15</f>
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <f>Table13162015[[#This Row],[Level]]*1 + 15</f>
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
+        <v>67.5</v>
+      </c>
+      <c r="G8">
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
+        <v>67.5</v>
+      </c>
+      <c r="H8">
+        <f>Table13162015[[#This Row],[Level]]*1.25 + 15</f>
+        <v>58.75</v>
+      </c>
+      <c r="I8">
+        <f>Table13162015[[#This Row],[Level]]*1 + 15</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>99</v>
+      </c>
+      <c r="B9">
+        <f>Table13162015[[#This Row],[Level]]*50 + 100</f>
+        <v>5050</v>
+      </c>
+      <c r="C9">
+        <f>Table13162015[[#This Row],[Level]]*15+100</f>
+        <v>1585</v>
+      </c>
+      <c r="D9">
+        <f>Table13162015[[#This Row],[Level]]*1+ 15</f>
+        <v>114</v>
+      </c>
+      <c r="E9">
+        <f>Table13162015[[#This Row],[Level]]*1 + 15</f>
+        <v>114</v>
+      </c>
+      <c r="F9">
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
+        <v>163.5</v>
+      </c>
+      <c r="G9">
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
+        <v>163.5</v>
+      </c>
+      <c r="H9">
+        <f>Table13162015[[#This Row],[Level]]*1.25 + 15</f>
+        <v>138.75</v>
+      </c>
+      <c r="I9">
+        <f>Table13162015[[#This Row],[Level]]*1 + 15</f>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1">
+        <f>Table13162015[[#This Row],[Level]]*50 + 100</f>
+        <v>1100</v>
+      </c>
+      <c r="C10" s="1">
+        <f>Table13162015[[#This Row],[Level]]*15+100</f>
+        <v>400</v>
+      </c>
+      <c r="D10" s="1">
+        <f>Table13162015[[#This Row],[Level]]*1+ 15</f>
+        <v>35</v>
+      </c>
+      <c r="E10" s="1">
+        <f>Table13162015[[#This Row],[Level]]*1 + 15</f>
+        <v>35</v>
+      </c>
+      <c r="F10" s="1">
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
+        <v>45</v>
+      </c>
+      <c r="G10" s="1">
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
+        <v>45</v>
+      </c>
+      <c r="H10" s="1">
+        <f>Table13162015[[#This Row],[Level]]*1.25 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="I10" s="1">
+        <f>Table13162015[[#This Row],[Level]]*1 + 15</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CE9C02-0686-4D94-800E-4766BA124417}">
+  <dimension ref="A2:J16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <f>SUM(Table16821[[#This Row],[HP]:[LUK]])</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <f>Table131618[[#This Row],[Level]]*75 + 500</f>
+        <v>575</v>
+      </c>
+      <c r="C8">
+        <f>Table131618[[#This Row],[Level]]*10+20</f>
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <f>Table131618[[#This Row],[Level]]*1.5+ 15</f>
+        <v>16.5</v>
+      </c>
+      <c r="E8">
+        <f>Table131618[[#This Row],[Level]]*1.5 + 15</f>
+        <v>16.5</v>
+      </c>
+      <c r="F8">
+        <f>Table131618[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+      <c r="G8">
+        <f>Table131618[[#This Row],[Level]]*1.5 + 15</f>
+        <v>16.5</v>
+      </c>
+      <c r="H8">
+        <f>Table131618[[#This Row],[Level]]*1.375 + 15</f>
+        <v>16.375</v>
+      </c>
+      <c r="I8">
+        <f>Table131618[[#This Row],[Level]]*1.125 + 15</f>
+        <v>16.125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <f>Table131618[[#This Row],[Level]]*75 + 500</f>
+        <v>1625</v>
+      </c>
+      <c r="C9">
+        <f>Table131618[[#This Row],[Level]]*10+20</f>
+        <v>170</v>
+      </c>
+      <c r="D9">
+        <f>Table131618[[#This Row],[Level]]*1.5+ 15</f>
+        <v>37.5</v>
+      </c>
+      <c r="E9">
+        <f>Table131618[[#This Row],[Level]]*1.5 + 15</f>
+        <v>37.5</v>
+      </c>
+      <c r="F9">
+        <f>Table131618[[#This Row],[Level]]*1 + 15</f>
+        <v>30</v>
+      </c>
+      <c r="G9">
+        <f>Table131618[[#This Row],[Level]]*1.5 + 15</f>
+        <v>37.5</v>
+      </c>
+      <c r="H9">
+        <f>Table131618[[#This Row],[Level]]*1.375 + 15</f>
+        <v>35.625</v>
+      </c>
+      <c r="I9">
+        <f>Table131618[[#This Row],[Level]]*1.125 + 15</f>
+        <v>31.875</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <f>Table131618[[#This Row],[Level]]*75 + 500</f>
+        <v>2375</v>
+      </c>
+      <c r="C10">
+        <f>Table131618[[#This Row],[Level]]*10+20</f>
+        <v>270</v>
+      </c>
+      <c r="D10">
+        <f>Table131618[[#This Row],[Level]]*1.5+ 15</f>
+        <v>52.5</v>
+      </c>
+      <c r="E10">
+        <f>Table131618[[#This Row],[Level]]*1.5 + 15</f>
+        <v>52.5</v>
+      </c>
+      <c r="F10">
+        <f>Table131618[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="G10">
+        <f>Table131618[[#This Row],[Level]]*1.5 + 15</f>
+        <v>52.5</v>
+      </c>
+      <c r="H10">
+        <f>Table131618[[#This Row],[Level]]*1.375 + 15</f>
+        <v>49.375</v>
+      </c>
+      <c r="I10">
+        <f>Table131618[[#This Row],[Level]]*1.125 + 15</f>
+        <v>43.125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>35</v>
+      </c>
+      <c r="B11">
+        <f>Table131618[[#This Row],[Level]]*75 + 500</f>
+        <v>3125</v>
+      </c>
+      <c r="C11">
+        <f>Table131618[[#This Row],[Level]]*10+20</f>
+        <v>370</v>
+      </c>
+      <c r="D11">
+        <f>Table131618[[#This Row],[Level]]*1.5+ 15</f>
+        <v>67.5</v>
+      </c>
+      <c r="E11">
+        <f>Table131618[[#This Row],[Level]]*1.5 + 15</f>
+        <v>67.5</v>
+      </c>
+      <c r="F11">
+        <f>Table131618[[#This Row],[Level]]*1 + 15</f>
+        <v>50</v>
+      </c>
+      <c r="G11">
+        <f>Table131618[[#This Row],[Level]]*1.5 + 15</f>
+        <v>67.5</v>
+      </c>
+      <c r="H11">
+        <f>Table131618[[#This Row],[Level]]*1.375 + 15</f>
+        <v>63.125</v>
+      </c>
+      <c r="I11">
+        <f>Table131618[[#This Row],[Level]]*1.125 + 15</f>
+        <v>54.375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <f>Table131618[[#This Row],[Level]]*75 + 500</f>
+        <v>2000</v>
+      </c>
+      <c r="C12">
+        <f>Table131618[[#This Row],[Level]]*10+20</f>
+        <v>220</v>
+      </c>
+      <c r="D12">
+        <f>Table131618[[#This Row],[Level]]*1.5+ 15</f>
+        <v>45</v>
+      </c>
+      <c r="E12">
+        <f>Table131618[[#This Row],[Level]]*1.5 + 15</f>
+        <v>45</v>
+      </c>
+      <c r="F12">
+        <f>Table131618[[#This Row],[Level]]*1 + 15</f>
+        <v>35</v>
+      </c>
+      <c r="G12">
+        <f>Table131618[[#This Row],[Level]]*1.5 + 15</f>
+        <v>45</v>
+      </c>
+      <c r="H12">
+        <f>Table131618[[#This Row],[Level]]*1.375 + 15</f>
+        <v>42.5</v>
+      </c>
+      <c r="I12">
+        <f>Table131618[[#This Row],[Level]]*1.125 + 15</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>20</v>
+      </c>
+      <c r="B16" s="3">
+        <f>Table1922[Level]*75 + 500</f>
+        <v>2000</v>
+      </c>
+      <c r="C16" s="3">
+        <f>Table1922[[#This Row],[Level]]*10 + 20</f>
+        <v>220</v>
+      </c>
+      <c r="D16" s="3">
+        <v>75</v>
+      </c>
+      <c r="E16" s="3">
+        <v>71</v>
+      </c>
+      <c r="F16" s="3">
+        <v>35</v>
+      </c>
+      <c r="G16" s="3">
+        <v>61</v>
+      </c>
+      <c r="H16" s="3">
+        <v>42.5</v>
+      </c>
+      <c r="I16" s="4">
+        <v>37.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED846686-A238-4174-849F-9F6770BD1F9B}">
+  <dimension ref="A1:T9"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:T4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="I1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R3" t="s">
+        <v>7</v>
+      </c>
+      <c r="S3" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
+        <v>150</v>
+      </c>
+      <c r="C4">
+        <f>Table131620[[#This Row],[Level]]*15+100</f>
+        <v>115</v>
+      </c>
+      <c r="D4">
+        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>16.5</v>
+      </c>
+      <c r="G4">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>16.5</v>
+      </c>
+      <c r="H4">
+        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
+        <v>16.25</v>
+      </c>
+      <c r="I4">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+      <c r="L4" s="2">
+        <v>20</v>
+      </c>
+      <c r="M4" s="3">
+        <f>Table19[Level]*50 + 100</f>
+        <v>1100</v>
+      </c>
+      <c r="N4" s="3">
+        <f>Table19[[#This Row],[Level]]*15+100</f>
+        <v>400</v>
+      </c>
+      <c r="O4" s="3">
+        <f>Table19[[#This Row],[Level]]*1+ 15</f>
+        <v>35</v>
+      </c>
+      <c r="P4" s="3">
+        <f>Table19[[#This Row],[Level]]*1 + 15 + 6</f>
+        <v>41</v>
+      </c>
+      <c r="Q4" s="3">
+        <f>Table19[[#This Row],[Level]]*1.5 + 15 + 40</f>
+        <v>85</v>
+      </c>
+      <c r="R4" s="3">
+        <f>Table19[[#This Row],[Level]]*1.5 + 15 + 12</f>
+        <v>57</v>
+      </c>
+      <c r="S4" s="3">
+        <f>Table19[[#This Row],[Level]]*1.25 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="T4" s="4">
+        <f>Table19[Level] + 15</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
+        <v>850</v>
+      </c>
+      <c r="C5">
+        <f>Table131620[[#This Row],[Level]]*15+100</f>
+        <v>325</v>
+      </c>
+      <c r="D5">
+        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>37.5</v>
+      </c>
+      <c r="G5">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>37.5</v>
+      </c>
+      <c r="H5">
+        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
+        <v>33.75</v>
+      </c>
+      <c r="I5">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
+        <v>1350</v>
+      </c>
+      <c r="C6">
+        <f>Table131620[[#This Row],[Level]]*15+100</f>
+        <v>475</v>
+      </c>
+      <c r="D6">
+        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+        <v>40</v>
+      </c>
+      <c r="E6">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>52.5</v>
+      </c>
+      <c r="G6">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>52.5</v>
+      </c>
+      <c r="H6">
+        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+      <c r="I6">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>35</v>
+      </c>
+      <c r="B7">
+        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
+        <v>1850</v>
+      </c>
+      <c r="C7">
+        <f>Table131620[[#This Row],[Level]]*15+100</f>
+        <v>625</v>
+      </c>
+      <c r="D7">
+        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+        <v>50</v>
+      </c>
+      <c r="E7">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>67.5</v>
+      </c>
+      <c r="G7">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>67.5</v>
+      </c>
+      <c r="H7">
+        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
+        <v>58.75</v>
+      </c>
+      <c r="I7">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>99</v>
+      </c>
+      <c r="B8">
+        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
+        <v>5050</v>
+      </c>
+      <c r="C8">
+        <f>Table131620[[#This Row],[Level]]*15+100</f>
+        <v>1585</v>
+      </c>
+      <c r="D8">
+        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+        <v>114</v>
+      </c>
+      <c r="E8">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>114</v>
+      </c>
+      <c r="F8">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>163.5</v>
+      </c>
+      <c r="G8">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>163.5</v>
+      </c>
+      <c r="H8">
+        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
+        <v>138.75</v>
+      </c>
+      <c r="I8">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1">
+        <f>Table131620[[#This Row],[Level]]*50 + 100</f>
+        <v>1100</v>
+      </c>
+      <c r="C9" s="1">
+        <f>Table131620[[#This Row],[Level]]*15+100</f>
+        <v>400</v>
+      </c>
+      <c r="D9" s="1">
+        <f>Table131620[[#This Row],[Level]]*1+ 15</f>
+        <v>35</v>
+      </c>
+      <c r="E9" s="1">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>35</v>
+      </c>
+      <c r="F9" s="1">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>45</v>
+      </c>
+      <c r="G9" s="1">
+        <f>Table131620[[#This Row],[Level]]*1.5 + 15</f>
+        <v>45</v>
+      </c>
+      <c r="H9" s="1">
+        <f>Table131620[[#This Row],[Level]]*1.25 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="I9" s="1">
+        <f>Table131620[[#This Row],[Level]]*1 + 15</f>
+        <v>35</v>
+      </c>
+      <c r="K9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4195E475-9F10-4DD8-82F0-E47D9A595A6E}">
   <dimension ref="A2:S17"/>
   <sheetViews>

</xml_diff>

<commit_message>
Finished Sidezones 1 and 2. Thinking about class quests in town
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="2" activeTab="4" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="2" activeTab="6" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Skeleton Soldier" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="40">
   <si>
     <t>Skeletons are the most basic undead, they have low magical attributes, agility, and luck.</t>
   </si>
@@ -136,6 +136,21 @@
   <si>
     <t>Sidequest: Tech 2 Gear. Iron Spear: 30, Body: 11/11, Helm: 6/2, Heavy Shield: 9/3</t>
   </si>
+  <si>
+    <t>Goblin Grunt</t>
+  </si>
+  <si>
+    <t>Goblin Grunts use crude iron daggers, crude shield, crude mail, and crude helmets</t>
+  </si>
+  <si>
+    <t>25atk/5agi, 17def/16mdf</t>
+  </si>
+  <si>
+    <t>Goblin Shaman use their divine powers to heal and curse enemies</t>
+  </si>
+  <si>
+    <t>They use a 2-handed faith light balanced armor: 40 Faith, 14/13</t>
+  </si>
 </sst>
 </file>
 
@@ -211,7 +226,91 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="99">
+  <dxfs count="115">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -541,99 +640,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1021,6 +1027,63 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1047,7 +1110,7 @@
     <tableColumn id="7" xr3:uid="{F9852B29-E77D-4E17-A56E-5F0C649FA862}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{9A914BFF-1060-46E4-B8F9-412BD9293C3D}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2F83B650-811D-4FEE-92D5-03D4DC4376E5}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="98">
+    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="114">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1068,7 +1131,7 @@
     <tableColumn id="7" xr3:uid="{AEFF5C29-BE6A-4CF8-A2BB-F6B076077DA9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{4DE9B01E-67F2-4136-ADC3-60389FB67DCC}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{F5A82F03-513C-46D4-9F91-470F0060526B}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="16">
+    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="63">
       <calculatedColumnFormula>SUM(Table16821[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1077,22 +1140,22 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="15" tableBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="62" tableBorderDxfId="61">
   <autoFilter ref="A15:I16" xr:uid="{434CBBE2-2F8D-4EEB-895C-68FC850EF1FD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="59">
       <calculatedColumnFormula>Table1922[Level]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="11">
+    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="58">
       <calculatedColumnFormula>Table1922[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="55"/>
+    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="54"/>
+    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="53"/>
+    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1103,28 +1166,28 @@
   <autoFilter ref="A3:I9" xr:uid="{A90D1C2A-DBF9-4EEF-ACC2-3DC17C207301}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BD3505AC-AE6D-4947-A74E-A6C2D68658F1}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="73">
+    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="51">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="72">
+    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="50">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="71">
+    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="49">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="70">
+    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="48">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="69">
+    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="47">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="68">
+    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="46">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="67">
+    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="45">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="66">
+    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="44">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1133,32 +1196,32 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="65" tableBorderDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="43" tableBorderDxfId="42">
   <autoFilter ref="L3:T4" xr:uid="{5D2C3EA8-1297-4C77-AF32-84E50F8232C5}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="62">
+    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="40">
       <calculatedColumnFormula>Table19[Level]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="61">
+    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="39">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="60">
+    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="38">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="59">
+    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="37">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1 + 15 + 6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="58">
+    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="36">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="57">
+    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="35">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="56">
+    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="34">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="55">
+    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="33">
       <calculatedColumnFormula>Table19[Level] + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1167,8 +1230,8 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DE335D90-A9BD-40A2-B9C7-73CA6E6CAB11}" name="Table15" displayName="Table15" ref="A4:J7" totalsRowShown="0">
-  <autoFilter ref="A4:J7" xr:uid="{CE759384-ADAA-40BA-B9E0-40CE462A16EC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DE335D90-A9BD-40A2-B9C7-73CA6E6CAB11}" name="Table15" displayName="Table15" ref="A4:J8" totalsRowShown="0">
+  <autoFilter ref="A4:J8" xr:uid="{CE759384-ADAA-40BA-B9E0-40CE462A16EC}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{DAE2EC63-1D40-4ED3-8C7B-1C8C0375CA6B}" name="Name"/>
     <tableColumn id="2" xr3:uid="{0BF5F099-BE0D-4349-90FC-65863CB0E17C}" name="HP"/>
@@ -1179,7 +1242,7 @@
     <tableColumn id="7" xr3:uid="{22216E02-260E-4471-8BB1-4E6E1250BAC9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{DC2670AC-8DF2-47F7-A3F6-EE7896309BC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{749652E2-F6CF-428C-B67C-FD0B1EFCCBBF}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="54">
+    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="32">
       <calculatedColumnFormula>SUM(Table15[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1188,32 +1251,32 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{11E951F1-5D13-41C6-A7E5-8F4298DA5463}" name="Table13167" displayName="Table13167" ref="A11:I16" totalsRowShown="0">
-  <autoFilter ref="A11:I16" xr:uid="{A1CF627F-8D28-44AD-9A35-411103976FCA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{11E951F1-5D13-41C6-A7E5-8F4298DA5463}" name="Table13167" displayName="Table13167" ref="A15:I20" totalsRowShown="0">
+  <autoFilter ref="A15:I20" xr:uid="{A1CF627F-8D28-44AD-9A35-411103976FCA}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F14CC326-DE44-48D8-856F-8DCDCFC89CAD}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="53">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="52">
+    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="31">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*63-100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="30">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="51">
+    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="29">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="50">
+    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="28">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="27">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="26">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="25">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="49">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="48">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="47">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="46">
+    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="24">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1226,29 +1289,97 @@
   <autoFilter ref="K11:S17" xr:uid="{EAF9FB6A-F011-40E3-AB2F-E53826722AFB}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DF3E0800-6EE4-4E1B-BA6F-0194351D6E7C}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="45">
+    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="23">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*56.25+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="44">
+    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="22">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="43">
+    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="21">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="42">
+    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="20">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="41">
+    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="19">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="40">
+    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="18">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="39">
+    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="17">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="38">
+    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="16">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{57801F89-51BE-4BC1-9BA3-39DF9D564857}" name="Table1316717" displayName="Table1316717" ref="A26:I31" totalsRowShown="0">
+  <autoFilter ref="A26:I31" xr:uid="{870F76F2-5EA7-4FD7-B1F9-507D64592088}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{3C04B742-338A-4366-BF3D-C5BC13023785}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="15">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*63+100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="14">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="7">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="6">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="13">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="12">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="11">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="10">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6BE19079-7252-4251-9EA9-046E7A11042F}" name="Table13167173" displayName="Table13167173" ref="A36:I41" totalsRowShown="0">
+  <autoFilter ref="A36:I41" xr:uid="{9BD043AF-0D77-4FF4-B2F9-B4AC3C3F1F82}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{7BB908A3-05D7-4357-920B-BF4C6BC20C06}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="3">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*56.5+200</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="8">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*12.5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="5">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="0">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1 + 15+14</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="4">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="1">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.5+ 15+13</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="9">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="2">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.375 + 15+40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1260,28 +1391,28 @@
   <autoFilter ref="A8:I13" xr:uid="{67385006-CBB9-4472-99D4-7881E042769D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FD96F8F7-CCAB-44FA-B525-A5081670706A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="97">
+    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="113">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="96">
+    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="112">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="95">
+    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="111">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="94">
+    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="110">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="93">
+    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="109">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="92">
+    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="108">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="91">
+    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="107">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="90">
+    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="106">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1294,28 +1425,28 @@
   <autoFilter ref="K8:S13" xr:uid="{AB7E938D-7ACC-4BFB-A6B9-682B8B29CEF2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{66EB8EF1-BCF4-44F7-B8A6-3C3B425F8FF5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="89">
+    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="105">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*56.25+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="88">
+    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="104">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="87">
+    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="103">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25+ 15+30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="86">
+    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="102">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25 + 15+33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="85">
+    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="101">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="84">
+    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="100">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="83">
+    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="99">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="82">
+    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="98">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1336,7 +1467,7 @@
     <tableColumn id="7" xr3:uid="{3A2FD57C-060A-462E-8BB9-B06F717E9D20}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{ED9393EA-F7F9-4661-8D0B-0D9246DDABF8}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{6F56342F-5442-42CD-8B6C-D98B6D6C0C56}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="81">
+    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="97">
       <calculatedColumnFormula>SUM(Table16[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1349,28 +1480,28 @@
   <autoFilter ref="A8:I13" xr:uid="{7BE337CC-37BD-4688-B60D-A66F4420668B}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{71340E4C-6101-4C59-8ED7-689E2AD5A962}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="35">
+    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="96">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*63-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="80">
+    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="95">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="79">
+    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="94">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="78">
+    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="93">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="77">
+    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="92">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="76">
+    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="91">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="75">
+    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="90">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="74">
+    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="89">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1391,7 +1522,7 @@
     <tableColumn id="7" xr3:uid="{4899BF24-9D2A-4CC0-AE35-4F49604AAC5A}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{CB1CC6BA-1D38-4B74-9BC6-7057FB9773EE}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{C47FADF6-C526-4188-9187-383757CE17C1}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="37">
+    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="88">
       <calculatedColumnFormula>SUM(Table168[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1404,28 +1535,28 @@
   <autoFilter ref="A9:I14" xr:uid="{06A56D17-07E5-4650-8EE9-7EA8F94D4020}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A2BE27C9-9DAE-49F5-9A70-C6CF7428BF31}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="34">
+    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="87">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="33">
+    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="86">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="32">
+    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="85">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="36">
+    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="84">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="31">
+    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="83">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.375+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="30">
+    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="82">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="29">
+    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="81">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="28">
+    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="80">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1438,28 +1569,28 @@
   <autoFilter ref="A4:I10" xr:uid="{A1EAC62C-C07D-464E-91B1-4A34E6604BA2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{430FD3D4-914C-4309-B2E6-6F01B5CAED94}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="27">
+    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="79">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="26">
+    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="78">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="25">
+    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="77">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="24">
+    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="76">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="23">
+    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="75">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="22">
+    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="74">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="21">
+    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="73">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="20">
+    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="72">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1472,28 +1603,28 @@
   <autoFilter ref="A7:I12" xr:uid="{9BE7336F-352A-4FAE-B0E4-61965FC814C7}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B8DA50BB-4379-43D1-879B-CDBE6D82C13A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="19">
+    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="71">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="18">
+    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="70">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="69">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="68">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="17">
+    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="67">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="66">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="65">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="64">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2630,7 +2761,7 @@
   <dimension ref="A2:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:J7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3226,8 +3357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CE9C02-0686-4D94-800E-4766BA124417}">
   <dimension ref="A2:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3596,7 +3727,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:T4"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3939,10 +4070,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4195E475-9F10-4DD8-82F0-E47D9A595A6E}">
-  <dimension ref="A2:S17"/>
+  <dimension ref="A2:S41"/>
   <sheetViews>
-    <sheetView topLeftCell="J7" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4058,69 +4189,65 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
         <v>2</v>
       </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
-      </c>
       <c r="G7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H7">
         <v>3</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J7" s="1">
         <f>SUM(Table15[[#This Row],[HP]:[LUK]])</f>
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1">
+        <f>SUM(Table15[[#This Row],[HP]:[LUK]])</f>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" t="s">
-        <v>9</v>
-      </c>
       <c r="K11" t="s">
         <v>12</v>
       </c>
@@ -4150,41 +4277,6 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12">
-        <f>Table13167[[#This Row],[Level]]*56.25-100</f>
-        <v>-43.75</v>
-      </c>
-      <c r="C12">
-        <f>Table13167[[#This Row],[Level]]*10</f>
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <f>Table13167[[#This Row],[Level]]*1.375+ 15</f>
-        <v>16.375</v>
-      </c>
-      <c r="E12">
-        <f>Table13167[[#This Row],[Level]]*1.25 + 15</f>
-        <v>16.25</v>
-      </c>
-      <c r="F12">
-        <f>Table13167[[#This Row],[Level]]*1 + 15</f>
-        <v>16</v>
-      </c>
-      <c r="G12">
-        <f>Table13167[[#This Row],[Level]]*1.25+ 15</f>
-        <v>16.25</v>
-      </c>
-      <c r="H12">
-        <f>Table13167[[#This Row],[Level]]*1.5 + 15</f>
-        <v>16.5</v>
-      </c>
-      <c r="I12">
-        <f>Table13167[[#This Row],[Level]]*1.125 + 15</f>
-        <v>16.125</v>
-      </c>
       <c r="K12">
         <v>1</v>
       </c>
@@ -4222,40 +4314,8 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <f>Table13167[[#This Row],[Level]]*56.25-100</f>
-        <v>462.5</v>
-      </c>
-      <c r="C13">
-        <f>Table13167[[#This Row],[Level]]*10</f>
-        <v>100</v>
-      </c>
-      <c r="D13">
-        <f>Table13167[[#This Row],[Level]]*1.375+ 15</f>
-        <v>28.75</v>
-      </c>
-      <c r="E13">
-        <f>Table13167[[#This Row],[Level]]*1.25 + 15</f>
-        <v>27.5</v>
-      </c>
-      <c r="F13">
-        <f>Table13167[[#This Row],[Level]]*1 + 15</f>
-        <v>25</v>
-      </c>
-      <c r="G13">
-        <f>Table13167[[#This Row],[Level]]*1.25+ 15</f>
-        <v>27.5</v>
-      </c>
-      <c r="H13">
-        <f>Table13167[[#This Row],[Level]]*1.5 + 15</f>
-        <v>30</v>
-      </c>
-      <c r="I13">
-        <f>Table13167[[#This Row],[Level]]*1.125 + 15</f>
-        <v>26.25</v>
+      <c r="A13" t="s">
+        <v>19</v>
       </c>
       <c r="K13">
         <v>10</v>
@@ -4294,40 +4354,8 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>25</v>
-      </c>
-      <c r="B14">
-        <f>Table13167[[#This Row],[Level]]*56.25-100</f>
-        <v>1306.25</v>
-      </c>
-      <c r="C14">
-        <f>Table13167[[#This Row],[Level]]*10</f>
-        <v>250</v>
-      </c>
-      <c r="D14">
-        <f>Table13167[[#This Row],[Level]]*1.375+ 15</f>
-        <v>49.375</v>
-      </c>
-      <c r="E14">
-        <f>Table13167[[#This Row],[Level]]*1.25 + 15</f>
-        <v>46.25</v>
-      </c>
-      <c r="F14">
-        <f>Table13167[[#This Row],[Level]]*1 + 15</f>
-        <v>40</v>
-      </c>
-      <c r="G14">
-        <f>Table13167[[#This Row],[Level]]*1.25+ 15</f>
-        <v>46.25</v>
-      </c>
-      <c r="H14">
-        <f>Table13167[[#This Row],[Level]]*1.5 + 15</f>
-        <v>52.5</v>
-      </c>
-      <c r="I14">
-        <f>Table13167[[#This Row],[Level]]*1.125 + 15</f>
-        <v>43.125</v>
+      <c r="A14" t="s">
+        <v>20</v>
       </c>
       <c r="K14">
         <v>25</v>
@@ -4366,40 +4394,32 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>35</v>
-      </c>
-      <c r="B15">
-        <f>Table13167[[#This Row],[Level]]*56.25-100</f>
-        <v>1868.75</v>
-      </c>
-      <c r="C15">
-        <f>Table13167[[#This Row],[Level]]*10</f>
-        <v>350</v>
-      </c>
-      <c r="D15">
-        <f>Table13167[[#This Row],[Level]]*1.375+ 15</f>
-        <v>63.125</v>
-      </c>
-      <c r="E15">
-        <f>Table13167[[#This Row],[Level]]*1.25 + 15</f>
-        <v>58.75</v>
-      </c>
-      <c r="F15">
-        <f>Table13167[[#This Row],[Level]]*1 + 15</f>
-        <v>50</v>
-      </c>
-      <c r="G15">
-        <f>Table13167[[#This Row],[Level]]*1.25+ 15</f>
-        <v>58.75</v>
-      </c>
-      <c r="H15">
-        <f>Table13167[[#This Row],[Level]]*1.5 + 15</f>
-        <v>67.5</v>
-      </c>
-      <c r="I15">
-        <f>Table13167[[#This Row],[Level]]*1.125 + 15</f>
-        <v>54.375</v>
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" t="s">
+        <v>9</v>
       </c>
       <c r="K15">
         <v>35</v>
@@ -4439,39 +4459,39 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="B16">
-        <f>Table13167[[#This Row],[Level]]*56.25-100</f>
-        <v>5468.75</v>
+        <f>Table13167[[#This Row],[Level]]*63-100</f>
+        <v>-37</v>
       </c>
       <c r="C16">
         <f>Table13167[[#This Row],[Level]]*10</f>
-        <v>990</v>
+        <v>10</v>
       </c>
       <c r="D16">
         <f>Table13167[[#This Row],[Level]]*1.375+ 15</f>
-        <v>151.125</v>
+        <v>16.375</v>
       </c>
       <c r="E16">
-        <f>Table13167[[#This Row],[Level]]*1.25 + 15</f>
-        <v>138.75</v>
+        <f>Table13167[[#This Row],[Level]]*1.375 + 15</f>
+        <v>16.375</v>
       </c>
       <c r="F16">
         <f>Table13167[[#This Row],[Level]]*1 + 15</f>
-        <v>114</v>
+        <v>16</v>
       </c>
       <c r="G16">
         <f>Table13167[[#This Row],[Level]]*1.25+ 15</f>
-        <v>138.75</v>
+        <v>16.25</v>
       </c>
       <c r="H16">
-        <f>Table13167[[#This Row],[Level]]*1.5 + 15</f>
-        <v>163.5</v>
+        <f>Table13167[[#This Row],[Level]]*1.25 + 15</f>
+        <v>16.25</v>
       </c>
       <c r="I16">
         <f>Table13167[[#This Row],[Level]]*1.125 + 15</f>
-        <v>126.375</v>
+        <v>16.125</v>
       </c>
       <c r="K16">
         <v>99</v>
@@ -4509,7 +4529,42 @@
         <v>126.375</v>
       </c>
     </row>
-    <row r="17" spans="11:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <f>Table13167[[#This Row],[Level]]*63</f>
+        <v>630</v>
+      </c>
+      <c r="C17">
+        <f>Table13167[[#This Row],[Level]]*10</f>
+        <v>100</v>
+      </c>
+      <c r="D17">
+        <f>Table13167[[#This Row],[Level]]*1.375+ 15</f>
+        <v>28.75</v>
+      </c>
+      <c r="E17">
+        <f>Table13167[[#This Row],[Level]]*1.375 + 15</f>
+        <v>28.75</v>
+      </c>
+      <c r="F17">
+        <f>Table13167[[#This Row],[Level]]*1 + 15</f>
+        <v>25</v>
+      </c>
+      <c r="G17">
+        <f>Table13167[[#This Row],[Level]]*1.25+ 15</f>
+        <v>27.5</v>
+      </c>
+      <c r="H17">
+        <f>Table13167[[#This Row],[Level]]*1.25 + 15</f>
+        <v>27.5</v>
+      </c>
+      <c r="I17">
+        <f>Table13167[[#This Row],[Level]]*1.125 + 15</f>
+        <v>26.25</v>
+      </c>
       <c r="K17">
         <v>3</v>
       </c>
@@ -4546,12 +4601,573 @@
         <v>18.375</v>
       </c>
     </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <f>Table13167[[#This Row],[Level]]*63-100</f>
+        <v>1475</v>
+      </c>
+      <c r="C18">
+        <f>Table13167[[#This Row],[Level]]*10</f>
+        <v>250</v>
+      </c>
+      <c r="D18">
+        <f>Table13167[[#This Row],[Level]]*1.375+ 15</f>
+        <v>49.375</v>
+      </c>
+      <c r="E18">
+        <f>Table13167[[#This Row],[Level]]*1.375 + 15</f>
+        <v>49.375</v>
+      </c>
+      <c r="F18">
+        <f>Table13167[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="G18">
+        <f>Table13167[[#This Row],[Level]]*1.25+ 15</f>
+        <v>46.25</v>
+      </c>
+      <c r="H18">
+        <f>Table13167[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+      <c r="I18">
+        <f>Table13167[[#This Row],[Level]]*1.125 + 15</f>
+        <v>43.125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>35</v>
+      </c>
+      <c r="B19">
+        <f>Table13167[[#This Row],[Level]]*63-100</f>
+        <v>2105</v>
+      </c>
+      <c r="C19">
+        <f>Table13167[[#This Row],[Level]]*10</f>
+        <v>350</v>
+      </c>
+      <c r="D19">
+        <f>Table13167[[#This Row],[Level]]*1.375+ 15</f>
+        <v>63.125</v>
+      </c>
+      <c r="E19">
+        <f>Table13167[[#This Row],[Level]]*1.375 + 15</f>
+        <v>63.125</v>
+      </c>
+      <c r="F19">
+        <f>Table13167[[#This Row],[Level]]*1 + 15</f>
+        <v>50</v>
+      </c>
+      <c r="G19">
+        <f>Table13167[[#This Row],[Level]]*1.25+ 15</f>
+        <v>58.75</v>
+      </c>
+      <c r="H19">
+        <f>Table13167[[#This Row],[Level]]*1.25 + 15</f>
+        <v>58.75</v>
+      </c>
+      <c r="I19">
+        <f>Table13167[[#This Row],[Level]]*1.125 + 15</f>
+        <v>54.375</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>99</v>
+      </c>
+      <c r="B20">
+        <f>Table13167[[#This Row],[Level]]*63-100</f>
+        <v>6137</v>
+      </c>
+      <c r="C20">
+        <f>Table13167[[#This Row],[Level]]*10</f>
+        <v>990</v>
+      </c>
+      <c r="D20">
+        <f>Table13167[[#This Row],[Level]]*1.375+ 15</f>
+        <v>151.125</v>
+      </c>
+      <c r="E20">
+        <f>Table13167[[#This Row],[Level]]*1.375 + 15</f>
+        <v>151.125</v>
+      </c>
+      <c r="F20">
+        <f>Table13167[[#This Row],[Level]]*1 + 15</f>
+        <v>114</v>
+      </c>
+      <c r="G20">
+        <f>Table13167[[#This Row],[Level]]*1.25+ 15</f>
+        <v>138.75</v>
+      </c>
+      <c r="H20">
+        <f>Table13167[[#This Row],[Level]]*1.25 + 15</f>
+        <v>138.75</v>
+      </c>
+      <c r="I20">
+        <f>Table13167[[#This Row],[Level]]*1.125 + 15</f>
+        <v>126.375</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <f>Table1316717[[#This Row],[Level]]*63+100</f>
+        <v>163</v>
+      </c>
+      <c r="C27">
+        <f>Table1316717[[#This Row],[Level]]*10</f>
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <f>Table1316717[[#This Row],[Level]]*1.375+ 15</f>
+        <v>16.375</v>
+      </c>
+      <c r="E27">
+        <f>Table1316717[[#This Row],[Level]]*1.375 + 15</f>
+        <v>16.375</v>
+      </c>
+      <c r="F27">
+        <f>Table1316717[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+      <c r="G27">
+        <f>Table1316717[[#This Row],[Level]]*1.25+ 15</f>
+        <v>16.25</v>
+      </c>
+      <c r="H27">
+        <f>Table1316717[[#This Row],[Level]]*1.25 + 15</f>
+        <v>16.25</v>
+      </c>
+      <c r="I27">
+        <f>Table1316717[[#This Row],[Level]]*1.125 + 15</f>
+        <v>16.125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <f>Table1316717[[#This Row],[Level]]*63+100</f>
+        <v>730</v>
+      </c>
+      <c r="C28">
+        <f>Table1316717[[#This Row],[Level]]*10</f>
+        <v>100</v>
+      </c>
+      <c r="D28">
+        <f>Table1316717[[#This Row],[Level]]*1.375+ 15</f>
+        <v>28.75</v>
+      </c>
+      <c r="E28">
+        <f>Table1316717[[#This Row],[Level]]*1.375 + 15</f>
+        <v>28.75</v>
+      </c>
+      <c r="F28">
+        <f>Table1316717[[#This Row],[Level]]*1 + 15</f>
+        <v>25</v>
+      </c>
+      <c r="G28">
+        <f>Table1316717[[#This Row],[Level]]*1.25+ 15</f>
+        <v>27.5</v>
+      </c>
+      <c r="H28">
+        <f>Table1316717[[#This Row],[Level]]*1.25 + 15</f>
+        <v>27.5</v>
+      </c>
+      <c r="I28">
+        <f>Table1316717[[#This Row],[Level]]*1.125 + 15</f>
+        <v>26.25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <f>Table1316717[[#This Row],[Level]]*63+100</f>
+        <v>1675</v>
+      </c>
+      <c r="C29">
+        <f>Table1316717[[#This Row],[Level]]*10</f>
+        <v>250</v>
+      </c>
+      <c r="D29">
+        <f>Table1316717[[#This Row],[Level]]*1.375+ 15</f>
+        <v>49.375</v>
+      </c>
+      <c r="E29">
+        <f>Table1316717[[#This Row],[Level]]*1.375 + 15</f>
+        <v>49.375</v>
+      </c>
+      <c r="F29">
+        <f>Table1316717[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="G29">
+        <f>Table1316717[[#This Row],[Level]]*1.25+ 15</f>
+        <v>46.25</v>
+      </c>
+      <c r="H29">
+        <f>Table1316717[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+      <c r="I29">
+        <f>Table1316717[[#This Row],[Level]]*1.125 + 15</f>
+        <v>43.125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>35</v>
+      </c>
+      <c r="B30">
+        <f>Table1316717[[#This Row],[Level]]*63+100</f>
+        <v>2305</v>
+      </c>
+      <c r="C30">
+        <f>Table1316717[[#This Row],[Level]]*10</f>
+        <v>350</v>
+      </c>
+      <c r="D30">
+        <f>Table1316717[[#This Row],[Level]]*1.375+ 15</f>
+        <v>63.125</v>
+      </c>
+      <c r="E30">
+        <f>Table1316717[[#This Row],[Level]]*1.375 + 15</f>
+        <v>63.125</v>
+      </c>
+      <c r="F30">
+        <f>Table1316717[[#This Row],[Level]]*1 + 15</f>
+        <v>50</v>
+      </c>
+      <c r="G30">
+        <f>Table1316717[[#This Row],[Level]]*1.25+ 15</f>
+        <v>58.75</v>
+      </c>
+      <c r="H30">
+        <f>Table1316717[[#This Row],[Level]]*1.25 + 15</f>
+        <v>58.75</v>
+      </c>
+      <c r="I30">
+        <f>Table1316717[[#This Row],[Level]]*1.125 + 15</f>
+        <v>54.375</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>99</v>
+      </c>
+      <c r="B31">
+        <f>Table1316717[[#This Row],[Level]]*63+100</f>
+        <v>6337</v>
+      </c>
+      <c r="C31">
+        <f>Table1316717[[#This Row],[Level]]*10</f>
+        <v>990</v>
+      </c>
+      <c r="D31">
+        <f>Table1316717[[#This Row],[Level]]*1.375+ 15</f>
+        <v>151.125</v>
+      </c>
+      <c r="E31">
+        <f>Table1316717[[#This Row],[Level]]*1.375 + 15</f>
+        <v>151.125</v>
+      </c>
+      <c r="F31">
+        <f>Table1316717[[#This Row],[Level]]*1 + 15</f>
+        <v>114</v>
+      </c>
+      <c r="G31">
+        <f>Table1316717[[#This Row],[Level]]*1.25+ 15</f>
+        <v>138.75</v>
+      </c>
+      <c r="H31">
+        <f>Table1316717[[#This Row],[Level]]*1.25 + 15</f>
+        <v>138.75</v>
+      </c>
+      <c r="I31">
+        <f>Table1316717[[#This Row],[Level]]*1.125 + 15</f>
+        <v>126.375</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>5</v>
+      </c>
+      <c r="F36" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" t="s">
+        <v>8</v>
+      </c>
+      <c r="I36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <f>Table13167173[[#This Row],[Level]]*56.5+200</f>
+        <v>256.5</v>
+      </c>
+      <c r="C37">
+        <f>Table13167173[[#This Row],[Level]]*12.5</f>
+        <v>12.5</v>
+      </c>
+      <c r="D37">
+        <f>Table13167173[[#This Row],[Level]]*1+ 15</f>
+        <v>16</v>
+      </c>
+      <c r="E37">
+        <f>Table13167173[[#This Row],[Level]]*1 + 15+14</f>
+        <v>30</v>
+      </c>
+      <c r="F37">
+        <f>Table13167173[[#This Row],[Level]]*1.125 + 15</f>
+        <v>16.125</v>
+      </c>
+      <c r="G37">
+        <f>Table13167173[[#This Row],[Level]]*1.5+ 15+13</f>
+        <v>29.5</v>
+      </c>
+      <c r="H37">
+        <f>Table13167173[[#This Row],[Level]]*1.25 + 15</f>
+        <v>16.25</v>
+      </c>
+      <c r="I37">
+        <f>Table13167173[[#This Row],[Level]]*1.375 + 15+40</f>
+        <v>56.375</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>10</v>
+      </c>
+      <c r="B38">
+        <f>Table13167173[[#This Row],[Level]]*56.5+200</f>
+        <v>765</v>
+      </c>
+      <c r="C38">
+        <f>Table13167173[[#This Row],[Level]]*12.5+100</f>
+        <v>225</v>
+      </c>
+      <c r="D38">
+        <f>Table13167173[[#This Row],[Level]]*1+ 15</f>
+        <v>25</v>
+      </c>
+      <c r="E38">
+        <f>Table13167173[[#This Row],[Level]]*1 + 15+14</f>
+        <v>39</v>
+      </c>
+      <c r="F38">
+        <f>Table13167173[[#This Row],[Level]]*1.125 + 15</f>
+        <v>26.25</v>
+      </c>
+      <c r="G38">
+        <f>Table13167173[[#This Row],[Level]]*1.5+ 15+13</f>
+        <v>43</v>
+      </c>
+      <c r="H38">
+        <f>Table13167173[[#This Row],[Level]]*1.25 + 15</f>
+        <v>27.5</v>
+      </c>
+      <c r="I38">
+        <f>Table13167173[[#This Row],[Level]]*1.375 + 15+40</f>
+        <v>68.75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>25</v>
+      </c>
+      <c r="B39">
+        <f>Table13167173[[#This Row],[Level]]*56.5+200</f>
+        <v>1612.5</v>
+      </c>
+      <c r="C39">
+        <f>Table13167173[[#This Row],[Level]]*12.5</f>
+        <v>312.5</v>
+      </c>
+      <c r="D39">
+        <f>Table13167173[[#This Row],[Level]]*1+ 15</f>
+        <v>40</v>
+      </c>
+      <c r="E39">
+        <f>Table13167173[[#This Row],[Level]]*1 + 15+14</f>
+        <v>54</v>
+      </c>
+      <c r="F39">
+        <f>Table13167173[[#This Row],[Level]]*1.125 + 15</f>
+        <v>43.125</v>
+      </c>
+      <c r="G39">
+        <f>Table13167173[[#This Row],[Level]]*1.5+ 15+13</f>
+        <v>65.5</v>
+      </c>
+      <c r="H39">
+        <f>Table13167173[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+      <c r="I39">
+        <f>Table13167173[[#This Row],[Level]]*1.375 + 15+40</f>
+        <v>89.375</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>35</v>
+      </c>
+      <c r="B40">
+        <f>Table13167173[[#This Row],[Level]]*56.5+200</f>
+        <v>2177.5</v>
+      </c>
+      <c r="C40">
+        <f>Table13167173[[#This Row],[Level]]*12.5</f>
+        <v>437.5</v>
+      </c>
+      <c r="D40">
+        <f>Table13167173[[#This Row],[Level]]*1+ 15</f>
+        <v>50</v>
+      </c>
+      <c r="E40">
+        <f>Table13167173[[#This Row],[Level]]*1 + 15+14</f>
+        <v>64</v>
+      </c>
+      <c r="F40">
+        <f>Table13167173[[#This Row],[Level]]*1.125 + 15</f>
+        <v>54.375</v>
+      </c>
+      <c r="G40">
+        <f>Table13167173[[#This Row],[Level]]*1.5+ 15+13</f>
+        <v>80.5</v>
+      </c>
+      <c r="H40">
+        <f>Table13167173[[#This Row],[Level]]*1.25 + 15</f>
+        <v>58.75</v>
+      </c>
+      <c r="I40">
+        <f>Table13167173[[#This Row],[Level]]*1.375 + 15+40</f>
+        <v>103.125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>20</v>
+      </c>
+      <c r="B41">
+        <f>Table13167173[[#This Row],[Level]]*56.5+200</f>
+        <v>1330</v>
+      </c>
+      <c r="C41">
+        <f>Table13167173[[#This Row],[Level]]*12.5</f>
+        <v>250</v>
+      </c>
+      <c r="D41">
+        <f>Table13167173[[#This Row],[Level]]*1+ 15</f>
+        <v>35</v>
+      </c>
+      <c r="E41">
+        <f>Table13167173[[#This Row],[Level]]*1 + 15+14</f>
+        <v>49</v>
+      </c>
+      <c r="F41">
+        <f>Table13167173[[#This Row],[Level]]*1.125 + 15</f>
+        <v>37.5</v>
+      </c>
+      <c r="G41">
+        <f>Table13167173[[#This Row],[Level]]*1.5+ 15+13</f>
+        <v>58</v>
+      </c>
+      <c r="H41">
+        <f>Table13167173[[#This Row],[Level]]*1.25 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="I41">
+        <f>Table13167173[[#This Row],[Level]]*1.375 + 15+40</f>
+        <v>82.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="3">
+  <tableParts count="5">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished Fort Reon exterior, working on first floor, deciding on 3 skills for the skill quests in basement
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -9,16 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="2" activeTab="6" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Skeleton Soldier" sheetId="1" r:id="rId1"/>
-    <sheet name="Zombie" sheetId="5" r:id="rId2"/>
-    <sheet name="SpiritPuppet" sheetId="6" r:id="rId3"/>
-    <sheet name="Acolyte" sheetId="7" r:id="rId4"/>
-    <sheet name="Death Knight" sheetId="8" r:id="rId5"/>
-    <sheet name="VillianCanson" sheetId="4" r:id="rId6"/>
-    <sheet name="Goblin" sheetId="2" r:id="rId7"/>
+    <sheet name="Skeleton Swordsman" sheetId="9" r:id="rId2"/>
+    <sheet name="Skeleton Mage" sheetId="10" r:id="rId3"/>
+    <sheet name="Zombie" sheetId="5" r:id="rId4"/>
+    <sheet name="SpiritPuppet" sheetId="6" r:id="rId5"/>
+    <sheet name="Acolyte" sheetId="7" r:id="rId6"/>
+    <sheet name="Death Knight" sheetId="8" r:id="rId7"/>
+    <sheet name="VillianCanson" sheetId="4" r:id="rId8"/>
+    <sheet name="Goblin" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="44">
   <si>
     <t>Skeletons are the most basic undead, they have low magical attributes, agility, and luck.</t>
   </si>
@@ -151,6 +153,18 @@
   <si>
     <t>They use a 2-handed faith light balanced armor: 40 Faith, 14/13</t>
   </si>
+  <si>
+    <t>Skeleton Swordsmans are a more advanced type of undead than skeleton soldiers</t>
+  </si>
+  <si>
+    <t>2handed sword: 40, Heavy iron plate -&gt; (no shield) 21/7</t>
+  </si>
+  <si>
+    <t>Skeleton mages are a high tier undead that are capable of gathering mana, an extreme rarity amongst golems. Important for logistics of an undead army</t>
+  </si>
+  <si>
+    <t>2handed staff: 40, Heavy iron plate -&gt; (no shield) 4/14</t>
+  </si>
 </sst>
 </file>
 
@@ -226,7 +240,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="115">
+  <dxfs count="133">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1084,6 +1128,30 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1110,7 +1178,7 @@
     <tableColumn id="7" xr3:uid="{F9852B29-E77D-4E17-A56E-5F0C649FA862}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{9A914BFF-1060-46E4-B8F9-412BD9293C3D}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2F83B650-811D-4FEE-92D5-03D4DC4376E5}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="114">
+    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="132">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1119,6 +1187,129 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{0A2DAD7E-8DB8-432C-AD24-4A1116190AFC}" name="Table168" displayName="Table168" ref="A6:J7" totalsRowShown="0">
+  <autoFilter ref="A6:J7" xr:uid="{3F070465-048B-4A60-A5D6-289DD81841E3}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{46422AF1-99B7-4965-8F6A-D256072E575C}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{0A71C80C-CA2E-4E72-9D93-350B3DA84447}" name="HP"/>
+    <tableColumn id="3" xr3:uid="{DF6C3EB9-3A52-40CE-AC4E-B7F04A1EBB64}" name="MP"/>
+    <tableColumn id="4" xr3:uid="{F31DDD26-7F37-4DBC-8236-79185692625B}" name="ATK"/>
+    <tableColumn id="5" xr3:uid="{34BB612C-EF90-4001-865D-C0BBE9DDE35C}" name="DEF"/>
+    <tableColumn id="6" xr3:uid="{3C2ED426-96C6-4371-9F06-FA42D5AE2877}" name="MAT"/>
+    <tableColumn id="7" xr3:uid="{4899BF24-9D2A-4CC0-AE35-4F49604AAC5A}" name="MDF"/>
+    <tableColumn id="8" xr3:uid="{CB1CC6BA-1D38-4B74-9BC6-7057FB9773EE}" name="AGI"/>
+    <tableColumn id="9" xr3:uid="{C47FADF6-C526-4188-9187-383757CE17C1}" name="LUK"/>
+    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="98">
+      <calculatedColumnFormula>SUM(Table168[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{E50ECAD0-74A3-4ED4-B8F9-3CED6CCBE3D4}" name="Table13161013" displayName="Table13161013" ref="A9:I15" totalsRowShown="0">
+  <autoFilter ref="A9:I15" xr:uid="{06A56D17-07E5-4650-8EE9-7EA8F94D4020}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{A2BE27C9-9DAE-49F5-9A70-C6CF7428BF31}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="97">
+      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="96">
+      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*10+20</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="95">
+      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="94">
+      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="93">
+      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.375+15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="92">
+      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="91">
+      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="90">
+      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{537551B7-B0FC-43E4-9401-043CCFC4A3B0}" name="Table13162015" displayName="Table13162015" ref="A4:I10" totalsRowShown="0">
+  <autoFilter ref="A4:I10" xr:uid="{A1EAC62C-C07D-464E-91B1-4A34E6604BA2}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{430FD3D4-914C-4309-B2E6-6F01B5CAED94}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="89">
+      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="88">
+      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*15+100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="87">
+      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="86">
+      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="85">
+      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="84">
+      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="83">
+      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="82">
+      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{F3CEF94F-0A77-45F7-9EF0-B6E7B4DA3B1F}" name="Table131618" displayName="Table131618" ref="A7:I12" totalsRowShown="0">
+  <autoFilter ref="A7:I12" xr:uid="{9BE7336F-352A-4FAE-B0E4-61965FC814C7}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{B8DA50BB-4379-43D1-879B-CDBE6D82C13A}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="81">
+      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="80">
+      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*10+20</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="79">
+      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="78">
+      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="77">
+      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="76">
+      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="75">
+      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="74">
+      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{6BEAD6DA-F1CC-4DB1-9830-FAC45EABEE4E}" name="Table16821" displayName="Table16821" ref="A4:J5" totalsRowShown="0">
   <autoFilter ref="A4:J5" xr:uid="{0874E50B-9ED5-4CBB-94CE-FE34DD543476}"/>
   <tableColumns count="10">
@@ -1131,7 +1322,7 @@
     <tableColumn id="7" xr3:uid="{AEFF5C29-BE6A-4CF8-A2BB-F6B076077DA9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{4DE9B01E-67F2-4136-ADC3-60389FB67DCC}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{F5A82F03-513C-46D4-9F91-470F0060526B}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="63">
+    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="73">
       <calculatedColumnFormula>SUM(Table16821[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1139,55 +1330,55 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="62" tableBorderDxfId="61">
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="72" tableBorderDxfId="71">
   <autoFilter ref="A15:I16" xr:uid="{434CBBE2-2F8D-4EEB-895C-68FC850EF1FD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="59">
+    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="69">
       <calculatedColumnFormula>Table1922[Level]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="58">
+    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="68">
       <calculatedColumnFormula>Table1922[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="55"/>
-    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="54"/>
-    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="53"/>
-    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="63"/>
+    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BACB03CE-1DAD-4E5F-8D00-25D6D07FC945}" name="Table131620" displayName="Table131620" ref="A3:I9" totalsRowShown="0">
   <autoFilter ref="A3:I9" xr:uid="{A90D1C2A-DBF9-4EEF-ACC2-3DC17C207301}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BD3505AC-AE6D-4947-A74E-A6C2D68658F1}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="51">
+    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="61">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="50">
+    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="60">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="49">
+    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="59">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="48">
+    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="58">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="47">
+    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="57">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="46">
+    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="56">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="45">
+    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="55">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="44">
+    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="54">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1195,33 +1386,33 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="43" tableBorderDxfId="42">
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="53" tableBorderDxfId="52">
   <autoFilter ref="L3:T4" xr:uid="{5D2C3EA8-1297-4C77-AF32-84E50F8232C5}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="40">
+    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="50">
       <calculatedColumnFormula>Table19[Level]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="39">
+    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="49">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="38">
+    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="48">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="37">
+    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="47">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1 + 15 + 6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="36">
+    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="46">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="35">
+    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="45">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="34">
+    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="44">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="33">
+    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="43">
       <calculatedColumnFormula>Table19[Level] + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1229,7 +1420,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DE335D90-A9BD-40A2-B9C7-73CA6E6CAB11}" name="Table15" displayName="Table15" ref="A4:J8" totalsRowShown="0">
   <autoFilter ref="A4:J8" xr:uid="{CE759384-ADAA-40BA-B9E0-40CE462A16EC}"/>
   <tableColumns count="10">
@@ -1242,7 +1433,7 @@
     <tableColumn id="7" xr3:uid="{22216E02-260E-4471-8BB1-4E6E1250BAC9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{DC2670AC-8DF2-47F7-A3F6-EE7896309BC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{749652E2-F6CF-428C-B67C-FD0B1EFCCBBF}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="32">
+    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="42">
       <calculatedColumnFormula>SUM(Table15[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1250,136 +1441,34 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{11E951F1-5D13-41C6-A7E5-8F4298DA5463}" name="Table13167" displayName="Table13167" ref="A15:I20" totalsRowShown="0">
   <autoFilter ref="A15:I20" xr:uid="{A1CF627F-8D28-44AD-9A35-411103976FCA}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F14CC326-DE44-48D8-856F-8DCDCFC89CAD}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="31">
+    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="41">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*63-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="30">
+    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="40">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="29">
+    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="39">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="28">
+    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="38">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="27">
+    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="37">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="26">
+    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="36">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="25">
+    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="35">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="24">
+    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="34">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{60D4A7A8-82BF-4B58-A912-589523D22F05}" name="Table131679" displayName="Table131679" ref="K11:S17" totalsRowShown="0">
-  <autoFilter ref="K11:S17" xr:uid="{EAF9FB6A-F011-40E3-AB2F-E53826722AFB}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{DF3E0800-6EE4-4E1B-BA6F-0194351D6E7C}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="23">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*56.25+100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="22">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*10</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="21">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="20">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="19">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="18">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="17">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="16">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{57801F89-51BE-4BC1-9BA3-39DF9D564857}" name="Table1316717" displayName="Table1316717" ref="A26:I31" totalsRowShown="0">
-  <autoFilter ref="A26:I31" xr:uid="{870F76F2-5EA7-4FD7-B1F9-507D64592088}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{3C04B742-338A-4366-BF3D-C5BC13023785}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="15">
-      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*63+100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="14">
-      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*10</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="7">
-      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="6">
-      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="13">
-      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="12">
-      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="11">
-      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="10">
-      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6BE19079-7252-4251-9EA9-046E7A11042F}" name="Table13167173" displayName="Table13167173" ref="A36:I41" totalsRowShown="0">
-  <autoFilter ref="A36:I41" xr:uid="{9BD043AF-0D77-4FF4-B2F9-B4AC3C3F1F82}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{7BB908A3-05D7-4357-920B-BF4C6BC20C06}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="3">
-      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*56.5+200</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="8">
-      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*12.5</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="5">
-      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="0">
-      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1 + 15+14</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="4">
-      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="1">
-      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.5+ 15+13</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="9">
-      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="2">
-      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.375 + 15+40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1391,29 +1480,131 @@
   <autoFilter ref="A8:I13" xr:uid="{67385006-CBB9-4472-99D4-7881E042769D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FD96F8F7-CCAB-44FA-B525-A5081670706A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="113">
+    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="131">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="112">
+    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="130">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="111">
+    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="129">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="110">
+    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="128">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="109">
+    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="127">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="108">
+    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="126">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="107">
+    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="125">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="106">
+    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="124">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{60D4A7A8-82BF-4B58-A912-589523D22F05}" name="Table131679" displayName="Table131679" ref="K11:S17" totalsRowShown="0">
+  <autoFilter ref="K11:S17" xr:uid="{EAF9FB6A-F011-40E3-AB2F-E53826722AFB}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{DF3E0800-6EE4-4E1B-BA6F-0194351D6E7C}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="33">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*56.25+100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="32">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="31">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="30">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="29">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="28">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="27">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="26">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{57801F89-51BE-4BC1-9BA3-39DF9D564857}" name="Table1316717" displayName="Table1316717" ref="A26:I31" totalsRowShown="0">
+  <autoFilter ref="A26:I31" xr:uid="{870F76F2-5EA7-4FD7-B1F9-507D64592088}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{3C04B742-338A-4366-BF3D-C5BC13023785}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="25">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*63+100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="24">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="23">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="22">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="21">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="20">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="19">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="18">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6BE19079-7252-4251-9EA9-046E7A11042F}" name="Table13167173" displayName="Table13167173" ref="A36:I41" totalsRowShown="0">
+  <autoFilter ref="A36:I41" xr:uid="{9BD043AF-0D77-4FF4-B2F9-B4AC3C3F1F82}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{7BB908A3-05D7-4357-920B-BF4C6BC20C06}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="17">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*56.5+200</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="16">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*12.5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="15">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="14">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1 + 15+14</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="13">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="12">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.5+ 15+13</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="11">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="10">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.375 + 15+40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1421,32 +1612,32 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{7268DD6D-84F4-43D7-A05F-EB56AE11DFF7}" name="Table131611" displayName="Table131611" ref="K8:S13" totalsRowShown="0">
-  <autoFilter ref="K8:S13" xr:uid="{AB7E938D-7ACC-4BFB-A6B9-682B8B29CEF2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{7268DD6D-84F4-43D7-A05F-EB56AE11DFF7}" name="Table131611" displayName="Table131611" ref="K8:S14" totalsRowShown="0">
+  <autoFilter ref="K8:S14" xr:uid="{AB7E938D-7ACC-4BFB-A6B9-682B8B29CEF2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{66EB8EF1-BCF4-44F7-B8A6-3C3B425F8FF5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="105">
+    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="123">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*56.25+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="104">
+    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="122">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="103">
+    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="121">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25+ 15+30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="102">
+    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="120">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25 + 15+33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="101">
+    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="119">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="100">
-      <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="99">
+    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="118">
+      <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1+15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="117">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="98">
+    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="116">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1455,6 +1646,116 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{FD9E665F-9A0B-404A-95E4-EDBB03CAF48D}" name="Table114" displayName="Table114" ref="A4:J5" totalsRowShown="0">
+  <autoFilter ref="A4:J5" xr:uid="{E9278F13-379F-448A-A51E-94066E7C03F7}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{5FC81D18-62EF-448A-9E55-8A9C52D43090}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{0E78CA4E-A74F-419A-9E47-7AE45C542639}" name="HP"/>
+    <tableColumn id="3" xr3:uid="{95DB8F2F-7F57-4056-AD97-739982489212}" name="MP"/>
+    <tableColumn id="4" xr3:uid="{EE075CA3-304F-4DCB-AB35-0B55B867F191}" name="ATK"/>
+    <tableColumn id="5" xr3:uid="{FD5AB016-A5A2-4D6F-B6CB-B99FE33534FF}" name="DEF"/>
+    <tableColumn id="6" xr3:uid="{C2B0F5C0-8020-4DE8-8CAF-E2EF237A54C7}" name="MAT"/>
+    <tableColumn id="7" xr3:uid="{F833922A-76F9-427C-8462-D94DE51D0477}" name="MDF"/>
+    <tableColumn id="8" xr3:uid="{203171A1-C88B-4F81-ADC2-1EE072D645F3}" name="AGI"/>
+    <tableColumn id="9" xr3:uid="{34003EF6-E9A5-4584-A186-09DFF4EC11C7}" name="LUK"/>
+    <tableColumn id="10" xr3:uid="{C4602156-F897-42BE-8F3F-411E13EEB095}" name="Total" dataDxfId="115">
+      <calculatedColumnFormula>SUM(Table114[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{244DE9F1-262D-4253-A743-41598B2E31D8}" name="Table13161123" displayName="Table13161123" ref="A8:I14" totalsRowShown="0">
+  <autoFilter ref="A8:I14" xr:uid="{D3C3F418-ED32-4504-9D73-88545A192967}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{13E0AF4A-AA83-489A-A156-B01D4F48D2F5}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{B970139F-8BB5-4CE6-92F8-79E3236AC62B}" name="HP" dataDxfId="9">
+      <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*63+300</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{7BCF83B8-7492-4991-A008-F212725940B9}" name="MP" dataDxfId="114">
+      <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{33220A80-38D8-4480-ACC7-DF484072C96B}" name="ATK" dataDxfId="113">
+      <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.5+ 15+40</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{36708515-5004-4705-A558-44B59D0CE676}" name="DEF" dataDxfId="112">
+      <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25 + 15+21</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{11729EA3-08C4-4E0B-B5EE-5B3C08A31A9C}" name="MAT" dataDxfId="111">
+      <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{B179D090-E484-4663-937A-480D1164D655}" name="MDF" dataDxfId="110">
+      <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25+15 + 7</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{28323AD0-B3BD-401F-A237-92C8B8D70FEA}" name="AGI" dataDxfId="109">
+      <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{657BED8B-4C8A-42DC-BECD-5EEF9D1B7F37}" name="LUK" dataDxfId="108">
+      <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{C6DB90FA-47BB-4001-850B-2E17AF4D6004}" name="Table11412" displayName="Table11412" ref="A4:J5" totalsRowShown="0">
+  <autoFilter ref="A4:J5" xr:uid="{DFE1AD4A-B881-42F7-AAE6-39AE9A965177}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{E4B7B88D-C722-46AF-A0B0-1626D101562F}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{66DF6FD9-5382-4400-BDCD-999E4BAAD10E}" name="HP"/>
+    <tableColumn id="3" xr3:uid="{51EB43B9-01BB-4061-9E8A-340E86516E96}" name="MP"/>
+    <tableColumn id="4" xr3:uid="{C1B55568-DE47-4E09-8DF1-04C8D85529DC}" name="ATK"/>
+    <tableColumn id="5" xr3:uid="{B6CC6D9E-EACE-49C0-97AE-A601A0EC3165}" name="DEF"/>
+    <tableColumn id="6" xr3:uid="{2264D5A1-C893-4362-97B8-7E20FC5D2A58}" name="MAT"/>
+    <tableColumn id="7" xr3:uid="{D1DFC0D2-A987-4E3F-BA23-52162FB0C0BA}" name="MDF"/>
+    <tableColumn id="8" xr3:uid="{AB6209DB-CCCB-4C37-B455-4C7652E0DAC9}" name="AGI"/>
+    <tableColumn id="9" xr3:uid="{2CD4CD14-92FD-41A7-9CCD-1329B5A77390}" name="LUK"/>
+    <tableColumn id="10" xr3:uid="{3B2C0A10-5038-4C21-BAC5-12FB16275D2E}" name="Total" dataDxfId="8">
+      <calculatedColumnFormula>SUM(Table11412[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{004CE0C0-6517-463C-8F96-51BDA9C554B5}" name="Table1316112324" displayName="Table1316112324" ref="A8:I14" totalsRowShown="0">
+  <autoFilter ref="A8:I14" xr:uid="{43F790D1-EA7B-4BAE-8A37-7CAD791E8821}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{F6E842E1-B25F-4CA1-9107-AC7179420C29}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{EFB2F0D5-318D-4A65-BA2B-20ADDE071648}" name="HP" dataDxfId="5">
+      <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{0D914B89-2678-453F-BC18-571DCD45E628}" name="MP" dataDxfId="3">
+      <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*13.75 + 80</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{6FBD2F64-5B1C-4035-BB1A-AFB092DB60C3}" name="ATK" dataDxfId="4">
+      <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{7E0AF3FC-CC5D-4A6A-A4A2-DE278DEC4062}" name="DEF" dataDxfId="0">
+      <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1 + 15 + 4</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{3AF4D559-893B-4D50-BCB4-A1BD1FAF2F23}" name="MAT" dataDxfId="2">
+      <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{6E9418A6-75AC-4541-9029-814EC5C06E70}" name="MDF" dataDxfId="1">
+      <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.375+15 + 14</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{CD605BEE-D561-4A2C-8D06-8E9AD70C32AC}" name="AGI" dataDxfId="7">
+      <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{E26506B2-F488-4AA4-AC87-819A22964609}" name="LUK" dataDxfId="6">
+      <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{671A73B1-117F-4F40-B5B7-178F8355834B}" name="Table16" displayName="Table16" ref="A5:J6" totalsRowShown="0">
   <autoFilter ref="A5:J6" xr:uid="{6C0AACD2-FA3F-4094-92F8-D2B9E23D5ABC}"/>
   <tableColumns count="10">
@@ -1467,131 +1768,8 @@
     <tableColumn id="7" xr3:uid="{3A2FD57C-060A-462E-8BB9-B06F717E9D20}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{ED9393EA-F7F9-4661-8D0B-0D9246DDABF8}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{6F56342F-5442-42CD-8B6C-D98B6D6C0C56}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="97">
+    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="107">
       <calculatedColumnFormula>SUM(Table16[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0489A86C-0040-4142-8D05-11877F6AC5E6}" name="Table131610" displayName="Table131610" ref="A8:I13" totalsRowShown="0">
-  <autoFilter ref="A8:I13" xr:uid="{7BE337CC-37BD-4688-B60D-A66F4420668B}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{71340E4C-6101-4C59-8ED7-689E2AD5A962}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="96">
-      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*63-100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="95">
-      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*10</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="94">
-      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="93">
-      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="92">
-      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="91">
-      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="90">
-      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="89">
-      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{0A2DAD7E-8DB8-432C-AD24-4A1116190AFC}" name="Table168" displayName="Table168" ref="A6:J7" totalsRowShown="0">
-  <autoFilter ref="A6:J7" xr:uid="{3F070465-048B-4A60-A5D6-289DD81841E3}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{46422AF1-99B7-4965-8F6A-D256072E575C}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{0A71C80C-CA2E-4E72-9D93-350B3DA84447}" name="HP"/>
-    <tableColumn id="3" xr3:uid="{DF6C3EB9-3A52-40CE-AC4E-B7F04A1EBB64}" name="MP"/>
-    <tableColumn id="4" xr3:uid="{F31DDD26-7F37-4DBC-8236-79185692625B}" name="ATK"/>
-    <tableColumn id="5" xr3:uid="{34BB612C-EF90-4001-865D-C0BBE9DDE35C}" name="DEF"/>
-    <tableColumn id="6" xr3:uid="{3C2ED426-96C6-4371-9F06-FA42D5AE2877}" name="MAT"/>
-    <tableColumn id="7" xr3:uid="{4899BF24-9D2A-4CC0-AE35-4F49604AAC5A}" name="MDF"/>
-    <tableColumn id="8" xr3:uid="{CB1CC6BA-1D38-4B74-9BC6-7057FB9773EE}" name="AGI"/>
-    <tableColumn id="9" xr3:uid="{C47FADF6-C526-4188-9187-383757CE17C1}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="88">
-      <calculatedColumnFormula>SUM(Table168[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{E50ECAD0-74A3-4ED4-B8F9-3CED6CCBE3D4}" name="Table13161013" displayName="Table13161013" ref="A9:I14" totalsRowShown="0">
-  <autoFilter ref="A9:I14" xr:uid="{06A56D17-07E5-4650-8EE9-7EA8F94D4020}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A2BE27C9-9DAE-49F5-9A70-C6CF7428BF31}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="87">
-      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="86">
-      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*10+20</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="85">
-      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="84">
-      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="83">
-      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.375+15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="82">
-      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="81">
-      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="80">
-      <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{537551B7-B0FC-43E4-9401-043CCFC4A3B0}" name="Table13162015" displayName="Table13162015" ref="A4:I10" totalsRowShown="0">
-  <autoFilter ref="A4:I10" xr:uid="{A1EAC62C-C07D-464E-91B1-4A34E6604BA2}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{430FD3D4-914C-4309-B2E6-6F01B5CAED94}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="79">
-      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="78">
-      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*15+100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="77">
-      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="76">
-      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="75">
-      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="74">
-      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="73">
-      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="72">
-      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1599,33 +1777,33 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{F3CEF94F-0A77-45F7-9EF0-B6E7B4DA3B1F}" name="Table131618" displayName="Table131618" ref="A7:I12" totalsRowShown="0">
-  <autoFilter ref="A7:I12" xr:uid="{9BE7336F-352A-4FAE-B0E4-61965FC814C7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0489A86C-0040-4142-8D05-11877F6AC5E6}" name="Table131610" displayName="Table131610" ref="A8:I13" totalsRowShown="0">
+  <autoFilter ref="A8:I13" xr:uid="{7BE337CC-37BD-4688-B60D-A66F4420668B}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B8DA50BB-4379-43D1-879B-CDBE6D82C13A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="71">
-      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="70">
-      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*10+20</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="69">
-      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="68">
-      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="67">
-      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="66">
-      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="65">
-      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="64">
-      <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{71340E4C-6101-4C59-8ED7-689E2AD5A962}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="106">
+      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*63-100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="105">
+      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="104">
+      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="103">
+      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="102">
+      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="101">
+      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="100">
+      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="99">
+      <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1929,10 +2107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F7AABB-3532-4A29-877B-ED130C7A9042}">
-  <dimension ref="A2:S13"/>
+  <dimension ref="A2:S14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2138,8 +2316,8 @@
         <v>1</v>
       </c>
       <c r="Q9">
-        <f>Table131611[[#This Row],[Level]]*1</f>
-        <v>1</v>
+        <f>Table131611[[#This Row],[Level]]*1+15</f>
+        <v>16</v>
       </c>
       <c r="R9">
         <f>Table131611[[#This Row],[Level]]*1 + 15</f>
@@ -2210,8 +2388,8 @@
         <v>10</v>
       </c>
       <c r="Q10">
-        <f>Table131611[[#This Row],[Level]]*1</f>
-        <v>10</v>
+        <f>Table131611[[#This Row],[Level]]*1+15</f>
+        <v>25</v>
       </c>
       <c r="R10">
         <f>Table131611[[#This Row],[Level]]*1 + 15</f>
@@ -2282,8 +2460,8 @@
         <v>25</v>
       </c>
       <c r="Q11">
-        <f>Table131611[[#This Row],[Level]]*1</f>
-        <v>25</v>
+        <f>Table131611[[#This Row],[Level]]*1+15</f>
+        <v>40</v>
       </c>
       <c r="R11">
         <f>Table131611[[#This Row],[Level]]*1 + 15</f>
@@ -2354,8 +2532,8 @@
         <v>35</v>
       </c>
       <c r="Q12">
-        <f>Table131611[[#This Row],[Level]]*1</f>
-        <v>35</v>
+        <f>Table131611[[#This Row],[Level]]*1+15</f>
+        <v>50</v>
       </c>
       <c r="R12">
         <f>Table131611[[#This Row],[Level]]*1 + 15</f>
@@ -2426,8 +2604,8 @@
         <v>99</v>
       </c>
       <c r="Q13">
-        <f>Table131611[[#This Row],[Level]]*1</f>
-        <v>99</v>
+        <f>Table131611[[#This Row],[Level]]*1+15</f>
+        <v>114</v>
       </c>
       <c r="R13">
         <f>Table131611[[#This Row],[Level]]*1 + 15</f>
@@ -2436,6 +2614,43 @@
       <c r="S13">
         <f>Table131611[[#This Row],[Level]]*1</f>
         <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>15</v>
+      </c>
+      <c r="L14" s="1">
+        <f>Table131611[[#This Row],[Level]]*56.25+200</f>
+        <v>1043.75</v>
+      </c>
+      <c r="M14" s="1">
+        <f>Table131611[[#This Row],[Level]]*10</f>
+        <v>150</v>
+      </c>
+      <c r="N14" s="1">
+        <f>Table131611[[#This Row],[Level]]*1.25+ 15+30</f>
+        <v>63.75</v>
+      </c>
+      <c r="O14" s="1">
+        <f>Table131611[[#This Row],[Level]]*1.25 + 15+33</f>
+        <v>66.75</v>
+      </c>
+      <c r="P14" s="1">
+        <f>Table131611[[#This Row],[Level]]*1</f>
+        <v>15</v>
+      </c>
+      <c r="Q14" s="1">
+        <f>Table131611[[#This Row],[Level]]*1+15</f>
+        <v>30</v>
+      </c>
+      <c r="R14" s="1">
+        <f>Table131611[[#This Row],[Level]]*1 + 15</f>
+        <v>30</v>
+      </c>
+      <c r="S14" s="1">
+        <f>Table131611[[#This Row],[Level]]*1</f>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2449,6 +2664,696 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8DFDAFD-5CD5-4F03-8B08-1FCB08CB3DEC}">
+  <dimension ref="A2:J17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <f>SUM(Table114[[#This Row],[HP]:[LUK]])</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <f>Table13161123[[#This Row],[Level]]*63+300</f>
+        <v>363</v>
+      </c>
+      <c r="C9">
+        <f>Table13161123[[#This Row],[Level]]*10</f>
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <f>Table13161123[[#This Row],[Level]]*1.5+ 15+40</f>
+        <v>56.5</v>
+      </c>
+      <c r="E9">
+        <f>Table13161123[[#This Row],[Level]]*1.25 + 15+21</f>
+        <v>37.25</v>
+      </c>
+      <c r="F9">
+        <f>Table13161123[[#This Row],[Level]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f>Table13161123[[#This Row],[Level]]*1.25+15 + 7</f>
+        <v>23.25</v>
+      </c>
+      <c r="H9">
+        <f>Table13161123[[#This Row],[Level]]*1.25 + 15</f>
+        <v>16.25</v>
+      </c>
+      <c r="I9">
+        <f>Table13161123[[#This Row],[Level]]*1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <f>Table13161123[[#This Row],[Level]]*63+300</f>
+        <v>930</v>
+      </c>
+      <c r="C10">
+        <f>Table13161123[[#This Row],[Level]]*10</f>
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <f>Table13161123[[#This Row],[Level]]*1.5+ 15+40</f>
+        <v>70</v>
+      </c>
+      <c r="E10">
+        <f>Table13161123[[#This Row],[Level]]*1.25 + 15+21</f>
+        <v>48.5</v>
+      </c>
+      <c r="F10">
+        <f>Table13161123[[#This Row],[Level]]*1</f>
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <f>Table13161123[[#This Row],[Level]]*1.25+15 + 7</f>
+        <v>34.5</v>
+      </c>
+      <c r="H10">
+        <f>Table13161123[[#This Row],[Level]]*1.25 + 15</f>
+        <v>27.5</v>
+      </c>
+      <c r="I10">
+        <f>Table13161123[[#This Row],[Level]]*1</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <f>Table13161123[[#This Row],[Level]]*63+300</f>
+        <v>1875</v>
+      </c>
+      <c r="C11">
+        <f>Table13161123[[#This Row],[Level]]*10</f>
+        <v>250</v>
+      </c>
+      <c r="D11">
+        <f>Table13161123[[#This Row],[Level]]*1.5+ 15+40</f>
+        <v>92.5</v>
+      </c>
+      <c r="E11">
+        <f>Table13161123[[#This Row],[Level]]*1.25 + 15+21</f>
+        <v>67.25</v>
+      </c>
+      <c r="F11">
+        <f>Table13161123[[#This Row],[Level]]*1</f>
+        <v>25</v>
+      </c>
+      <c r="G11">
+        <f>Table13161123[[#This Row],[Level]]*1.25+15 + 7</f>
+        <v>53.25</v>
+      </c>
+      <c r="H11">
+        <f>Table13161123[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+      <c r="I11">
+        <f>Table13161123[[#This Row],[Level]]*1</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <f>Table13161123[[#This Row],[Level]]*63+300</f>
+        <v>2505</v>
+      </c>
+      <c r="C12">
+        <f>Table13161123[[#This Row],[Level]]*10</f>
+        <v>350</v>
+      </c>
+      <c r="D12">
+        <f>Table13161123[[#This Row],[Level]]*1.5+ 15+40</f>
+        <v>107.5</v>
+      </c>
+      <c r="E12">
+        <f>Table13161123[[#This Row],[Level]]*1.25 + 15+21</f>
+        <v>79.75</v>
+      </c>
+      <c r="F12">
+        <f>Table13161123[[#This Row],[Level]]*1</f>
+        <v>35</v>
+      </c>
+      <c r="G12">
+        <f>Table13161123[[#This Row],[Level]]*1.25+15 + 7</f>
+        <v>65.75</v>
+      </c>
+      <c r="H12">
+        <f>Table13161123[[#This Row],[Level]]*1.25 + 15</f>
+        <v>58.75</v>
+      </c>
+      <c r="I12">
+        <f>Table13161123[[#This Row],[Level]]*1</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>99</v>
+      </c>
+      <c r="B13">
+        <f>Table13161123[[#This Row],[Level]]*63+300</f>
+        <v>6537</v>
+      </c>
+      <c r="C13">
+        <f>Table13161123[[#This Row],[Level]]*10</f>
+        <v>990</v>
+      </c>
+      <c r="D13">
+        <f>Table13161123[[#This Row],[Level]]*1.5+ 15+40</f>
+        <v>203.5</v>
+      </c>
+      <c r="E13">
+        <f>Table13161123[[#This Row],[Level]]*1.25 + 15+21</f>
+        <v>159.75</v>
+      </c>
+      <c r="F13">
+        <f>Table13161123[[#This Row],[Level]]*1</f>
+        <v>99</v>
+      </c>
+      <c r="G13">
+        <f>Table13161123[[#This Row],[Level]]*1.25+15 + 7</f>
+        <v>145.75</v>
+      </c>
+      <c r="H13">
+        <f>Table13161123[[#This Row],[Level]]*1.25 + 15</f>
+        <v>138.75</v>
+      </c>
+      <c r="I13">
+        <f>Table13161123[[#This Row],[Level]]*1</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <f>Table13161123[[#This Row],[Level]]*63+300</f>
+        <v>1245</v>
+      </c>
+      <c r="C14" s="1">
+        <f>Table13161123[[#This Row],[Level]]*10</f>
+        <v>150</v>
+      </c>
+      <c r="D14" s="1">
+        <f>Table13161123[[#This Row],[Level]]*1.5+ 15+40</f>
+        <v>77.5</v>
+      </c>
+      <c r="E14" s="1">
+        <f>Table13161123[[#This Row],[Level]]*1.25 + 15+21</f>
+        <v>54.75</v>
+      </c>
+      <c r="F14" s="1">
+        <f>Table13161123[[#This Row],[Level]]*1</f>
+        <v>15</v>
+      </c>
+      <c r="G14" s="1">
+        <f>Table13161123[[#This Row],[Level]]*1.25+15 + 7</f>
+        <v>40.75</v>
+      </c>
+      <c r="H14" s="1">
+        <f>Table13161123[[#This Row],[Level]]*1.25 + 15</f>
+        <v>33.75</v>
+      </c>
+      <c r="I14" s="1">
+        <f>Table13161123[[#This Row],[Level]]*1</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63963E77-5E81-4490-B187-3082B2132C5A}">
+  <dimension ref="A3:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <f>SUM(Table11412[[#This Row],[HP]:[LUK]])</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <f>Table1316112324[[#This Row],[Level]]*50 + 100</f>
+        <v>150</v>
+      </c>
+      <c r="C9">
+        <f>Table1316112324[[#This Row],[Level]]*13.75 + 80</f>
+        <v>93.75</v>
+      </c>
+      <c r="D9">
+        <f>Table1316112324[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <f>Table1316112324[[#This Row],[Level]]*1 + 15 + 4</f>
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <f>Table1316112324[[#This Row],[Level]]*1.5 + 15 + 40</f>
+        <v>56.5</v>
+      </c>
+      <c r="G9">
+        <f>Table1316112324[[#This Row],[Level]]*1.375+15 + 14</f>
+        <v>30.375</v>
+      </c>
+      <c r="H9">
+        <f>Table1316112324[[#This Row],[Level]]*1.25 + 15</f>
+        <v>16.25</v>
+      </c>
+      <c r="I9">
+        <f>Table1316112324[[#This Row],[Level]]*1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <f>Table1316112324[[#This Row],[Level]]*50 + 100</f>
+        <v>600</v>
+      </c>
+      <c r="C10">
+        <f>Table1316112324[[#This Row],[Level]]*13.75 + 80</f>
+        <v>217.5</v>
+      </c>
+      <c r="D10">
+        <f>Table1316112324[[#This Row],[Level]]*1 + 15</f>
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <f>Table1316112324[[#This Row],[Level]]*1 + 15 + 4</f>
+        <v>29</v>
+      </c>
+      <c r="F10">
+        <f>Table1316112324[[#This Row],[Level]]*1.5 + 15 + 40</f>
+        <v>70</v>
+      </c>
+      <c r="G10">
+        <f>Table1316112324[[#This Row],[Level]]*1.375+15 + 14</f>
+        <v>42.75</v>
+      </c>
+      <c r="H10">
+        <f>Table1316112324[[#This Row],[Level]]*1.25 + 15</f>
+        <v>27.5</v>
+      </c>
+      <c r="I10">
+        <f>Table1316112324[[#This Row],[Level]]*1</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <f>Table1316112324[[#This Row],[Level]]*50 + 100</f>
+        <v>1350</v>
+      </c>
+      <c r="C11">
+        <f>Table1316112324[[#This Row],[Level]]*13.75 + 80</f>
+        <v>423.75</v>
+      </c>
+      <c r="D11">
+        <f>Table1316112324[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="E11">
+        <f>Table1316112324[[#This Row],[Level]]*1 + 15 + 4</f>
+        <v>44</v>
+      </c>
+      <c r="F11">
+        <f>Table1316112324[[#This Row],[Level]]*1.5 + 15 + 40</f>
+        <v>92.5</v>
+      </c>
+      <c r="G11">
+        <f>Table1316112324[[#This Row],[Level]]*1.375+15 + 14</f>
+        <v>63.375</v>
+      </c>
+      <c r="H11">
+        <f>Table1316112324[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+      <c r="I11">
+        <f>Table1316112324[[#This Row],[Level]]*1</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <f>Table1316112324[[#This Row],[Level]]*50 + 100</f>
+        <v>1850</v>
+      </c>
+      <c r="C12">
+        <f>Table1316112324[[#This Row],[Level]]*13.75 + 80</f>
+        <v>561.25</v>
+      </c>
+      <c r="D12">
+        <f>Table1316112324[[#This Row],[Level]]*1 + 15</f>
+        <v>50</v>
+      </c>
+      <c r="E12">
+        <f>Table1316112324[[#This Row],[Level]]*1 + 15 + 4</f>
+        <v>54</v>
+      </c>
+      <c r="F12">
+        <f>Table1316112324[[#This Row],[Level]]*1.5 + 15 + 40</f>
+        <v>107.5</v>
+      </c>
+      <c r="G12">
+        <f>Table1316112324[[#This Row],[Level]]*1.375+15 + 14</f>
+        <v>77.125</v>
+      </c>
+      <c r="H12">
+        <f>Table1316112324[[#This Row],[Level]]*1.25 + 15</f>
+        <v>58.75</v>
+      </c>
+      <c r="I12">
+        <f>Table1316112324[[#This Row],[Level]]*1</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>99</v>
+      </c>
+      <c r="B13">
+        <f>Table1316112324[[#This Row],[Level]]*50 + 100</f>
+        <v>5050</v>
+      </c>
+      <c r="C13">
+        <f>Table1316112324[[#This Row],[Level]]*13.75 + 80</f>
+        <v>1441.25</v>
+      </c>
+      <c r="D13">
+        <f>Table1316112324[[#This Row],[Level]]*1 + 15</f>
+        <v>114</v>
+      </c>
+      <c r="E13">
+        <f>Table1316112324[[#This Row],[Level]]*1 + 15 + 4</f>
+        <v>118</v>
+      </c>
+      <c r="F13">
+        <f>Table1316112324[[#This Row],[Level]]*1.5 + 15 + 40</f>
+        <v>203.5</v>
+      </c>
+      <c r="G13">
+        <f>Table1316112324[[#This Row],[Level]]*1.375+15 + 14</f>
+        <v>165.125</v>
+      </c>
+      <c r="H13">
+        <f>Table1316112324[[#This Row],[Level]]*1.25 + 15</f>
+        <v>138.75</v>
+      </c>
+      <c r="I13">
+        <f>Table1316112324[[#This Row],[Level]]*1</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <f>Table1316112324[[#This Row],[Level]]*50 + 100</f>
+        <v>850</v>
+      </c>
+      <c r="C14" s="1">
+        <f>Table1316112324[[#This Row],[Level]]*13.75 + 80</f>
+        <v>286.25</v>
+      </c>
+      <c r="D14" s="1">
+        <f>Table1316112324[[#This Row],[Level]]*1 + 15</f>
+        <v>30</v>
+      </c>
+      <c r="E14" s="1">
+        <f>Table1316112324[[#This Row],[Level]]*1 + 15 + 4</f>
+        <v>34</v>
+      </c>
+      <c r="F14" s="1">
+        <f>Table1316112324[[#This Row],[Level]]*1.5 + 15 + 40</f>
+        <v>77.5</v>
+      </c>
+      <c r="G14" s="1">
+        <f>Table1316112324[[#This Row],[Level]]*1.375+15 + 14</f>
+        <v>49.625</v>
+      </c>
+      <c r="H14" s="1">
+        <f>Table1316112324[[#This Row],[Level]]*1.25 + 15</f>
+        <v>33.75</v>
+      </c>
+      <c r="I14" s="1">
+        <f>Table1316112324[[#This Row],[Level]]*1</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FEB1284-A899-416A-A581-E0E1F5719020}">
   <dimension ref="A2:J13"/>
   <sheetViews>
@@ -2756,12 +3661,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9807F697-48C3-4A93-87DF-719DC89F6DFD}">
-  <dimension ref="A2:J14"/>
+  <dimension ref="A2:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3058,6 +3963,43 @@
       <c r="I14">
         <f>Table13161013[[#This Row],[Level]]*1.5+15</f>
         <v>163.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1">
+        <f>Table13161013[[#This Row],[Level]]*56.25-100</f>
+        <v>743.75</v>
+      </c>
+      <c r="C15" s="1">
+        <f>Table13161013[[#This Row],[Level]]*10+20</f>
+        <v>170</v>
+      </c>
+      <c r="D15" s="1">
+        <f>Table13161013[[#This Row],[Level]]*1+ 15</f>
+        <v>30</v>
+      </c>
+      <c r="E15" s="1">
+        <f>Table13161013[[#This Row],[Level]]*1 + 15</f>
+        <v>30</v>
+      </c>
+      <c r="F15" s="1">
+        <f>Table13161013[[#This Row],[Level]]*1.375+15</f>
+        <v>35.625</v>
+      </c>
+      <c r="G15" s="1">
+        <f>Table13161013[[#This Row],[Level]]*1.5+15</f>
+        <v>37.5</v>
+      </c>
+      <c r="H15" s="1">
+        <f>Table13161013[[#This Row],[Level]]*1.125 + 15</f>
+        <v>31.875</v>
+      </c>
+      <c r="I15" s="1">
+        <f>Table13161013[[#This Row],[Level]]*1.5+15</f>
+        <v>37.5</v>
       </c>
     </row>
   </sheetData>
@@ -3069,7 +4011,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA7AE8E-3CBD-43D4-8334-3506A3BDF6FA}">
   <dimension ref="A2:I13"/>
   <sheetViews>
@@ -3353,12 +4295,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CE9C02-0686-4D94-800E-4766BA124417}">
   <dimension ref="A2:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3722,7 +4664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED846686-A238-4174-849F-9F6770BD1F9B}">
   <dimension ref="A1:T9"/>
   <sheetViews>
@@ -4068,12 +5010,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4195E475-9F10-4DD8-82F0-E47D9A595A6E}">
   <dimension ref="A2:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Scripted prison rescue scene
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="3" activeTab="7" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="7" activeTab="8" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Skeleton Soldier" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="54">
   <si>
     <t>Skeletons are the most basic undead, they have low magical attributes, agility, and luck.</t>
   </si>
@@ -195,6 +195,9 @@
   <si>
     <t>Bounded Wind Spirit</t>
   </si>
+  <si>
+    <t>In fort: 30MAT, 7/21</t>
+  </si>
 </sst>
 </file>
 
@@ -380,24 +383,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1263,6 +1248,24 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1475,7 +1478,7 @@
     <tableColumn id="7" xr3:uid="{20C5D094-BAF0-471C-ACF3-C6658991DB5F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{E08E2AF0-56DD-4A69-A536-27139D793022}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{12AD8606-1127-4E5B-BA2C-872780F22F9E}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{5E2EF778-63AE-48B7-9F49-0D2AFEBD66A1}" name="Total" dataDxfId="8">
+    <tableColumn id="10" xr3:uid="{5E2EF778-63AE-48B7-9F49-0D2AFEBD66A1}" name="Total" dataDxfId="88">
       <calculatedColumnFormula>SUM(Table1682630[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1488,28 +1491,28 @@
   <autoFilter ref="A8:I14" xr:uid="{299912CC-280B-49E1-8859-432D05893259}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4F0B657F-C9A5-4A73-AAA3-27D307385193}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{526284E7-597F-4726-AB18-230CA03461B1}" name="HP" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{526284E7-597F-4726-AB18-230CA03461B1}" name="HP" dataDxfId="87">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*63+ 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E7BA3C7A-2677-415F-BA47-A4E88679B948}" name="MP" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{E7BA3C7A-2677-415F-BA47-A4E88679B948}" name="MP" dataDxfId="86">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE7BE678-2229-44F6-8732-71214FB69DD7}" name="ATK" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{AE7BE678-2229-44F6-8732-71214FB69DD7}" name="ATK" dataDxfId="85">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+ 15+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4715E3DB-8817-43D5-9074-9FB5F0BEF5B4}" name="DEF" dataDxfId="6">
+    <tableColumn id="5" xr3:uid="{4715E3DB-8817-43D5-9074-9FB5F0BEF5B4}" name="DEF" dataDxfId="84">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1 + 15+12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9CE76933-D045-418B-A975-378EEA51D856}" name="MAT" dataDxfId="5">
+    <tableColumn id="6" xr3:uid="{9CE76933-D045-418B-A975-378EEA51D856}" name="MAT" dataDxfId="83">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244B9611-6CB0-4946-B5CD-7D42311C7D7E}" name="MDF" dataDxfId="4">
+    <tableColumn id="7" xr3:uid="{244B9611-6CB0-4946-B5CD-7D42311C7D7E}" name="MDF" dataDxfId="82">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+15+11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32550C13-49BB-41D2-BA0A-26798830A0FD}" name="AGI" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{32550C13-49BB-41D2-BA0A-26798830A0FD}" name="AGI" dataDxfId="81">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{BB22F289-8AF5-4DD6-877B-F09520710555}" name="LUK" dataDxfId="3">
+    <tableColumn id="9" xr3:uid="{BB22F289-8AF5-4DD6-877B-F09520710555}" name="LUK" dataDxfId="80">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+15+20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1522,28 +1525,28 @@
   <autoFilter ref="A4:I10" xr:uid="{A1EAC62C-C07D-464E-91B1-4A34E6604BA2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{430FD3D4-914C-4309-B2E6-6F01B5CAED94}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="88">
+    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="79">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="87">
+    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="78">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="86">
+    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="77">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="85">
-      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="84">
-      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="83">
-      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="82">
+    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="0">
+      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15 + 7</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="2">
+      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15 + 30</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="1">
+      <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15 + 21</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="76">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="81">
+    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="75">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1556,28 +1559,28 @@
   <autoFilter ref="A7:I12" xr:uid="{9BE7336F-352A-4FAE-B0E4-61965FC814C7}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B8DA50BB-4379-43D1-879B-CDBE6D82C13A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="80">
+    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="74">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="79">
+    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="73">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="78">
+    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="72">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="77">
+    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="71">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="76">
+    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="70">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="75">
+    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="69">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="74">
+    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="68">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="73">
+    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="67">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1632,7 +1635,7 @@
     <tableColumn id="7" xr3:uid="{AEFF5C29-BE6A-4CF8-A2BB-F6B076077DA9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{4DE9B01E-67F2-4136-ADC3-60389FB67DCC}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{F5A82F03-513C-46D4-9F91-470F0060526B}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="72">
+    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="66">
       <calculatedColumnFormula>SUM(Table16821[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1641,22 +1644,22 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="71" tableBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="65" tableBorderDxfId="64">
   <autoFilter ref="A15:I16" xr:uid="{434CBBE2-2F8D-4EEB-895C-68FC850EF1FD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="68">
+    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="62">
       <calculatedColumnFormula>Table1922[Level]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="67">
+    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="61">
       <calculatedColumnFormula>Table1922[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="66"/>
-    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="65"/>
-    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="64"/>
-    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="63"/>
-    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="62"/>
-    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="58"/>
+    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="57"/>
+    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="56"/>
+    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1667,28 +1670,28 @@
   <autoFilter ref="A3:I9" xr:uid="{A90D1C2A-DBF9-4EEF-ACC2-3DC17C207301}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BD3505AC-AE6D-4947-A74E-A6C2D68658F1}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="60">
+    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="54">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="59">
+    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="53">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="58">
+    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="52">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="57">
+    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="51">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="56">
+    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="50">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="55">
+    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="49">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="54">
+    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="48">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="53">
+    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="47">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1697,32 +1700,32 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="52" tableBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="46" tableBorderDxfId="45">
   <autoFilter ref="L3:T4" xr:uid="{5D2C3EA8-1297-4C77-AF32-84E50F8232C5}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="49">
+    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="43">
       <calculatedColumnFormula>Table19[Level]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="48">
+    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="42">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="47">
+    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="41">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="46">
+    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="40">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1 + 15 + 6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="45">
+    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="39">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="44">
+    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="38">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="43">
+    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="37">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="42">
+    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="36">
       <calculatedColumnFormula>Table19[Level] + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1743,7 +1746,7 @@
     <tableColumn id="7" xr3:uid="{22216E02-260E-4471-8BB1-4E6E1250BAC9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{DC2670AC-8DF2-47F7-A3F6-EE7896309BC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{749652E2-F6CF-428C-B67C-FD0B1EFCCBBF}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="41">
+    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="35">
       <calculatedColumnFormula>SUM(Table15[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1756,28 +1759,28 @@
   <autoFilter ref="A15:I20" xr:uid="{A1CF627F-8D28-44AD-9A35-411103976FCA}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F14CC326-DE44-48D8-856F-8DCDCFC89CAD}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="40">
+    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="34">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*63-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="39">
+    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="33">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="38">
+    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="32">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="37">
+    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="31">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="36">
+    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="30">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="35">
+    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="29">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="34">
+    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="28">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="33">
+    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="27">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1790,28 +1793,28 @@
   <autoFilter ref="K11:S17" xr:uid="{EAF9FB6A-F011-40E3-AB2F-E53826722AFB}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DF3E0800-6EE4-4E1B-BA6F-0194351D6E7C}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="32">
+    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="26">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*56.25+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="31">
+    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="25">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="30">
+    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="24">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="29">
+    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="23">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="28">
+    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="22">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="27">
+    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="21">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="26">
+    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="20">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="25">
+    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="19">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1824,28 +1827,28 @@
   <autoFilter ref="A26:I31" xr:uid="{870F76F2-5EA7-4FD7-B1F9-507D64592088}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{3C04B742-338A-4366-BF3D-C5BC13023785}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="24">
+    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="18">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*63+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="23">
+    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="17">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="22">
+    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="16">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="21">
+    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="15">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="20">
+    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="14">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="19">
+    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="13">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="18">
+    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="12">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="17">
+    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="11">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1858,28 +1861,28 @@
   <autoFilter ref="A36:I41" xr:uid="{9BD043AF-0D77-4FF4-B2F9-B4AC3C3F1F82}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{7BB908A3-05D7-4357-920B-BF4C6BC20C06}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="16">
+    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="10">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*56.5+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="15">
+    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="9">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*12.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="14">
+    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="8">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="13">
+    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="7">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1 + 15+14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="6">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="5">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.5+ 15+13</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="10">
+    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="4">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="9">
+    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="3">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.375 + 15+40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6800,8 +6803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{553D32E0-5A99-4BFF-A02D-6B35D71614A2}">
   <dimension ref="A2:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7148,10 +7151,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA7AE8E-3CBD-43D4-8334-3506A3BDF6FA}">
-  <dimension ref="A2:I13"/>
+  <dimension ref="A2:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7212,16 +7215,16 @@
         <v>16</v>
       </c>
       <c r="E5">
-        <f>Table13162015[[#This Row],[Level]]*1 + 15</f>
-        <v>16</v>
+        <f>Table13162015[[#This Row],[Level]]*1 + 15 + 7</f>
+        <v>23</v>
       </c>
       <c r="F5">
-        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
-        <v>16.5</v>
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15 + 30</f>
+        <v>46.5</v>
       </c>
       <c r="G5">
-        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
-        <v>16.5</v>
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15 + 21</f>
+        <v>37.5</v>
       </c>
       <c r="H5">
         <f>Table13162015[[#This Row],[Level]]*1.25 + 15</f>
@@ -7249,16 +7252,16 @@
         <v>30</v>
       </c>
       <c r="E6">
-        <f>Table13162015[[#This Row],[Level]]*1 + 15</f>
-        <v>30</v>
+        <f>Table13162015[[#This Row],[Level]]*1 + 15 + 7</f>
+        <v>37</v>
       </c>
       <c r="F6">
-        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
-        <v>37.5</v>
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15 + 30</f>
+        <v>67.5</v>
       </c>
       <c r="G6">
-        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
-        <v>37.5</v>
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15 + 21</f>
+        <v>58.5</v>
       </c>
       <c r="H6">
         <f>Table13162015[[#This Row],[Level]]*1.25 + 15</f>
@@ -7286,16 +7289,16 @@
         <v>40</v>
       </c>
       <c r="E7">
-        <f>Table13162015[[#This Row],[Level]]*1 + 15</f>
-        <v>40</v>
+        <f>Table13162015[[#This Row],[Level]]*1 + 15 + 7</f>
+        <v>47</v>
       </c>
       <c r="F7">
-        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
-        <v>52.5</v>
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15 + 30</f>
+        <v>82.5</v>
       </c>
       <c r="G7">
-        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
-        <v>52.5</v>
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15 + 21</f>
+        <v>73.5</v>
       </c>
       <c r="H7">
         <f>Table13162015[[#This Row],[Level]]*1.25 + 15</f>
@@ -7323,16 +7326,16 @@
         <v>50</v>
       </c>
       <c r="E8">
-        <f>Table13162015[[#This Row],[Level]]*1 + 15</f>
-        <v>50</v>
+        <f>Table13162015[[#This Row],[Level]]*1 + 15 + 7</f>
+        <v>57</v>
       </c>
       <c r="F8">
-        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
-        <v>67.5</v>
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15 + 30</f>
+        <v>97.5</v>
       </c>
       <c r="G8">
-        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
-        <v>67.5</v>
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15 + 21</f>
+        <v>88.5</v>
       </c>
       <c r="H8">
         <f>Table13162015[[#This Row],[Level]]*1.25 + 15</f>
@@ -7360,16 +7363,16 @@
         <v>114</v>
       </c>
       <c r="E9">
-        <f>Table13162015[[#This Row],[Level]]*1 + 15</f>
-        <v>114</v>
+        <f>Table13162015[[#This Row],[Level]]*1 + 15 + 7</f>
+        <v>121</v>
       </c>
       <c r="F9">
-        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
-        <v>163.5</v>
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15 + 30</f>
+        <v>193.5</v>
       </c>
       <c r="G9">
-        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
-        <v>163.5</v>
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15 + 21</f>
+        <v>184.5</v>
       </c>
       <c r="H9">
         <f>Table13162015[[#This Row],[Level]]*1.25 + 15</f>
@@ -7397,16 +7400,16 @@
         <v>35</v>
       </c>
       <c r="E10" s="1">
-        <f>Table13162015[[#This Row],[Level]]*1 + 15</f>
-        <v>35</v>
+        <f>Table13162015[[#This Row],[Level]]*1 + 15 + 7</f>
+        <v>42</v>
       </c>
       <c r="F10" s="1">
-        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
-        <v>45</v>
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15 + 30</f>
+        <v>75</v>
       </c>
       <c r="G10" s="1">
-        <f>Table13162015[[#This Row],[Level]]*1.5 + 15</f>
-        <v>45</v>
+        <f>Table13162015[[#This Row],[Level]]*1.5 + 15 + 21</f>
+        <v>66</v>
       </c>
       <c r="H10" s="1">
         <f>Table13162015[[#This Row],[Level]]*1.25 + 15</f>
@@ -7420,6 +7423,11 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mapped second floor, TODO: Script battle with necromancer and battle with Death Lord
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="7" activeTab="8" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="7" activeTab="11" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Skeleton Soldier" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,8 @@
     <sheet name="Acolyte" sheetId="7" r:id="rId9"/>
     <sheet name="Death Knight" sheetId="8" r:id="rId10"/>
     <sheet name="VillianCanson" sheetId="4" r:id="rId11"/>
-    <sheet name="Goblin" sheetId="2" r:id="rId12"/>
+    <sheet name="Death Lord" sheetId="15" r:id="rId12"/>
+    <sheet name="Goblin" sheetId="2" r:id="rId13"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="55">
   <si>
     <t>Skeletons are the most basic undead, they have low magical attributes, agility, and luck.</t>
   </si>
@@ -198,6 +199,9 @@
   <si>
     <t>In fort: 30MAT, 7/21</t>
   </si>
+  <si>
+    <t>Death Lords are giant undead</t>
+  </si>
 </sst>
 </file>
 
@@ -273,112 +277,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="160">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="180">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -696,6 +595,105 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1009,6 +1007,328 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -1292,7 +1612,7 @@
     <tableColumn id="7" xr3:uid="{F9852B29-E77D-4E17-A56E-5F0C649FA862}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{9A914BFF-1060-46E4-B8F9-412BD9293C3D}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2F83B650-811D-4FEE-92D5-03D4DC4376E5}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="159">
+    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="179">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1313,7 +1633,7 @@
     <tableColumn id="7" xr3:uid="{3A2FD57C-060A-462E-8BB9-B06F717E9D20}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{ED9393EA-F7F9-4661-8D0B-0D9246DDABF8}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{6F56342F-5442-42CD-8B6C-D98B6D6C0C56}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="115">
+    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="135">
       <calculatedColumnFormula>SUM(Table16[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1326,28 +1646,28 @@
   <autoFilter ref="A8:I13" xr:uid="{7BE337CC-37BD-4688-B60D-A66F4420668B}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{71340E4C-6101-4C59-8ED7-689E2AD5A962}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="114">
+    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="134">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*63-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="113">
+    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="133">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="112">
+    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="132">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="111">
+    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="131">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="110">
+    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="130">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="109">
+    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="129">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="108">
+    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="128">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="107">
+    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="127">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1368,7 +1688,7 @@
     <tableColumn id="7" xr3:uid="{4899BF24-9D2A-4CC0-AE35-4F49604AAC5A}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{CB1CC6BA-1D38-4B74-9BC6-7057FB9773EE}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{C47FADF6-C526-4188-9187-383757CE17C1}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="106">
+    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="126">
       <calculatedColumnFormula>SUM(Table168[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1381,28 +1701,28 @@
   <autoFilter ref="A9:I15" xr:uid="{06A56D17-07E5-4650-8EE9-7EA8F94D4020}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A2BE27C9-9DAE-49F5-9A70-C6CF7428BF31}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="105">
+    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="125">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="104">
+    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="124">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="103">
+    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="123">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="102">
+    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="122">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="101">
+    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="121">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.375+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="100">
+    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="120">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="99">
+    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="119">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="98">
+    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="118">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1423,7 +1743,7 @@
     <tableColumn id="7" xr3:uid="{60AD88FB-4685-412B-B5FD-BF8412C6B8E2}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{6A88D48C-D864-4F16-BEF2-BA88783A3FF3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{D40BD230-6392-4A28-A29D-F13EFE35C95E}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A0E09B2B-FD41-413F-8063-62214E990751}" name="Total" dataDxfId="97">
+    <tableColumn id="10" xr3:uid="{A0E09B2B-FD41-413F-8063-62214E990751}" name="Total" dataDxfId="117">
       <calculatedColumnFormula>SUM(Table16826[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1436,28 +1756,28 @@
   <autoFilter ref="A8:I14" xr:uid="{F7062CBA-4FAA-4900-9D3A-5C6613BCB6CE}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{ADCB4852-D3A0-456B-A8BD-E5F74BDBB762}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{ED76047D-1BC2-4C1B-B9B0-58BE0ACDDA48}" name="HP" dataDxfId="96">
+    <tableColumn id="2" xr3:uid="{ED76047D-1BC2-4C1B-B9B0-58BE0ACDDA48}" name="HP" dataDxfId="116">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EC859C53-0BA5-45D1-868B-F22DC8CE7D25}" name="MP" dataDxfId="95">
+    <tableColumn id="3" xr3:uid="{EC859C53-0BA5-45D1-868B-F22DC8CE7D25}" name="MP" dataDxfId="115">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DED33AB9-A2BB-4F9E-AA6D-02F8D1D65CD1}" name="ATK" dataDxfId="94">
+    <tableColumn id="4" xr3:uid="{DED33AB9-A2BB-4F9E-AA6D-02F8D1D65CD1}" name="ATK" dataDxfId="114">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.375+ 15+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{329B716D-9CA6-4546-AB13-92D88BE40F5F}" name="DEF" dataDxfId="93">
+    <tableColumn id="5" xr3:uid="{329B716D-9CA6-4546-AB13-92D88BE40F5F}" name="DEF" dataDxfId="113">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1 + 15+12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{67F8198A-5FC2-4C6D-9558-68B3141EA756}" name="MAT" dataDxfId="92">
+    <tableColumn id="6" xr3:uid="{67F8198A-5FC2-4C6D-9558-68B3141EA756}" name="MAT" dataDxfId="112">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C70F5BF6-63B0-44C1-862D-25E3FB55320F}" name="MDF" dataDxfId="91">
+    <tableColumn id="7" xr3:uid="{C70F5BF6-63B0-44C1-862D-25E3FB55320F}" name="MDF" dataDxfId="111">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.5+15+11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AB20AF53-453C-4266-A46B-40E693C91985}" name="AGI" dataDxfId="90">
+    <tableColumn id="8" xr3:uid="{AB20AF53-453C-4266-A46B-40E693C91985}" name="AGI" dataDxfId="110">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7FC46A31-F9F1-432E-B399-0823E198FE0A}" name="LUK" dataDxfId="89">
+    <tableColumn id="9" xr3:uid="{7FC46A31-F9F1-432E-B399-0823E198FE0A}" name="LUK" dataDxfId="109">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.5+15+20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1478,7 +1798,7 @@
     <tableColumn id="7" xr3:uid="{20C5D094-BAF0-471C-ACF3-C6658991DB5F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{E08E2AF0-56DD-4A69-A536-27139D793022}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{12AD8606-1127-4E5B-BA2C-872780F22F9E}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{5E2EF778-63AE-48B7-9F49-0D2AFEBD66A1}" name="Total" dataDxfId="88">
+    <tableColumn id="10" xr3:uid="{5E2EF778-63AE-48B7-9F49-0D2AFEBD66A1}" name="Total" dataDxfId="108">
       <calculatedColumnFormula>SUM(Table1682630[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1491,28 +1811,28 @@
   <autoFilter ref="A8:I14" xr:uid="{299912CC-280B-49E1-8859-432D05893259}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4F0B657F-C9A5-4A73-AAA3-27D307385193}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{526284E7-597F-4726-AB18-230CA03461B1}" name="HP" dataDxfId="87">
+    <tableColumn id="2" xr3:uid="{526284E7-597F-4726-AB18-230CA03461B1}" name="HP" dataDxfId="107">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*63+ 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E7BA3C7A-2677-415F-BA47-A4E88679B948}" name="MP" dataDxfId="86">
+    <tableColumn id="3" xr3:uid="{E7BA3C7A-2677-415F-BA47-A4E88679B948}" name="MP" dataDxfId="106">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE7BE678-2229-44F6-8732-71214FB69DD7}" name="ATK" dataDxfId="85">
+    <tableColumn id="4" xr3:uid="{AE7BE678-2229-44F6-8732-71214FB69DD7}" name="ATK" dataDxfId="105">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+ 15+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4715E3DB-8817-43D5-9074-9FB5F0BEF5B4}" name="DEF" dataDxfId="84">
+    <tableColumn id="5" xr3:uid="{4715E3DB-8817-43D5-9074-9FB5F0BEF5B4}" name="DEF" dataDxfId="104">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1 + 15+12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9CE76933-D045-418B-A975-378EEA51D856}" name="MAT" dataDxfId="83">
+    <tableColumn id="6" xr3:uid="{9CE76933-D045-418B-A975-378EEA51D856}" name="MAT" dataDxfId="103">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244B9611-6CB0-4946-B5CD-7D42311C7D7E}" name="MDF" dataDxfId="82">
+    <tableColumn id="7" xr3:uid="{244B9611-6CB0-4946-B5CD-7D42311C7D7E}" name="MDF" dataDxfId="102">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+15+11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32550C13-49BB-41D2-BA0A-26798830A0FD}" name="AGI" dataDxfId="81">
+    <tableColumn id="8" xr3:uid="{32550C13-49BB-41D2-BA0A-26798830A0FD}" name="AGI" dataDxfId="101">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{BB22F289-8AF5-4DD6-877B-F09520710555}" name="LUK" dataDxfId="80">
+    <tableColumn id="9" xr3:uid="{BB22F289-8AF5-4DD6-877B-F09520710555}" name="LUK" dataDxfId="100">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+15+20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1525,28 +1845,28 @@
   <autoFilter ref="A4:I10" xr:uid="{A1EAC62C-C07D-464E-91B1-4A34E6604BA2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{430FD3D4-914C-4309-B2E6-6F01B5CAED94}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="79">
+    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="99">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="78">
+    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="98">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="77">
+    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="97">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="96">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15 + 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="95">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15 + 30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="1">
+    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="94">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15 + 21</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="76">
+    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="93">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="75">
+    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="92">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1559,28 +1879,28 @@
   <autoFilter ref="A7:I12" xr:uid="{9BE7336F-352A-4FAE-B0E4-61965FC814C7}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B8DA50BB-4379-43D1-879B-CDBE6D82C13A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="74">
+    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="91">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="73">
+    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="90">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="72">
+    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="89">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="71">
+    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="88">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="70">
+    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="87">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="69">
+    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="86">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="68">
+    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="85">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="67">
+    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="84">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1593,28 +1913,28 @@
   <autoFilter ref="A8:I13" xr:uid="{67385006-CBB9-4472-99D4-7881E042769D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FD96F8F7-CCAB-44FA-B525-A5081670706A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="158">
+    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="178">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="157">
+    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="177">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="156">
+    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="176">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="155">
+    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="175">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="154">
+    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="174">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="153">
+    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="173">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="152">
+    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="172">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="151">
+    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="171">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1635,7 +1955,7 @@
     <tableColumn id="7" xr3:uid="{AEFF5C29-BE6A-4CF8-A2BB-F6B076077DA9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{4DE9B01E-67F2-4136-ADC3-60389FB67DCC}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{F5A82F03-513C-46D4-9F91-470F0060526B}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="66">
+    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="83">
       <calculatedColumnFormula>SUM(Table16821[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1644,22 +1964,22 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="65" tableBorderDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="82" tableBorderDxfId="81">
   <autoFilter ref="A15:I16" xr:uid="{434CBBE2-2F8D-4EEB-895C-68FC850EF1FD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="62">
+    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="79">
       <calculatedColumnFormula>Table1922[Level]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="61">
+    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="78">
       <calculatedColumnFormula>Table1922[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="60"/>
-    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="59"/>
-    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="58"/>
-    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="57"/>
-    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="56"/>
-    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="75"/>
+    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="74"/>
+    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="73"/>
+    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1670,28 +1990,28 @@
   <autoFilter ref="A3:I9" xr:uid="{A90D1C2A-DBF9-4EEF-ACC2-3DC17C207301}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BD3505AC-AE6D-4947-A74E-A6C2D68658F1}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="54">
+    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="71">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="53">
+    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="70">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="52">
+    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="69">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="51">
+    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="68">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="50">
+    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="67">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="49">
+    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="66">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="48">
+    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="65">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="47">
+    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="64">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1700,32 +2020,32 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="46" tableBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="63" tableBorderDxfId="62">
   <autoFilter ref="L3:T4" xr:uid="{5D2C3EA8-1297-4C77-AF32-84E50F8232C5}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="43">
+    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="60">
       <calculatedColumnFormula>Table19[Level]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="42">
+    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="59">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="41">
+    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="58">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="40">
+    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="57">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1 + 15 + 6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="39">
+    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="56">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="38">
+    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="55">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="37">
+    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="54">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="36">
+    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="53">
       <calculatedColumnFormula>Table19[Level] + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1734,6 +2054,87 @@
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{41A82D08-9A09-4219-84C8-447F62C5E4A5}" name="Table13161833" displayName="Table13161833" ref="A7:I12" totalsRowShown="0">
+  <autoFilter ref="A7:I12" xr:uid="{553298A4-7E43-42CF-9EEB-1F9E7E6BAD27}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{2AA35C8B-719C-4BA6-9CDF-2963E1C9F233}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{C087FAFA-9653-40EC-B4B9-5CB8F9D7255E}" name="HP" dataDxfId="19">
+      <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{0004B47B-3968-4C5A-BE6C-B822A307D7C5}" name="MP" dataDxfId="18">
+      <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*10+20</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{67EC8D91-0122-40D7-87D0-A3AB6788CE9D}" name="ATK" dataDxfId="0">
+      <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{E9988E54-33D6-41EB-B6BE-6E832544E18C}" name="DEF" dataDxfId="17">
+      <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{16D71A55-372C-4029-A831-ECF2325E46C4}" name="MAT" dataDxfId="16">
+      <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{1802FB48-B110-4DBF-A8F2-64CD4890E741}" name="MDF" dataDxfId="15">
+      <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{350CA8CC-761C-4994-9D80-14685787EF3D}" name="AGI" dataDxfId="14">
+      <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{B578CF58-136A-41B9-800E-D75836A4CDD1}" name="LUK" dataDxfId="13">
+      <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{B310FA79-C251-4887-8BA0-13EFC898E0EE}" name="Table1682134" displayName="Table1682134" ref="A4:J5" totalsRowShown="0">
+  <autoFilter ref="A4:J5" xr:uid="{A196C7A4-18CB-4B62-A1B5-F180559CC24F}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{5856C6A7-86D8-4034-9C75-EF0B447521E9}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{0323D56B-1230-40A6-9F39-A1F15B999EB9}" name="HP"/>
+    <tableColumn id="3" xr3:uid="{5047D0C1-3B69-43A4-8BB7-50413F800B48}" name="MP"/>
+    <tableColumn id="4" xr3:uid="{35844843-6592-40C2-87B2-39C1F8EAC612}" name="ATK"/>
+    <tableColumn id="5" xr3:uid="{1408F78D-2392-49EF-BC8D-CA3D7292C8AF}" name="DEF"/>
+    <tableColumn id="6" xr3:uid="{4D9C5D96-8CD0-4851-8FE4-5E19474329C4}" name="MAT"/>
+    <tableColumn id="7" xr3:uid="{5A405725-30A7-487F-95BF-061F71CA9C61}" name="MDF"/>
+    <tableColumn id="8" xr3:uid="{644DEF70-6EBD-403E-904B-6C30E5FBEA48}" name="AGI"/>
+    <tableColumn id="9" xr3:uid="{BA93DA54-96B9-48D1-80BB-C266771E13F1}" name="LUK"/>
+    <tableColumn id="10" xr3:uid="{3EBB17A5-47EA-458B-83A5-7056BE67D25F}" name="Total" dataDxfId="12">
+      <calculatedColumnFormula>SUM(Table1682134[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{A7C0F3AC-4E86-430D-AE55-8604641B493E}" name="Table192235" displayName="Table192235" ref="A15:I16" totalsRowShown="0" dataDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="A15:I16" xr:uid="{D0DF3ED4-9A21-493B-88F4-CE5814AF31C9}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{A78A876E-6C8B-4FC8-BFD4-A9BC80EA3FC2}" name="Level" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{4B423FFC-D037-484D-A927-2F66E15D422A}" name="HP" dataDxfId="8">
+      <calculatedColumnFormula>(Table192235[Level]*75 + 500)*2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{B695FEDE-EC59-44D8-AE99-CBF568DE5C93}" name="MP" dataDxfId="7">
+      <calculatedColumnFormula>Table192235[[#This Row],[Level]]*14 + 80</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{160D5D77-34E8-44F3-B51D-7CC0736DDCB1}" name="ATK" dataDxfId="6">
+      <calculatedColumnFormula>Table192235[[#This Row],[Level]]*1.5+ 15 + 50</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{559DAC37-CD6A-449F-AFF0-355ADE7CED80}" name="DEF" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{EEC344A5-27A5-450E-B795-04D237DD063F}" name="MAT" dataDxfId="4">
+      <calculatedColumnFormula>Table192235[Level]*1.5+15+50</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{54363CA4-9EE5-495F-8323-6C0C1261453C}" name="MDF" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{26B56E9D-2FCD-4476-A6CF-8F2EDC965246}" name="AGI" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{95814D66-3343-4190-9BF4-F4E45AB27D95}" name="LUK" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DE335D90-A9BD-40A2-B9C7-73CA6E6CAB11}" name="Table15" displayName="Table15" ref="A4:J8" totalsRowShown="0">
   <autoFilter ref="A4:J8" xr:uid="{CE759384-ADAA-40BA-B9E0-40CE462A16EC}"/>
   <tableColumns count="10">
@@ -1746,110 +2147,8 @@
     <tableColumn id="7" xr3:uid="{22216E02-260E-4471-8BB1-4E6E1250BAC9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{DC2670AC-8DF2-47F7-A3F6-EE7896309BC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{749652E2-F6CF-428C-B67C-FD0B1EFCCBBF}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="35">
+    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="52">
       <calculatedColumnFormula>SUM(Table15[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{11E951F1-5D13-41C6-A7E5-8F4298DA5463}" name="Table13167" displayName="Table13167" ref="A15:I20" totalsRowShown="0">
-  <autoFilter ref="A15:I20" xr:uid="{A1CF627F-8D28-44AD-9A35-411103976FCA}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{F14CC326-DE44-48D8-856F-8DCDCFC89CAD}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="34">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*63-100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="33">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*10</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="32">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="31">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="30">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="29">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="28">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="27">
-      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{60D4A7A8-82BF-4B58-A912-589523D22F05}" name="Table131679" displayName="Table131679" ref="K11:S17" totalsRowShown="0">
-  <autoFilter ref="K11:S17" xr:uid="{EAF9FB6A-F011-40E3-AB2F-E53826722AFB}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{DF3E0800-6EE4-4E1B-BA6F-0194351D6E7C}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="26">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*56.25+100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="25">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*10</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="24">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="23">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="22">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="21">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="20">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="19">
-      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{57801F89-51BE-4BC1-9BA3-39DF9D564857}" name="Table1316717" displayName="Table1316717" ref="A26:I31" totalsRowShown="0">
-  <autoFilter ref="A26:I31" xr:uid="{870F76F2-5EA7-4FD7-B1F9-507D64592088}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{3C04B742-338A-4366-BF3D-C5BC13023785}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="18">
-      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*63+100</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="17">
-      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*10</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="16">
-      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="15">
-      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="14">
-      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="13">
-      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="12">
-      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="11">
-      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1857,33 +2156,67 @@
 </file>
 
 <file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6BE19079-7252-4251-9EA9-046E7A11042F}" name="Table13167173" displayName="Table13167173" ref="A36:I41" totalsRowShown="0">
-  <autoFilter ref="A36:I41" xr:uid="{9BD043AF-0D77-4FF4-B2F9-B4AC3C3F1F82}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{11E951F1-5D13-41C6-A7E5-8F4298DA5463}" name="Table13167" displayName="Table13167" ref="A15:I20" totalsRowShown="0">
+  <autoFilter ref="A15:I20" xr:uid="{A1CF627F-8D28-44AD-9A35-411103976FCA}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{7BB908A3-05D7-4357-920B-BF4C6BC20C06}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="10">
-      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*56.5+200</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="9">
-      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*12.5</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="8">
-      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="7">
-      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1 + 15+14</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="6">
-      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="5">
-      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.5+ 15+13</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="4">
-      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="3">
-      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.375 + 15+40</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{F14CC326-DE44-48D8-856F-8DCDCFC89CAD}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="51">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*63-100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="50">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="49">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="48">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="47">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="46">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="45">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="44">
+      <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{60D4A7A8-82BF-4B58-A912-589523D22F05}" name="Table131679" displayName="Table131679" ref="K11:S17" totalsRowShown="0">
+  <autoFilter ref="K11:S17" xr:uid="{EAF9FB6A-F011-40E3-AB2F-E53826722AFB}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{DF3E0800-6EE4-4E1B-BA6F-0194351D6E7C}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="43">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*56.25+100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="42">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="41">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="40">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="39">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="38">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="37">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="36">
+      <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1895,29 +2228,97 @@
   <autoFilter ref="K8:S14" xr:uid="{AB7E938D-7ACC-4BFB-A6B9-682B8B29CEF2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{66EB8EF1-BCF4-44F7-B8A6-3C3B425F8FF5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="150">
+    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="170">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*56.25+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="149">
+    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="169">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="148">
+    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="168">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25+ 15+30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="147">
+    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="167">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25 + 15+33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="146">
+    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="166">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="145">
+    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="165">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="144">
+    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="164">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="143">
+    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="163">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{57801F89-51BE-4BC1-9BA3-39DF9D564857}" name="Table1316717" displayName="Table1316717" ref="A26:I31" totalsRowShown="0">
+  <autoFilter ref="A26:I31" xr:uid="{870F76F2-5EA7-4FD7-B1F9-507D64592088}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{3C04B742-338A-4366-BF3D-C5BC13023785}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="35">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*63+100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="34">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="33">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="32">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="31">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="30">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="29">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="28">
+      <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6BE19079-7252-4251-9EA9-046E7A11042F}" name="Table13167173" displayName="Table13167173" ref="A36:I41" totalsRowShown="0">
+  <autoFilter ref="A36:I41" xr:uid="{9BD043AF-0D77-4FF4-B2F9-B4AC3C3F1F82}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{7BB908A3-05D7-4357-920B-BF4C6BC20C06}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="27">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*56.5+200</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="26">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*12.5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="25">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="24">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1 + 15+14</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="23">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="22">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.5+ 15+13</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="21">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="20">
+      <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.375 + 15+40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1937,7 +2338,7 @@
     <tableColumn id="7" xr3:uid="{F833922A-76F9-427C-8462-D94DE51D0477}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{203171A1-C88B-4F81-ADC2-1EE072D645F3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{34003EF6-E9A5-4584-A186-09DFF4EC11C7}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{C4602156-F897-42BE-8F3F-411E13EEB095}" name="Total" dataDxfId="142">
+    <tableColumn id="10" xr3:uid="{C4602156-F897-42BE-8F3F-411E13EEB095}" name="Total" dataDxfId="162">
       <calculatedColumnFormula>SUM(Table114[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1950,28 +2351,28 @@
   <autoFilter ref="A8:I14" xr:uid="{D3C3F418-ED32-4504-9D73-88545A192967}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{13E0AF4A-AA83-489A-A156-B01D4F48D2F5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{B970139F-8BB5-4CE6-92F8-79E3236AC62B}" name="HP" dataDxfId="141">
+    <tableColumn id="2" xr3:uid="{B970139F-8BB5-4CE6-92F8-79E3236AC62B}" name="HP" dataDxfId="161">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*63+300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7BCF83B8-7492-4991-A008-F212725940B9}" name="MP" dataDxfId="140">
+    <tableColumn id="3" xr3:uid="{7BCF83B8-7492-4991-A008-F212725940B9}" name="MP" dataDxfId="160">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{33220A80-38D8-4480-ACC7-DF484072C96B}" name="ATK" dataDxfId="139">
+    <tableColumn id="4" xr3:uid="{33220A80-38D8-4480-ACC7-DF484072C96B}" name="ATK" dataDxfId="159">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.5+ 15+40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{36708515-5004-4705-A558-44B59D0CE676}" name="DEF" dataDxfId="138">
+    <tableColumn id="5" xr3:uid="{36708515-5004-4705-A558-44B59D0CE676}" name="DEF" dataDxfId="158">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25 + 15+21</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{11729EA3-08C4-4E0B-B5EE-5B3C08A31A9C}" name="MAT" dataDxfId="137">
+    <tableColumn id="6" xr3:uid="{11729EA3-08C4-4E0B-B5EE-5B3C08A31A9C}" name="MAT" dataDxfId="157">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B179D090-E484-4663-937A-480D1164D655}" name="MDF" dataDxfId="136">
+    <tableColumn id="7" xr3:uid="{B179D090-E484-4663-937A-480D1164D655}" name="MDF" dataDxfId="156">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25+15 + 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{28323AD0-B3BD-401F-A237-92C8B8D70FEA}" name="AGI" dataDxfId="135">
+    <tableColumn id="8" xr3:uid="{28323AD0-B3BD-401F-A237-92C8B8D70FEA}" name="AGI" dataDxfId="155">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{657BED8B-4C8A-42DC-BECD-5EEF9D1B7F37}" name="LUK" dataDxfId="134">
+    <tableColumn id="9" xr3:uid="{657BED8B-4C8A-42DC-BECD-5EEF9D1B7F37}" name="LUK" dataDxfId="154">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1992,7 +2393,7 @@
     <tableColumn id="7" xr3:uid="{D1DFC0D2-A987-4E3F-BA23-52162FB0C0BA}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{AB6209DB-CCCB-4C37-B455-4C7652E0DAC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2CD4CD14-92FD-41A7-9CCD-1329B5A77390}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{3B2C0A10-5038-4C21-BAC5-12FB16275D2E}" name="Total" dataDxfId="133">
+    <tableColumn id="10" xr3:uid="{3B2C0A10-5038-4C21-BAC5-12FB16275D2E}" name="Total" dataDxfId="153">
       <calculatedColumnFormula>SUM(Table11412[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2005,28 +2406,28 @@
   <autoFilter ref="A8:I14" xr:uid="{43F790D1-EA7B-4BAE-8A37-7CAD791E8821}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F6E842E1-B25F-4CA1-9107-AC7179420C29}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EFB2F0D5-318D-4A65-BA2B-20ADDE071648}" name="HP" dataDxfId="132">
+    <tableColumn id="2" xr3:uid="{EFB2F0D5-318D-4A65-BA2B-20ADDE071648}" name="HP" dataDxfId="152">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0D914B89-2678-453F-BC18-571DCD45E628}" name="MP" dataDxfId="131">
+    <tableColumn id="3" xr3:uid="{0D914B89-2678-453F-BC18-571DCD45E628}" name="MP" dataDxfId="151">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*13.75 + 80</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{6FBD2F64-5B1C-4035-BB1A-AFB092DB60C3}" name="ATK" dataDxfId="130">
+    <tableColumn id="4" xr3:uid="{6FBD2F64-5B1C-4035-BB1A-AFB092DB60C3}" name="ATK" dataDxfId="150">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7E0AF3FC-CC5D-4A6A-A4A2-DE278DEC4062}" name="DEF" dataDxfId="129">
+    <tableColumn id="5" xr3:uid="{7E0AF3FC-CC5D-4A6A-A4A2-DE278DEC4062}" name="DEF" dataDxfId="149">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1 + 15 + 4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3AF4D559-893B-4D50-BCB4-A1BD1FAF2F23}" name="MAT" dataDxfId="128">
+    <tableColumn id="6" xr3:uid="{3AF4D559-893B-4D50-BCB4-A1BD1FAF2F23}" name="MAT" dataDxfId="148">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6E9418A6-75AC-4541-9029-814EC5C06E70}" name="MDF" dataDxfId="127">
+    <tableColumn id="7" xr3:uid="{6E9418A6-75AC-4541-9029-814EC5C06E70}" name="MDF" dataDxfId="147">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.375+15 + 14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD605BEE-D561-4A2C-8D06-8E9AD70C32AC}" name="AGI" dataDxfId="126">
+    <tableColumn id="8" xr3:uid="{CD605BEE-D561-4A2C-8D06-8E9AD70C32AC}" name="AGI" dataDxfId="146">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E26506B2-F488-4AA4-AC87-819A22964609}" name="LUK" dataDxfId="125">
+    <tableColumn id="9" xr3:uid="{E26506B2-F488-4AA4-AC87-819A22964609}" name="LUK" dataDxfId="145">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2047,7 +2448,7 @@
     <tableColumn id="7" xr3:uid="{E91A64A8-F750-4893-9958-7C6ABC37405F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{3832FF0E-95E5-4B1F-B122-1EAFBF719DE3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{237404A9-EB50-465E-89AF-7167C57AFB99}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{927EBD24-571F-408C-A33B-59C753D9D96D}" name="Total" dataDxfId="124">
+    <tableColumn id="10" xr3:uid="{927EBD24-571F-408C-A33B-59C753D9D96D}" name="Total" dataDxfId="144">
       <calculatedColumnFormula>SUM(Table1141219[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2060,28 +2461,28 @@
   <autoFilter ref="A7:I13" xr:uid="{2539D8EE-2982-4734-B28B-342036FEDAC6}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FEE8F081-132E-4ED3-8FFD-2CF48368B2CC}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A79BC043-DB1A-48B4-AC21-AD31632979A6}" name="HP" dataDxfId="123">
+    <tableColumn id="2" xr3:uid="{A79BC043-DB1A-48B4-AC21-AD31632979A6}" name="HP" dataDxfId="143">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*63 + 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{42935B44-C727-42B0-B48E-0369818BF78A}" name="MP" dataDxfId="122">
+    <tableColumn id="3" xr3:uid="{42935B44-C727-42B0-B48E-0369818BF78A}" name="MP" dataDxfId="142">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{FC4572C7-88EC-4981-A6ED-43397844845B}" name="ATK" dataDxfId="121">
+    <tableColumn id="4" xr3:uid="{FC4572C7-88EC-4981-A6ED-43397844845B}" name="ATK" dataDxfId="141">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C8D61CEB-FFEC-42C3-9123-5140E65C1A2C}" name="DEF" dataDxfId="120">
+    <tableColumn id="5" xr3:uid="{C8D61CEB-FFEC-42C3-9123-5140E65C1A2C}" name="DEF" dataDxfId="140">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.375 + 15 + 19</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8C971683-28D2-4474-83CA-936F352F1324}" name="MAT" dataDxfId="119">
+    <tableColumn id="6" xr3:uid="{8C971683-28D2-4474-83CA-936F352F1324}" name="MAT" dataDxfId="139">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3371862A-9CF2-47CA-A149-4921E3B33162}" name="MDF" dataDxfId="118">
+    <tableColumn id="7" xr3:uid="{3371862A-9CF2-47CA-A149-4921E3B33162}" name="MDF" dataDxfId="138">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.375+15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC6AC739-B4C9-47A6-9472-439C60B629A0}" name="AGI" dataDxfId="117">
+    <tableColumn id="8" xr3:uid="{AC6AC739-B4C9-47A6-9472-439C60B629A0}" name="AGI" dataDxfId="137">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E727A271-B479-47C0-A557-227ABD8EC0AC}" name="LUK" dataDxfId="116">
+    <tableColumn id="9" xr3:uid="{E727A271-B479-47C0-A557-227ABD8EC0AC}" name="LUK" dataDxfId="136">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2947,7 +3348,7 @@
   <dimension ref="A2:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="A2" sqref="A2:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3316,7 +3717,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="L3" sqref="L3:T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3658,6 +4059,372 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5005335F-A4EA-4889-9D4A-6AE8EF295080}">
+  <dimension ref="A2:J16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <f>SUM(Table1682134[[#This Row],[HP]:[LUK]])</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <f>Table13161833[[#This Row],[Level]]*75 + 500</f>
+        <v>575</v>
+      </c>
+      <c r="C8">
+        <f>Table13161833[[#This Row],[Level]]*10+20</f>
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <f>Table13161833[[#This Row],[Level]]*1.5+ 15</f>
+        <v>16.5</v>
+      </c>
+      <c r="E8">
+        <f>Table13161833[[#This Row],[Level]]*1.5 + 15</f>
+        <v>16.5</v>
+      </c>
+      <c r="F8">
+        <f>Table13161833[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+      <c r="G8">
+        <f>Table13161833[[#This Row],[Level]]*1.5 + 15</f>
+        <v>16.5</v>
+      </c>
+      <c r="H8">
+        <f>Table13161833[[#This Row],[Level]]*1.375 + 15</f>
+        <v>16.375</v>
+      </c>
+      <c r="I8">
+        <f>Table13161833[[#This Row],[Level]]*1.125 + 15</f>
+        <v>16.125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <f>Table13161833[[#This Row],[Level]]*75 + 500</f>
+        <v>1625</v>
+      </c>
+      <c r="C9">
+        <f>Table13161833[[#This Row],[Level]]*10+20</f>
+        <v>170</v>
+      </c>
+      <c r="D9">
+        <f>Table13161833[[#This Row],[Level]]*1.5+ 15</f>
+        <v>37.5</v>
+      </c>
+      <c r="E9">
+        <f>Table13161833[[#This Row],[Level]]*1.5 + 15</f>
+        <v>37.5</v>
+      </c>
+      <c r="F9">
+        <f>Table13161833[[#This Row],[Level]]*1 + 15</f>
+        <v>30</v>
+      </c>
+      <c r="G9">
+        <f>Table13161833[[#This Row],[Level]]*1.5 + 15</f>
+        <v>37.5</v>
+      </c>
+      <c r="H9">
+        <f>Table13161833[[#This Row],[Level]]*1.375 + 15</f>
+        <v>35.625</v>
+      </c>
+      <c r="I9">
+        <f>Table13161833[[#This Row],[Level]]*1.125 + 15</f>
+        <v>31.875</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <f>Table13161833[[#This Row],[Level]]*75 + 500</f>
+        <v>2375</v>
+      </c>
+      <c r="C10">
+        <f>Table13161833[[#This Row],[Level]]*10+20</f>
+        <v>270</v>
+      </c>
+      <c r="D10">
+        <f>Table13161833[[#This Row],[Level]]*1.5+ 15</f>
+        <v>52.5</v>
+      </c>
+      <c r="E10">
+        <f>Table13161833[[#This Row],[Level]]*1.5 + 15</f>
+        <v>52.5</v>
+      </c>
+      <c r="F10">
+        <f>Table13161833[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="G10">
+        <f>Table13161833[[#This Row],[Level]]*1.5 + 15</f>
+        <v>52.5</v>
+      </c>
+      <c r="H10">
+        <f>Table13161833[[#This Row],[Level]]*1.375 + 15</f>
+        <v>49.375</v>
+      </c>
+      <c r="I10">
+        <f>Table13161833[[#This Row],[Level]]*1.125 + 15</f>
+        <v>43.125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>35</v>
+      </c>
+      <c r="B11">
+        <f>Table13161833[[#This Row],[Level]]*75 + 500</f>
+        <v>3125</v>
+      </c>
+      <c r="C11">
+        <f>Table13161833[[#This Row],[Level]]*10+20</f>
+        <v>370</v>
+      </c>
+      <c r="D11">
+        <f>Table13161833[[#This Row],[Level]]*1.5+ 15</f>
+        <v>67.5</v>
+      </c>
+      <c r="E11">
+        <f>Table13161833[[#This Row],[Level]]*1.5 + 15</f>
+        <v>67.5</v>
+      </c>
+      <c r="F11">
+        <f>Table13161833[[#This Row],[Level]]*1 + 15</f>
+        <v>50</v>
+      </c>
+      <c r="G11">
+        <f>Table13161833[[#This Row],[Level]]*1.5 + 15</f>
+        <v>67.5</v>
+      </c>
+      <c r="H11">
+        <f>Table13161833[[#This Row],[Level]]*1.375 + 15</f>
+        <v>63.125</v>
+      </c>
+      <c r="I11">
+        <f>Table13161833[[#This Row],[Level]]*1.125 + 15</f>
+        <v>54.375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <f>Table13161833[[#This Row],[Level]]*75 + 500</f>
+        <v>2000</v>
+      </c>
+      <c r="C12">
+        <f>Table13161833[[#This Row],[Level]]*10+20</f>
+        <v>220</v>
+      </c>
+      <c r="D12">
+        <f>Table13161833[[#This Row],[Level]]*1.5+ 15</f>
+        <v>45</v>
+      </c>
+      <c r="E12">
+        <f>Table13161833[[#This Row],[Level]]*1.5 + 15</f>
+        <v>45</v>
+      </c>
+      <c r="F12">
+        <f>Table13161833[[#This Row],[Level]]*1 + 15</f>
+        <v>35</v>
+      </c>
+      <c r="G12">
+        <f>Table13161833[[#This Row],[Level]]*1.5 + 15</f>
+        <v>45</v>
+      </c>
+      <c r="H12">
+        <f>Table13161833[[#This Row],[Level]]*1.375 + 15</f>
+        <v>42.5</v>
+      </c>
+      <c r="I12">
+        <f>Table13161833[[#This Row],[Level]]*1.125 + 15</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>20</v>
+      </c>
+      <c r="B16" s="3">
+        <f>(Table192235[Level]*75 + 500)*2</f>
+        <v>4000</v>
+      </c>
+      <c r="C16" s="3">
+        <f>Table192235[[#This Row],[Level]]*14 + 80</f>
+        <v>360</v>
+      </c>
+      <c r="D16" s="3">
+        <f>Table192235[[#This Row],[Level]]*1.5+ 15 + 50</f>
+        <v>95</v>
+      </c>
+      <c r="E16" s="3">
+        <v>75</v>
+      </c>
+      <c r="F16" s="3">
+        <f>Table192235[Level]*1.5+15+50</f>
+        <v>95</v>
+      </c>
+      <c r="G16" s="3">
+        <v>75</v>
+      </c>
+      <c r="H16" s="3">
+        <v>42.5</v>
+      </c>
+      <c r="I16" s="4">
+        <v>37.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4195E475-9F10-4DD8-82F0-E47D9A595A6E}">
   <dimension ref="A2:S41"/>
   <sheetViews>
@@ -7153,7 +7920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA7AE8E-3CBD-43D4-8334-3506A3BDF6FA}">
   <dimension ref="A2:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Working on main plot's script. Really long conversations are really long
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="7" activeTab="11" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="8" activeTab="13" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Skeleton Soldier" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="VillianCanson" sheetId="4" r:id="rId11"/>
     <sheet name="Death Lord" sheetId="15" r:id="rId12"/>
     <sheet name="Goblin" sheetId="2" r:id="rId13"/>
+    <sheet name="Slimes" sheetId="16" r:id="rId14"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="56">
   <si>
     <t>Skeletons are the most basic undead, they have low magical attributes, agility, and luck.</t>
   </si>
@@ -202,6 +203,9 @@
   <si>
     <t>Death Lords are giant undead</t>
   </si>
+  <si>
+    <t>Slime</t>
+  </si>
 </sst>
 </file>
 
@@ -277,7 +281,130 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="180">
+  <dxfs count="189">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -598,102 +725,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1612,7 +1643,7 @@
     <tableColumn id="7" xr3:uid="{F9852B29-E77D-4E17-A56E-5F0C649FA862}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{9A914BFF-1060-46E4-B8F9-412BD9293C3D}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2F83B650-811D-4FEE-92D5-03D4DC4376E5}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="179">
+    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="188">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1633,7 +1664,7 @@
     <tableColumn id="7" xr3:uid="{3A2FD57C-060A-462E-8BB9-B06F717E9D20}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{ED9393EA-F7F9-4661-8D0B-0D9246DDABF8}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{6F56342F-5442-42CD-8B6C-D98B6D6C0C56}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="135">
+    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="144">
       <calculatedColumnFormula>SUM(Table16[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1646,28 +1677,28 @@
   <autoFilter ref="A8:I13" xr:uid="{7BE337CC-37BD-4688-B60D-A66F4420668B}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{71340E4C-6101-4C59-8ED7-689E2AD5A962}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="134">
+    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="143">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*63-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="133">
+    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="142">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="132">
+    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="141">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="131">
+    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="140">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="130">
+    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="139">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="129">
+    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="138">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="128">
+    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="137">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="127">
+    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="136">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1688,7 +1719,7 @@
     <tableColumn id="7" xr3:uid="{4899BF24-9D2A-4CC0-AE35-4F49604AAC5A}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{CB1CC6BA-1D38-4B74-9BC6-7057FB9773EE}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{C47FADF6-C526-4188-9187-383757CE17C1}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="126">
+    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="135">
       <calculatedColumnFormula>SUM(Table168[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1701,28 +1732,28 @@
   <autoFilter ref="A9:I15" xr:uid="{06A56D17-07E5-4650-8EE9-7EA8F94D4020}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A2BE27C9-9DAE-49F5-9A70-C6CF7428BF31}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="125">
+    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="134">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="124">
+    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="133">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="123">
+    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="132">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="122">
+    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="131">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="121">
+    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="130">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.375+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="120">
+    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="129">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="119">
+    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="128">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="118">
+    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="127">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1743,7 +1774,7 @@
     <tableColumn id="7" xr3:uid="{60AD88FB-4685-412B-B5FD-BF8412C6B8E2}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{6A88D48C-D864-4F16-BEF2-BA88783A3FF3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{D40BD230-6392-4A28-A29D-F13EFE35C95E}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A0E09B2B-FD41-413F-8063-62214E990751}" name="Total" dataDxfId="117">
+    <tableColumn id="10" xr3:uid="{A0E09B2B-FD41-413F-8063-62214E990751}" name="Total" dataDxfId="126">
       <calculatedColumnFormula>SUM(Table16826[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1756,28 +1787,28 @@
   <autoFilter ref="A8:I14" xr:uid="{F7062CBA-4FAA-4900-9D3A-5C6613BCB6CE}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{ADCB4852-D3A0-456B-A8BD-E5F74BDBB762}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{ED76047D-1BC2-4C1B-B9B0-58BE0ACDDA48}" name="HP" dataDxfId="116">
+    <tableColumn id="2" xr3:uid="{ED76047D-1BC2-4C1B-B9B0-58BE0ACDDA48}" name="HP" dataDxfId="125">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EC859C53-0BA5-45D1-868B-F22DC8CE7D25}" name="MP" dataDxfId="115">
+    <tableColumn id="3" xr3:uid="{EC859C53-0BA5-45D1-868B-F22DC8CE7D25}" name="MP" dataDxfId="124">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DED33AB9-A2BB-4F9E-AA6D-02F8D1D65CD1}" name="ATK" dataDxfId="114">
+    <tableColumn id="4" xr3:uid="{DED33AB9-A2BB-4F9E-AA6D-02F8D1D65CD1}" name="ATK" dataDxfId="123">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.375+ 15+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{329B716D-9CA6-4546-AB13-92D88BE40F5F}" name="DEF" dataDxfId="113">
+    <tableColumn id="5" xr3:uid="{329B716D-9CA6-4546-AB13-92D88BE40F5F}" name="DEF" dataDxfId="122">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1 + 15+12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{67F8198A-5FC2-4C6D-9558-68B3141EA756}" name="MAT" dataDxfId="112">
+    <tableColumn id="6" xr3:uid="{67F8198A-5FC2-4C6D-9558-68B3141EA756}" name="MAT" dataDxfId="121">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C70F5BF6-63B0-44C1-862D-25E3FB55320F}" name="MDF" dataDxfId="111">
+    <tableColumn id="7" xr3:uid="{C70F5BF6-63B0-44C1-862D-25E3FB55320F}" name="MDF" dataDxfId="120">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.5+15+11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AB20AF53-453C-4266-A46B-40E693C91985}" name="AGI" dataDxfId="110">
+    <tableColumn id="8" xr3:uid="{AB20AF53-453C-4266-A46B-40E693C91985}" name="AGI" dataDxfId="119">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7FC46A31-F9F1-432E-B399-0823E198FE0A}" name="LUK" dataDxfId="109">
+    <tableColumn id="9" xr3:uid="{7FC46A31-F9F1-432E-B399-0823E198FE0A}" name="LUK" dataDxfId="118">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.5+15+20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1798,7 +1829,7 @@
     <tableColumn id="7" xr3:uid="{20C5D094-BAF0-471C-ACF3-C6658991DB5F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{E08E2AF0-56DD-4A69-A536-27139D793022}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{12AD8606-1127-4E5B-BA2C-872780F22F9E}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{5E2EF778-63AE-48B7-9F49-0D2AFEBD66A1}" name="Total" dataDxfId="108">
+    <tableColumn id="10" xr3:uid="{5E2EF778-63AE-48B7-9F49-0D2AFEBD66A1}" name="Total" dataDxfId="117">
       <calculatedColumnFormula>SUM(Table1682630[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1811,28 +1842,28 @@
   <autoFilter ref="A8:I14" xr:uid="{299912CC-280B-49E1-8859-432D05893259}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4F0B657F-C9A5-4A73-AAA3-27D307385193}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{526284E7-597F-4726-AB18-230CA03461B1}" name="HP" dataDxfId="107">
+    <tableColumn id="2" xr3:uid="{526284E7-597F-4726-AB18-230CA03461B1}" name="HP" dataDxfId="116">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*63+ 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E7BA3C7A-2677-415F-BA47-A4E88679B948}" name="MP" dataDxfId="106">
+    <tableColumn id="3" xr3:uid="{E7BA3C7A-2677-415F-BA47-A4E88679B948}" name="MP" dataDxfId="115">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE7BE678-2229-44F6-8732-71214FB69DD7}" name="ATK" dataDxfId="105">
+    <tableColumn id="4" xr3:uid="{AE7BE678-2229-44F6-8732-71214FB69DD7}" name="ATK" dataDxfId="114">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+ 15+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4715E3DB-8817-43D5-9074-9FB5F0BEF5B4}" name="DEF" dataDxfId="104">
+    <tableColumn id="5" xr3:uid="{4715E3DB-8817-43D5-9074-9FB5F0BEF5B4}" name="DEF" dataDxfId="113">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1 + 15+12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9CE76933-D045-418B-A975-378EEA51D856}" name="MAT" dataDxfId="103">
+    <tableColumn id="6" xr3:uid="{9CE76933-D045-418B-A975-378EEA51D856}" name="MAT" dataDxfId="112">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244B9611-6CB0-4946-B5CD-7D42311C7D7E}" name="MDF" dataDxfId="102">
+    <tableColumn id="7" xr3:uid="{244B9611-6CB0-4946-B5CD-7D42311C7D7E}" name="MDF" dataDxfId="111">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+15+11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32550C13-49BB-41D2-BA0A-26798830A0FD}" name="AGI" dataDxfId="101">
+    <tableColumn id="8" xr3:uid="{32550C13-49BB-41D2-BA0A-26798830A0FD}" name="AGI" dataDxfId="110">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{BB22F289-8AF5-4DD6-877B-F09520710555}" name="LUK" dataDxfId="100">
+    <tableColumn id="9" xr3:uid="{BB22F289-8AF5-4DD6-877B-F09520710555}" name="LUK" dataDxfId="109">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+15+20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1845,28 +1876,28 @@
   <autoFilter ref="A4:I10" xr:uid="{A1EAC62C-C07D-464E-91B1-4A34E6604BA2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{430FD3D4-914C-4309-B2E6-6F01B5CAED94}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="99">
+    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="108">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="98">
+    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="107">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="97">
+    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="106">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="96">
+    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="105">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15 + 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="95">
+    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="104">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15 + 30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="94">
+    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="103">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15 + 21</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="93">
+    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="102">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="92">
+    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="101">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1879,28 +1910,28 @@
   <autoFilter ref="A7:I12" xr:uid="{9BE7336F-352A-4FAE-B0E4-61965FC814C7}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B8DA50BB-4379-43D1-879B-CDBE6D82C13A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="91">
+    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="100">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="90">
+    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="99">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="89">
+    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="98">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="88">
+    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="97">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="87">
+    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="96">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="86">
+    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="95">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="85">
+    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="94">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="84">
+    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="93">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1913,28 +1944,28 @@
   <autoFilter ref="A8:I13" xr:uid="{67385006-CBB9-4472-99D4-7881E042769D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FD96F8F7-CCAB-44FA-B525-A5081670706A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="178">
+    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="187">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="177">
+    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="186">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="176">
+    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="185">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="175">
+    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="184">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="174">
+    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="183">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="173">
+    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="182">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="172">
+    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="181">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="171">
+    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="180">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1955,7 +1986,7 @@
     <tableColumn id="7" xr3:uid="{AEFF5C29-BE6A-4CF8-A2BB-F6B076077DA9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{4DE9B01E-67F2-4136-ADC3-60389FB67DCC}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{F5A82F03-513C-46D4-9F91-470F0060526B}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="83">
+    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="92">
       <calculatedColumnFormula>SUM(Table16821[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1964,22 +1995,22 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="82" tableBorderDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="91" tableBorderDxfId="90">
   <autoFilter ref="A15:I16" xr:uid="{434CBBE2-2F8D-4EEB-895C-68FC850EF1FD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="79">
+    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="89"/>
+    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="88">
       <calculatedColumnFormula>Table1922[Level]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="78">
+    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="87">
       <calculatedColumnFormula>Table1922[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="76"/>
-    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="75"/>
-    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="74"/>
-    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="73"/>
-    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="72"/>
+    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="86"/>
+    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="85"/>
+    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="84"/>
+    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="83"/>
+    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="82"/>
+    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1990,28 +2021,28 @@
   <autoFilter ref="A3:I9" xr:uid="{A90D1C2A-DBF9-4EEF-ACC2-3DC17C207301}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BD3505AC-AE6D-4947-A74E-A6C2D68658F1}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="71">
+    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="80">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="70">
+    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="79">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="69">
+    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="78">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="68">
+    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="77">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="67">
+    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="76">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="66">
+    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="75">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="65">
+    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="74">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="64">
+    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="73">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2020,32 +2051,32 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="63" tableBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="72" tableBorderDxfId="71">
   <autoFilter ref="L3:T4" xr:uid="{5D2C3EA8-1297-4C77-AF32-84E50F8232C5}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="60">
+    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="69">
       <calculatedColumnFormula>Table19[Level]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="59">
+    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="68">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="58">
+    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="67">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="57">
+    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="66">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1 + 15 + 6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="56">
+    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="65">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="55">
+    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="64">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="54">
+    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="63">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="53">
+    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="62">
       <calculatedColumnFormula>Table19[Level] + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2058,28 +2089,28 @@
   <autoFilter ref="A7:I12" xr:uid="{553298A4-7E43-42CF-9EEB-1F9E7E6BAD27}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2AA35C8B-719C-4BA6-9CDF-2963E1C9F233}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C087FAFA-9653-40EC-B4B9-5CB8F9D7255E}" name="HP" dataDxfId="19">
+    <tableColumn id="2" xr3:uid="{C087FAFA-9653-40EC-B4B9-5CB8F9D7255E}" name="HP" dataDxfId="61">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0004B47B-3968-4C5A-BE6C-B822A307D7C5}" name="MP" dataDxfId="18">
+    <tableColumn id="3" xr3:uid="{0004B47B-3968-4C5A-BE6C-B822A307D7C5}" name="MP" dataDxfId="60">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{67EC8D91-0122-40D7-87D0-A3AB6788CE9D}" name="ATK" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{67EC8D91-0122-40D7-87D0-A3AB6788CE9D}" name="ATK" dataDxfId="59">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E9988E54-33D6-41EB-B6BE-6E832544E18C}" name="DEF" dataDxfId="17">
+    <tableColumn id="5" xr3:uid="{E9988E54-33D6-41EB-B6BE-6E832544E18C}" name="DEF" dataDxfId="58">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{16D71A55-372C-4029-A831-ECF2325E46C4}" name="MAT" dataDxfId="16">
+    <tableColumn id="6" xr3:uid="{16D71A55-372C-4029-A831-ECF2325E46C4}" name="MAT" dataDxfId="57">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{1802FB48-B110-4DBF-A8F2-64CD4890E741}" name="MDF" dataDxfId="15">
+    <tableColumn id="7" xr3:uid="{1802FB48-B110-4DBF-A8F2-64CD4890E741}" name="MDF" dataDxfId="56">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{350CA8CC-761C-4994-9D80-14685787EF3D}" name="AGI" dataDxfId="14">
+    <tableColumn id="8" xr3:uid="{350CA8CC-761C-4994-9D80-14685787EF3D}" name="AGI" dataDxfId="55">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B578CF58-136A-41B9-800E-D75836A4CDD1}" name="LUK" dataDxfId="13">
+    <tableColumn id="9" xr3:uid="{B578CF58-136A-41B9-800E-D75836A4CDD1}" name="LUK" dataDxfId="54">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2100,7 +2131,7 @@
     <tableColumn id="7" xr3:uid="{5A405725-30A7-487F-95BF-061F71CA9C61}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{644DEF70-6EBD-403E-904B-6C30E5FBEA48}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{BA93DA54-96B9-48D1-80BB-C266771E13F1}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{3EBB17A5-47EA-458B-83A5-7056BE67D25F}" name="Total" dataDxfId="12">
+    <tableColumn id="10" xr3:uid="{3EBB17A5-47EA-458B-83A5-7056BE67D25F}" name="Total" dataDxfId="53">
       <calculatedColumnFormula>SUM(Table1682134[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2109,26 +2140,26 @@
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{A7C0F3AC-4E86-430D-AE55-8604641B493E}" name="Table192235" displayName="Table192235" ref="A15:I16" totalsRowShown="0" dataDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{A7C0F3AC-4E86-430D-AE55-8604641B493E}" name="Table192235" displayName="Table192235" ref="A15:I16" totalsRowShown="0" dataDxfId="52" tableBorderDxfId="51">
   <autoFilter ref="A15:I16" xr:uid="{D0DF3ED4-9A21-493B-88F4-CE5814AF31C9}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A78A876E-6C8B-4FC8-BFD4-A9BC80EA3FC2}" name="Level" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{4B423FFC-D037-484D-A927-2F66E15D422A}" name="HP" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{A78A876E-6C8B-4FC8-BFD4-A9BC80EA3FC2}" name="Level" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{4B423FFC-D037-484D-A927-2F66E15D422A}" name="HP" dataDxfId="49">
       <calculatedColumnFormula>(Table192235[Level]*75 + 500)*2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B695FEDE-EC59-44D8-AE99-CBF568DE5C93}" name="MP" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{B695FEDE-EC59-44D8-AE99-CBF568DE5C93}" name="MP" dataDxfId="48">
       <calculatedColumnFormula>Table192235[[#This Row],[Level]]*14 + 80</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{160D5D77-34E8-44F3-B51D-7CC0736DDCB1}" name="ATK" dataDxfId="6">
+    <tableColumn id="4" xr3:uid="{160D5D77-34E8-44F3-B51D-7CC0736DDCB1}" name="ATK" dataDxfId="47">
       <calculatedColumnFormula>Table192235[[#This Row],[Level]]*1.5+ 15 + 50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{559DAC37-CD6A-449F-AFF0-355ADE7CED80}" name="DEF" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{EEC344A5-27A5-450E-B795-04D237DD063F}" name="MAT" dataDxfId="4">
+    <tableColumn id="5" xr3:uid="{559DAC37-CD6A-449F-AFF0-355ADE7CED80}" name="DEF" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{EEC344A5-27A5-450E-B795-04D237DD063F}" name="MAT" dataDxfId="45">
       <calculatedColumnFormula>Table192235[Level]*1.5+15+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{54363CA4-9EE5-495F-8323-6C0C1261453C}" name="MDF" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{26B56E9D-2FCD-4476-A6CF-8F2EDC965246}" name="AGI" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{95814D66-3343-4190-9BF4-F4E45AB27D95}" name="LUK" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{54363CA4-9EE5-495F-8323-6C0C1261453C}" name="MDF" dataDxfId="44"/>
+    <tableColumn id="8" xr3:uid="{26B56E9D-2FCD-4476-A6CF-8F2EDC965246}" name="AGI" dataDxfId="43"/>
+    <tableColumn id="9" xr3:uid="{95814D66-3343-4190-9BF4-F4E45AB27D95}" name="LUK" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2147,7 +2178,7 @@
     <tableColumn id="7" xr3:uid="{22216E02-260E-4471-8BB1-4E6E1250BAC9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{DC2670AC-8DF2-47F7-A3F6-EE7896309BC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{749652E2-F6CF-428C-B67C-FD0B1EFCCBBF}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="52">
+    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="41">
       <calculatedColumnFormula>SUM(Table15[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2160,28 +2191,28 @@
   <autoFilter ref="A15:I20" xr:uid="{A1CF627F-8D28-44AD-9A35-411103976FCA}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F14CC326-DE44-48D8-856F-8DCDCFC89CAD}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="51">
+    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="40">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*63-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="50">
+    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="39">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="49">
+    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="38">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="48">
+    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="37">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="47">
+    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="36">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="46">
+    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="35">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="45">
+    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="34">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="44">
+    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="33">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2194,28 +2225,28 @@
   <autoFilter ref="K11:S17" xr:uid="{EAF9FB6A-F011-40E3-AB2F-E53826722AFB}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DF3E0800-6EE4-4E1B-BA6F-0194351D6E7C}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="43">
+    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="32">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*56.25+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="42">
+    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="31">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="41">
+    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="30">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="40">
+    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="29">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="39">
+    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="28">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="38">
+    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="27">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="37">
+    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="26">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="36">
+    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="25">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2228,28 +2259,28 @@
   <autoFilter ref="K8:S14" xr:uid="{AB7E938D-7ACC-4BFB-A6B9-682B8B29CEF2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{66EB8EF1-BCF4-44F7-B8A6-3C3B425F8FF5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="170">
+    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="179">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*56.25+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="169">
+    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="178">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="168">
+    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="177">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25+ 15+30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="167">
+    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="176">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25 + 15+33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="166">
+    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="175">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="165">
+    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="174">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="164">
+    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="173">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="163">
+    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="172">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2262,28 +2293,28 @@
   <autoFilter ref="A26:I31" xr:uid="{870F76F2-5EA7-4FD7-B1F9-507D64592088}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{3C04B742-338A-4366-BF3D-C5BC13023785}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="35">
+    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="24">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*63+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="34">
+    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="23">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="33">
+    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="22">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="32">
+    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="21">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="31">
+    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="20">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="30">
+    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="19">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="29">
+    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="18">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="28">
+    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="17">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2296,29 +2327,84 @@
   <autoFilter ref="A36:I41" xr:uid="{9BD043AF-0D77-4FF4-B2F9-B4AC3C3F1F82}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{7BB908A3-05D7-4357-920B-BF4C6BC20C06}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="27">
+    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="16">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*56.5+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="26">
+    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="15">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*12.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="25">
+    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="14">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="24">
+    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="13">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1 + 15+14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="23">
+    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="12">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="22">
+    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="11">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.5+ 15+13</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="21">
+    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="10">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="20">
+    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="9">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.375 + 15+40</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{E4471554-FCCF-4CBD-B1D2-34C3D61042AD}" name="Table168213429" displayName="Table168213429" ref="A3:J4" totalsRowShown="0">
+  <autoFilter ref="A3:J4" xr:uid="{B7276DA8-436B-4A87-A068-359A8A999C7E}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{5B20A54B-B88D-4A60-AC76-0D908355E6BA}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{68EBB8E2-05D1-4EDB-9CDA-3AD9FF254CCC}" name="HP"/>
+    <tableColumn id="3" xr3:uid="{8A304FC7-0E71-4252-847F-360347B995ED}" name="MP"/>
+    <tableColumn id="4" xr3:uid="{7083D6DB-67C9-429B-B586-FA259E20A040}" name="ATK"/>
+    <tableColumn id="5" xr3:uid="{32627FC9-83F7-4B6B-BCEF-A7C48D737A49}" name="DEF"/>
+    <tableColumn id="6" xr3:uid="{25B3F460-3592-4647-BCA0-54E890CB0695}" name="MAT"/>
+    <tableColumn id="7" xr3:uid="{09E4151E-54A0-41FF-BA5B-3B1C748DA23D}" name="MDF"/>
+    <tableColumn id="8" xr3:uid="{909575E0-EC13-4E35-A35F-2451A5741589}" name="AGI"/>
+    <tableColumn id="9" xr3:uid="{2CDCF32E-D8FC-48D9-A28D-8D9C5F3EB001}" name="LUK"/>
+    <tableColumn id="10" xr3:uid="{001DA1BB-34DD-4786-BDE4-23C510900A3D}" name="Total" dataDxfId="8">
+      <calculatedColumnFormula>SUM(Table168213429[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table33.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{E8776A97-35F2-43E5-8B1D-D6E628AF44FA}" name="Table1316183336" displayName="Table1316183336" ref="A7:I12" totalsRowShown="0">
+  <autoFilter ref="A7:I12" xr:uid="{4ED64482-035D-49B9-A477-A1D5AEB4A5A4}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{141B0E2E-D4F3-4884-86FD-AAD67C363749}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{D4B50877-EF56-4EF7-8C6D-9928A6D654F6}" name="HP" dataDxfId="4">
+      <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*88</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{F4B06187-BE28-4283-9518-F773FE75C2BF}" name="MP" dataDxfId="7">
+      <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{91A68FC7-5F16-4880-AE82-97341814BB95}" name="ATK" dataDxfId="3">
+      <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*4.5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{2BCD0E58-85DE-4C10-BFBC-AF77BC569C92}" name="DEF" dataDxfId="2">
+      <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*4.5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{7C48A1FC-CE8F-4CDD-9A3D-308B46D78A48}" name="MAT" dataDxfId="6">
+      <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{474D8178-EA8C-4322-93C3-B7F6EBA88102}" name="MDF" dataDxfId="1">
+      <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*4.5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{257B31D9-5838-45E0-A56E-9B1566E1A34A}" name="AGI" dataDxfId="0">
+      <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1.5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{17960EB4-4250-49DB-9A6B-455B9913B04B}" name="LUK" dataDxfId="5">
+      <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1.125</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2338,7 +2424,7 @@
     <tableColumn id="7" xr3:uid="{F833922A-76F9-427C-8462-D94DE51D0477}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{203171A1-C88B-4F81-ADC2-1EE072D645F3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{34003EF6-E9A5-4584-A186-09DFF4EC11C7}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{C4602156-F897-42BE-8F3F-411E13EEB095}" name="Total" dataDxfId="162">
+    <tableColumn id="10" xr3:uid="{C4602156-F897-42BE-8F3F-411E13EEB095}" name="Total" dataDxfId="171">
       <calculatedColumnFormula>SUM(Table114[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2351,28 +2437,28 @@
   <autoFilter ref="A8:I14" xr:uid="{D3C3F418-ED32-4504-9D73-88545A192967}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{13E0AF4A-AA83-489A-A156-B01D4F48D2F5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{B970139F-8BB5-4CE6-92F8-79E3236AC62B}" name="HP" dataDxfId="161">
+    <tableColumn id="2" xr3:uid="{B970139F-8BB5-4CE6-92F8-79E3236AC62B}" name="HP" dataDxfId="170">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*63+300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7BCF83B8-7492-4991-A008-F212725940B9}" name="MP" dataDxfId="160">
+    <tableColumn id="3" xr3:uid="{7BCF83B8-7492-4991-A008-F212725940B9}" name="MP" dataDxfId="169">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{33220A80-38D8-4480-ACC7-DF484072C96B}" name="ATK" dataDxfId="159">
+    <tableColumn id="4" xr3:uid="{33220A80-38D8-4480-ACC7-DF484072C96B}" name="ATK" dataDxfId="168">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.5+ 15+40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{36708515-5004-4705-A558-44B59D0CE676}" name="DEF" dataDxfId="158">
+    <tableColumn id="5" xr3:uid="{36708515-5004-4705-A558-44B59D0CE676}" name="DEF" dataDxfId="167">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25 + 15+21</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{11729EA3-08C4-4E0B-B5EE-5B3C08A31A9C}" name="MAT" dataDxfId="157">
+    <tableColumn id="6" xr3:uid="{11729EA3-08C4-4E0B-B5EE-5B3C08A31A9C}" name="MAT" dataDxfId="166">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B179D090-E484-4663-937A-480D1164D655}" name="MDF" dataDxfId="156">
+    <tableColumn id="7" xr3:uid="{B179D090-E484-4663-937A-480D1164D655}" name="MDF" dataDxfId="165">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25+15 + 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{28323AD0-B3BD-401F-A237-92C8B8D70FEA}" name="AGI" dataDxfId="155">
+    <tableColumn id="8" xr3:uid="{28323AD0-B3BD-401F-A237-92C8B8D70FEA}" name="AGI" dataDxfId="164">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{657BED8B-4C8A-42DC-BECD-5EEF9D1B7F37}" name="LUK" dataDxfId="154">
+    <tableColumn id="9" xr3:uid="{657BED8B-4C8A-42DC-BECD-5EEF9D1B7F37}" name="LUK" dataDxfId="163">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2393,7 +2479,7 @@
     <tableColumn id="7" xr3:uid="{D1DFC0D2-A987-4E3F-BA23-52162FB0C0BA}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{AB6209DB-CCCB-4C37-B455-4C7652E0DAC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2CD4CD14-92FD-41A7-9CCD-1329B5A77390}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{3B2C0A10-5038-4C21-BAC5-12FB16275D2E}" name="Total" dataDxfId="153">
+    <tableColumn id="10" xr3:uid="{3B2C0A10-5038-4C21-BAC5-12FB16275D2E}" name="Total" dataDxfId="162">
       <calculatedColumnFormula>SUM(Table11412[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2406,28 +2492,28 @@
   <autoFilter ref="A8:I14" xr:uid="{43F790D1-EA7B-4BAE-8A37-7CAD791E8821}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F6E842E1-B25F-4CA1-9107-AC7179420C29}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EFB2F0D5-318D-4A65-BA2B-20ADDE071648}" name="HP" dataDxfId="152">
+    <tableColumn id="2" xr3:uid="{EFB2F0D5-318D-4A65-BA2B-20ADDE071648}" name="HP" dataDxfId="161">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0D914B89-2678-453F-BC18-571DCD45E628}" name="MP" dataDxfId="151">
+    <tableColumn id="3" xr3:uid="{0D914B89-2678-453F-BC18-571DCD45E628}" name="MP" dataDxfId="160">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*13.75 + 80</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{6FBD2F64-5B1C-4035-BB1A-AFB092DB60C3}" name="ATK" dataDxfId="150">
+    <tableColumn id="4" xr3:uid="{6FBD2F64-5B1C-4035-BB1A-AFB092DB60C3}" name="ATK" dataDxfId="159">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7E0AF3FC-CC5D-4A6A-A4A2-DE278DEC4062}" name="DEF" dataDxfId="149">
+    <tableColumn id="5" xr3:uid="{7E0AF3FC-CC5D-4A6A-A4A2-DE278DEC4062}" name="DEF" dataDxfId="158">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1 + 15 + 4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3AF4D559-893B-4D50-BCB4-A1BD1FAF2F23}" name="MAT" dataDxfId="148">
+    <tableColumn id="6" xr3:uid="{3AF4D559-893B-4D50-BCB4-A1BD1FAF2F23}" name="MAT" dataDxfId="157">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6E9418A6-75AC-4541-9029-814EC5C06E70}" name="MDF" dataDxfId="147">
+    <tableColumn id="7" xr3:uid="{6E9418A6-75AC-4541-9029-814EC5C06E70}" name="MDF" dataDxfId="156">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.375+15 + 14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD605BEE-D561-4A2C-8D06-8E9AD70C32AC}" name="AGI" dataDxfId="146">
+    <tableColumn id="8" xr3:uid="{CD605BEE-D561-4A2C-8D06-8E9AD70C32AC}" name="AGI" dataDxfId="155">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E26506B2-F488-4AA4-AC87-819A22964609}" name="LUK" dataDxfId="145">
+    <tableColumn id="9" xr3:uid="{E26506B2-F488-4AA4-AC87-819A22964609}" name="LUK" dataDxfId="154">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2448,7 +2534,7 @@
     <tableColumn id="7" xr3:uid="{E91A64A8-F750-4893-9958-7C6ABC37405F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{3832FF0E-95E5-4B1F-B122-1EAFBF719DE3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{237404A9-EB50-465E-89AF-7167C57AFB99}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{927EBD24-571F-408C-A33B-59C753D9D96D}" name="Total" dataDxfId="144">
+    <tableColumn id="10" xr3:uid="{927EBD24-571F-408C-A33B-59C753D9D96D}" name="Total" dataDxfId="153">
       <calculatedColumnFormula>SUM(Table1141219[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2461,28 +2547,28 @@
   <autoFilter ref="A7:I13" xr:uid="{2539D8EE-2982-4734-B28B-342036FEDAC6}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FEE8F081-132E-4ED3-8FFD-2CF48368B2CC}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A79BC043-DB1A-48B4-AC21-AD31632979A6}" name="HP" dataDxfId="143">
+    <tableColumn id="2" xr3:uid="{A79BC043-DB1A-48B4-AC21-AD31632979A6}" name="HP" dataDxfId="152">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*63 + 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{42935B44-C727-42B0-B48E-0369818BF78A}" name="MP" dataDxfId="142">
+    <tableColumn id="3" xr3:uid="{42935B44-C727-42B0-B48E-0369818BF78A}" name="MP" dataDxfId="151">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{FC4572C7-88EC-4981-A6ED-43397844845B}" name="ATK" dataDxfId="141">
+    <tableColumn id="4" xr3:uid="{FC4572C7-88EC-4981-A6ED-43397844845B}" name="ATK" dataDxfId="150">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C8D61CEB-FFEC-42C3-9123-5140E65C1A2C}" name="DEF" dataDxfId="140">
+    <tableColumn id="5" xr3:uid="{C8D61CEB-FFEC-42C3-9123-5140E65C1A2C}" name="DEF" dataDxfId="149">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.375 + 15 + 19</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8C971683-28D2-4474-83CA-936F352F1324}" name="MAT" dataDxfId="139">
+    <tableColumn id="6" xr3:uid="{8C971683-28D2-4474-83CA-936F352F1324}" name="MAT" dataDxfId="148">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3371862A-9CF2-47CA-A149-4921E3B33162}" name="MDF" dataDxfId="138">
+    <tableColumn id="7" xr3:uid="{3371862A-9CF2-47CA-A149-4921E3B33162}" name="MDF" dataDxfId="147">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.375+15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC6AC739-B4C9-47A6-9472-439C60B629A0}" name="AGI" dataDxfId="137">
+    <tableColumn id="8" xr3:uid="{AC6AC739-B4C9-47A6-9472-439C60B629A0}" name="AGI" dataDxfId="146">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E727A271-B479-47C0-A557-227ABD8EC0AC}" name="LUK" dataDxfId="136">
+    <tableColumn id="9" xr3:uid="{E727A271-B479-47C0-A557-227ABD8EC0AC}" name="LUK" dataDxfId="145">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4062,8 +4148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5005335F-A4EA-4889-9D4A-6AE8EF295080}">
   <dimension ref="A2:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5528,6 +5614,304 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6D1546-413F-4D33-8AC9-20828C70BDCB}">
+  <dimension ref="A3:J12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <f>SUM(Table168213429[[#This Row],[HP]:[LUK]])</f>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <f>Table1316183336[[#This Row],[Level]]*88</f>
+        <v>88</v>
+      </c>
+      <c r="C8">
+        <f>Table1316183336[[#This Row],[Level]]*10</f>
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
+        <v>4.5</v>
+      </c>
+      <c r="E8">
+        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
+        <v>4.5</v>
+      </c>
+      <c r="F8">
+        <f>Table1316183336[[#This Row],[Level]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
+        <v>4.5</v>
+      </c>
+      <c r="H8">
+        <f>Table1316183336[[#This Row],[Level]]*1.5</f>
+        <v>1.5</v>
+      </c>
+      <c r="I8">
+        <f>Table1316183336[[#This Row],[Level]]*1.125</f>
+        <v>1.125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <f>Table1316183336[[#This Row],[Level]]*88</f>
+        <v>1320</v>
+      </c>
+      <c r="C9">
+        <f>Table1316183336[[#This Row],[Level]]*10</f>
+        <v>150</v>
+      </c>
+      <c r="D9">
+        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
+        <v>67.5</v>
+      </c>
+      <c r="E9">
+        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
+        <v>67.5</v>
+      </c>
+      <c r="F9">
+        <f>Table1316183336[[#This Row],[Level]]*1</f>
+        <v>15</v>
+      </c>
+      <c r="G9">
+        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
+        <v>67.5</v>
+      </c>
+      <c r="H9">
+        <f>Table1316183336[[#This Row],[Level]]*1.5</f>
+        <v>22.5</v>
+      </c>
+      <c r="I9">
+        <f>Table1316183336[[#This Row],[Level]]*1.125</f>
+        <v>16.875</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <f>Table1316183336[[#This Row],[Level]]*88</f>
+        <v>2200</v>
+      </c>
+      <c r="C10">
+        <f>Table1316183336[[#This Row],[Level]]*10</f>
+        <v>250</v>
+      </c>
+      <c r="D10">
+        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
+        <v>112.5</v>
+      </c>
+      <c r="E10">
+        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
+        <v>112.5</v>
+      </c>
+      <c r="F10">
+        <f>Table1316183336[[#This Row],[Level]]*1</f>
+        <v>25</v>
+      </c>
+      <c r="G10">
+        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
+        <v>112.5</v>
+      </c>
+      <c r="H10">
+        <f>Table1316183336[[#This Row],[Level]]*1.5</f>
+        <v>37.5</v>
+      </c>
+      <c r="I10">
+        <f>Table1316183336[[#This Row],[Level]]*1.125</f>
+        <v>28.125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>35</v>
+      </c>
+      <c r="B11">
+        <f>Table1316183336[[#This Row],[Level]]*88</f>
+        <v>3080</v>
+      </c>
+      <c r="C11">
+        <f>Table1316183336[[#This Row],[Level]]*10</f>
+        <v>350</v>
+      </c>
+      <c r="D11">
+        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
+        <v>157.5</v>
+      </c>
+      <c r="E11">
+        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
+        <v>157.5</v>
+      </c>
+      <c r="F11">
+        <f>Table1316183336[[#This Row],[Level]]*1</f>
+        <v>35</v>
+      </c>
+      <c r="G11">
+        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
+        <v>157.5</v>
+      </c>
+      <c r="H11">
+        <f>Table1316183336[[#This Row],[Level]]*1.5</f>
+        <v>52.5</v>
+      </c>
+      <c r="I11">
+        <f>Table1316183336[[#This Row],[Level]]*1.125</f>
+        <v>39.375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <f>Table1316183336[[#This Row],[Level]]*88</f>
+        <v>1760</v>
+      </c>
+      <c r="C12">
+        <f>Table1316183336[[#This Row],[Level]]*10</f>
+        <v>200</v>
+      </c>
+      <c r="D12">
+        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
+        <v>90</v>
+      </c>
+      <c r="E12">
+        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
+        <v>90</v>
+      </c>
+      <c r="F12">
+        <f>Table1316183336[[#This Row],[Level]]*1</f>
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
+        <v>90</v>
+      </c>
+      <c r="H12">
+        <f>Table1316183336[[#This Row],[Level]]*1.5</f>
+        <v>30</v>
+      </c>
+      <c r="I12">
+        <f>Table1316183336[[#This Row],[Level]]*1.125</f>
+        <v>22.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8DFDAFD-5CD5-4F03-8B08-1FCB08CB3DEC}">
   <dimension ref="A2:J17"/>

</xml_diff>

<commit_message>
Made several of Veronica's skills. Finished working on two small side areas in fort reon. Still have to add loot and all of teh single encounters in fort reon. Made slime monster to hunt, not so overpowered anymore
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -2382,28 +2382,28 @@
   <autoFilter ref="A7:I12" xr:uid="{4ED64482-035D-49B9-A477-A1D5AEB4A5A4}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{141B0E2E-D4F3-4884-86FD-AAD67C363749}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{D4B50877-EF56-4EF7-8C6D-9928A6D654F6}" name="HP" dataDxfId="4">
-      <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*88</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{D4B50877-EF56-4EF7-8C6D-9928A6D654F6}" name="HP" dataDxfId="0">
+      <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*125</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{F4B06187-BE28-4283-9518-F773FE75C2BF}" name="MP" dataDxfId="7">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{91A68FC7-5F16-4880-AE82-97341814BB95}" name="ATK" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{91A68FC7-5F16-4880-AE82-97341814BB95}" name="ATK" dataDxfId="6">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*4.5</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{2BCD0E58-85DE-4C10-BFBC-AF77BC569C92}" name="DEF" dataDxfId="2">
-      <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*4.5</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{7C48A1FC-CE8F-4CDD-9A3D-308B46D78A48}" name="MAT" dataDxfId="6">
+      <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*6</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{7C48A1FC-CE8F-4CDD-9A3D-308B46D78A48}" name="MAT" dataDxfId="5">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{474D8178-EA8C-4322-93C3-B7F6EBA88102}" name="MDF" dataDxfId="1">
-      <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*4.5</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{257B31D9-5838-45E0-A56E-9B1566E1A34A}" name="AGI" dataDxfId="0">
+      <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*6</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{257B31D9-5838-45E0-A56E-9B1566E1A34A}" name="AGI" dataDxfId="4">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{17960EB4-4250-49DB-9A6B-455B9913B04B}" name="LUK" dataDxfId="5">
+    <tableColumn id="9" xr3:uid="{17960EB4-4250-49DB-9A6B-455B9913B04B}" name="LUK" dataDxfId="3">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1.125</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5619,7 +5619,7 @@
   <dimension ref="A3:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5661,7 +5661,7 @@
         <v>55</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -5670,13 +5670,13 @@
         <v>15</v>
       </c>
       <c r="E4">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H4">
         <v>5</v>
@@ -5686,7 +5686,7 @@
       </c>
       <c r="J4">
         <f>SUM(Table168213429[[#This Row],[HP]:[LUK]])</f>
-        <v>61</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -5723,8 +5723,8 @@
         <v>1</v>
       </c>
       <c r="B8">
-        <f>Table1316183336[[#This Row],[Level]]*88</f>
-        <v>88</v>
+        <f>Table1316183336[[#This Row],[Level]]*125</f>
+        <v>125</v>
       </c>
       <c r="C8">
         <f>Table1316183336[[#This Row],[Level]]*10</f>
@@ -5735,16 +5735,16 @@
         <v>4.5</v>
       </c>
       <c r="E8">
-        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
-        <v>4.5</v>
+        <f>Table1316183336[[#This Row],[Level]]*6</f>
+        <v>6</v>
       </c>
       <c r="F8">
         <f>Table1316183336[[#This Row],[Level]]*1</f>
         <v>1</v>
       </c>
       <c r="G8">
-        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
-        <v>4.5</v>
+        <f>Table1316183336[[#This Row],[Level]]*6</f>
+        <v>6</v>
       </c>
       <c r="H8">
         <f>Table1316183336[[#This Row],[Level]]*1.5</f>
@@ -5760,8 +5760,8 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <f>Table1316183336[[#This Row],[Level]]*88</f>
-        <v>1320</v>
+        <f>Table1316183336[[#This Row],[Level]]*125</f>
+        <v>1875</v>
       </c>
       <c r="C9">
         <f>Table1316183336[[#This Row],[Level]]*10</f>
@@ -5772,16 +5772,16 @@
         <v>67.5</v>
       </c>
       <c r="E9">
-        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
-        <v>67.5</v>
+        <f>Table1316183336[[#This Row],[Level]]*6</f>
+        <v>90</v>
       </c>
       <c r="F9">
         <f>Table1316183336[[#This Row],[Level]]*1</f>
         <v>15</v>
       </c>
       <c r="G9">
-        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
-        <v>67.5</v>
+        <f>Table1316183336[[#This Row],[Level]]*6</f>
+        <v>90</v>
       </c>
       <c r="H9">
         <f>Table1316183336[[#This Row],[Level]]*1.5</f>
@@ -5797,8 +5797,8 @@
         <v>25</v>
       </c>
       <c r="B10">
-        <f>Table1316183336[[#This Row],[Level]]*88</f>
-        <v>2200</v>
+        <f>Table1316183336[[#This Row],[Level]]*125</f>
+        <v>3125</v>
       </c>
       <c r="C10">
         <f>Table1316183336[[#This Row],[Level]]*10</f>
@@ -5809,16 +5809,16 @@
         <v>112.5</v>
       </c>
       <c r="E10">
-        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
-        <v>112.5</v>
+        <f>Table1316183336[[#This Row],[Level]]*6</f>
+        <v>150</v>
       </c>
       <c r="F10">
         <f>Table1316183336[[#This Row],[Level]]*1</f>
         <v>25</v>
       </c>
       <c r="G10">
-        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
-        <v>112.5</v>
+        <f>Table1316183336[[#This Row],[Level]]*6</f>
+        <v>150</v>
       </c>
       <c r="H10">
         <f>Table1316183336[[#This Row],[Level]]*1.5</f>
@@ -5834,8 +5834,8 @@
         <v>35</v>
       </c>
       <c r="B11">
-        <f>Table1316183336[[#This Row],[Level]]*88</f>
-        <v>3080</v>
+        <f>Table1316183336[[#This Row],[Level]]*125</f>
+        <v>4375</v>
       </c>
       <c r="C11">
         <f>Table1316183336[[#This Row],[Level]]*10</f>
@@ -5846,16 +5846,16 @@
         <v>157.5</v>
       </c>
       <c r="E11">
-        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
-        <v>157.5</v>
+        <f>Table1316183336[[#This Row],[Level]]*6</f>
+        <v>210</v>
       </c>
       <c r="F11">
         <f>Table1316183336[[#This Row],[Level]]*1</f>
         <v>35</v>
       </c>
       <c r="G11">
-        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
-        <v>157.5</v>
+        <f>Table1316183336[[#This Row],[Level]]*6</f>
+        <v>210</v>
       </c>
       <c r="H11">
         <f>Table1316183336[[#This Row],[Level]]*1.5</f>
@@ -5871,8 +5871,8 @@
         <v>20</v>
       </c>
       <c r="B12">
-        <f>Table1316183336[[#This Row],[Level]]*88</f>
-        <v>1760</v>
+        <f>Table1316183336[[#This Row],[Level]]*125</f>
+        <v>2500</v>
       </c>
       <c r="C12">
         <f>Table1316183336[[#This Row],[Level]]*10</f>
@@ -5883,16 +5883,16 @@
         <v>90</v>
       </c>
       <c r="E12">
-        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
-        <v>90</v>
+        <f>Table1316183336[[#This Row],[Level]]*6</f>
+        <v>120</v>
       </c>
       <c r="F12">
         <f>Table1316183336[[#This Row],[Level]]*1</f>
         <v>20</v>
       </c>
       <c r="G12">
-        <f>Table1316183336[[#This Row],[Level]]*4.5</f>
-        <v>90</v>
+        <f>Table1316183336[[#This Row],[Level]]*6</f>
+        <v>120</v>
       </c>
       <c r="H12">
         <f>Table1316183336[[#This Row],[Level]]*1.5</f>

</xml_diff>

<commit_message>
Finished adding loot to Fort Reon interior, add loot to exterior, place pick ups around fort (like on tables). Working on mapping road towards Tellren city
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="8" activeTab="13" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="8" activeTab="14" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Skeleton Soldier" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="Death Lord" sheetId="15" r:id="rId12"/>
     <sheet name="Goblin" sheetId="2" r:id="rId13"/>
     <sheet name="Slimes" sheetId="16" r:id="rId14"/>
+    <sheet name="Corpse Eater" sheetId="17" r:id="rId15"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="57">
   <si>
     <t>Skeletons are the most basic undead, they have low magical attributes, agility, and luck.</t>
   </si>
@@ -206,6 +207,9 @@
   <si>
     <t>Slime</t>
   </si>
+  <si>
+    <t>Corpse Eater</t>
+  </si>
 </sst>
 </file>
 
@@ -281,7 +285,34 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="189">
+  <dxfs count="198">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1643,7 +1674,7 @@
     <tableColumn id="7" xr3:uid="{F9852B29-E77D-4E17-A56E-5F0C649FA862}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{9A914BFF-1060-46E4-B8F9-412BD9293C3D}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2F83B650-811D-4FEE-92D5-03D4DC4376E5}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="188">
+    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="197">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1664,7 +1695,7 @@
     <tableColumn id="7" xr3:uid="{3A2FD57C-060A-462E-8BB9-B06F717E9D20}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{ED9393EA-F7F9-4661-8D0B-0D9246DDABF8}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{6F56342F-5442-42CD-8B6C-D98B6D6C0C56}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="144">
+    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="153">
       <calculatedColumnFormula>SUM(Table16[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1677,28 +1708,28 @@
   <autoFilter ref="A8:I13" xr:uid="{7BE337CC-37BD-4688-B60D-A66F4420668B}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{71340E4C-6101-4C59-8ED7-689E2AD5A962}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="143">
+    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="152">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*63-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="142">
+    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="151">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="141">
+    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="150">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="140">
+    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="149">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="139">
+    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="148">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="138">
+    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="147">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="137">
+    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="146">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="136">
+    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="145">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1719,7 +1750,7 @@
     <tableColumn id="7" xr3:uid="{4899BF24-9D2A-4CC0-AE35-4F49604AAC5A}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{CB1CC6BA-1D38-4B74-9BC6-7057FB9773EE}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{C47FADF6-C526-4188-9187-383757CE17C1}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="135">
+    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="144">
       <calculatedColumnFormula>SUM(Table168[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1732,28 +1763,28 @@
   <autoFilter ref="A9:I15" xr:uid="{06A56D17-07E5-4650-8EE9-7EA8F94D4020}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A2BE27C9-9DAE-49F5-9A70-C6CF7428BF31}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="134">
+    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="143">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="133">
+    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="142">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="132">
+    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="141">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="131">
+    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="140">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="130">
+    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="139">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.375+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="129">
+    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="138">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="128">
+    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="137">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="127">
+    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="136">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1774,7 +1805,7 @@
     <tableColumn id="7" xr3:uid="{60AD88FB-4685-412B-B5FD-BF8412C6B8E2}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{6A88D48C-D864-4F16-BEF2-BA88783A3FF3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{D40BD230-6392-4A28-A29D-F13EFE35C95E}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A0E09B2B-FD41-413F-8063-62214E990751}" name="Total" dataDxfId="126">
+    <tableColumn id="10" xr3:uid="{A0E09B2B-FD41-413F-8063-62214E990751}" name="Total" dataDxfId="135">
       <calculatedColumnFormula>SUM(Table16826[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1787,28 +1818,28 @@
   <autoFilter ref="A8:I14" xr:uid="{F7062CBA-4FAA-4900-9D3A-5C6613BCB6CE}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{ADCB4852-D3A0-456B-A8BD-E5F74BDBB762}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{ED76047D-1BC2-4C1B-B9B0-58BE0ACDDA48}" name="HP" dataDxfId="125">
+    <tableColumn id="2" xr3:uid="{ED76047D-1BC2-4C1B-B9B0-58BE0ACDDA48}" name="HP" dataDxfId="134">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EC859C53-0BA5-45D1-868B-F22DC8CE7D25}" name="MP" dataDxfId="124">
+    <tableColumn id="3" xr3:uid="{EC859C53-0BA5-45D1-868B-F22DC8CE7D25}" name="MP" dataDxfId="133">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DED33AB9-A2BB-4F9E-AA6D-02F8D1D65CD1}" name="ATK" dataDxfId="123">
+    <tableColumn id="4" xr3:uid="{DED33AB9-A2BB-4F9E-AA6D-02F8D1D65CD1}" name="ATK" dataDxfId="132">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.375+ 15+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{329B716D-9CA6-4546-AB13-92D88BE40F5F}" name="DEF" dataDxfId="122">
+    <tableColumn id="5" xr3:uid="{329B716D-9CA6-4546-AB13-92D88BE40F5F}" name="DEF" dataDxfId="131">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1 + 15+12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{67F8198A-5FC2-4C6D-9558-68B3141EA756}" name="MAT" dataDxfId="121">
+    <tableColumn id="6" xr3:uid="{67F8198A-5FC2-4C6D-9558-68B3141EA756}" name="MAT" dataDxfId="130">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C70F5BF6-63B0-44C1-862D-25E3FB55320F}" name="MDF" dataDxfId="120">
+    <tableColumn id="7" xr3:uid="{C70F5BF6-63B0-44C1-862D-25E3FB55320F}" name="MDF" dataDxfId="129">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.5+15+11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AB20AF53-453C-4266-A46B-40E693C91985}" name="AGI" dataDxfId="119">
+    <tableColumn id="8" xr3:uid="{AB20AF53-453C-4266-A46B-40E693C91985}" name="AGI" dataDxfId="128">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7FC46A31-F9F1-432E-B399-0823E198FE0A}" name="LUK" dataDxfId="118">
+    <tableColumn id="9" xr3:uid="{7FC46A31-F9F1-432E-B399-0823E198FE0A}" name="LUK" dataDxfId="127">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.5+15+20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1829,7 +1860,7 @@
     <tableColumn id="7" xr3:uid="{20C5D094-BAF0-471C-ACF3-C6658991DB5F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{E08E2AF0-56DD-4A69-A536-27139D793022}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{12AD8606-1127-4E5B-BA2C-872780F22F9E}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{5E2EF778-63AE-48B7-9F49-0D2AFEBD66A1}" name="Total" dataDxfId="117">
+    <tableColumn id="10" xr3:uid="{5E2EF778-63AE-48B7-9F49-0D2AFEBD66A1}" name="Total" dataDxfId="126">
       <calculatedColumnFormula>SUM(Table1682630[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1842,28 +1873,28 @@
   <autoFilter ref="A8:I14" xr:uid="{299912CC-280B-49E1-8859-432D05893259}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4F0B657F-C9A5-4A73-AAA3-27D307385193}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{526284E7-597F-4726-AB18-230CA03461B1}" name="HP" dataDxfId="116">
+    <tableColumn id="2" xr3:uid="{526284E7-597F-4726-AB18-230CA03461B1}" name="HP" dataDxfId="125">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*63+ 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E7BA3C7A-2677-415F-BA47-A4E88679B948}" name="MP" dataDxfId="115">
+    <tableColumn id="3" xr3:uid="{E7BA3C7A-2677-415F-BA47-A4E88679B948}" name="MP" dataDxfId="124">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE7BE678-2229-44F6-8732-71214FB69DD7}" name="ATK" dataDxfId="114">
+    <tableColumn id="4" xr3:uid="{AE7BE678-2229-44F6-8732-71214FB69DD7}" name="ATK" dataDxfId="123">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+ 15+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4715E3DB-8817-43D5-9074-9FB5F0BEF5B4}" name="DEF" dataDxfId="113">
+    <tableColumn id="5" xr3:uid="{4715E3DB-8817-43D5-9074-9FB5F0BEF5B4}" name="DEF" dataDxfId="122">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1 + 15+12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9CE76933-D045-418B-A975-378EEA51D856}" name="MAT" dataDxfId="112">
+    <tableColumn id="6" xr3:uid="{9CE76933-D045-418B-A975-378EEA51D856}" name="MAT" dataDxfId="121">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244B9611-6CB0-4946-B5CD-7D42311C7D7E}" name="MDF" dataDxfId="111">
+    <tableColumn id="7" xr3:uid="{244B9611-6CB0-4946-B5CD-7D42311C7D7E}" name="MDF" dataDxfId="120">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+15+11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32550C13-49BB-41D2-BA0A-26798830A0FD}" name="AGI" dataDxfId="110">
+    <tableColumn id="8" xr3:uid="{32550C13-49BB-41D2-BA0A-26798830A0FD}" name="AGI" dataDxfId="119">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{BB22F289-8AF5-4DD6-877B-F09520710555}" name="LUK" dataDxfId="109">
+    <tableColumn id="9" xr3:uid="{BB22F289-8AF5-4DD6-877B-F09520710555}" name="LUK" dataDxfId="118">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+15+20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1876,28 +1907,28 @@
   <autoFilter ref="A4:I10" xr:uid="{A1EAC62C-C07D-464E-91B1-4A34E6604BA2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{430FD3D4-914C-4309-B2E6-6F01B5CAED94}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="108">
+    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="117">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="107">
+    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="116">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="106">
+    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="115">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="105">
+    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="114">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15 + 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="104">
+    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="113">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15 + 30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="103">
+    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="112">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15 + 21</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="102">
+    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="111">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="101">
+    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="110">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1910,28 +1941,28 @@
   <autoFilter ref="A7:I12" xr:uid="{9BE7336F-352A-4FAE-B0E4-61965FC814C7}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B8DA50BB-4379-43D1-879B-CDBE6D82C13A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="100">
+    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="109">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="99">
+    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="108">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="98">
+    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="107">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="97">
+    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="106">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="96">
+    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="105">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="95">
+    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="104">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="94">
+    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="103">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="93">
+    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="102">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1944,28 +1975,28 @@
   <autoFilter ref="A8:I13" xr:uid="{67385006-CBB9-4472-99D4-7881E042769D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FD96F8F7-CCAB-44FA-B525-A5081670706A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="187">
+    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="196">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="186">
+    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="195">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="185">
+    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="194">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="184">
+    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="193">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="183">
+    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="192">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="182">
+    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="191">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="181">
+    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="190">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="180">
+    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="189">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1986,7 +2017,7 @@
     <tableColumn id="7" xr3:uid="{AEFF5C29-BE6A-4CF8-A2BB-F6B076077DA9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{4DE9B01E-67F2-4136-ADC3-60389FB67DCC}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{F5A82F03-513C-46D4-9F91-470F0060526B}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="92">
+    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="101">
       <calculatedColumnFormula>SUM(Table16821[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1995,22 +2026,22 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="91" tableBorderDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="100" tableBorderDxfId="99">
   <autoFilter ref="A15:I16" xr:uid="{434CBBE2-2F8D-4EEB-895C-68FC850EF1FD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="89"/>
-    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="88">
+    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="98"/>
+    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="97">
       <calculatedColumnFormula>Table1922[Level]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="87">
+    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="96">
       <calculatedColumnFormula>Table1922[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="86"/>
-    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="85"/>
-    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="84"/>
-    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="83"/>
-    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="82"/>
-    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="81"/>
+    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="95"/>
+    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="94"/>
+    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="93"/>
+    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="92"/>
+    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="91"/>
+    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2021,28 +2052,28 @@
   <autoFilter ref="A3:I9" xr:uid="{A90D1C2A-DBF9-4EEF-ACC2-3DC17C207301}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BD3505AC-AE6D-4947-A74E-A6C2D68658F1}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="80">
+    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="89">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="79">
+    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="88">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="78">
+    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="87">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="77">
+    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="86">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="76">
+    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="85">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="75">
+    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="84">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="74">
+    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="83">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="73">
+    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="82">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2051,32 +2082,32 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="72" tableBorderDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="81" tableBorderDxfId="80">
   <autoFilter ref="L3:T4" xr:uid="{5D2C3EA8-1297-4C77-AF32-84E50F8232C5}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="70"/>
-    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="69">
+    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="79"/>
+    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="78">
       <calculatedColumnFormula>Table19[Level]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="68">
+    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="77">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="67">
+    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="76">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="66">
+    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="75">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1 + 15 + 6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="65">
+    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="74">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="64">
+    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="73">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="63">
+    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="72">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="62">
+    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="71">
       <calculatedColumnFormula>Table19[Level] + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2089,28 +2120,28 @@
   <autoFilter ref="A7:I12" xr:uid="{553298A4-7E43-42CF-9EEB-1F9E7E6BAD27}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2AA35C8B-719C-4BA6-9CDF-2963E1C9F233}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C087FAFA-9653-40EC-B4B9-5CB8F9D7255E}" name="HP" dataDxfId="61">
+    <tableColumn id="2" xr3:uid="{C087FAFA-9653-40EC-B4B9-5CB8F9D7255E}" name="HP" dataDxfId="70">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0004B47B-3968-4C5A-BE6C-B822A307D7C5}" name="MP" dataDxfId="60">
+    <tableColumn id="3" xr3:uid="{0004B47B-3968-4C5A-BE6C-B822A307D7C5}" name="MP" dataDxfId="69">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{67EC8D91-0122-40D7-87D0-A3AB6788CE9D}" name="ATK" dataDxfId="59">
+    <tableColumn id="4" xr3:uid="{67EC8D91-0122-40D7-87D0-A3AB6788CE9D}" name="ATK" dataDxfId="68">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E9988E54-33D6-41EB-B6BE-6E832544E18C}" name="DEF" dataDxfId="58">
+    <tableColumn id="5" xr3:uid="{E9988E54-33D6-41EB-B6BE-6E832544E18C}" name="DEF" dataDxfId="67">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{16D71A55-372C-4029-A831-ECF2325E46C4}" name="MAT" dataDxfId="57">
+    <tableColumn id="6" xr3:uid="{16D71A55-372C-4029-A831-ECF2325E46C4}" name="MAT" dataDxfId="66">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{1802FB48-B110-4DBF-A8F2-64CD4890E741}" name="MDF" dataDxfId="56">
+    <tableColumn id="7" xr3:uid="{1802FB48-B110-4DBF-A8F2-64CD4890E741}" name="MDF" dataDxfId="65">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{350CA8CC-761C-4994-9D80-14685787EF3D}" name="AGI" dataDxfId="55">
+    <tableColumn id="8" xr3:uid="{350CA8CC-761C-4994-9D80-14685787EF3D}" name="AGI" dataDxfId="64">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B578CF58-136A-41B9-800E-D75836A4CDD1}" name="LUK" dataDxfId="54">
+    <tableColumn id="9" xr3:uid="{B578CF58-136A-41B9-800E-D75836A4CDD1}" name="LUK" dataDxfId="63">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2131,7 +2162,7 @@
     <tableColumn id="7" xr3:uid="{5A405725-30A7-487F-95BF-061F71CA9C61}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{644DEF70-6EBD-403E-904B-6C30E5FBEA48}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{BA93DA54-96B9-48D1-80BB-C266771E13F1}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{3EBB17A5-47EA-458B-83A5-7056BE67D25F}" name="Total" dataDxfId="53">
+    <tableColumn id="10" xr3:uid="{3EBB17A5-47EA-458B-83A5-7056BE67D25F}" name="Total" dataDxfId="62">
       <calculatedColumnFormula>SUM(Table1682134[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2140,26 +2171,26 @@
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{A7C0F3AC-4E86-430D-AE55-8604641B493E}" name="Table192235" displayName="Table192235" ref="A15:I16" totalsRowShown="0" dataDxfId="52" tableBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{A7C0F3AC-4E86-430D-AE55-8604641B493E}" name="Table192235" displayName="Table192235" ref="A15:I16" totalsRowShown="0" dataDxfId="61" tableBorderDxfId="60">
   <autoFilter ref="A15:I16" xr:uid="{D0DF3ED4-9A21-493B-88F4-CE5814AF31C9}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A78A876E-6C8B-4FC8-BFD4-A9BC80EA3FC2}" name="Level" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{4B423FFC-D037-484D-A927-2F66E15D422A}" name="HP" dataDxfId="49">
+    <tableColumn id="1" xr3:uid="{A78A876E-6C8B-4FC8-BFD4-A9BC80EA3FC2}" name="Level" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{4B423FFC-D037-484D-A927-2F66E15D422A}" name="HP" dataDxfId="58">
       <calculatedColumnFormula>(Table192235[Level]*75 + 500)*2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B695FEDE-EC59-44D8-AE99-CBF568DE5C93}" name="MP" dataDxfId="48">
+    <tableColumn id="3" xr3:uid="{B695FEDE-EC59-44D8-AE99-CBF568DE5C93}" name="MP" dataDxfId="57">
       <calculatedColumnFormula>Table192235[[#This Row],[Level]]*14 + 80</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{160D5D77-34E8-44F3-B51D-7CC0736DDCB1}" name="ATK" dataDxfId="47">
+    <tableColumn id="4" xr3:uid="{160D5D77-34E8-44F3-B51D-7CC0736DDCB1}" name="ATK" dataDxfId="56">
       <calculatedColumnFormula>Table192235[[#This Row],[Level]]*1.5+ 15 + 50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{559DAC37-CD6A-449F-AFF0-355ADE7CED80}" name="DEF" dataDxfId="46"/>
-    <tableColumn id="6" xr3:uid="{EEC344A5-27A5-450E-B795-04D237DD063F}" name="MAT" dataDxfId="45">
+    <tableColumn id="5" xr3:uid="{559DAC37-CD6A-449F-AFF0-355ADE7CED80}" name="DEF" dataDxfId="55"/>
+    <tableColumn id="6" xr3:uid="{EEC344A5-27A5-450E-B795-04D237DD063F}" name="MAT" dataDxfId="54">
       <calculatedColumnFormula>Table192235[Level]*1.5+15+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{54363CA4-9EE5-495F-8323-6C0C1261453C}" name="MDF" dataDxfId="44"/>
-    <tableColumn id="8" xr3:uid="{26B56E9D-2FCD-4476-A6CF-8F2EDC965246}" name="AGI" dataDxfId="43"/>
-    <tableColumn id="9" xr3:uid="{95814D66-3343-4190-9BF4-F4E45AB27D95}" name="LUK" dataDxfId="42"/>
+    <tableColumn id="7" xr3:uid="{54363CA4-9EE5-495F-8323-6C0C1261453C}" name="MDF" dataDxfId="53"/>
+    <tableColumn id="8" xr3:uid="{26B56E9D-2FCD-4476-A6CF-8F2EDC965246}" name="AGI" dataDxfId="52"/>
+    <tableColumn id="9" xr3:uid="{95814D66-3343-4190-9BF4-F4E45AB27D95}" name="LUK" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2178,7 +2209,7 @@
     <tableColumn id="7" xr3:uid="{22216E02-260E-4471-8BB1-4E6E1250BAC9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{DC2670AC-8DF2-47F7-A3F6-EE7896309BC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{749652E2-F6CF-428C-B67C-FD0B1EFCCBBF}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="41">
+    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="50">
       <calculatedColumnFormula>SUM(Table15[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2191,28 +2222,28 @@
   <autoFilter ref="A15:I20" xr:uid="{A1CF627F-8D28-44AD-9A35-411103976FCA}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F14CC326-DE44-48D8-856F-8DCDCFC89CAD}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="40">
+    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="49">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*63-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="39">
+    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="48">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="38">
+    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="47">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="37">
+    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="46">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="36">
+    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="45">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="35">
+    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="44">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="34">
+    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="43">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="33">
+    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="42">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2225,28 +2256,28 @@
   <autoFilter ref="K11:S17" xr:uid="{EAF9FB6A-F011-40E3-AB2F-E53826722AFB}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DF3E0800-6EE4-4E1B-BA6F-0194351D6E7C}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="32">
+    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="41">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*56.25+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="31">
+    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="40">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="30">
+    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="39">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="29">
+    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="38">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="28">
+    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="37">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="27">
+    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="36">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="26">
+    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="35">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="25">
+    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="34">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2259,28 +2290,28 @@
   <autoFilter ref="K8:S14" xr:uid="{AB7E938D-7ACC-4BFB-A6B9-682B8B29CEF2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{66EB8EF1-BCF4-44F7-B8A6-3C3B425F8FF5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="179">
+    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="188">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*56.25+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="178">
+    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="187">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="177">
+    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="186">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25+ 15+30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="176">
+    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="185">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25 + 15+33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="175">
+    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="184">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="174">
+    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="183">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="173">
+    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="182">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="172">
+    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="181">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2293,28 +2324,28 @@
   <autoFilter ref="A26:I31" xr:uid="{870F76F2-5EA7-4FD7-B1F9-507D64592088}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{3C04B742-338A-4366-BF3D-C5BC13023785}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="24">
+    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="33">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*63+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="23">
+    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="32">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="22">
+    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="31">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="21">
+    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="30">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="20">
+    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="29">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="19">
+    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="28">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="18">
+    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="27">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="17">
+    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="26">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2327,28 +2358,28 @@
   <autoFilter ref="A36:I41" xr:uid="{9BD043AF-0D77-4FF4-B2F9-B4AC3C3F1F82}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{7BB908A3-05D7-4357-920B-BF4C6BC20C06}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="16">
+    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="25">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*56.5+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="15">
+    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="24">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*12.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="14">
+    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="23">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="13">
+    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="22">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1 + 15+14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="21">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="20">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.5+ 15+13</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="10">
+    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="19">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="9">
+    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="18">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.375 + 15+40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2369,7 +2400,7 @@
     <tableColumn id="7" xr3:uid="{09E4151E-54A0-41FF-BA5B-3B1C748DA23D}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{909575E0-EC13-4E35-A35F-2451A5741589}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2CDCF32E-D8FC-48D9-A28D-8D9C5F3EB001}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{001DA1BB-34DD-4786-BDE4-23C510900A3D}" name="Total" dataDxfId="8">
+    <tableColumn id="10" xr3:uid="{001DA1BB-34DD-4786-BDE4-23C510900A3D}" name="Total" dataDxfId="17">
       <calculatedColumnFormula>SUM(Table168213429[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2382,29 +2413,84 @@
   <autoFilter ref="A7:I12" xr:uid="{4ED64482-035D-49B9-A477-A1D5AEB4A5A4}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{141B0E2E-D4F3-4884-86FD-AAD67C363749}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{D4B50877-EF56-4EF7-8C6D-9928A6D654F6}" name="HP" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{D4B50877-EF56-4EF7-8C6D-9928A6D654F6}" name="HP" dataDxfId="16">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*125</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F4B06187-BE28-4283-9518-F773FE75C2BF}" name="MP" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{F4B06187-BE28-4283-9518-F773FE75C2BF}" name="MP" dataDxfId="15">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{91A68FC7-5F16-4880-AE82-97341814BB95}" name="ATK" dataDxfId="6">
+    <tableColumn id="4" xr3:uid="{91A68FC7-5F16-4880-AE82-97341814BB95}" name="ATK" dataDxfId="14">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*4.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{2BCD0E58-85DE-4C10-BFBC-AF77BC569C92}" name="DEF" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{2BCD0E58-85DE-4C10-BFBC-AF77BC569C92}" name="DEF" dataDxfId="13">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7C48A1FC-CE8F-4CDD-9A3D-308B46D78A48}" name="MAT" dataDxfId="5">
+    <tableColumn id="6" xr3:uid="{7C48A1FC-CE8F-4CDD-9A3D-308B46D78A48}" name="MAT" dataDxfId="12">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{474D8178-EA8C-4322-93C3-B7F6EBA88102}" name="MDF" dataDxfId="1">
+    <tableColumn id="7" xr3:uid="{474D8178-EA8C-4322-93C3-B7F6EBA88102}" name="MDF" dataDxfId="11">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{257B31D9-5838-45E0-A56E-9B1566E1A34A}" name="AGI" dataDxfId="4">
+    <tableColumn id="8" xr3:uid="{257B31D9-5838-45E0-A56E-9B1566E1A34A}" name="AGI" dataDxfId="10">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{17960EB4-4250-49DB-9A6B-455B9913B04B}" name="LUK" dataDxfId="3">
+    <tableColumn id="9" xr3:uid="{17960EB4-4250-49DB-9A6B-455B9913B04B}" name="LUK" dataDxfId="9">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1.125</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table34.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{1BF38CE5-AE76-4D55-A7A1-A0031AB12082}" name="Table16821342932" displayName="Table16821342932" ref="A2:J3" totalsRowShown="0">
+  <autoFilter ref="A2:J3" xr:uid="{7DA0C592-B226-4929-8531-42F076DA52EC}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{3A64E47E-25C8-4094-A361-6EFD40EA5158}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{0CA8146C-91BF-4F90-B048-1F984082990B}" name="HP"/>
+    <tableColumn id="3" xr3:uid="{CE821208-5046-4677-97B3-53026C5E6EB5}" name="MP"/>
+    <tableColumn id="4" xr3:uid="{BCDAC572-3A17-4261-A6F7-47414761764B}" name="ATK"/>
+    <tableColumn id="5" xr3:uid="{E65F8E36-7291-4370-8BAA-C711A8B38D65}" name="DEF"/>
+    <tableColumn id="6" xr3:uid="{23BEB1EA-9AE5-41A1-95A0-F6255A1D9952}" name="MAT"/>
+    <tableColumn id="7" xr3:uid="{07EA0638-8880-4944-AC9E-13E3F1B9F651}" name="MDF"/>
+    <tableColumn id="8" xr3:uid="{AA18E602-126F-4D69-9CC8-C097E8EB9C70}" name="AGI"/>
+    <tableColumn id="9" xr3:uid="{5563B0CB-2EA7-4851-8D1F-D77E0F90CBAD}" name="LUK"/>
+    <tableColumn id="10" xr3:uid="{2D960B43-0F76-4936-9508-4D501A79A83C}" name="Total" dataDxfId="8">
+      <calculatedColumnFormula>SUM(Table16821342932[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table35.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="36" xr:uid="{FB5A8576-9AFA-4611-8031-671097B463A2}" name="Table131618333637" displayName="Table131618333637" ref="A5:I10" totalsRowShown="0">
+  <autoFilter ref="A5:I10" xr:uid="{2922C913-6AE8-4B89-BDA6-9F44D59987D8}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{3D67222C-6501-4A5D-A9FC-528EE591A288}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{EE3E4CCC-C404-4B78-AAB4-3B38166E23BA}" name="HP" dataDxfId="6">
+      <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{DE5141FB-3B4E-46D4-9E0D-AF1DEE998B4A}" name="MP" dataDxfId="7">
+      <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{404B3E88-DF62-4AA0-82D6-C21C2BCA762B}" name="ATK" dataDxfId="5">
+      <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*4.5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{342B3F39-F7A2-45D8-9CD4-39B5ABC72D2F}" name="DEF" dataDxfId="4">
+      <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{CD819DB3-9F2E-4428-AAFC-72776ECB8EAF}" name="MAT" dataDxfId="3">
+      <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{270DF964-8095-43FD-B050-DD4A2A138F32}" name="MDF" dataDxfId="2">
+      <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{4F4D3B2A-5B86-4AB7-A97E-18E2868266B8}" name="AGI" dataDxfId="1">
+      <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*6</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{0178CE2D-63C5-426A-A081-D62E62FF91AC}" name="LUK" dataDxfId="0">
+      <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*1.5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2424,7 +2510,7 @@
     <tableColumn id="7" xr3:uid="{F833922A-76F9-427C-8462-D94DE51D0477}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{203171A1-C88B-4F81-ADC2-1EE072D645F3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{34003EF6-E9A5-4584-A186-09DFF4EC11C7}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{C4602156-F897-42BE-8F3F-411E13EEB095}" name="Total" dataDxfId="171">
+    <tableColumn id="10" xr3:uid="{C4602156-F897-42BE-8F3F-411E13EEB095}" name="Total" dataDxfId="180">
       <calculatedColumnFormula>SUM(Table114[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2437,28 +2523,28 @@
   <autoFilter ref="A8:I14" xr:uid="{D3C3F418-ED32-4504-9D73-88545A192967}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{13E0AF4A-AA83-489A-A156-B01D4F48D2F5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{B970139F-8BB5-4CE6-92F8-79E3236AC62B}" name="HP" dataDxfId="170">
+    <tableColumn id="2" xr3:uid="{B970139F-8BB5-4CE6-92F8-79E3236AC62B}" name="HP" dataDxfId="179">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*63+300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7BCF83B8-7492-4991-A008-F212725940B9}" name="MP" dataDxfId="169">
+    <tableColumn id="3" xr3:uid="{7BCF83B8-7492-4991-A008-F212725940B9}" name="MP" dataDxfId="178">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{33220A80-38D8-4480-ACC7-DF484072C96B}" name="ATK" dataDxfId="168">
+    <tableColumn id="4" xr3:uid="{33220A80-38D8-4480-ACC7-DF484072C96B}" name="ATK" dataDxfId="177">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.5+ 15+40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{36708515-5004-4705-A558-44B59D0CE676}" name="DEF" dataDxfId="167">
+    <tableColumn id="5" xr3:uid="{36708515-5004-4705-A558-44B59D0CE676}" name="DEF" dataDxfId="176">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25 + 15+21</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{11729EA3-08C4-4E0B-B5EE-5B3C08A31A9C}" name="MAT" dataDxfId="166">
+    <tableColumn id="6" xr3:uid="{11729EA3-08C4-4E0B-B5EE-5B3C08A31A9C}" name="MAT" dataDxfId="175">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B179D090-E484-4663-937A-480D1164D655}" name="MDF" dataDxfId="165">
+    <tableColumn id="7" xr3:uid="{B179D090-E484-4663-937A-480D1164D655}" name="MDF" dataDxfId="174">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25+15 + 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{28323AD0-B3BD-401F-A237-92C8B8D70FEA}" name="AGI" dataDxfId="164">
+    <tableColumn id="8" xr3:uid="{28323AD0-B3BD-401F-A237-92C8B8D70FEA}" name="AGI" dataDxfId="173">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{657BED8B-4C8A-42DC-BECD-5EEF9D1B7F37}" name="LUK" dataDxfId="163">
+    <tableColumn id="9" xr3:uid="{657BED8B-4C8A-42DC-BECD-5EEF9D1B7F37}" name="LUK" dataDxfId="172">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2479,7 +2565,7 @@
     <tableColumn id="7" xr3:uid="{D1DFC0D2-A987-4E3F-BA23-52162FB0C0BA}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{AB6209DB-CCCB-4C37-B455-4C7652E0DAC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2CD4CD14-92FD-41A7-9CCD-1329B5A77390}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{3B2C0A10-5038-4C21-BAC5-12FB16275D2E}" name="Total" dataDxfId="162">
+    <tableColumn id="10" xr3:uid="{3B2C0A10-5038-4C21-BAC5-12FB16275D2E}" name="Total" dataDxfId="171">
       <calculatedColumnFormula>SUM(Table11412[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2492,28 +2578,28 @@
   <autoFilter ref="A8:I14" xr:uid="{43F790D1-EA7B-4BAE-8A37-7CAD791E8821}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F6E842E1-B25F-4CA1-9107-AC7179420C29}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EFB2F0D5-318D-4A65-BA2B-20ADDE071648}" name="HP" dataDxfId="161">
+    <tableColumn id="2" xr3:uid="{EFB2F0D5-318D-4A65-BA2B-20ADDE071648}" name="HP" dataDxfId="170">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0D914B89-2678-453F-BC18-571DCD45E628}" name="MP" dataDxfId="160">
+    <tableColumn id="3" xr3:uid="{0D914B89-2678-453F-BC18-571DCD45E628}" name="MP" dataDxfId="169">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*13.75 + 80</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{6FBD2F64-5B1C-4035-BB1A-AFB092DB60C3}" name="ATK" dataDxfId="159">
+    <tableColumn id="4" xr3:uid="{6FBD2F64-5B1C-4035-BB1A-AFB092DB60C3}" name="ATK" dataDxfId="168">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7E0AF3FC-CC5D-4A6A-A4A2-DE278DEC4062}" name="DEF" dataDxfId="158">
+    <tableColumn id="5" xr3:uid="{7E0AF3FC-CC5D-4A6A-A4A2-DE278DEC4062}" name="DEF" dataDxfId="167">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1 + 15 + 4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3AF4D559-893B-4D50-BCB4-A1BD1FAF2F23}" name="MAT" dataDxfId="157">
+    <tableColumn id="6" xr3:uid="{3AF4D559-893B-4D50-BCB4-A1BD1FAF2F23}" name="MAT" dataDxfId="166">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6E9418A6-75AC-4541-9029-814EC5C06E70}" name="MDF" dataDxfId="156">
+    <tableColumn id="7" xr3:uid="{6E9418A6-75AC-4541-9029-814EC5C06E70}" name="MDF" dataDxfId="165">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.375+15 + 14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD605BEE-D561-4A2C-8D06-8E9AD70C32AC}" name="AGI" dataDxfId="155">
+    <tableColumn id="8" xr3:uid="{CD605BEE-D561-4A2C-8D06-8E9AD70C32AC}" name="AGI" dataDxfId="164">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E26506B2-F488-4AA4-AC87-819A22964609}" name="LUK" dataDxfId="154">
+    <tableColumn id="9" xr3:uid="{E26506B2-F488-4AA4-AC87-819A22964609}" name="LUK" dataDxfId="163">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2534,7 +2620,7 @@
     <tableColumn id="7" xr3:uid="{E91A64A8-F750-4893-9958-7C6ABC37405F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{3832FF0E-95E5-4B1F-B122-1EAFBF719DE3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{237404A9-EB50-465E-89AF-7167C57AFB99}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{927EBD24-571F-408C-A33B-59C753D9D96D}" name="Total" dataDxfId="153">
+    <tableColumn id="10" xr3:uid="{927EBD24-571F-408C-A33B-59C753D9D96D}" name="Total" dataDxfId="162">
       <calculatedColumnFormula>SUM(Table1141219[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2547,28 +2633,28 @@
   <autoFilter ref="A7:I13" xr:uid="{2539D8EE-2982-4734-B28B-342036FEDAC6}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FEE8F081-132E-4ED3-8FFD-2CF48368B2CC}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A79BC043-DB1A-48B4-AC21-AD31632979A6}" name="HP" dataDxfId="152">
+    <tableColumn id="2" xr3:uid="{A79BC043-DB1A-48B4-AC21-AD31632979A6}" name="HP" dataDxfId="161">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*63 + 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{42935B44-C727-42B0-B48E-0369818BF78A}" name="MP" dataDxfId="151">
+    <tableColumn id="3" xr3:uid="{42935B44-C727-42B0-B48E-0369818BF78A}" name="MP" dataDxfId="160">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{FC4572C7-88EC-4981-A6ED-43397844845B}" name="ATK" dataDxfId="150">
+    <tableColumn id="4" xr3:uid="{FC4572C7-88EC-4981-A6ED-43397844845B}" name="ATK" dataDxfId="159">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C8D61CEB-FFEC-42C3-9123-5140E65C1A2C}" name="DEF" dataDxfId="149">
+    <tableColumn id="5" xr3:uid="{C8D61CEB-FFEC-42C3-9123-5140E65C1A2C}" name="DEF" dataDxfId="158">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.375 + 15 + 19</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8C971683-28D2-4474-83CA-936F352F1324}" name="MAT" dataDxfId="148">
+    <tableColumn id="6" xr3:uid="{8C971683-28D2-4474-83CA-936F352F1324}" name="MAT" dataDxfId="157">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3371862A-9CF2-47CA-A149-4921E3B33162}" name="MDF" dataDxfId="147">
+    <tableColumn id="7" xr3:uid="{3371862A-9CF2-47CA-A149-4921E3B33162}" name="MDF" dataDxfId="156">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.375+15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC6AC739-B4C9-47A6-9472-439C60B629A0}" name="AGI" dataDxfId="146">
+    <tableColumn id="8" xr3:uid="{AC6AC739-B4C9-47A6-9472-439C60B629A0}" name="AGI" dataDxfId="155">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E727A271-B479-47C0-A557-227ABD8EC0AC}" name="LUK" dataDxfId="145">
+    <tableColumn id="9" xr3:uid="{E727A271-B479-47C0-A557-227ABD8EC0AC}" name="LUK" dataDxfId="154">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5618,8 +5704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6D1546-413F-4D33-8AC9-20828C70BDCB}">
   <dimension ref="A3:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5901,6 +5987,304 @@
       <c r="I12">
         <f>Table1316183336[[#This Row],[Level]]*1.125</f>
         <v>22.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76FD8A7-49F8-4714-9911-92DFAEEE64EB}">
+  <dimension ref="A2:J10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <f>SUM(Table16821342932[[#This Row],[HP]:[LUK]])</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <f>Table131618333637[[#This Row],[Level]]*100</f>
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <f>Table131618333637[[#This Row],[Level]]*10</f>
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <f>Table131618333637[[#This Row],[Level]]*4.5</f>
+        <v>4.5</v>
+      </c>
+      <c r="E6">
+        <f>Table131618333637[[#This Row],[Level]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <f>Table131618333637[[#This Row],[Level]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <f>Table131618333637[[#This Row],[Level]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <f>Table131618333637[[#This Row],[Level]]*6</f>
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <f>Table131618333637[[#This Row],[Level]]*1.5</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <f>Table131618333637[[#This Row],[Level]]*100</f>
+        <v>1500</v>
+      </c>
+      <c r="C7">
+        <f>Table131618333637[[#This Row],[Level]]*10</f>
+        <v>150</v>
+      </c>
+      <c r="D7">
+        <f>Table131618333637[[#This Row],[Level]]*4.5</f>
+        <v>67.5</v>
+      </c>
+      <c r="E7">
+        <f>Table131618333637[[#This Row],[Level]]*3</f>
+        <v>45</v>
+      </c>
+      <c r="F7">
+        <f>Table131618333637[[#This Row],[Level]]*3</f>
+        <v>45</v>
+      </c>
+      <c r="G7">
+        <f>Table131618333637[[#This Row],[Level]]*3</f>
+        <v>45</v>
+      </c>
+      <c r="H7">
+        <f>Table131618333637[[#This Row],[Level]]*6</f>
+        <v>90</v>
+      </c>
+      <c r="I7">
+        <f>Table131618333637[[#This Row],[Level]]*1.5</f>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <f>Table131618333637[[#This Row],[Level]]*100</f>
+        <v>2500</v>
+      </c>
+      <c r="C8">
+        <f>Table131618333637[[#This Row],[Level]]*10</f>
+        <v>250</v>
+      </c>
+      <c r="D8">
+        <f>Table131618333637[[#This Row],[Level]]*4.5</f>
+        <v>112.5</v>
+      </c>
+      <c r="E8">
+        <f>Table131618333637[[#This Row],[Level]]*3</f>
+        <v>75</v>
+      </c>
+      <c r="F8">
+        <f>Table131618333637[[#This Row],[Level]]*3</f>
+        <v>75</v>
+      </c>
+      <c r="G8">
+        <f>Table131618333637[[#This Row],[Level]]*3</f>
+        <v>75</v>
+      </c>
+      <c r="H8">
+        <f>Table131618333637[[#This Row],[Level]]*6</f>
+        <v>150</v>
+      </c>
+      <c r="I8">
+        <f>Table131618333637[[#This Row],[Level]]*1.5</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <f>Table131618333637[[#This Row],[Level]]*100</f>
+        <v>3500</v>
+      </c>
+      <c r="C9">
+        <f>Table131618333637[[#This Row],[Level]]*10</f>
+        <v>350</v>
+      </c>
+      <c r="D9">
+        <f>Table131618333637[[#This Row],[Level]]*4.5</f>
+        <v>157.5</v>
+      </c>
+      <c r="E9">
+        <f>Table131618333637[[#This Row],[Level]]*3</f>
+        <v>105</v>
+      </c>
+      <c r="F9">
+        <f>Table131618333637[[#This Row],[Level]]*3</f>
+        <v>105</v>
+      </c>
+      <c r="G9">
+        <f>Table131618333637[[#This Row],[Level]]*3</f>
+        <v>105</v>
+      </c>
+      <c r="H9">
+        <f>Table131618333637[[#This Row],[Level]]*6</f>
+        <v>210</v>
+      </c>
+      <c r="I9">
+        <f>Table131618333637[[#This Row],[Level]]*1.5</f>
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <f>Table131618333637[[#This Row],[Level]]*100</f>
+        <v>2000</v>
+      </c>
+      <c r="C10">
+        <f>Table131618333637[[#This Row],[Level]]*10</f>
+        <v>200</v>
+      </c>
+      <c r="D10">
+        <f>Table131618333637[[#This Row],[Level]]*4.5</f>
+        <v>90</v>
+      </c>
+      <c r="E10">
+        <f>Table131618333637[[#This Row],[Level]]*3</f>
+        <v>60</v>
+      </c>
+      <c r="F10">
+        <f>Table131618333637[[#This Row],[Level]]*3</f>
+        <v>60</v>
+      </c>
+      <c r="G10">
+        <f>Table131618333637[[#This Row],[Level]]*3</f>
+        <v>60</v>
+      </c>
+      <c r="H10">
+        <f>Table131618333637[[#This Row],[Level]]*6</f>
+        <v>120</v>
+      </c>
+      <c r="I10">
+        <f>Table131618333637[[#This Row],[Level]]*1.5</f>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made interior map for Wynsia village, added Slime King. TODO: Fight with slimes, cutscene with villagers, craft a thunder sword, go fight pair of hunter slimes, then fight slime king
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="8" activeTab="14" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="8" activeTab="13" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Skeleton Soldier" sheetId="1" r:id="rId1"/>
@@ -2468,10 +2468,10 @@
   <autoFilter ref="A5:I10" xr:uid="{2922C913-6AE8-4B89-BDA6-9F44D59987D8}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{3D67222C-6501-4A5D-A9FC-528EE591A288}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EE3E4CCC-C404-4B78-AAB4-3B38166E23BA}" name="HP" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{EE3E4CCC-C404-4B78-AAB4-3B38166E23BA}" name="HP" dataDxfId="7">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DE5141FB-3B4E-46D4-9E0D-AF1DEE998B4A}" name="MP" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{DE5141FB-3B4E-46D4-9E0D-AF1DEE998B4A}" name="MP" dataDxfId="6">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{404B3E88-DF62-4AA0-82D6-C21C2BCA762B}" name="ATK" dataDxfId="5">
@@ -5704,8 +5704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6D1546-413F-4D33-8AC9-20828C70BDCB}">
   <dimension ref="A3:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5917,39 +5917,39 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B11">
         <f>Table1316183336[[#This Row],[Level]]*125</f>
-        <v>4375</v>
+        <v>3125</v>
       </c>
       <c r="C11">
         <f>Table1316183336[[#This Row],[Level]]*10</f>
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="D11">
         <f>Table1316183336[[#This Row],[Level]]*4.5</f>
-        <v>157.5</v>
+        <v>112.5</v>
       </c>
       <c r="E11">
         <f>Table1316183336[[#This Row],[Level]]*6</f>
-        <v>210</v>
+        <v>150</v>
       </c>
       <c r="F11">
         <f>Table1316183336[[#This Row],[Level]]*1</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="G11">
         <f>Table1316183336[[#This Row],[Level]]*6</f>
-        <v>210</v>
+        <v>150</v>
       </c>
       <c r="H11">
         <f>Table1316183336[[#This Row],[Level]]*1.5</f>
-        <v>52.5</v>
+        <v>37.5</v>
       </c>
       <c r="I11">
         <f>Table1316183336[[#This Row],[Level]]*1.125</f>
-        <v>39.375</v>
+        <v>28.125</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -6002,7 +6002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76FD8A7-49F8-4714-9911-92DFAEEE64EB}">
   <dimension ref="A2:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Done factoring goblin fights, consumable items, and item table and started working on road to Tellren
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="8" activeTab="13" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="14" activeTab="15" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Skeleton Soldier" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="Goblin" sheetId="2" r:id="rId13"/>
     <sheet name="Slimes" sheetId="16" r:id="rId14"/>
     <sheet name="Corpse Eater" sheetId="17" r:id="rId15"/>
+    <sheet name="Barren Wolf" sheetId="18" r:id="rId16"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="60">
   <si>
     <t>Skeletons are the most basic undead, they have low magical attributes, agility, and luck.</t>
   </si>
@@ -210,6 +211,15 @@
   <si>
     <t>Corpse Eater</t>
   </si>
+  <si>
+    <t>An Earth type monster, may look similar to normal wolfs but since it’s a monster it is much stronger</t>
+  </si>
+  <si>
+    <t>Barren Wolf</t>
+  </si>
+  <si>
+    <t>Alpha wolf should have mark enemy skill!</t>
+  </si>
 </sst>
 </file>
 
@@ -285,7 +295,34 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="198">
+  <dxfs count="207">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1674,7 +1711,7 @@
     <tableColumn id="7" xr3:uid="{F9852B29-E77D-4E17-A56E-5F0C649FA862}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{9A914BFF-1060-46E4-B8F9-412BD9293C3D}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2F83B650-811D-4FEE-92D5-03D4DC4376E5}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="197">
+    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="206">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1695,7 +1732,7 @@
     <tableColumn id="7" xr3:uid="{3A2FD57C-060A-462E-8BB9-B06F717E9D20}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{ED9393EA-F7F9-4661-8D0B-0D9246DDABF8}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{6F56342F-5442-42CD-8B6C-D98B6D6C0C56}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="153">
+    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="162">
       <calculatedColumnFormula>SUM(Table16[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1708,28 +1745,28 @@
   <autoFilter ref="A8:I13" xr:uid="{7BE337CC-37BD-4688-B60D-A66F4420668B}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{71340E4C-6101-4C59-8ED7-689E2AD5A962}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="152">
+    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="161">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*63-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="151">
+    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="160">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="150">
+    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="159">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="149">
+    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="158">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="148">
+    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="157">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="147">
+    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="156">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="146">
+    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="155">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="145">
+    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="154">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1750,7 +1787,7 @@
     <tableColumn id="7" xr3:uid="{4899BF24-9D2A-4CC0-AE35-4F49604AAC5A}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{CB1CC6BA-1D38-4B74-9BC6-7057FB9773EE}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{C47FADF6-C526-4188-9187-383757CE17C1}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="144">
+    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="153">
       <calculatedColumnFormula>SUM(Table168[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1763,28 +1800,28 @@
   <autoFilter ref="A9:I15" xr:uid="{06A56D17-07E5-4650-8EE9-7EA8F94D4020}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A2BE27C9-9DAE-49F5-9A70-C6CF7428BF31}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="143">
+    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="152">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="142">
+    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="151">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="141">
+    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="150">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="140">
+    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="149">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="139">
+    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="148">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.375+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="138">
+    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="147">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="137">
+    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="146">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="136">
+    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="145">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1805,7 +1842,7 @@
     <tableColumn id="7" xr3:uid="{60AD88FB-4685-412B-B5FD-BF8412C6B8E2}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{6A88D48C-D864-4F16-BEF2-BA88783A3FF3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{D40BD230-6392-4A28-A29D-F13EFE35C95E}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A0E09B2B-FD41-413F-8063-62214E990751}" name="Total" dataDxfId="135">
+    <tableColumn id="10" xr3:uid="{A0E09B2B-FD41-413F-8063-62214E990751}" name="Total" dataDxfId="144">
       <calculatedColumnFormula>SUM(Table16826[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1818,28 +1855,28 @@
   <autoFilter ref="A8:I14" xr:uid="{F7062CBA-4FAA-4900-9D3A-5C6613BCB6CE}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{ADCB4852-D3A0-456B-A8BD-E5F74BDBB762}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{ED76047D-1BC2-4C1B-B9B0-58BE0ACDDA48}" name="HP" dataDxfId="134">
+    <tableColumn id="2" xr3:uid="{ED76047D-1BC2-4C1B-B9B0-58BE0ACDDA48}" name="HP" dataDxfId="143">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EC859C53-0BA5-45D1-868B-F22DC8CE7D25}" name="MP" dataDxfId="133">
+    <tableColumn id="3" xr3:uid="{EC859C53-0BA5-45D1-868B-F22DC8CE7D25}" name="MP" dataDxfId="142">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DED33AB9-A2BB-4F9E-AA6D-02F8D1D65CD1}" name="ATK" dataDxfId="132">
+    <tableColumn id="4" xr3:uid="{DED33AB9-A2BB-4F9E-AA6D-02F8D1D65CD1}" name="ATK" dataDxfId="141">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.375+ 15+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{329B716D-9CA6-4546-AB13-92D88BE40F5F}" name="DEF" dataDxfId="131">
+    <tableColumn id="5" xr3:uid="{329B716D-9CA6-4546-AB13-92D88BE40F5F}" name="DEF" dataDxfId="140">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1 + 15+12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{67F8198A-5FC2-4C6D-9558-68B3141EA756}" name="MAT" dataDxfId="130">
+    <tableColumn id="6" xr3:uid="{67F8198A-5FC2-4C6D-9558-68B3141EA756}" name="MAT" dataDxfId="139">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C70F5BF6-63B0-44C1-862D-25E3FB55320F}" name="MDF" dataDxfId="129">
+    <tableColumn id="7" xr3:uid="{C70F5BF6-63B0-44C1-862D-25E3FB55320F}" name="MDF" dataDxfId="138">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.5+15+11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AB20AF53-453C-4266-A46B-40E693C91985}" name="AGI" dataDxfId="128">
+    <tableColumn id="8" xr3:uid="{AB20AF53-453C-4266-A46B-40E693C91985}" name="AGI" dataDxfId="137">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7FC46A31-F9F1-432E-B399-0823E198FE0A}" name="LUK" dataDxfId="127">
+    <tableColumn id="9" xr3:uid="{7FC46A31-F9F1-432E-B399-0823E198FE0A}" name="LUK" dataDxfId="136">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.5+15+20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1860,7 +1897,7 @@
     <tableColumn id="7" xr3:uid="{20C5D094-BAF0-471C-ACF3-C6658991DB5F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{E08E2AF0-56DD-4A69-A536-27139D793022}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{12AD8606-1127-4E5B-BA2C-872780F22F9E}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{5E2EF778-63AE-48B7-9F49-0D2AFEBD66A1}" name="Total" dataDxfId="126">
+    <tableColumn id="10" xr3:uid="{5E2EF778-63AE-48B7-9F49-0D2AFEBD66A1}" name="Total" dataDxfId="135">
       <calculatedColumnFormula>SUM(Table1682630[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1873,28 +1910,28 @@
   <autoFilter ref="A8:I14" xr:uid="{299912CC-280B-49E1-8859-432D05893259}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4F0B657F-C9A5-4A73-AAA3-27D307385193}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{526284E7-597F-4726-AB18-230CA03461B1}" name="HP" dataDxfId="125">
+    <tableColumn id="2" xr3:uid="{526284E7-597F-4726-AB18-230CA03461B1}" name="HP" dataDxfId="134">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*63+ 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E7BA3C7A-2677-415F-BA47-A4E88679B948}" name="MP" dataDxfId="124">
+    <tableColumn id="3" xr3:uid="{E7BA3C7A-2677-415F-BA47-A4E88679B948}" name="MP" dataDxfId="133">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE7BE678-2229-44F6-8732-71214FB69DD7}" name="ATK" dataDxfId="123">
+    <tableColumn id="4" xr3:uid="{AE7BE678-2229-44F6-8732-71214FB69DD7}" name="ATK" dataDxfId="132">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+ 15+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4715E3DB-8817-43D5-9074-9FB5F0BEF5B4}" name="DEF" dataDxfId="122">
+    <tableColumn id="5" xr3:uid="{4715E3DB-8817-43D5-9074-9FB5F0BEF5B4}" name="DEF" dataDxfId="131">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1 + 15+12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9CE76933-D045-418B-A975-378EEA51D856}" name="MAT" dataDxfId="121">
+    <tableColumn id="6" xr3:uid="{9CE76933-D045-418B-A975-378EEA51D856}" name="MAT" dataDxfId="130">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244B9611-6CB0-4946-B5CD-7D42311C7D7E}" name="MDF" dataDxfId="120">
+    <tableColumn id="7" xr3:uid="{244B9611-6CB0-4946-B5CD-7D42311C7D7E}" name="MDF" dataDxfId="129">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+15+11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32550C13-49BB-41D2-BA0A-26798830A0FD}" name="AGI" dataDxfId="119">
+    <tableColumn id="8" xr3:uid="{32550C13-49BB-41D2-BA0A-26798830A0FD}" name="AGI" dataDxfId="128">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{BB22F289-8AF5-4DD6-877B-F09520710555}" name="LUK" dataDxfId="118">
+    <tableColumn id="9" xr3:uid="{BB22F289-8AF5-4DD6-877B-F09520710555}" name="LUK" dataDxfId="127">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+15+20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1907,28 +1944,28 @@
   <autoFilter ref="A4:I10" xr:uid="{A1EAC62C-C07D-464E-91B1-4A34E6604BA2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{430FD3D4-914C-4309-B2E6-6F01B5CAED94}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="117">
+    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="126">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="116">
+    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="125">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="115">
+    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="124">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="114">
+    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="123">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15 + 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="113">
+    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="122">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15 + 30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="112">
+    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="121">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15 + 21</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="111">
+    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="120">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="110">
+    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="119">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1941,28 +1978,28 @@
   <autoFilter ref="A7:I12" xr:uid="{9BE7336F-352A-4FAE-B0E4-61965FC814C7}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B8DA50BB-4379-43D1-879B-CDBE6D82C13A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="109">
+    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="118">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="108">
+    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="117">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="107">
+    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="116">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="106">
+    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="115">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="105">
+    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="114">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="104">
+    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="113">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="103">
+    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="112">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="102">
+    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="111">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1975,28 +2012,28 @@
   <autoFilter ref="A8:I13" xr:uid="{67385006-CBB9-4472-99D4-7881E042769D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FD96F8F7-CCAB-44FA-B525-A5081670706A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="196">
+    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="205">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="195">
+    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="204">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="194">
+    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="203">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="193">
+    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="202">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="192">
+    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="201">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="191">
+    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="200">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="190">
+    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="199">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="189">
+    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="198">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2017,7 +2054,7 @@
     <tableColumn id="7" xr3:uid="{AEFF5C29-BE6A-4CF8-A2BB-F6B076077DA9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{4DE9B01E-67F2-4136-ADC3-60389FB67DCC}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{F5A82F03-513C-46D4-9F91-470F0060526B}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="101">
+    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="110">
       <calculatedColumnFormula>SUM(Table16821[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2026,22 +2063,22 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="100" tableBorderDxfId="99">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="109" tableBorderDxfId="108">
   <autoFilter ref="A15:I16" xr:uid="{434CBBE2-2F8D-4EEB-895C-68FC850EF1FD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="98"/>
-    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="97">
+    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="107"/>
+    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="106">
       <calculatedColumnFormula>Table1922[Level]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="96">
+    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="105">
       <calculatedColumnFormula>Table1922[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="95"/>
-    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="94"/>
-    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="93"/>
-    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="92"/>
-    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="91"/>
-    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="90"/>
+    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="104"/>
+    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="103"/>
+    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="102"/>
+    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="101"/>
+    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="100"/>
+    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="99"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2052,28 +2089,28 @@
   <autoFilter ref="A3:I9" xr:uid="{A90D1C2A-DBF9-4EEF-ACC2-3DC17C207301}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BD3505AC-AE6D-4947-A74E-A6C2D68658F1}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="89">
+    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="98">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="88">
+    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="97">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="87">
+    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="96">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="86">
+    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="95">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="85">
+    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="94">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="84">
+    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="93">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="83">
+    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="92">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="82">
+    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="91">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2082,32 +2119,32 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="81" tableBorderDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="90" tableBorderDxfId="89">
   <autoFilter ref="L3:T4" xr:uid="{5D2C3EA8-1297-4C77-AF32-84E50F8232C5}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="79"/>
-    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="78">
+    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="88"/>
+    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="87">
       <calculatedColumnFormula>Table19[Level]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="77">
+    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="86">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="76">
+    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="85">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="75">
+    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="84">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1 + 15 + 6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="74">
+    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="83">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="73">
+    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="82">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="72">
+    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="81">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="71">
+    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="80">
       <calculatedColumnFormula>Table19[Level] + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2120,28 +2157,28 @@
   <autoFilter ref="A7:I12" xr:uid="{553298A4-7E43-42CF-9EEB-1F9E7E6BAD27}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2AA35C8B-719C-4BA6-9CDF-2963E1C9F233}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C087FAFA-9653-40EC-B4B9-5CB8F9D7255E}" name="HP" dataDxfId="70">
+    <tableColumn id="2" xr3:uid="{C087FAFA-9653-40EC-B4B9-5CB8F9D7255E}" name="HP" dataDxfId="79">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0004B47B-3968-4C5A-BE6C-B822A307D7C5}" name="MP" dataDxfId="69">
+    <tableColumn id="3" xr3:uid="{0004B47B-3968-4C5A-BE6C-B822A307D7C5}" name="MP" dataDxfId="78">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{67EC8D91-0122-40D7-87D0-A3AB6788CE9D}" name="ATK" dataDxfId="68">
+    <tableColumn id="4" xr3:uid="{67EC8D91-0122-40D7-87D0-A3AB6788CE9D}" name="ATK" dataDxfId="77">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E9988E54-33D6-41EB-B6BE-6E832544E18C}" name="DEF" dataDxfId="67">
+    <tableColumn id="5" xr3:uid="{E9988E54-33D6-41EB-B6BE-6E832544E18C}" name="DEF" dataDxfId="76">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{16D71A55-372C-4029-A831-ECF2325E46C4}" name="MAT" dataDxfId="66">
+    <tableColumn id="6" xr3:uid="{16D71A55-372C-4029-A831-ECF2325E46C4}" name="MAT" dataDxfId="75">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{1802FB48-B110-4DBF-A8F2-64CD4890E741}" name="MDF" dataDxfId="65">
+    <tableColumn id="7" xr3:uid="{1802FB48-B110-4DBF-A8F2-64CD4890E741}" name="MDF" dataDxfId="74">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{350CA8CC-761C-4994-9D80-14685787EF3D}" name="AGI" dataDxfId="64">
+    <tableColumn id="8" xr3:uid="{350CA8CC-761C-4994-9D80-14685787EF3D}" name="AGI" dataDxfId="73">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B578CF58-136A-41B9-800E-D75836A4CDD1}" name="LUK" dataDxfId="63">
+    <tableColumn id="9" xr3:uid="{B578CF58-136A-41B9-800E-D75836A4CDD1}" name="LUK" dataDxfId="72">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2162,7 +2199,7 @@
     <tableColumn id="7" xr3:uid="{5A405725-30A7-487F-95BF-061F71CA9C61}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{644DEF70-6EBD-403E-904B-6C30E5FBEA48}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{BA93DA54-96B9-48D1-80BB-C266771E13F1}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{3EBB17A5-47EA-458B-83A5-7056BE67D25F}" name="Total" dataDxfId="62">
+    <tableColumn id="10" xr3:uid="{3EBB17A5-47EA-458B-83A5-7056BE67D25F}" name="Total" dataDxfId="71">
       <calculatedColumnFormula>SUM(Table1682134[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2171,26 +2208,26 @@
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{A7C0F3AC-4E86-430D-AE55-8604641B493E}" name="Table192235" displayName="Table192235" ref="A15:I16" totalsRowShown="0" dataDxfId="61" tableBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{A7C0F3AC-4E86-430D-AE55-8604641B493E}" name="Table192235" displayName="Table192235" ref="A15:I16" totalsRowShown="0" dataDxfId="70" tableBorderDxfId="69">
   <autoFilter ref="A15:I16" xr:uid="{D0DF3ED4-9A21-493B-88F4-CE5814AF31C9}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A78A876E-6C8B-4FC8-BFD4-A9BC80EA3FC2}" name="Level" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{4B423FFC-D037-484D-A927-2F66E15D422A}" name="HP" dataDxfId="58">
+    <tableColumn id="1" xr3:uid="{A78A876E-6C8B-4FC8-BFD4-A9BC80EA3FC2}" name="Level" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{4B423FFC-D037-484D-A927-2F66E15D422A}" name="HP" dataDxfId="67">
       <calculatedColumnFormula>(Table192235[Level]*75 + 500)*2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B695FEDE-EC59-44D8-AE99-CBF568DE5C93}" name="MP" dataDxfId="57">
+    <tableColumn id="3" xr3:uid="{B695FEDE-EC59-44D8-AE99-CBF568DE5C93}" name="MP" dataDxfId="66">
       <calculatedColumnFormula>Table192235[[#This Row],[Level]]*14 + 80</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{160D5D77-34E8-44F3-B51D-7CC0736DDCB1}" name="ATK" dataDxfId="56">
+    <tableColumn id="4" xr3:uid="{160D5D77-34E8-44F3-B51D-7CC0736DDCB1}" name="ATK" dataDxfId="65">
       <calculatedColumnFormula>Table192235[[#This Row],[Level]]*1.5+ 15 + 50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{559DAC37-CD6A-449F-AFF0-355ADE7CED80}" name="DEF" dataDxfId="55"/>
-    <tableColumn id="6" xr3:uid="{EEC344A5-27A5-450E-B795-04D237DD063F}" name="MAT" dataDxfId="54">
+    <tableColumn id="5" xr3:uid="{559DAC37-CD6A-449F-AFF0-355ADE7CED80}" name="DEF" dataDxfId="64"/>
+    <tableColumn id="6" xr3:uid="{EEC344A5-27A5-450E-B795-04D237DD063F}" name="MAT" dataDxfId="63">
       <calculatedColumnFormula>Table192235[Level]*1.5+15+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{54363CA4-9EE5-495F-8323-6C0C1261453C}" name="MDF" dataDxfId="53"/>
-    <tableColumn id="8" xr3:uid="{26B56E9D-2FCD-4476-A6CF-8F2EDC965246}" name="AGI" dataDxfId="52"/>
-    <tableColumn id="9" xr3:uid="{95814D66-3343-4190-9BF4-F4E45AB27D95}" name="LUK" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{54363CA4-9EE5-495F-8323-6C0C1261453C}" name="MDF" dataDxfId="62"/>
+    <tableColumn id="8" xr3:uid="{26B56E9D-2FCD-4476-A6CF-8F2EDC965246}" name="AGI" dataDxfId="61"/>
+    <tableColumn id="9" xr3:uid="{95814D66-3343-4190-9BF4-F4E45AB27D95}" name="LUK" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2209,7 +2246,7 @@
     <tableColumn id="7" xr3:uid="{22216E02-260E-4471-8BB1-4E6E1250BAC9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{DC2670AC-8DF2-47F7-A3F6-EE7896309BC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{749652E2-F6CF-428C-B67C-FD0B1EFCCBBF}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="50">
+    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="59">
       <calculatedColumnFormula>SUM(Table15[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2222,28 +2259,28 @@
   <autoFilter ref="A15:I20" xr:uid="{A1CF627F-8D28-44AD-9A35-411103976FCA}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F14CC326-DE44-48D8-856F-8DCDCFC89CAD}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="49">
+    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="58">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*63-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="48">
+    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="57">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="47">
+    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="56">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="46">
+    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="55">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="45">
+    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="54">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="44">
+    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="53">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="43">
+    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="52">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="42">
+    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="51">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2256,28 +2293,28 @@
   <autoFilter ref="K11:S17" xr:uid="{EAF9FB6A-F011-40E3-AB2F-E53826722AFB}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DF3E0800-6EE4-4E1B-BA6F-0194351D6E7C}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="41">
+    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="50">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*56.25+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="40">
+    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="49">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="39">
+    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="48">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="38">
+    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="47">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="37">
+    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="46">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="36">
+    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="45">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="35">
+    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="44">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="34">
+    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="43">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2290,28 +2327,28 @@
   <autoFilter ref="K8:S14" xr:uid="{AB7E938D-7ACC-4BFB-A6B9-682B8B29CEF2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{66EB8EF1-BCF4-44F7-B8A6-3C3B425F8FF5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="188">
+    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="197">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*56.25+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="187">
+    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="196">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="186">
+    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="195">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25+ 15+30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="185">
+    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="194">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25 + 15+33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="184">
+    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="193">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="183">
+    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="192">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="182">
+    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="191">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="181">
+    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="190">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2324,28 +2361,28 @@
   <autoFilter ref="A26:I31" xr:uid="{870F76F2-5EA7-4FD7-B1F9-507D64592088}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{3C04B742-338A-4366-BF3D-C5BC13023785}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="33">
+    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="42">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*63+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="32">
+    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="41">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="31">
+    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="40">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="30">
+    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="39">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="29">
+    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="38">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="28">
+    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="37">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="27">
+    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="36">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="26">
+    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="35">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2358,28 +2395,28 @@
   <autoFilter ref="A36:I41" xr:uid="{9BD043AF-0D77-4FF4-B2F9-B4AC3C3F1F82}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{7BB908A3-05D7-4357-920B-BF4C6BC20C06}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="25">
+    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="34">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*56.5+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="24">
+    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="33">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*12.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="23">
+    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="32">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="22">
+    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="31">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1 + 15+14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="21">
+    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="30">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="20">
+    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="29">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.5+ 15+13</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="19">
+    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="28">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="18">
+    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="27">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.375 + 15+40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2400,7 +2437,7 @@
     <tableColumn id="7" xr3:uid="{09E4151E-54A0-41FF-BA5B-3B1C748DA23D}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{909575E0-EC13-4E35-A35F-2451A5741589}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2CDCF32E-D8FC-48D9-A28D-8D9C5F3EB001}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{001DA1BB-34DD-4786-BDE4-23C510900A3D}" name="Total" dataDxfId="17">
+    <tableColumn id="10" xr3:uid="{001DA1BB-34DD-4786-BDE4-23C510900A3D}" name="Total" dataDxfId="26">
       <calculatedColumnFormula>SUM(Table168213429[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2413,28 +2450,28 @@
   <autoFilter ref="A7:I12" xr:uid="{4ED64482-035D-49B9-A477-A1D5AEB4A5A4}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{141B0E2E-D4F3-4884-86FD-AAD67C363749}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{D4B50877-EF56-4EF7-8C6D-9928A6D654F6}" name="HP" dataDxfId="16">
+    <tableColumn id="2" xr3:uid="{D4B50877-EF56-4EF7-8C6D-9928A6D654F6}" name="HP" dataDxfId="25">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*125</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F4B06187-BE28-4283-9518-F773FE75C2BF}" name="MP" dataDxfId="15">
+    <tableColumn id="3" xr3:uid="{F4B06187-BE28-4283-9518-F773FE75C2BF}" name="MP" dataDxfId="24">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{91A68FC7-5F16-4880-AE82-97341814BB95}" name="ATK" dataDxfId="14">
+    <tableColumn id="4" xr3:uid="{91A68FC7-5F16-4880-AE82-97341814BB95}" name="ATK" dataDxfId="23">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*4.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{2BCD0E58-85DE-4C10-BFBC-AF77BC569C92}" name="DEF" dataDxfId="13">
+    <tableColumn id="5" xr3:uid="{2BCD0E58-85DE-4C10-BFBC-AF77BC569C92}" name="DEF" dataDxfId="22">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7C48A1FC-CE8F-4CDD-9A3D-308B46D78A48}" name="MAT" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{7C48A1FC-CE8F-4CDD-9A3D-308B46D78A48}" name="MAT" dataDxfId="21">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{474D8178-EA8C-4322-93C3-B7F6EBA88102}" name="MDF" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{474D8178-EA8C-4322-93C3-B7F6EBA88102}" name="MDF" dataDxfId="20">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{257B31D9-5838-45E0-A56E-9B1566E1A34A}" name="AGI" dataDxfId="10">
+    <tableColumn id="8" xr3:uid="{257B31D9-5838-45E0-A56E-9B1566E1A34A}" name="AGI" dataDxfId="19">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{17960EB4-4250-49DB-9A6B-455B9913B04B}" name="LUK" dataDxfId="9">
+    <tableColumn id="9" xr3:uid="{17960EB4-4250-49DB-9A6B-455B9913B04B}" name="LUK" dataDxfId="18">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1.125</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2455,7 +2492,7 @@
     <tableColumn id="7" xr3:uid="{07EA0638-8880-4944-AC9E-13E3F1B9F651}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{AA18E602-126F-4D69-9CC8-C097E8EB9C70}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{5563B0CB-2EA7-4851-8D1F-D77E0F90CBAD}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{2D960B43-0F76-4936-9508-4D501A79A83C}" name="Total" dataDxfId="8">
+    <tableColumn id="10" xr3:uid="{2D960B43-0F76-4936-9508-4D501A79A83C}" name="Total" dataDxfId="17">
       <calculatedColumnFormula>SUM(Table16821342932[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2468,29 +2505,84 @@
   <autoFilter ref="A5:I10" xr:uid="{2922C913-6AE8-4B89-BDA6-9F44D59987D8}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{3D67222C-6501-4A5D-A9FC-528EE591A288}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EE3E4CCC-C404-4B78-AAB4-3B38166E23BA}" name="HP" dataDxfId="7">
+    <tableColumn id="2" xr3:uid="{EE3E4CCC-C404-4B78-AAB4-3B38166E23BA}" name="HP" dataDxfId="16">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DE5141FB-3B4E-46D4-9E0D-AF1DEE998B4A}" name="MP" dataDxfId="6">
+    <tableColumn id="3" xr3:uid="{DE5141FB-3B4E-46D4-9E0D-AF1DEE998B4A}" name="MP" dataDxfId="15">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{404B3E88-DF62-4AA0-82D6-C21C2BCA762B}" name="ATK" dataDxfId="5">
+    <tableColumn id="4" xr3:uid="{404B3E88-DF62-4AA0-82D6-C21C2BCA762B}" name="ATK" dataDxfId="14">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*4.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{342B3F39-F7A2-45D8-9CD4-39B5ABC72D2F}" name="DEF" dataDxfId="4">
+    <tableColumn id="5" xr3:uid="{342B3F39-F7A2-45D8-9CD4-39B5ABC72D2F}" name="DEF" dataDxfId="13">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{CD819DB3-9F2E-4428-AAFC-72776ECB8EAF}" name="MAT" dataDxfId="3">
+    <tableColumn id="6" xr3:uid="{CD819DB3-9F2E-4428-AAFC-72776ECB8EAF}" name="MAT" dataDxfId="12">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{270DF964-8095-43FD-B050-DD4A2A138F32}" name="MDF" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{270DF964-8095-43FD-B050-DD4A2A138F32}" name="MDF" dataDxfId="11">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4F4D3B2A-5B86-4AB7-A97E-18E2868266B8}" name="AGI" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{4F4D3B2A-5B86-4AB7-A97E-18E2868266B8}" name="AGI" dataDxfId="10">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{0178CE2D-63C5-426A-A081-D62E62FF91AC}" name="LUK" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{0178CE2D-63C5-426A-A081-D62E62FF91AC}" name="LUK" dataDxfId="9">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*1.5</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table36.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{D8FF574E-7CB5-44ED-ACC1-441286183A98}" name="Table1682134293227" displayName="Table1682134293227" ref="A3:J4" totalsRowShown="0">
+  <autoFilter ref="A3:J4" xr:uid="{8A31C229-01C6-437B-9E04-6F843FD0C86C}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{F3569224-AAE7-4DCF-97C9-1036932CDEE2}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{6E383D0B-96C5-451F-A34A-04D1D515E64F}" name="HP"/>
+    <tableColumn id="3" xr3:uid="{388E448C-9DA4-4F05-A4ED-52905AE0B683}" name="MP"/>
+    <tableColumn id="4" xr3:uid="{ACBE6513-AE17-4148-984B-3642C7E81A30}" name="ATK"/>
+    <tableColumn id="5" xr3:uid="{232AF18F-B72F-4887-8648-9A98555B95F0}" name="DEF"/>
+    <tableColumn id="6" xr3:uid="{8F2BC7A2-DB88-42F9-9985-4935DC400D24}" name="MAT"/>
+    <tableColumn id="7" xr3:uid="{C374A90B-690A-432C-974A-C8A7D22E367F}" name="MDF"/>
+    <tableColumn id="8" xr3:uid="{05C64890-0DC2-4577-975E-95477DCED789}" name="AGI"/>
+    <tableColumn id="9" xr3:uid="{CE6AAEA9-D599-4B9B-BD40-7E602F47088C}" name="LUK"/>
+    <tableColumn id="10" xr3:uid="{30017AE7-6C23-415F-A2EA-70EA09C835E6}" name="Total" dataDxfId="8">
+      <calculatedColumnFormula>SUM(Table1682134293227[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table37.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{74260B06-AD17-472A-BF93-18F4B0E61A60}" name="Table13161833363738" displayName="Table13161833363738" ref="A6:I11" totalsRowShown="0">
+  <autoFilter ref="A6:I11" xr:uid="{D09397F4-7631-4CD3-AF40-3B14C64478EE}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{BF4E6A79-8CCF-498E-B3B0-FA782AB06519}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{37E52E57-C499-4FFB-AC3F-20E63EEA4D3A}" name="HP" dataDxfId="5">
+      <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*87.5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{D29F5CDE-1200-4C77-A4BA-0DE4F7C46627}" name="MP" dataDxfId="7">
+      <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{9701140A-64F9-4967-9DEE-3460411D91C1}" name="ATK" dataDxfId="4">
+      <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*6</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{F90A425E-E031-4255-8AF9-DAD672F8DD7D}" name="DEF" dataDxfId="1">
+      <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*4.5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{255210A0-6EB8-4CFB-84DD-42C88AEAF7AA}" name="MAT" dataDxfId="2">
+      <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{91177FDD-F316-4D6B-A547-FC5FA6DAC266}" name="MDF" dataDxfId="0">
+      <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{ADA902F7-B7D7-4B1B-A144-E5252296AB61}" name="AGI" dataDxfId="6">
+      <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*6</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{78273DA6-F2CA-4999-B4EA-F6C044BC41AB}" name="LUK" dataDxfId="3">
+      <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2510,7 +2602,7 @@
     <tableColumn id="7" xr3:uid="{F833922A-76F9-427C-8462-D94DE51D0477}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{203171A1-C88B-4F81-ADC2-1EE072D645F3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{34003EF6-E9A5-4584-A186-09DFF4EC11C7}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{C4602156-F897-42BE-8F3F-411E13EEB095}" name="Total" dataDxfId="180">
+    <tableColumn id="10" xr3:uid="{C4602156-F897-42BE-8F3F-411E13EEB095}" name="Total" dataDxfId="189">
       <calculatedColumnFormula>SUM(Table114[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2523,28 +2615,28 @@
   <autoFilter ref="A8:I14" xr:uid="{D3C3F418-ED32-4504-9D73-88545A192967}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{13E0AF4A-AA83-489A-A156-B01D4F48D2F5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{B970139F-8BB5-4CE6-92F8-79E3236AC62B}" name="HP" dataDxfId="179">
+    <tableColumn id="2" xr3:uid="{B970139F-8BB5-4CE6-92F8-79E3236AC62B}" name="HP" dataDxfId="188">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*63+300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7BCF83B8-7492-4991-A008-F212725940B9}" name="MP" dataDxfId="178">
+    <tableColumn id="3" xr3:uid="{7BCF83B8-7492-4991-A008-F212725940B9}" name="MP" dataDxfId="187">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{33220A80-38D8-4480-ACC7-DF484072C96B}" name="ATK" dataDxfId="177">
+    <tableColumn id="4" xr3:uid="{33220A80-38D8-4480-ACC7-DF484072C96B}" name="ATK" dataDxfId="186">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.5+ 15+40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{36708515-5004-4705-A558-44B59D0CE676}" name="DEF" dataDxfId="176">
+    <tableColumn id="5" xr3:uid="{36708515-5004-4705-A558-44B59D0CE676}" name="DEF" dataDxfId="185">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25 + 15+21</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{11729EA3-08C4-4E0B-B5EE-5B3C08A31A9C}" name="MAT" dataDxfId="175">
+    <tableColumn id="6" xr3:uid="{11729EA3-08C4-4E0B-B5EE-5B3C08A31A9C}" name="MAT" dataDxfId="184">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B179D090-E484-4663-937A-480D1164D655}" name="MDF" dataDxfId="174">
+    <tableColumn id="7" xr3:uid="{B179D090-E484-4663-937A-480D1164D655}" name="MDF" dataDxfId="183">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25+15 + 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{28323AD0-B3BD-401F-A237-92C8B8D70FEA}" name="AGI" dataDxfId="173">
+    <tableColumn id="8" xr3:uid="{28323AD0-B3BD-401F-A237-92C8B8D70FEA}" name="AGI" dataDxfId="182">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{657BED8B-4C8A-42DC-BECD-5EEF9D1B7F37}" name="LUK" dataDxfId="172">
+    <tableColumn id="9" xr3:uid="{657BED8B-4C8A-42DC-BECD-5EEF9D1B7F37}" name="LUK" dataDxfId="181">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2565,7 +2657,7 @@
     <tableColumn id="7" xr3:uid="{D1DFC0D2-A987-4E3F-BA23-52162FB0C0BA}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{AB6209DB-CCCB-4C37-B455-4C7652E0DAC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2CD4CD14-92FD-41A7-9CCD-1329B5A77390}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{3B2C0A10-5038-4C21-BAC5-12FB16275D2E}" name="Total" dataDxfId="171">
+    <tableColumn id="10" xr3:uid="{3B2C0A10-5038-4C21-BAC5-12FB16275D2E}" name="Total" dataDxfId="180">
       <calculatedColumnFormula>SUM(Table11412[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2578,28 +2670,28 @@
   <autoFilter ref="A8:I14" xr:uid="{43F790D1-EA7B-4BAE-8A37-7CAD791E8821}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F6E842E1-B25F-4CA1-9107-AC7179420C29}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EFB2F0D5-318D-4A65-BA2B-20ADDE071648}" name="HP" dataDxfId="170">
+    <tableColumn id="2" xr3:uid="{EFB2F0D5-318D-4A65-BA2B-20ADDE071648}" name="HP" dataDxfId="179">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0D914B89-2678-453F-BC18-571DCD45E628}" name="MP" dataDxfId="169">
+    <tableColumn id="3" xr3:uid="{0D914B89-2678-453F-BC18-571DCD45E628}" name="MP" dataDxfId="178">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*13.75 + 80</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{6FBD2F64-5B1C-4035-BB1A-AFB092DB60C3}" name="ATK" dataDxfId="168">
+    <tableColumn id="4" xr3:uid="{6FBD2F64-5B1C-4035-BB1A-AFB092DB60C3}" name="ATK" dataDxfId="177">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7E0AF3FC-CC5D-4A6A-A4A2-DE278DEC4062}" name="DEF" dataDxfId="167">
+    <tableColumn id="5" xr3:uid="{7E0AF3FC-CC5D-4A6A-A4A2-DE278DEC4062}" name="DEF" dataDxfId="176">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1 + 15 + 4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3AF4D559-893B-4D50-BCB4-A1BD1FAF2F23}" name="MAT" dataDxfId="166">
+    <tableColumn id="6" xr3:uid="{3AF4D559-893B-4D50-BCB4-A1BD1FAF2F23}" name="MAT" dataDxfId="175">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6E9418A6-75AC-4541-9029-814EC5C06E70}" name="MDF" dataDxfId="165">
+    <tableColumn id="7" xr3:uid="{6E9418A6-75AC-4541-9029-814EC5C06E70}" name="MDF" dataDxfId="174">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.375+15 + 14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD605BEE-D561-4A2C-8D06-8E9AD70C32AC}" name="AGI" dataDxfId="164">
+    <tableColumn id="8" xr3:uid="{CD605BEE-D561-4A2C-8D06-8E9AD70C32AC}" name="AGI" dataDxfId="173">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E26506B2-F488-4AA4-AC87-819A22964609}" name="LUK" dataDxfId="163">
+    <tableColumn id="9" xr3:uid="{E26506B2-F488-4AA4-AC87-819A22964609}" name="LUK" dataDxfId="172">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2620,7 +2712,7 @@
     <tableColumn id="7" xr3:uid="{E91A64A8-F750-4893-9958-7C6ABC37405F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{3832FF0E-95E5-4B1F-B122-1EAFBF719DE3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{237404A9-EB50-465E-89AF-7167C57AFB99}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{927EBD24-571F-408C-A33B-59C753D9D96D}" name="Total" dataDxfId="162">
+    <tableColumn id="10" xr3:uid="{927EBD24-571F-408C-A33B-59C753D9D96D}" name="Total" dataDxfId="171">
       <calculatedColumnFormula>SUM(Table1141219[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2633,28 +2725,28 @@
   <autoFilter ref="A7:I13" xr:uid="{2539D8EE-2982-4734-B28B-342036FEDAC6}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FEE8F081-132E-4ED3-8FFD-2CF48368B2CC}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A79BC043-DB1A-48B4-AC21-AD31632979A6}" name="HP" dataDxfId="161">
+    <tableColumn id="2" xr3:uid="{A79BC043-DB1A-48B4-AC21-AD31632979A6}" name="HP" dataDxfId="170">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*63 + 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{42935B44-C727-42B0-B48E-0369818BF78A}" name="MP" dataDxfId="160">
+    <tableColumn id="3" xr3:uid="{42935B44-C727-42B0-B48E-0369818BF78A}" name="MP" dataDxfId="169">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{FC4572C7-88EC-4981-A6ED-43397844845B}" name="ATK" dataDxfId="159">
+    <tableColumn id="4" xr3:uid="{FC4572C7-88EC-4981-A6ED-43397844845B}" name="ATK" dataDxfId="168">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C8D61CEB-FFEC-42C3-9123-5140E65C1A2C}" name="DEF" dataDxfId="158">
+    <tableColumn id="5" xr3:uid="{C8D61CEB-FFEC-42C3-9123-5140E65C1A2C}" name="DEF" dataDxfId="167">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.375 + 15 + 19</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8C971683-28D2-4474-83CA-936F352F1324}" name="MAT" dataDxfId="157">
+    <tableColumn id="6" xr3:uid="{8C971683-28D2-4474-83CA-936F352F1324}" name="MAT" dataDxfId="166">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3371862A-9CF2-47CA-A149-4921E3B33162}" name="MDF" dataDxfId="156">
+    <tableColumn id="7" xr3:uid="{3371862A-9CF2-47CA-A149-4921E3B33162}" name="MDF" dataDxfId="165">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.375+15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC6AC739-B4C9-47A6-9472-439C60B629A0}" name="AGI" dataDxfId="155">
+    <tableColumn id="8" xr3:uid="{AC6AC739-B4C9-47A6-9472-439C60B629A0}" name="AGI" dataDxfId="164">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E727A271-B479-47C0-A557-227ABD8EC0AC}" name="LUK" dataDxfId="154">
+    <tableColumn id="9" xr3:uid="{E727A271-B479-47C0-A557-227ABD8EC0AC}" name="LUK" dataDxfId="163">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2962,7 +3054,7 @@
   <dimension ref="A2:S14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3520,7 +3612,7 @@
   <dimension ref="A2:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J17"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3888,8 +3980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED846686-A238-4174-849F-9F6770BD1F9B}">
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:T3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4235,7 +4327,7 @@
   <dimension ref="A2:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:I12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5704,8 +5796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6D1546-413F-4D33-8AC9-20828C70BDCB}">
   <dimension ref="A3:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5753,16 +5845,16 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E4">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H4">
         <v>5</v>
@@ -5772,7 +5864,7 @@
       </c>
       <c r="J4">
         <f>SUM(Table168213429[[#This Row],[HP]:[LUK]])</f>
-        <v>79</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -6003,7 +6095,7 @@
   <dimension ref="A2:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6051,26 +6143,26 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F3">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G3">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I3">
         <v>5</v>
       </c>
       <c r="J3">
         <f>SUM(Table16821342932[[#This Row],[HP]:[LUK]])</f>
-        <v>81</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -6285,6 +6377,314 @@
       <c r="I10">
         <f>Table131618333637[[#This Row],[Level]]*1.5</f>
         <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F7754B-A2F6-4572-9750-3C214A463E7D}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>40</v>
+      </c>
+      <c r="E4">
+        <v>28</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>32</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <f>SUM(Table1682134293227[[#This Row],[HP]:[LUK]])</f>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <f>Table13161833363738[[#This Row],[Level]]*87.5</f>
+        <v>87.5</v>
+      </c>
+      <c r="C7">
+        <f>Table13161833363738[[#This Row],[Level]]*10</f>
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <f>Table13161833363738[[#This Row],[Level]]*6</f>
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <f>Table13161833363738[[#This Row],[Level]]*4.5</f>
+        <v>4.5</v>
+      </c>
+      <c r="F7">
+        <f>Table13161833363738[[#This Row],[Level]]*1</f>
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f>Table13161833363738[[#This Row],[Level]]*3</f>
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <f>Table13161833363738[[#This Row],[Level]]*6</f>
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <f>Table13161833363738[[#This Row],[Level]]*1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <f>Table13161833363738[[#This Row],[Level]]*87.5</f>
+        <v>1312.5</v>
+      </c>
+      <c r="C8">
+        <f>Table13161833363738[[#This Row],[Level]]*10</f>
+        <v>150</v>
+      </c>
+      <c r="D8">
+        <f>Table13161833363738[[#This Row],[Level]]*6</f>
+        <v>90</v>
+      </c>
+      <c r="E8">
+        <f>Table13161833363738[[#This Row],[Level]]*4.5</f>
+        <v>67.5</v>
+      </c>
+      <c r="F8">
+        <f>Table13161833363738[[#This Row],[Level]]*1</f>
+        <v>15</v>
+      </c>
+      <c r="G8">
+        <f>Table13161833363738[[#This Row],[Level]]*3</f>
+        <v>45</v>
+      </c>
+      <c r="H8">
+        <f>Table13161833363738[[#This Row],[Level]]*6</f>
+        <v>90</v>
+      </c>
+      <c r="I8">
+        <f>Table13161833363738[[#This Row],[Level]]*1</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <f>Table13161833363738[[#This Row],[Level]]*87.5</f>
+        <v>2187.5</v>
+      </c>
+      <c r="C9">
+        <f>Table13161833363738[[#This Row],[Level]]*10</f>
+        <v>250</v>
+      </c>
+      <c r="D9">
+        <f>Table13161833363738[[#This Row],[Level]]*6</f>
+        <v>150</v>
+      </c>
+      <c r="E9">
+        <f>Table13161833363738[[#This Row],[Level]]*4.5</f>
+        <v>112.5</v>
+      </c>
+      <c r="F9">
+        <f>Table13161833363738[[#This Row],[Level]]*1</f>
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <f>Table13161833363738[[#This Row],[Level]]*3</f>
+        <v>75</v>
+      </c>
+      <c r="H9">
+        <f>Table13161833363738[[#This Row],[Level]]*6</f>
+        <v>150</v>
+      </c>
+      <c r="I9">
+        <f>Table13161833363738[[#This Row],[Level]]*1</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <f>Table13161833363738[[#This Row],[Level]]*87.5</f>
+        <v>3062.5</v>
+      </c>
+      <c r="C10">
+        <f>Table13161833363738[[#This Row],[Level]]*10</f>
+        <v>350</v>
+      </c>
+      <c r="D10">
+        <f>Table13161833363738[[#This Row],[Level]]*6</f>
+        <v>210</v>
+      </c>
+      <c r="E10">
+        <f>Table13161833363738[[#This Row],[Level]]*4.5</f>
+        <v>157.5</v>
+      </c>
+      <c r="F10">
+        <f>Table13161833363738[[#This Row],[Level]]*1</f>
+        <v>35</v>
+      </c>
+      <c r="G10">
+        <f>Table13161833363738[[#This Row],[Level]]*3</f>
+        <v>105</v>
+      </c>
+      <c r="H10">
+        <f>Table13161833363738[[#This Row],[Level]]*6</f>
+        <v>210</v>
+      </c>
+      <c r="I10">
+        <f>Table13161833363738[[#This Row],[Level]]*1</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <f>Table13161833363738[[#This Row],[Level]]*87.5</f>
+        <v>1750</v>
+      </c>
+      <c r="C11">
+        <f>Table13161833363738[[#This Row],[Level]]*10</f>
+        <v>200</v>
+      </c>
+      <c r="D11">
+        <f>Table13161833363738[[#This Row],[Level]]*6</f>
+        <v>120</v>
+      </c>
+      <c r="E11">
+        <f>Table13161833363738[[#This Row],[Level]]*4.5</f>
+        <v>90</v>
+      </c>
+      <c r="F11">
+        <f>Table13161833363738[[#This Row],[Level]]*1</f>
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <f>Table13161833363738[[#This Row],[Level]]*3</f>
+        <v>60</v>
+      </c>
+      <c r="H11">
+        <f>Table13161833363738[[#This Row],[Level]]*6</f>
+        <v>120</v>
+      </c>
+      <c r="I11">
+        <f>Table13161833363738[[#This Row],[Level]]*1</f>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made wolf enemies, preliminary map for Road to Tellren, next map is Tellren South Outskirts
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -212,13 +212,13 @@
     <t>Corpse Eater</t>
   </si>
   <si>
-    <t>An Earth type monster, may look similar to normal wolfs but since it’s a monster it is much stronger</t>
-  </si>
-  <si>
     <t>Barren Wolf</t>
   </si>
   <si>
     <t>Alpha wolf should have mark enemy skill!</t>
+  </si>
+  <si>
+    <t>An Earth type monster, may look similar to normal wolfs but since it’s a monster it is much stronger. Base Level 2</t>
   </si>
 </sst>
 </file>
@@ -2560,28 +2560,28 @@
   <autoFilter ref="A6:I11" xr:uid="{D09397F4-7631-4CD3-AF40-3B14C64478EE}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BF4E6A79-8CCF-498E-B3B0-FA782AB06519}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{37E52E57-C499-4FFB-AC3F-20E63EEA4D3A}" name="HP" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{37E52E57-C499-4FFB-AC3F-20E63EEA4D3A}" name="HP" dataDxfId="7">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*87.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D29F5CDE-1200-4C77-A4BA-0DE4F7C46627}" name="MP" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{D29F5CDE-1200-4C77-A4BA-0DE4F7C46627}" name="MP" dataDxfId="6">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{9701140A-64F9-4967-9DEE-3460411D91C1}" name="ATK" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{9701140A-64F9-4967-9DEE-3460411D91C1}" name="ATK" dataDxfId="5">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F90A425E-E031-4255-8AF9-DAD672F8DD7D}" name="DEF" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{F90A425E-E031-4255-8AF9-DAD672F8DD7D}" name="DEF" dataDxfId="4">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*4.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{255210A0-6EB8-4CFB-84DD-42C88AEAF7AA}" name="MAT" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{255210A0-6EB8-4CFB-84DD-42C88AEAF7AA}" name="MAT" dataDxfId="3">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{91177FDD-F316-4D6B-A547-FC5FA6DAC266}" name="MDF" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{91177FDD-F316-4D6B-A547-FC5FA6DAC266}" name="MDF" dataDxfId="2">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{ADA902F7-B7D7-4B1B-A144-E5252296AB61}" name="AGI" dataDxfId="6">
+    <tableColumn id="8" xr3:uid="{ADA902F7-B7D7-4B1B-A144-E5252296AB61}" name="AGI" dataDxfId="1">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{78273DA6-F2CA-4999-B4EA-F6C044BC41AB}" name="LUK" dataDxfId="3">
+    <tableColumn id="9" xr3:uid="{78273DA6-F2CA-4999-B4EA-F6C044BC41AB}" name="LUK" dataDxfId="0">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6393,19 +6393,19 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -6442,7 +6442,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4">
         <v>8</v>

</xml_diff>

<commit_message>
Connected Tellren City to rest of maps. Time for lots of cutscenes!
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -2722,19 +2722,19 @@
     <tableColumn id="4" xr3:uid="{D98F9CCD-2FEF-4FB2-B5AD-D2A6B610781B}" name="ATK" dataDxfId="13">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CF1AF448-2207-48D1-8FE3-0A6B5DE3511C}" name="DEF" dataDxfId="10">
+    <tableColumn id="5" xr3:uid="{CF1AF448-2207-48D1-8FE3-0A6B5DE3511C}" name="DEF" dataDxfId="12">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1 + 15 + 10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A632BAA7-E71C-41F8-B5B0-90891BB5BA9B}" name="MAT" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{A632BAA7-E71C-41F8-B5B0-90891BB5BA9B}" name="MAT" dataDxfId="11">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E76132BC-BC67-4915-8112-E0B292C65C91}" name="MDF" dataDxfId="9">
+    <tableColumn id="7" xr3:uid="{E76132BC-BC67-4915-8112-E0B292C65C91}" name="MDF" dataDxfId="10">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1 + 15 + 8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B25B7E33-B3CF-4D3D-9A14-3CE5B75535E8}" name="AGI" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{B25B7E33-B3CF-4D3D-9A14-3CE5B75535E8}" name="AGI" dataDxfId="9">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{40820F61-4B4C-4B23-95CF-AD5CDE975F4A}" name="LUK" dataDxfId="11">
+    <tableColumn id="9" xr3:uid="{40820F61-4B4C-4B23-95CF-AD5CDE975F4A}" name="LUK" dataDxfId="8">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2777,19 +2777,19 @@
     <tableColumn id="4" xr3:uid="{F3186E07-87BD-4E53-8F85-AB4798362B0C}" name="ATK" dataDxfId="5">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{22ED75D6-B85C-4DF9-BC39-4154BAF3990E}" name="DEF" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{22ED75D6-B85C-4DF9-BC39-4154BAF3990E}" name="DEF" dataDxfId="4">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1 + 15 + 4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B2DFC87A-2BEE-4B5A-AF53-4E18078ABC1B}" name="MAT" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{B2DFC87A-2BEE-4B5A-AF53-4E18078ABC1B}" name="MAT" dataDxfId="3">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.375 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{8FF82542-4129-4E67-AA7B-7CB38D8FB051}" name="MDF" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{8FF82542-4129-4E67-AA7B-7CB38D8FB051}" name="MDF" dataDxfId="2">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.375 + 15 + 14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{85F4097E-90A5-4A7C-B184-42B110E62300}" name="AGI" dataDxfId="4">
+    <tableColumn id="8" xr3:uid="{85F4097E-90A5-4A7C-B184-42B110E62300}" name="AGI" dataDxfId="1">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E1A21F56-D819-4CE3-9122-F47B8A4039A9}" name="LUK" dataDxfId="3">
+    <tableColumn id="9" xr3:uid="{E1A21F56-D819-4CE3-9122-F47B8A4039A9}" name="LUK" dataDxfId="0">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6887,8 +6887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDEC26FB-B5E4-44F5-B062-22E344453193}">
   <dimension ref="A2:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Working on tranquil hills. Added more dialogue in Tellren city
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="12" activeTab="17" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="12" activeTab="16" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Skeleton Soldier" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="70">
   <si>
     <t>Skeletons are the most basic undead, they have low magical attributes, agility, and luck.</t>
   </si>
@@ -246,6 +246,12 @@
   <si>
     <t>Lightning Behemoth</t>
   </si>
+  <si>
+    <t>Mercenary Priest, hammer -&gt; 40, 19/5</t>
+  </si>
+  <si>
+    <t>Mercenary Mage. Same equips</t>
+  </si>
 </sst>
 </file>
 
@@ -321,7 +327,31 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="240">
+  <dxfs count="248">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1836,7 +1866,7 @@
     <tableColumn id="7" xr3:uid="{F9852B29-E77D-4E17-A56E-5F0C649FA862}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{9A914BFF-1060-46E4-B8F9-412BD9293C3D}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2F83B650-811D-4FEE-92D5-03D4DC4376E5}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="239">
+    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="247">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1857,7 +1887,7 @@
     <tableColumn id="7" xr3:uid="{3A2FD57C-060A-462E-8BB9-B06F717E9D20}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{ED9393EA-F7F9-4661-8D0B-0D9246DDABF8}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{6F56342F-5442-42CD-8B6C-D98B6D6C0C56}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="195">
+    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="203">
       <calculatedColumnFormula>SUM(Table16[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1870,28 +1900,28 @@
   <autoFilter ref="A8:I13" xr:uid="{7BE337CC-37BD-4688-B60D-A66F4420668B}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{71340E4C-6101-4C59-8ED7-689E2AD5A962}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="194">
+    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="202">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*63-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="193">
+    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="201">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="192">
+    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="200">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="191">
+    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="199">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="190">
+    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="198">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="189">
+    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="197">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="188">
+    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="196">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="187">
+    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="195">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1912,7 +1942,7 @@
     <tableColumn id="7" xr3:uid="{4899BF24-9D2A-4CC0-AE35-4F49604AAC5A}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{CB1CC6BA-1D38-4B74-9BC6-7057FB9773EE}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{C47FADF6-C526-4188-9187-383757CE17C1}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="186">
+    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="194">
       <calculatedColumnFormula>SUM(Table168[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1925,28 +1955,28 @@
   <autoFilter ref="A9:I15" xr:uid="{06A56D17-07E5-4650-8EE9-7EA8F94D4020}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A2BE27C9-9DAE-49F5-9A70-C6CF7428BF31}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="185">
+    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="193">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="184">
+    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="192">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="183">
+    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="191">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="182">
+    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="190">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="181">
+    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="189">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.375+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="180">
+    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="188">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="179">
+    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="187">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="178">
+    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="186">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1967,7 +1997,7 @@
     <tableColumn id="7" xr3:uid="{60AD88FB-4685-412B-B5FD-BF8412C6B8E2}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{6A88D48C-D864-4F16-BEF2-BA88783A3FF3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{D40BD230-6392-4A28-A29D-F13EFE35C95E}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A0E09B2B-FD41-413F-8063-62214E990751}" name="Total" dataDxfId="177">
+    <tableColumn id="10" xr3:uid="{A0E09B2B-FD41-413F-8063-62214E990751}" name="Total" dataDxfId="185">
       <calculatedColumnFormula>SUM(Table16826[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1980,28 +2010,28 @@
   <autoFilter ref="A8:I14" xr:uid="{F7062CBA-4FAA-4900-9D3A-5C6613BCB6CE}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{ADCB4852-D3A0-456B-A8BD-E5F74BDBB762}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{ED76047D-1BC2-4C1B-B9B0-58BE0ACDDA48}" name="HP" dataDxfId="176">
+    <tableColumn id="2" xr3:uid="{ED76047D-1BC2-4C1B-B9B0-58BE0ACDDA48}" name="HP" dataDxfId="184">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EC859C53-0BA5-45D1-868B-F22DC8CE7D25}" name="MP" dataDxfId="175">
+    <tableColumn id="3" xr3:uid="{EC859C53-0BA5-45D1-868B-F22DC8CE7D25}" name="MP" dataDxfId="183">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DED33AB9-A2BB-4F9E-AA6D-02F8D1D65CD1}" name="ATK" dataDxfId="174">
+    <tableColumn id="4" xr3:uid="{DED33AB9-A2BB-4F9E-AA6D-02F8D1D65CD1}" name="ATK" dataDxfId="182">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.375+ 15+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{329B716D-9CA6-4546-AB13-92D88BE40F5F}" name="DEF" dataDxfId="173">
+    <tableColumn id="5" xr3:uid="{329B716D-9CA6-4546-AB13-92D88BE40F5F}" name="DEF" dataDxfId="181">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1 + 15+12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{67F8198A-5FC2-4C6D-9558-68B3141EA756}" name="MAT" dataDxfId="172">
+    <tableColumn id="6" xr3:uid="{67F8198A-5FC2-4C6D-9558-68B3141EA756}" name="MAT" dataDxfId="180">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C70F5BF6-63B0-44C1-862D-25E3FB55320F}" name="MDF" dataDxfId="171">
+    <tableColumn id="7" xr3:uid="{C70F5BF6-63B0-44C1-862D-25E3FB55320F}" name="MDF" dataDxfId="179">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.5+15+11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AB20AF53-453C-4266-A46B-40E693C91985}" name="AGI" dataDxfId="170">
+    <tableColumn id="8" xr3:uid="{AB20AF53-453C-4266-A46B-40E693C91985}" name="AGI" dataDxfId="178">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7FC46A31-F9F1-432E-B399-0823E198FE0A}" name="LUK" dataDxfId="169">
+    <tableColumn id="9" xr3:uid="{7FC46A31-F9F1-432E-B399-0823E198FE0A}" name="LUK" dataDxfId="177">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.5+15+20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2022,7 +2052,7 @@
     <tableColumn id="7" xr3:uid="{20C5D094-BAF0-471C-ACF3-C6658991DB5F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{E08E2AF0-56DD-4A69-A536-27139D793022}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{12AD8606-1127-4E5B-BA2C-872780F22F9E}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{5E2EF778-63AE-48B7-9F49-0D2AFEBD66A1}" name="Total" dataDxfId="168">
+    <tableColumn id="10" xr3:uid="{5E2EF778-63AE-48B7-9F49-0D2AFEBD66A1}" name="Total" dataDxfId="176">
       <calculatedColumnFormula>SUM(Table1682630[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2035,28 +2065,28 @@
   <autoFilter ref="A8:I14" xr:uid="{299912CC-280B-49E1-8859-432D05893259}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4F0B657F-C9A5-4A73-AAA3-27D307385193}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{526284E7-597F-4726-AB18-230CA03461B1}" name="HP" dataDxfId="167">
+    <tableColumn id="2" xr3:uid="{526284E7-597F-4726-AB18-230CA03461B1}" name="HP" dataDxfId="175">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*63+ 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E7BA3C7A-2677-415F-BA47-A4E88679B948}" name="MP" dataDxfId="166">
+    <tableColumn id="3" xr3:uid="{E7BA3C7A-2677-415F-BA47-A4E88679B948}" name="MP" dataDxfId="174">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE7BE678-2229-44F6-8732-71214FB69DD7}" name="ATK" dataDxfId="165">
+    <tableColumn id="4" xr3:uid="{AE7BE678-2229-44F6-8732-71214FB69DD7}" name="ATK" dataDxfId="173">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+ 15+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4715E3DB-8817-43D5-9074-9FB5F0BEF5B4}" name="DEF" dataDxfId="164">
+    <tableColumn id="5" xr3:uid="{4715E3DB-8817-43D5-9074-9FB5F0BEF5B4}" name="DEF" dataDxfId="172">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1 + 15+12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9CE76933-D045-418B-A975-378EEA51D856}" name="MAT" dataDxfId="163">
+    <tableColumn id="6" xr3:uid="{9CE76933-D045-418B-A975-378EEA51D856}" name="MAT" dataDxfId="171">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244B9611-6CB0-4946-B5CD-7D42311C7D7E}" name="MDF" dataDxfId="162">
+    <tableColumn id="7" xr3:uid="{244B9611-6CB0-4946-B5CD-7D42311C7D7E}" name="MDF" dataDxfId="170">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+15+11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32550C13-49BB-41D2-BA0A-26798830A0FD}" name="AGI" dataDxfId="161">
+    <tableColumn id="8" xr3:uid="{32550C13-49BB-41D2-BA0A-26798830A0FD}" name="AGI" dataDxfId="169">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{BB22F289-8AF5-4DD6-877B-F09520710555}" name="LUK" dataDxfId="160">
+    <tableColumn id="9" xr3:uid="{BB22F289-8AF5-4DD6-877B-F09520710555}" name="LUK" dataDxfId="168">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+15+20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2069,28 +2099,28 @@
   <autoFilter ref="A4:I10" xr:uid="{A1EAC62C-C07D-464E-91B1-4A34E6604BA2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{430FD3D4-914C-4309-B2E6-6F01B5CAED94}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="159">
+    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="167">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="158">
+    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="166">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="157">
+    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="165">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="156">
+    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="164">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15 + 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="155">
+    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="163">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15 + 30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="154">
+    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="162">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15 + 21</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="153">
+    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="161">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="152">
+    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="160">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2103,28 +2133,28 @@
   <autoFilter ref="A7:I12" xr:uid="{9BE7336F-352A-4FAE-B0E4-61965FC814C7}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B8DA50BB-4379-43D1-879B-CDBE6D82C13A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="151">
+    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="159">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="150">
+    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="158">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="149">
+    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="157">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="148">
+    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="156">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="147">
+    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="155">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="146">
+    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="154">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="145">
+    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="153">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="144">
+    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="152">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2137,28 +2167,28 @@
   <autoFilter ref="A8:I13" xr:uid="{67385006-CBB9-4472-99D4-7881E042769D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FD96F8F7-CCAB-44FA-B525-A5081670706A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="238">
+    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="246">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="237">
+    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="245">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="236">
+    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="244">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="235">
+    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="243">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="234">
+    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="242">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="233">
+    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="241">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="232">
+    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="240">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="231">
+    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="239">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2179,7 +2209,7 @@
     <tableColumn id="7" xr3:uid="{AEFF5C29-BE6A-4CF8-A2BB-F6B076077DA9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{4DE9B01E-67F2-4136-ADC3-60389FB67DCC}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{F5A82F03-513C-46D4-9F91-470F0060526B}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="143">
+    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="151">
       <calculatedColumnFormula>SUM(Table16821[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2188,22 +2218,22 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="142" tableBorderDxfId="141">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="150" tableBorderDxfId="149">
   <autoFilter ref="A15:I16" xr:uid="{434CBBE2-2F8D-4EEB-895C-68FC850EF1FD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="140"/>
-    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="139">
+    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="148"/>
+    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="147">
       <calculatedColumnFormula>Table1922[Level]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="138">
+    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="146">
       <calculatedColumnFormula>Table1922[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="137"/>
-    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="136"/>
-    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="135"/>
-    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="134"/>
-    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="133"/>
-    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="132"/>
+    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="145"/>
+    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="144"/>
+    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="143"/>
+    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="142"/>
+    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="141"/>
+    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="140"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2214,28 +2244,28 @@
   <autoFilter ref="A3:I9" xr:uid="{A90D1C2A-DBF9-4EEF-ACC2-3DC17C207301}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BD3505AC-AE6D-4947-A74E-A6C2D68658F1}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="131">
+    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="139">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="130">
+    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="138">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="129">
+    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="137">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="128">
+    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="136">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="127">
+    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="135">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="126">
+    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="134">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="125">
+    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="133">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="124">
+    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="132">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2244,32 +2274,32 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="123" tableBorderDxfId="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="131" tableBorderDxfId="130">
   <autoFilter ref="L3:T4" xr:uid="{5D2C3EA8-1297-4C77-AF32-84E50F8232C5}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="121"/>
-    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="120">
+    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="129"/>
+    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="128">
       <calculatedColumnFormula>Table19[Level]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="119">
+    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="127">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="118">
+    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="126">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="117">
+    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="125">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1 + 15 + 6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="116">
+    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="124">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="115">
+    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="123">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="114">
+    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="122">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="113">
+    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="121">
       <calculatedColumnFormula>Table19[Level] + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2282,28 +2312,28 @@
   <autoFilter ref="A7:I12" xr:uid="{553298A4-7E43-42CF-9EEB-1F9E7E6BAD27}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2AA35C8B-719C-4BA6-9CDF-2963E1C9F233}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C087FAFA-9653-40EC-B4B9-5CB8F9D7255E}" name="HP" dataDxfId="112">
+    <tableColumn id="2" xr3:uid="{C087FAFA-9653-40EC-B4B9-5CB8F9D7255E}" name="HP" dataDxfId="120">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0004B47B-3968-4C5A-BE6C-B822A307D7C5}" name="MP" dataDxfId="111">
+    <tableColumn id="3" xr3:uid="{0004B47B-3968-4C5A-BE6C-B822A307D7C5}" name="MP" dataDxfId="119">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{67EC8D91-0122-40D7-87D0-A3AB6788CE9D}" name="ATK" dataDxfId="110">
+    <tableColumn id="4" xr3:uid="{67EC8D91-0122-40D7-87D0-A3AB6788CE9D}" name="ATK" dataDxfId="118">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E9988E54-33D6-41EB-B6BE-6E832544E18C}" name="DEF" dataDxfId="109">
+    <tableColumn id="5" xr3:uid="{E9988E54-33D6-41EB-B6BE-6E832544E18C}" name="DEF" dataDxfId="117">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{16D71A55-372C-4029-A831-ECF2325E46C4}" name="MAT" dataDxfId="108">
+    <tableColumn id="6" xr3:uid="{16D71A55-372C-4029-A831-ECF2325E46C4}" name="MAT" dataDxfId="116">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{1802FB48-B110-4DBF-A8F2-64CD4890E741}" name="MDF" dataDxfId="107">
+    <tableColumn id="7" xr3:uid="{1802FB48-B110-4DBF-A8F2-64CD4890E741}" name="MDF" dataDxfId="115">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{350CA8CC-761C-4994-9D80-14685787EF3D}" name="AGI" dataDxfId="106">
+    <tableColumn id="8" xr3:uid="{350CA8CC-761C-4994-9D80-14685787EF3D}" name="AGI" dataDxfId="114">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B578CF58-136A-41B9-800E-D75836A4CDD1}" name="LUK" dataDxfId="105">
+    <tableColumn id="9" xr3:uid="{B578CF58-136A-41B9-800E-D75836A4CDD1}" name="LUK" dataDxfId="113">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2324,7 +2354,7 @@
     <tableColumn id="7" xr3:uid="{5A405725-30A7-487F-95BF-061F71CA9C61}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{644DEF70-6EBD-403E-904B-6C30E5FBEA48}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{BA93DA54-96B9-48D1-80BB-C266771E13F1}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{3EBB17A5-47EA-458B-83A5-7056BE67D25F}" name="Total" dataDxfId="104">
+    <tableColumn id="10" xr3:uid="{3EBB17A5-47EA-458B-83A5-7056BE67D25F}" name="Total" dataDxfId="112">
       <calculatedColumnFormula>SUM(Table1682134[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2333,26 +2363,26 @@
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{A7C0F3AC-4E86-430D-AE55-8604641B493E}" name="Table192235" displayName="Table192235" ref="A15:I16" totalsRowShown="0" dataDxfId="103" tableBorderDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{A7C0F3AC-4E86-430D-AE55-8604641B493E}" name="Table192235" displayName="Table192235" ref="A15:I16" totalsRowShown="0" dataDxfId="111" tableBorderDxfId="110">
   <autoFilter ref="A15:I16" xr:uid="{D0DF3ED4-9A21-493B-88F4-CE5814AF31C9}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A78A876E-6C8B-4FC8-BFD4-A9BC80EA3FC2}" name="Level" dataDxfId="101"/>
-    <tableColumn id="2" xr3:uid="{4B423FFC-D037-484D-A927-2F66E15D422A}" name="HP" dataDxfId="100">
+    <tableColumn id="1" xr3:uid="{A78A876E-6C8B-4FC8-BFD4-A9BC80EA3FC2}" name="Level" dataDxfId="109"/>
+    <tableColumn id="2" xr3:uid="{4B423FFC-D037-484D-A927-2F66E15D422A}" name="HP" dataDxfId="108">
       <calculatedColumnFormula>(Table192235[Level]*75 + 500)*2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B695FEDE-EC59-44D8-AE99-CBF568DE5C93}" name="MP" dataDxfId="99">
+    <tableColumn id="3" xr3:uid="{B695FEDE-EC59-44D8-AE99-CBF568DE5C93}" name="MP" dataDxfId="107">
       <calculatedColumnFormula>Table192235[[#This Row],[Level]]*14 + 80</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{160D5D77-34E8-44F3-B51D-7CC0736DDCB1}" name="ATK" dataDxfId="98">
+    <tableColumn id="4" xr3:uid="{160D5D77-34E8-44F3-B51D-7CC0736DDCB1}" name="ATK" dataDxfId="106">
       <calculatedColumnFormula>Table192235[[#This Row],[Level]]*1.5+ 15 + 50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{559DAC37-CD6A-449F-AFF0-355ADE7CED80}" name="DEF" dataDxfId="97"/>
-    <tableColumn id="6" xr3:uid="{EEC344A5-27A5-450E-B795-04D237DD063F}" name="MAT" dataDxfId="96">
+    <tableColumn id="5" xr3:uid="{559DAC37-CD6A-449F-AFF0-355ADE7CED80}" name="DEF" dataDxfId="105"/>
+    <tableColumn id="6" xr3:uid="{EEC344A5-27A5-450E-B795-04D237DD063F}" name="MAT" dataDxfId="104">
       <calculatedColumnFormula>Table192235[Level]*1.5+15+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{54363CA4-9EE5-495F-8323-6C0C1261453C}" name="MDF" dataDxfId="95"/>
-    <tableColumn id="8" xr3:uid="{26B56E9D-2FCD-4476-A6CF-8F2EDC965246}" name="AGI" dataDxfId="94"/>
-    <tableColumn id="9" xr3:uid="{95814D66-3343-4190-9BF4-F4E45AB27D95}" name="LUK" dataDxfId="93"/>
+    <tableColumn id="7" xr3:uid="{54363CA4-9EE5-495F-8323-6C0C1261453C}" name="MDF" dataDxfId="103"/>
+    <tableColumn id="8" xr3:uid="{26B56E9D-2FCD-4476-A6CF-8F2EDC965246}" name="AGI" dataDxfId="102"/>
+    <tableColumn id="9" xr3:uid="{95814D66-3343-4190-9BF4-F4E45AB27D95}" name="LUK" dataDxfId="101"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2371,7 +2401,7 @@
     <tableColumn id="7" xr3:uid="{22216E02-260E-4471-8BB1-4E6E1250BAC9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{DC2670AC-8DF2-47F7-A3F6-EE7896309BC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{749652E2-F6CF-428C-B67C-FD0B1EFCCBBF}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="92">
+    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="100">
       <calculatedColumnFormula>SUM(Table15[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2384,28 +2414,28 @@
   <autoFilter ref="A15:I20" xr:uid="{A1CF627F-8D28-44AD-9A35-411103976FCA}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F14CC326-DE44-48D8-856F-8DCDCFC89CAD}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="91">
+    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="99">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*63-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="90">
+    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="98">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="89">
+    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="97">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="88">
+    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="96">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="87">
+    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="95">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="86">
+    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="94">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="85">
+    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="93">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="84">
+    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="92">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2418,28 +2448,28 @@
   <autoFilter ref="K11:S17" xr:uid="{EAF9FB6A-F011-40E3-AB2F-E53826722AFB}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DF3E0800-6EE4-4E1B-BA6F-0194351D6E7C}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="83">
+    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="91">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*56.25+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="82">
+    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="90">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="81">
+    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="89">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="80">
+    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="88">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="79">
+    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="87">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="78">
+    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="86">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="77">
+    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="85">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="76">
+    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="84">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2452,28 +2482,28 @@
   <autoFilter ref="K8:S14" xr:uid="{AB7E938D-7ACC-4BFB-A6B9-682B8B29CEF2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{66EB8EF1-BCF4-44F7-B8A6-3C3B425F8FF5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="230">
+    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="238">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*56.25+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="229">
+    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="237">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="228">
+    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="236">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25+ 15+30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="227">
+    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="235">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25 + 15+33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="226">
+    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="234">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="225">
+    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="233">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="224">
+    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="232">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="223">
+    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="231">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2486,28 +2516,28 @@
   <autoFilter ref="A26:I31" xr:uid="{870F76F2-5EA7-4FD7-B1F9-507D64592088}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{3C04B742-338A-4366-BF3D-C5BC13023785}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="75">
+    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="83">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*63+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="74">
+    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="82">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="73">
+    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="81">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="72">
+    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="80">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="71">
+    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="79">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="70">
+    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="78">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="69">
+    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="77">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="68">
+    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="76">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2520,28 +2550,28 @@
   <autoFilter ref="A36:I41" xr:uid="{9BD043AF-0D77-4FF4-B2F9-B4AC3C3F1F82}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{7BB908A3-05D7-4357-920B-BF4C6BC20C06}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="67">
+    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="75">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*56.5+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="66">
+    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="74">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*12.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="65">
+    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="73">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="64">
+    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="72">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1 + 15+14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="63">
+    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="71">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="62">
+    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="70">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.5+ 15+13</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="61">
+    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="69">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="60">
+    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="68">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.375 + 15+40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2562,7 +2592,7 @@
     <tableColumn id="7" xr3:uid="{09E4151E-54A0-41FF-BA5B-3B1C748DA23D}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{909575E0-EC13-4E35-A35F-2451A5741589}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2CDCF32E-D8FC-48D9-A28D-8D9C5F3EB001}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{001DA1BB-34DD-4786-BDE4-23C510900A3D}" name="Total" dataDxfId="59">
+    <tableColumn id="10" xr3:uid="{001DA1BB-34DD-4786-BDE4-23C510900A3D}" name="Total" dataDxfId="67">
       <calculatedColumnFormula>SUM(Table168213429[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2575,28 +2605,28 @@
   <autoFilter ref="A7:I12" xr:uid="{4ED64482-035D-49B9-A477-A1D5AEB4A5A4}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{141B0E2E-D4F3-4884-86FD-AAD67C363749}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{D4B50877-EF56-4EF7-8C6D-9928A6D654F6}" name="HP" dataDxfId="58">
+    <tableColumn id="2" xr3:uid="{D4B50877-EF56-4EF7-8C6D-9928A6D654F6}" name="HP" dataDxfId="66">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*125</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F4B06187-BE28-4283-9518-F773FE75C2BF}" name="MP" dataDxfId="57">
+    <tableColumn id="3" xr3:uid="{F4B06187-BE28-4283-9518-F773FE75C2BF}" name="MP" dataDxfId="65">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{91A68FC7-5F16-4880-AE82-97341814BB95}" name="ATK" dataDxfId="56">
+    <tableColumn id="4" xr3:uid="{91A68FC7-5F16-4880-AE82-97341814BB95}" name="ATK" dataDxfId="64">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*4.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{2BCD0E58-85DE-4C10-BFBC-AF77BC569C92}" name="DEF" dataDxfId="55">
+    <tableColumn id="5" xr3:uid="{2BCD0E58-85DE-4C10-BFBC-AF77BC569C92}" name="DEF" dataDxfId="63">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7C48A1FC-CE8F-4CDD-9A3D-308B46D78A48}" name="MAT" dataDxfId="54">
+    <tableColumn id="6" xr3:uid="{7C48A1FC-CE8F-4CDD-9A3D-308B46D78A48}" name="MAT" dataDxfId="62">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{474D8178-EA8C-4322-93C3-B7F6EBA88102}" name="MDF" dataDxfId="53">
+    <tableColumn id="7" xr3:uid="{474D8178-EA8C-4322-93C3-B7F6EBA88102}" name="MDF" dataDxfId="61">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{257B31D9-5838-45E0-A56E-9B1566E1A34A}" name="AGI" dataDxfId="52">
+    <tableColumn id="8" xr3:uid="{257B31D9-5838-45E0-A56E-9B1566E1A34A}" name="AGI" dataDxfId="60">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{17960EB4-4250-49DB-9A6B-455B9913B04B}" name="LUK" dataDxfId="51">
+    <tableColumn id="9" xr3:uid="{17960EB4-4250-49DB-9A6B-455B9913B04B}" name="LUK" dataDxfId="59">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1.125</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2617,7 +2647,7 @@
     <tableColumn id="7" xr3:uid="{07EA0638-8880-4944-AC9E-13E3F1B9F651}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{AA18E602-126F-4D69-9CC8-C097E8EB9C70}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{5563B0CB-2EA7-4851-8D1F-D77E0F90CBAD}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{2D960B43-0F76-4936-9508-4D501A79A83C}" name="Total" dataDxfId="50">
+    <tableColumn id="10" xr3:uid="{2D960B43-0F76-4936-9508-4D501A79A83C}" name="Total" dataDxfId="58">
       <calculatedColumnFormula>SUM(Table16821342932[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2630,28 +2660,28 @@
   <autoFilter ref="A5:I10" xr:uid="{2922C913-6AE8-4B89-BDA6-9F44D59987D8}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{3D67222C-6501-4A5D-A9FC-528EE591A288}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EE3E4CCC-C404-4B78-AAB4-3B38166E23BA}" name="HP" dataDxfId="49">
+    <tableColumn id="2" xr3:uid="{EE3E4CCC-C404-4B78-AAB4-3B38166E23BA}" name="HP" dataDxfId="57">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DE5141FB-3B4E-46D4-9E0D-AF1DEE998B4A}" name="MP" dataDxfId="48">
+    <tableColumn id="3" xr3:uid="{DE5141FB-3B4E-46D4-9E0D-AF1DEE998B4A}" name="MP" dataDxfId="56">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{404B3E88-DF62-4AA0-82D6-C21C2BCA762B}" name="ATK" dataDxfId="47">
+    <tableColumn id="4" xr3:uid="{404B3E88-DF62-4AA0-82D6-C21C2BCA762B}" name="ATK" dataDxfId="55">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*4.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{342B3F39-F7A2-45D8-9CD4-39B5ABC72D2F}" name="DEF" dataDxfId="46">
+    <tableColumn id="5" xr3:uid="{342B3F39-F7A2-45D8-9CD4-39B5ABC72D2F}" name="DEF" dataDxfId="54">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{CD819DB3-9F2E-4428-AAFC-72776ECB8EAF}" name="MAT" dataDxfId="45">
+    <tableColumn id="6" xr3:uid="{CD819DB3-9F2E-4428-AAFC-72776ECB8EAF}" name="MAT" dataDxfId="53">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{270DF964-8095-43FD-B050-DD4A2A138F32}" name="MDF" dataDxfId="44">
+    <tableColumn id="7" xr3:uid="{270DF964-8095-43FD-B050-DD4A2A138F32}" name="MDF" dataDxfId="52">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4F4D3B2A-5B86-4AB7-A97E-18E2868266B8}" name="AGI" dataDxfId="43">
+    <tableColumn id="8" xr3:uid="{4F4D3B2A-5B86-4AB7-A97E-18E2868266B8}" name="AGI" dataDxfId="51">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{0178CE2D-63C5-426A-A081-D62E62FF91AC}" name="LUK" dataDxfId="42">
+    <tableColumn id="9" xr3:uid="{0178CE2D-63C5-426A-A081-D62E62FF91AC}" name="LUK" dataDxfId="50">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*1.5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2672,7 +2702,7 @@
     <tableColumn id="7" xr3:uid="{C374A90B-690A-432C-974A-C8A7D22E367F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{05C64890-0DC2-4577-975E-95477DCED789}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{CE6AAEA9-D599-4B9B-BD40-7E602F47088C}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{30017AE7-6C23-415F-A2EA-70EA09C835E6}" name="Total" dataDxfId="41">
+    <tableColumn id="10" xr3:uid="{30017AE7-6C23-415F-A2EA-70EA09C835E6}" name="Total" dataDxfId="49">
       <calculatedColumnFormula>SUM(Table1682134293227[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2685,28 +2715,28 @@
   <autoFilter ref="A6:I11" xr:uid="{D09397F4-7631-4CD3-AF40-3B14C64478EE}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BF4E6A79-8CCF-498E-B3B0-FA782AB06519}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{37E52E57-C499-4FFB-AC3F-20E63EEA4D3A}" name="HP" dataDxfId="40">
+    <tableColumn id="2" xr3:uid="{37E52E57-C499-4FFB-AC3F-20E63EEA4D3A}" name="HP" dataDxfId="48">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*87.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D29F5CDE-1200-4C77-A4BA-0DE4F7C46627}" name="MP" dataDxfId="39">
+    <tableColumn id="3" xr3:uid="{D29F5CDE-1200-4C77-A4BA-0DE4F7C46627}" name="MP" dataDxfId="47">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{9701140A-64F9-4967-9DEE-3460411D91C1}" name="ATK" dataDxfId="38">
+    <tableColumn id="4" xr3:uid="{9701140A-64F9-4967-9DEE-3460411D91C1}" name="ATK" dataDxfId="46">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F90A425E-E031-4255-8AF9-DAD672F8DD7D}" name="DEF" dataDxfId="37">
+    <tableColumn id="5" xr3:uid="{F90A425E-E031-4255-8AF9-DAD672F8DD7D}" name="DEF" dataDxfId="45">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*4.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{255210A0-6EB8-4CFB-84DD-42C88AEAF7AA}" name="MAT" dataDxfId="36">
+    <tableColumn id="6" xr3:uid="{255210A0-6EB8-4CFB-84DD-42C88AEAF7AA}" name="MAT" dataDxfId="44">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{91177FDD-F316-4D6B-A547-FC5FA6DAC266}" name="MDF" dataDxfId="35">
+    <tableColumn id="7" xr3:uid="{91177FDD-F316-4D6B-A547-FC5FA6DAC266}" name="MDF" dataDxfId="43">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{ADA902F7-B7D7-4B1B-A144-E5252296AB61}" name="AGI" dataDxfId="34">
+    <tableColumn id="8" xr3:uid="{ADA902F7-B7D7-4B1B-A144-E5252296AB61}" name="AGI" dataDxfId="42">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{78273DA6-F2CA-4999-B4EA-F6C044BC41AB}" name="LUK" dataDxfId="33">
+    <tableColumn id="9" xr3:uid="{78273DA6-F2CA-4999-B4EA-F6C044BC41AB}" name="LUK" dataDxfId="41">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2715,32 +2745,32 @@
 </file>
 
 <file path=xl/tables/table38.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{DC830F9D-6D0E-4024-B70E-0F7651ABC56D}" name="Table131639" displayName="Table131639" ref="A4:I7" totalsRowShown="0">
-  <autoFilter ref="A4:I7" xr:uid="{DD778A26-93EC-4B14-A9D1-160AE03B48D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{DC830F9D-6D0E-4024-B70E-0F7651ABC56D}" name="Table131639" displayName="Table131639" ref="A4:I9" totalsRowShown="0">
+  <autoFilter ref="A4:I9" xr:uid="{DD778A26-93EC-4B14-A9D1-160AE03B48D3}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F0A3DB96-38E4-4CD0-BAF6-C8BB768B1256}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{07B77441-F84C-41C6-A00C-B69369FBF0F1}" name="HP" dataDxfId="32">
+    <tableColumn id="2" xr3:uid="{07B77441-F84C-41C6-A00C-B69369FBF0F1}" name="HP" dataDxfId="40">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{2DBE06DE-38E0-4433-B590-3850C554BB8E}" name="MP" dataDxfId="31">
+    <tableColumn id="3" xr3:uid="{2DBE06DE-38E0-4433-B590-3850C554BB8E}" name="MP" dataDxfId="39">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DE8CC9D0-45D8-4F85-9317-09844C8D4DD7}" name="ATK" dataDxfId="30">
+    <tableColumn id="4" xr3:uid="{DE8CC9D0-45D8-4F85-9317-09844C8D4DD7}" name="ATK" dataDxfId="38">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1.375+ 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{9D33BCF5-CDB6-4BB0-8603-810E71EE1C47}" name="DEF" dataDxfId="29">
+    <tableColumn id="5" xr3:uid="{9D33BCF5-CDB6-4BB0-8603-810E71EE1C47}" name="DEF" dataDxfId="37">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1.375 + 15 + 19</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{1693AB2F-85DB-4286-A43C-82A15CDDA173}" name="MAT" dataDxfId="28">
+    <tableColumn id="6" xr3:uid="{1693AB2F-85DB-4286-A43C-82A15CDDA173}" name="MAT" dataDxfId="36">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{DCA68233-62C9-4E66-9306-24AE49EE344C}" name="MDF" dataDxfId="27">
+    <tableColumn id="7" xr3:uid="{DCA68233-62C9-4E66-9306-24AE49EE344C}" name="MDF" dataDxfId="35">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1 + 15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{60943D8A-0008-4FFE-AE90-4DDEB0149A21}" name="AGI" dataDxfId="26">
+    <tableColumn id="8" xr3:uid="{60943D8A-0008-4FFE-AE90-4DDEB0149A21}" name="AGI" dataDxfId="34">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E7EC6C93-3486-414B-87DB-F4D38BB2A0DC}" name="LUK" dataDxfId="25">
+    <tableColumn id="9" xr3:uid="{E7EC6C93-3486-414B-87DB-F4D38BB2A0DC}" name="LUK" dataDxfId="33">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2749,32 +2779,32 @@
 </file>
 
 <file path=xl/tables/table39.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="41" xr:uid="{3EDE85AD-4960-41AB-A603-4ABE8AAA49F8}" name="Table13182227" displayName="Table13182227" ref="A12:I15" totalsRowShown="0">
-  <autoFilter ref="A12:I15" xr:uid="{2A794F38-5DB8-40A3-A8E2-90B5A0A4A192}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="41" xr:uid="{3EDE85AD-4960-41AB-A603-4ABE8AAA49F8}" name="Table13182227" displayName="Table13182227" ref="A12:I16" totalsRowShown="0">
+  <autoFilter ref="A12:I16" xr:uid="{2A794F38-5DB8-40A3-A8E2-90B5A0A4A192}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{C5A2CF3A-0965-428C-AD05-883EDB0D400F}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C8840580-F723-4CA3-A107-42FCC677D424}" name="HP" dataDxfId="24">
+    <tableColumn id="2" xr3:uid="{C8840580-F723-4CA3-A107-42FCC677D424}" name="HP" dataDxfId="32">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*62.5+ 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5D9241C6-74A5-4C1F-A8F7-69DB1BDA83FE}" name="MP" dataDxfId="23">
+    <tableColumn id="3" xr3:uid="{5D9241C6-74A5-4C1F-A8F7-69DB1BDA83FE}" name="MP" dataDxfId="31">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*12.5+60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D98F9CCD-2FEF-4FB2-B5AD-D2A6B610781B}" name="ATK" dataDxfId="22">
+    <tableColumn id="4" xr3:uid="{D98F9CCD-2FEF-4FB2-B5AD-D2A6B610781B}" name="ATK" dataDxfId="30">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CF1AF448-2207-48D1-8FE3-0A6B5DE3511C}" name="DEF" dataDxfId="21">
+    <tableColumn id="5" xr3:uid="{CF1AF448-2207-48D1-8FE3-0A6B5DE3511C}" name="DEF" dataDxfId="29">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1 + 15 + 10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A632BAA7-E71C-41F8-B5B0-90891BB5BA9B}" name="MAT" dataDxfId="20">
+    <tableColumn id="6" xr3:uid="{A632BAA7-E71C-41F8-B5B0-90891BB5BA9B}" name="MAT" dataDxfId="28">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E76132BC-BC67-4915-8112-E0B292C65C91}" name="MDF" dataDxfId="19">
+    <tableColumn id="7" xr3:uid="{E76132BC-BC67-4915-8112-E0B292C65C91}" name="MDF" dataDxfId="27">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1 + 15 + 8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B25B7E33-B3CF-4D3D-9A14-3CE5B75535E8}" name="AGI" dataDxfId="18">
+    <tableColumn id="8" xr3:uid="{B25B7E33-B3CF-4D3D-9A14-3CE5B75535E8}" name="AGI" dataDxfId="26">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{40820F61-4B4C-4B23-95CF-AD5CDE975F4A}" name="LUK" dataDxfId="17">
+    <tableColumn id="9" xr3:uid="{40820F61-4B4C-4B23-95CF-AD5CDE975F4A}" name="LUK" dataDxfId="25">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2795,7 +2825,7 @@
     <tableColumn id="7" xr3:uid="{F833922A-76F9-427C-8462-D94DE51D0477}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{203171A1-C88B-4F81-ADC2-1EE072D645F3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{34003EF6-E9A5-4584-A186-09DFF4EC11C7}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{C4602156-F897-42BE-8F3F-411E13EEB095}" name="Total" dataDxfId="222">
+    <tableColumn id="10" xr3:uid="{C4602156-F897-42BE-8F3F-411E13EEB095}" name="Total" dataDxfId="230">
       <calculatedColumnFormula>SUM(Table114[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2804,32 +2834,32 @@
 </file>
 
 <file path=xl/tables/table40.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="43" xr:uid="{B712F8FC-9826-474C-B326-FF2E66C27FA3}" name="Table13162044" displayName="Table13162044" ref="A20:I23" totalsRowShown="0">
-  <autoFilter ref="A20:I23" xr:uid="{6015D08B-C4A1-43B9-B8BF-6F441CC08DCA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="43" xr:uid="{B712F8FC-9826-474C-B326-FF2E66C27FA3}" name="Table13162044" displayName="Table13162044" ref="A20:I24" totalsRowShown="0">
+  <autoFilter ref="A20:I24" xr:uid="{6015D08B-C4A1-43B9-B8BF-6F441CC08DCA}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D4205A68-390A-4750-8556-3B4847E58D16}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{D7D1DEBE-6CE0-4976-A401-D4F35A038AA9}" name="HP" dataDxfId="16">
+    <tableColumn id="2" xr3:uid="{D7D1DEBE-6CE0-4976-A401-D4F35A038AA9}" name="HP" dataDxfId="24">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{3CB0ED8A-F14B-4E5F-8474-F3034EA78A85}" name="MP" dataDxfId="15">
+    <tableColumn id="3" xr3:uid="{3CB0ED8A-F14B-4E5F-8474-F3034EA78A85}" name="MP" dataDxfId="23">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F3186E07-87BD-4E53-8F85-AB4798362B0C}" name="ATK" dataDxfId="14">
+    <tableColumn id="4" xr3:uid="{F3186E07-87BD-4E53-8F85-AB4798362B0C}" name="ATK" dataDxfId="22">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{22ED75D6-B85C-4DF9-BC39-4154BAF3990E}" name="DEF" dataDxfId="13">
+    <tableColumn id="5" xr3:uid="{22ED75D6-B85C-4DF9-BC39-4154BAF3990E}" name="DEF" dataDxfId="21">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1 + 15 + 4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B2DFC87A-2BEE-4B5A-AF53-4E18078ABC1B}" name="MAT" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{B2DFC87A-2BEE-4B5A-AF53-4E18078ABC1B}" name="MAT" dataDxfId="20">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.375 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{8FF82542-4129-4E67-AA7B-7CB38D8FB051}" name="MDF" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{8FF82542-4129-4E67-AA7B-7CB38D8FB051}" name="MDF" dataDxfId="19">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.375 + 15 + 14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{85F4097E-90A5-4A7C-B184-42B110E62300}" name="AGI" dataDxfId="10">
+    <tableColumn id="8" xr3:uid="{85F4097E-90A5-4A7C-B184-42B110E62300}" name="AGI" dataDxfId="18">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E1A21F56-D819-4CE3-9122-F47B8A4039A9}" name="LUK" dataDxfId="9">
+    <tableColumn id="9" xr3:uid="{E1A21F56-D819-4CE3-9122-F47B8A4039A9}" name="LUK" dataDxfId="17">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2838,6 +2868,40 @@
 </file>
 
 <file path=xl/tables/table41.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="40" xr:uid="{8A1F9CE0-57B7-46D3-A438-8752A6EBC657}" name="Table131822" displayName="Table131822" ref="A27:I30" totalsRowShown="0">
+  <autoFilter ref="A27:I30" xr:uid="{4506A984-1EE8-4D0B-9AFB-6DE5576F3317}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{97BB3945-930E-41A9-B479-678FD9D8EE85}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{2197951B-D7A2-413F-8152-C8BB282E3498}" name="HP" dataDxfId="7">
+      <calculatedColumnFormula>Table131822[[#This Row],[Level]]*62.5+ 300</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{54D89380-BDA0-4B18-8B8B-482E9AA62AD3}" name="MP" dataDxfId="6">
+      <calculatedColumnFormula>Table131822[[#This Row],[Level]]*12.5+60</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{DCD1A325-B7AE-4283-89E4-85446F157A12}" name="ATK" dataDxfId="5">
+      <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{1CD051D4-B531-4706-95A8-BBF452C5188D}" name="DEF" dataDxfId="0">
+      <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.25 + 15 + 19</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{E17A43F1-7669-40E6-BD8C-8623B203A60F}" name="MAT" dataDxfId="4">
+      <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{04F7D6BA-3673-4BE0-97CA-65C8DD4612E3}" name="MDF" dataDxfId="1">
+      <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.25 + 15 + 5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{7AA9AD24-2AFF-4204-AAEF-0CC3265C40FA}" name="AGI" dataDxfId="3">
+      <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{ABFCE932-20B6-4AEE-A261-B747D2EC6FA8}" name="LUK" dataDxfId="2">
+      <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table42.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="44" xr:uid="{63EFECE9-294D-4BD5-B983-D7DF0138B45B}" name="Table168213429322745" displayName="Table168213429322745" ref="A4:J6" totalsRowShown="0">
   <autoFilter ref="A4:J6" xr:uid="{9FA97447-7595-4CE0-9387-AEB91FE50244}"/>
   <tableColumns count="10">
@@ -2850,7 +2914,7 @@
     <tableColumn id="7" xr3:uid="{6B239F5E-F897-4532-B3C2-8B926BDED5BF}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{CB8FDC45-B604-4FEB-9A7B-367828FC7568}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{6C00B6B1-0959-4058-96EE-2711BA8C66BD}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{1803A62E-480C-481E-8063-2EB8C650EA1D}" name="Total" dataDxfId="8">
+    <tableColumn id="10" xr3:uid="{1803A62E-480C-481E-8063-2EB8C650EA1D}" name="Total" dataDxfId="16">
       <calculatedColumnFormula>SUM(Table168213429322745[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2858,33 +2922,33 @@
 </table>
 </file>
 
-<file path=xl/tables/table42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table43.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="46" xr:uid="{6B246BF5-6CE4-4B50-8843-8DACC434192B}" name="Table1316183336373847" displayName="Table1316183336373847" ref="A8:I13" totalsRowShown="0">
   <autoFilter ref="A8:I13" xr:uid="{F3DE48F5-A98B-4A15-8805-1948F568C45F}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2E01F6BC-B2F6-42D6-A20F-FDB9BA2D677A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{21915B10-9976-4EFE-936F-170B253E711B}" name="HP" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{21915B10-9976-4EFE-936F-170B253E711B}" name="HP" dataDxfId="15">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*168.75</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{052B9451-309F-4C84-8FC4-08AD4866120D}" name="MP" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{052B9451-309F-4C84-8FC4-08AD4866120D}" name="MP" dataDxfId="14">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{B73769F3-1F79-45AE-998C-FF1A9A557091}" name="ATK" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{B73769F3-1F79-45AE-998C-FF1A9A557091}" name="ATK" dataDxfId="13">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*3.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B5E81D1B-B382-4DF5-92BA-F92F12A23A07}" name="DEF" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{B5E81D1B-B382-4DF5-92BA-F92F12A23A07}" name="DEF" dataDxfId="12">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*4.75</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A815FA03-2618-4DC9-9734-50DCE6DA615F}" name="MAT" dataDxfId="6">
+    <tableColumn id="6" xr3:uid="{A815FA03-2618-4DC9-9734-50DCE6DA615F}" name="MAT" dataDxfId="11">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D8263081-7D11-47BB-9AEC-CE559647F35D}" name="MDF" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{D8263081-7D11-47BB-9AEC-CE559647F35D}" name="MDF" dataDxfId="10">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*4.75</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C838F145-4059-4C8C-8152-B8F66431FFE1}" name="AGI" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{C838F145-4059-4C8C-8152-B8F66431FFE1}" name="AGI" dataDxfId="9">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*3.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{431AC55C-A81C-4BB0-B544-6631F8331D55}" name="LUK" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{431AC55C-A81C-4BB0-B544-6631F8331D55}" name="LUK" dataDxfId="8">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*2.125</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2897,28 +2961,28 @@
   <autoFilter ref="A8:I14" xr:uid="{D3C3F418-ED32-4504-9D73-88545A192967}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{13E0AF4A-AA83-489A-A156-B01D4F48D2F5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{B970139F-8BB5-4CE6-92F8-79E3236AC62B}" name="HP" dataDxfId="221">
+    <tableColumn id="2" xr3:uid="{B970139F-8BB5-4CE6-92F8-79E3236AC62B}" name="HP" dataDxfId="229">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*63+300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7BCF83B8-7492-4991-A008-F212725940B9}" name="MP" dataDxfId="220">
+    <tableColumn id="3" xr3:uid="{7BCF83B8-7492-4991-A008-F212725940B9}" name="MP" dataDxfId="228">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{33220A80-38D8-4480-ACC7-DF484072C96B}" name="ATK" dataDxfId="219">
+    <tableColumn id="4" xr3:uid="{33220A80-38D8-4480-ACC7-DF484072C96B}" name="ATK" dataDxfId="227">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.5+ 15+40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{36708515-5004-4705-A558-44B59D0CE676}" name="DEF" dataDxfId="218">
+    <tableColumn id="5" xr3:uid="{36708515-5004-4705-A558-44B59D0CE676}" name="DEF" dataDxfId="226">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25 + 15+21</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{11729EA3-08C4-4E0B-B5EE-5B3C08A31A9C}" name="MAT" dataDxfId="217">
+    <tableColumn id="6" xr3:uid="{11729EA3-08C4-4E0B-B5EE-5B3C08A31A9C}" name="MAT" dataDxfId="225">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B179D090-E484-4663-937A-480D1164D655}" name="MDF" dataDxfId="216">
+    <tableColumn id="7" xr3:uid="{B179D090-E484-4663-937A-480D1164D655}" name="MDF" dataDxfId="224">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25+15 + 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{28323AD0-B3BD-401F-A237-92C8B8D70FEA}" name="AGI" dataDxfId="215">
+    <tableColumn id="8" xr3:uid="{28323AD0-B3BD-401F-A237-92C8B8D70FEA}" name="AGI" dataDxfId="223">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{657BED8B-4C8A-42DC-BECD-5EEF9D1B7F37}" name="LUK" dataDxfId="214">
+    <tableColumn id="9" xr3:uid="{657BED8B-4C8A-42DC-BECD-5EEF9D1B7F37}" name="LUK" dataDxfId="222">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2939,7 +3003,7 @@
     <tableColumn id="7" xr3:uid="{D1DFC0D2-A987-4E3F-BA23-52162FB0C0BA}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{AB6209DB-CCCB-4C37-B455-4C7652E0DAC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2CD4CD14-92FD-41A7-9CCD-1329B5A77390}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{3B2C0A10-5038-4C21-BAC5-12FB16275D2E}" name="Total" dataDxfId="213">
+    <tableColumn id="10" xr3:uid="{3B2C0A10-5038-4C21-BAC5-12FB16275D2E}" name="Total" dataDxfId="221">
       <calculatedColumnFormula>SUM(Table11412[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2952,28 +3016,28 @@
   <autoFilter ref="A8:I14" xr:uid="{43F790D1-EA7B-4BAE-8A37-7CAD791E8821}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F6E842E1-B25F-4CA1-9107-AC7179420C29}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EFB2F0D5-318D-4A65-BA2B-20ADDE071648}" name="HP" dataDxfId="212">
+    <tableColumn id="2" xr3:uid="{EFB2F0D5-318D-4A65-BA2B-20ADDE071648}" name="HP" dataDxfId="220">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0D914B89-2678-453F-BC18-571DCD45E628}" name="MP" dataDxfId="211">
+    <tableColumn id="3" xr3:uid="{0D914B89-2678-453F-BC18-571DCD45E628}" name="MP" dataDxfId="219">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*13.75 + 80</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{6FBD2F64-5B1C-4035-BB1A-AFB092DB60C3}" name="ATK" dataDxfId="210">
+    <tableColumn id="4" xr3:uid="{6FBD2F64-5B1C-4035-BB1A-AFB092DB60C3}" name="ATK" dataDxfId="218">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7E0AF3FC-CC5D-4A6A-A4A2-DE278DEC4062}" name="DEF" dataDxfId="209">
+    <tableColumn id="5" xr3:uid="{7E0AF3FC-CC5D-4A6A-A4A2-DE278DEC4062}" name="DEF" dataDxfId="217">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1 + 15 + 4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3AF4D559-893B-4D50-BCB4-A1BD1FAF2F23}" name="MAT" dataDxfId="208">
+    <tableColumn id="6" xr3:uid="{3AF4D559-893B-4D50-BCB4-A1BD1FAF2F23}" name="MAT" dataDxfId="216">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6E9418A6-75AC-4541-9029-814EC5C06E70}" name="MDF" dataDxfId="207">
+    <tableColumn id="7" xr3:uid="{6E9418A6-75AC-4541-9029-814EC5C06E70}" name="MDF" dataDxfId="215">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.375+15 + 14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD605BEE-D561-4A2C-8D06-8E9AD70C32AC}" name="AGI" dataDxfId="206">
+    <tableColumn id="8" xr3:uid="{CD605BEE-D561-4A2C-8D06-8E9AD70C32AC}" name="AGI" dataDxfId="214">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E26506B2-F488-4AA4-AC87-819A22964609}" name="LUK" dataDxfId="205">
+    <tableColumn id="9" xr3:uid="{E26506B2-F488-4AA4-AC87-819A22964609}" name="LUK" dataDxfId="213">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2994,7 +3058,7 @@
     <tableColumn id="7" xr3:uid="{E91A64A8-F750-4893-9958-7C6ABC37405F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{3832FF0E-95E5-4B1F-B122-1EAFBF719DE3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{237404A9-EB50-465E-89AF-7167C57AFB99}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{927EBD24-571F-408C-A33B-59C753D9D96D}" name="Total" dataDxfId="204">
+    <tableColumn id="10" xr3:uid="{927EBD24-571F-408C-A33B-59C753D9D96D}" name="Total" dataDxfId="212">
       <calculatedColumnFormula>SUM(Table1141219[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3007,28 +3071,28 @@
   <autoFilter ref="A7:I13" xr:uid="{2539D8EE-2982-4734-B28B-342036FEDAC6}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FEE8F081-132E-4ED3-8FFD-2CF48368B2CC}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A79BC043-DB1A-48B4-AC21-AD31632979A6}" name="HP" dataDxfId="203">
+    <tableColumn id="2" xr3:uid="{A79BC043-DB1A-48B4-AC21-AD31632979A6}" name="HP" dataDxfId="211">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*63 + 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{42935B44-C727-42B0-B48E-0369818BF78A}" name="MP" dataDxfId="202">
+    <tableColumn id="3" xr3:uid="{42935B44-C727-42B0-B48E-0369818BF78A}" name="MP" dataDxfId="210">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{FC4572C7-88EC-4981-A6ED-43397844845B}" name="ATK" dataDxfId="201">
+    <tableColumn id="4" xr3:uid="{FC4572C7-88EC-4981-A6ED-43397844845B}" name="ATK" dataDxfId="209">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C8D61CEB-FFEC-42C3-9123-5140E65C1A2C}" name="DEF" dataDxfId="200">
+    <tableColumn id="5" xr3:uid="{C8D61CEB-FFEC-42C3-9123-5140E65C1A2C}" name="DEF" dataDxfId="208">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.375 + 15 + 19</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8C971683-28D2-4474-83CA-936F352F1324}" name="MAT" dataDxfId="199">
+    <tableColumn id="6" xr3:uid="{8C971683-28D2-4474-83CA-936F352F1324}" name="MAT" dataDxfId="207">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3371862A-9CF2-47CA-A149-4921E3B33162}" name="MDF" dataDxfId="198">
+    <tableColumn id="7" xr3:uid="{3371862A-9CF2-47CA-A149-4921E3B33162}" name="MDF" dataDxfId="206">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.375+15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC6AC739-B4C9-47A6-9472-439C60B629A0}" name="AGI" dataDxfId="197">
+    <tableColumn id="8" xr3:uid="{AC6AC739-B4C9-47A6-9472-439C60B629A0}" name="AGI" dataDxfId="205">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E727A271-B479-47C0-A557-227ABD8EC0AC}" name="LUK" dataDxfId="196">
+    <tableColumn id="9" xr3:uid="{E727A271-B479-47C0-A557-227ABD8EC0AC}" name="LUK" dataDxfId="204">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6980,10 +7044,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDEC26FB-B5E4-44F5-B062-22E344453193}">
-  <dimension ref="A2:I23"/>
+  <dimension ref="A2:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7138,6 +7202,80 @@
         <v>40</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1">
+        <f>Table131639[[#This Row],[Level]]*75 + 500</f>
+        <v>2150</v>
+      </c>
+      <c r="C8" s="1">
+        <f>Table131639[[#This Row],[Level]]*10+20</f>
+        <v>240</v>
+      </c>
+      <c r="D8" s="1">
+        <f>Table131639[[#This Row],[Level]]*1.375+ 15 + 40</f>
+        <v>85.25</v>
+      </c>
+      <c r="E8" s="1">
+        <f>Table131639[[#This Row],[Level]]*1.375 + 15 + 19</f>
+        <v>64.25</v>
+      </c>
+      <c r="F8" s="1">
+        <f>Table131639[[#This Row],[Level]]*1 + 15</f>
+        <v>37</v>
+      </c>
+      <c r="G8" s="1">
+        <f>Table131639[[#This Row],[Level]]*1 + 15 + 5</f>
+        <v>42</v>
+      </c>
+      <c r="H8" s="1">
+        <f>Table131639[[#This Row],[Level]]*1.25 + 15</f>
+        <v>42.5</v>
+      </c>
+      <c r="I8" s="1">
+        <f>Table131639[[#This Row],[Level]]*1.25 + 15</f>
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1">
+        <f>Table131639[[#This Row],[Level]]*75 + 500</f>
+        <v>2375</v>
+      </c>
+      <c r="C9" s="1">
+        <f>Table131639[[#This Row],[Level]]*10+20</f>
+        <v>270</v>
+      </c>
+      <c r="D9" s="1">
+        <f>Table131639[[#This Row],[Level]]*1.375+ 15 + 40</f>
+        <v>89.375</v>
+      </c>
+      <c r="E9" s="1">
+        <f>Table131639[[#This Row],[Level]]*1.375 + 15 + 19</f>
+        <v>68.375</v>
+      </c>
+      <c r="F9" s="1">
+        <f>Table131639[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="G9" s="1">
+        <f>Table131639[[#This Row],[Level]]*1 + 15 + 5</f>
+        <v>45</v>
+      </c>
+      <c r="H9" s="1">
+        <f>Table131639[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+      <c r="I9" s="1">
+        <f>Table131639[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+    </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
@@ -7283,9 +7421,51 @@
         <v>40</v>
       </c>
     </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1">
+        <f>Table13182227[[#This Row],[Level]]*62.5+ 300</f>
+        <v>1862.5</v>
+      </c>
+      <c r="C16" s="1">
+        <f>Table13182227[[#This Row],[Level]]*12.5+60</f>
+        <v>372.5</v>
+      </c>
+      <c r="D16" s="1">
+        <f>Table13182227[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+      <c r="E16" s="1">
+        <f>Table13182227[[#This Row],[Level]]*1 + 15 + 10</f>
+        <v>50</v>
+      </c>
+      <c r="F16" s="1">
+        <f>Table13182227[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+      <c r="G16" s="1">
+        <f>Table13182227[[#This Row],[Level]]*1 + 15 + 8</f>
+        <v>48</v>
+      </c>
+      <c r="H16" s="1">
+        <f>Table13182227[[#This Row],[Level]]*1.5 + 15 + 40</f>
+        <v>92.5</v>
+      </c>
+      <c r="I16" s="1">
+        <f>Table13182227[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -7428,12 +7608,195 @@
         <v>40</v>
       </c>
     </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1">
+        <f>Table13162044[[#This Row],[Level]]*50 + 100</f>
+        <v>1350</v>
+      </c>
+      <c r="C24" s="1">
+        <f>Table13162044[[#This Row],[Level]]*15+100</f>
+        <v>475</v>
+      </c>
+      <c r="D24" s="1">
+        <f>Table13162044[[#This Row],[Level]]*1+ 15</f>
+        <v>40</v>
+      </c>
+      <c r="E24" s="1">
+        <f>Table13162044[[#This Row],[Level]]*1 + 15 + 4</f>
+        <v>44</v>
+      </c>
+      <c r="F24" s="1">
+        <f>Table13162044[[#This Row],[Level]]*1.375 + 15 + 40</f>
+        <v>89.375</v>
+      </c>
+      <c r="G24" s="1">
+        <f>Table13162044[[#This Row],[Level]]*1.375 + 15 + 14</f>
+        <v>63.375</v>
+      </c>
+      <c r="H24" s="1">
+        <f>Table13162044[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+      <c r="I24" s="1">
+        <f>Table13162044[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <f>Table131822[[#This Row],[Level]]*62.5+ 300</f>
+        <v>362.5</v>
+      </c>
+      <c r="C28">
+        <f>Table131822[[#This Row],[Level]]*12.5+60</f>
+        <v>72.5</v>
+      </c>
+      <c r="D28">
+        <f>Table131822[[#This Row],[Level]]*1.125 + 15</f>
+        <v>16.125</v>
+      </c>
+      <c r="E28">
+        <f>Table131822[[#This Row],[Level]]*1.25 + 15 + 19</f>
+        <v>35.25</v>
+      </c>
+      <c r="F28">
+        <f>Table131822[[#This Row],[Level]]*1.125 + 15</f>
+        <v>16.125</v>
+      </c>
+      <c r="G28">
+        <f>Table131822[[#This Row],[Level]]*1.25 + 15 + 5</f>
+        <v>21.25</v>
+      </c>
+      <c r="H28">
+        <f>Table131822[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+      <c r="I28">
+        <f>Table131822[[#This Row],[Level]]*1.5 + 15 + 40</f>
+        <v>56.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>20</v>
+      </c>
+      <c r="B29">
+        <f>Table131822[[#This Row],[Level]]*62.5+ 300</f>
+        <v>1550</v>
+      </c>
+      <c r="C29">
+        <f>Table131822[[#This Row],[Level]]*12.5+60</f>
+        <v>310</v>
+      </c>
+      <c r="D29">
+        <f>Table131822[[#This Row],[Level]]*1.125 + 15</f>
+        <v>37.5</v>
+      </c>
+      <c r="E29">
+        <f>Table131822[[#This Row],[Level]]*1.25 + 15 + 19</f>
+        <v>59</v>
+      </c>
+      <c r="F29">
+        <f>Table131822[[#This Row],[Level]]*1.125 + 15</f>
+        <v>37.5</v>
+      </c>
+      <c r="G29">
+        <f>Table131822[[#This Row],[Level]]*1.25 + 15 + 5</f>
+        <v>45</v>
+      </c>
+      <c r="H29">
+        <f>Table131822[[#This Row],[Level]]*1 + 15</f>
+        <v>35</v>
+      </c>
+      <c r="I29">
+        <f>Table131822[[#This Row],[Level]]*1.5 + 15 + 40</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <f>Table131822[[#This Row],[Level]]*62.5+ 300</f>
+        <v>1862.5</v>
+      </c>
+      <c r="C30">
+        <f>Table131822[[#This Row],[Level]]*12.5+60</f>
+        <v>372.5</v>
+      </c>
+      <c r="D30">
+        <f>Table131822[[#This Row],[Level]]*1.125 + 15</f>
+        <v>43.125</v>
+      </c>
+      <c r="E30">
+        <f>Table131822[[#This Row],[Level]]*1.25 + 15 + 19</f>
+        <v>65.25</v>
+      </c>
+      <c r="F30">
+        <f>Table131822[[#This Row],[Level]]*1.125 + 15</f>
+        <v>43.125</v>
+      </c>
+      <c r="G30">
+        <f>Table131822[[#This Row],[Level]]*1.25 + 15 + 5</f>
+        <v>51.25</v>
+      </c>
+      <c r="H30">
+        <f>Table131822[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="I30">
+        <f>Table131822[[#This Row],[Level]]*1.5 + 15 + 40</f>
+        <v>92.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7442,7 +7805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832521D1-8A9A-424A-96D4-48DD11A591EE}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Finished writing encounter with Chelsea, writing prince's arrival
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="12" activeTab="16" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="12" activeTab="17" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Skeleton Soldier" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,8 @@
     <sheet name="Corpse Eater" sheetId="17" r:id="rId15"/>
     <sheet name="Barren Wolf" sheetId="18" r:id="rId16"/>
     <sheet name="BanditsAndMercenaries" sheetId="19" r:id="rId17"/>
-    <sheet name="Behemoth" sheetId="20" r:id="rId18"/>
+    <sheet name="Chelsea" sheetId="21" r:id="rId18"/>
+    <sheet name="Behemoth" sheetId="20" r:id="rId19"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="71">
   <si>
     <t>Skeletons are the most basic undead, they have low magical attributes, agility, and luck.</t>
   </si>
@@ -252,6 +253,9 @@
   <si>
     <t>Mercenary Mage. Same equips</t>
   </si>
+  <si>
+    <t>Chelsea, light phys armor, dual equipped daggers -&gt; 40, 10/8 + 8 + 8</t>
+  </si>
 </sst>
 </file>
 
@@ -327,7 +331,31 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="248">
+  <dxfs count="256">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1866,7 +1894,7 @@
     <tableColumn id="7" xr3:uid="{F9852B29-E77D-4E17-A56E-5F0C649FA862}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{9A914BFF-1060-46E4-B8F9-412BD9293C3D}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2F83B650-811D-4FEE-92D5-03D4DC4376E5}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="247">
+    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="255">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1887,7 +1915,7 @@
     <tableColumn id="7" xr3:uid="{3A2FD57C-060A-462E-8BB9-B06F717E9D20}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{ED9393EA-F7F9-4661-8D0B-0D9246DDABF8}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{6F56342F-5442-42CD-8B6C-D98B6D6C0C56}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="203">
+    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="211">
       <calculatedColumnFormula>SUM(Table16[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1900,28 +1928,28 @@
   <autoFilter ref="A8:I13" xr:uid="{7BE337CC-37BD-4688-B60D-A66F4420668B}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{71340E4C-6101-4C59-8ED7-689E2AD5A962}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="202">
+    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="210">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*63-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="201">
+    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="209">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="200">
+    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="208">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="199">
+    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="207">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="198">
+    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="206">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="197">
+    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="205">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="196">
+    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="204">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="195">
+    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="203">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1942,7 +1970,7 @@
     <tableColumn id="7" xr3:uid="{4899BF24-9D2A-4CC0-AE35-4F49604AAC5A}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{CB1CC6BA-1D38-4B74-9BC6-7057FB9773EE}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{C47FADF6-C526-4188-9187-383757CE17C1}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="194">
+    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="202">
       <calculatedColumnFormula>SUM(Table168[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1955,28 +1983,28 @@
   <autoFilter ref="A9:I15" xr:uid="{06A56D17-07E5-4650-8EE9-7EA8F94D4020}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A2BE27C9-9DAE-49F5-9A70-C6CF7428BF31}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="193">
+    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="201">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="192">
+    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="200">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="191">
+    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="199">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="190">
+    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="198">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="189">
+    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="197">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.375+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="188">
+    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="196">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="187">
+    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="195">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="186">
+    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="194">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1997,7 +2025,7 @@
     <tableColumn id="7" xr3:uid="{60AD88FB-4685-412B-B5FD-BF8412C6B8E2}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{6A88D48C-D864-4F16-BEF2-BA88783A3FF3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{D40BD230-6392-4A28-A29D-F13EFE35C95E}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A0E09B2B-FD41-413F-8063-62214E990751}" name="Total" dataDxfId="185">
+    <tableColumn id="10" xr3:uid="{A0E09B2B-FD41-413F-8063-62214E990751}" name="Total" dataDxfId="193">
       <calculatedColumnFormula>SUM(Table16826[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2010,28 +2038,28 @@
   <autoFilter ref="A8:I14" xr:uid="{F7062CBA-4FAA-4900-9D3A-5C6613BCB6CE}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{ADCB4852-D3A0-456B-A8BD-E5F74BDBB762}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{ED76047D-1BC2-4C1B-B9B0-58BE0ACDDA48}" name="HP" dataDxfId="184">
+    <tableColumn id="2" xr3:uid="{ED76047D-1BC2-4C1B-B9B0-58BE0ACDDA48}" name="HP" dataDxfId="192">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EC859C53-0BA5-45D1-868B-F22DC8CE7D25}" name="MP" dataDxfId="183">
+    <tableColumn id="3" xr3:uid="{EC859C53-0BA5-45D1-868B-F22DC8CE7D25}" name="MP" dataDxfId="191">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DED33AB9-A2BB-4F9E-AA6D-02F8D1D65CD1}" name="ATK" dataDxfId="182">
+    <tableColumn id="4" xr3:uid="{DED33AB9-A2BB-4F9E-AA6D-02F8D1D65CD1}" name="ATK" dataDxfId="190">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.375+ 15+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{329B716D-9CA6-4546-AB13-92D88BE40F5F}" name="DEF" dataDxfId="181">
+    <tableColumn id="5" xr3:uid="{329B716D-9CA6-4546-AB13-92D88BE40F5F}" name="DEF" dataDxfId="189">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1 + 15+12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{67F8198A-5FC2-4C6D-9558-68B3141EA756}" name="MAT" dataDxfId="180">
+    <tableColumn id="6" xr3:uid="{67F8198A-5FC2-4C6D-9558-68B3141EA756}" name="MAT" dataDxfId="188">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C70F5BF6-63B0-44C1-862D-25E3FB55320F}" name="MDF" dataDxfId="179">
+    <tableColumn id="7" xr3:uid="{C70F5BF6-63B0-44C1-862D-25E3FB55320F}" name="MDF" dataDxfId="187">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.5+15+11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AB20AF53-453C-4266-A46B-40E693C91985}" name="AGI" dataDxfId="178">
+    <tableColumn id="8" xr3:uid="{AB20AF53-453C-4266-A46B-40E693C91985}" name="AGI" dataDxfId="186">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7FC46A31-F9F1-432E-B399-0823E198FE0A}" name="LUK" dataDxfId="177">
+    <tableColumn id="9" xr3:uid="{7FC46A31-F9F1-432E-B399-0823E198FE0A}" name="LUK" dataDxfId="185">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.5+15+20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2052,7 +2080,7 @@
     <tableColumn id="7" xr3:uid="{20C5D094-BAF0-471C-ACF3-C6658991DB5F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{E08E2AF0-56DD-4A69-A536-27139D793022}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{12AD8606-1127-4E5B-BA2C-872780F22F9E}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{5E2EF778-63AE-48B7-9F49-0D2AFEBD66A1}" name="Total" dataDxfId="176">
+    <tableColumn id="10" xr3:uid="{5E2EF778-63AE-48B7-9F49-0D2AFEBD66A1}" name="Total" dataDxfId="184">
       <calculatedColumnFormula>SUM(Table1682630[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2065,28 +2093,28 @@
   <autoFilter ref="A8:I14" xr:uid="{299912CC-280B-49E1-8859-432D05893259}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4F0B657F-C9A5-4A73-AAA3-27D307385193}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{526284E7-597F-4726-AB18-230CA03461B1}" name="HP" dataDxfId="175">
+    <tableColumn id="2" xr3:uid="{526284E7-597F-4726-AB18-230CA03461B1}" name="HP" dataDxfId="183">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*63+ 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E7BA3C7A-2677-415F-BA47-A4E88679B948}" name="MP" dataDxfId="174">
+    <tableColumn id="3" xr3:uid="{E7BA3C7A-2677-415F-BA47-A4E88679B948}" name="MP" dataDxfId="182">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE7BE678-2229-44F6-8732-71214FB69DD7}" name="ATK" dataDxfId="173">
+    <tableColumn id="4" xr3:uid="{AE7BE678-2229-44F6-8732-71214FB69DD7}" name="ATK" dataDxfId="181">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+ 15+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4715E3DB-8817-43D5-9074-9FB5F0BEF5B4}" name="DEF" dataDxfId="172">
+    <tableColumn id="5" xr3:uid="{4715E3DB-8817-43D5-9074-9FB5F0BEF5B4}" name="DEF" dataDxfId="180">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1 + 15+12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9CE76933-D045-418B-A975-378EEA51D856}" name="MAT" dataDxfId="171">
+    <tableColumn id="6" xr3:uid="{9CE76933-D045-418B-A975-378EEA51D856}" name="MAT" dataDxfId="179">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244B9611-6CB0-4946-B5CD-7D42311C7D7E}" name="MDF" dataDxfId="170">
+    <tableColumn id="7" xr3:uid="{244B9611-6CB0-4946-B5CD-7D42311C7D7E}" name="MDF" dataDxfId="178">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+15+11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32550C13-49BB-41D2-BA0A-26798830A0FD}" name="AGI" dataDxfId="169">
+    <tableColumn id="8" xr3:uid="{32550C13-49BB-41D2-BA0A-26798830A0FD}" name="AGI" dataDxfId="177">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{BB22F289-8AF5-4DD6-877B-F09520710555}" name="LUK" dataDxfId="168">
+    <tableColumn id="9" xr3:uid="{BB22F289-8AF5-4DD6-877B-F09520710555}" name="LUK" dataDxfId="176">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+15+20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2099,28 +2127,28 @@
   <autoFilter ref="A4:I10" xr:uid="{A1EAC62C-C07D-464E-91B1-4A34E6604BA2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{430FD3D4-914C-4309-B2E6-6F01B5CAED94}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="167">
+    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="175">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="166">
+    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="174">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="165">
+    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="173">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="164">
+    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="172">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15 + 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="163">
+    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="171">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15 + 30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="162">
+    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="170">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15 + 21</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="161">
+    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="169">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="160">
+    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="168">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2133,28 +2161,28 @@
   <autoFilter ref="A7:I12" xr:uid="{9BE7336F-352A-4FAE-B0E4-61965FC814C7}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B8DA50BB-4379-43D1-879B-CDBE6D82C13A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="159">
+    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="167">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="158">
+    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="166">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="157">
+    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="165">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="156">
+    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="164">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="155">
+    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="163">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="154">
+    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="162">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="153">
+    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="161">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="152">
+    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="160">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2167,28 +2195,28 @@
   <autoFilter ref="A8:I13" xr:uid="{67385006-CBB9-4472-99D4-7881E042769D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FD96F8F7-CCAB-44FA-B525-A5081670706A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="246">
+    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="254">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="245">
+    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="253">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="244">
+    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="252">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="243">
+    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="251">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="242">
+    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="250">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="241">
+    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="249">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="240">
+    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="248">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="239">
+    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="247">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2209,7 +2237,7 @@
     <tableColumn id="7" xr3:uid="{AEFF5C29-BE6A-4CF8-A2BB-F6B076077DA9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{4DE9B01E-67F2-4136-ADC3-60389FB67DCC}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{F5A82F03-513C-46D4-9F91-470F0060526B}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="151">
+    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="159">
       <calculatedColumnFormula>SUM(Table16821[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2218,22 +2246,22 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="150" tableBorderDxfId="149">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="158" tableBorderDxfId="157">
   <autoFilter ref="A15:I16" xr:uid="{434CBBE2-2F8D-4EEB-895C-68FC850EF1FD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="148"/>
-    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="147">
+    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="156"/>
+    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="155">
       <calculatedColumnFormula>Table1922[Level]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="146">
+    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="154">
       <calculatedColumnFormula>Table1922[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="145"/>
-    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="144"/>
-    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="143"/>
-    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="142"/>
-    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="141"/>
-    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="140"/>
+    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="153"/>
+    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="152"/>
+    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="151"/>
+    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="150"/>
+    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="149"/>
+    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="148"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2244,28 +2272,28 @@
   <autoFilter ref="A3:I9" xr:uid="{A90D1C2A-DBF9-4EEF-ACC2-3DC17C207301}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BD3505AC-AE6D-4947-A74E-A6C2D68658F1}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="139">
+    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="147">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="138">
+    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="146">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="137">
+    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="145">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="136">
+    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="144">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="135">
+    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="143">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="134">
+    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="142">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="133">
+    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="141">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="132">
+    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="140">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2274,32 +2302,32 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="131" tableBorderDxfId="130">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="139" tableBorderDxfId="138">
   <autoFilter ref="L3:T4" xr:uid="{5D2C3EA8-1297-4C77-AF32-84E50F8232C5}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="129"/>
-    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="128">
+    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="137"/>
+    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="136">
       <calculatedColumnFormula>Table19[Level]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="127">
+    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="135">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="126">
+    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="134">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="125">
+    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="133">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1 + 15 + 6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="124">
+    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="132">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="123">
+    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="131">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="122">
+    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="130">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="121">
+    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="129">
       <calculatedColumnFormula>Table19[Level] + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2312,28 +2340,28 @@
   <autoFilter ref="A7:I12" xr:uid="{553298A4-7E43-42CF-9EEB-1F9E7E6BAD27}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2AA35C8B-719C-4BA6-9CDF-2963E1C9F233}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C087FAFA-9653-40EC-B4B9-5CB8F9D7255E}" name="HP" dataDxfId="120">
+    <tableColumn id="2" xr3:uid="{C087FAFA-9653-40EC-B4B9-5CB8F9D7255E}" name="HP" dataDxfId="128">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0004B47B-3968-4C5A-BE6C-B822A307D7C5}" name="MP" dataDxfId="119">
+    <tableColumn id="3" xr3:uid="{0004B47B-3968-4C5A-BE6C-B822A307D7C5}" name="MP" dataDxfId="127">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{67EC8D91-0122-40D7-87D0-A3AB6788CE9D}" name="ATK" dataDxfId="118">
+    <tableColumn id="4" xr3:uid="{67EC8D91-0122-40D7-87D0-A3AB6788CE9D}" name="ATK" dataDxfId="126">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E9988E54-33D6-41EB-B6BE-6E832544E18C}" name="DEF" dataDxfId="117">
+    <tableColumn id="5" xr3:uid="{E9988E54-33D6-41EB-B6BE-6E832544E18C}" name="DEF" dataDxfId="125">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{16D71A55-372C-4029-A831-ECF2325E46C4}" name="MAT" dataDxfId="116">
+    <tableColumn id="6" xr3:uid="{16D71A55-372C-4029-A831-ECF2325E46C4}" name="MAT" dataDxfId="124">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{1802FB48-B110-4DBF-A8F2-64CD4890E741}" name="MDF" dataDxfId="115">
+    <tableColumn id="7" xr3:uid="{1802FB48-B110-4DBF-A8F2-64CD4890E741}" name="MDF" dataDxfId="123">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{350CA8CC-761C-4994-9D80-14685787EF3D}" name="AGI" dataDxfId="114">
+    <tableColumn id="8" xr3:uid="{350CA8CC-761C-4994-9D80-14685787EF3D}" name="AGI" dataDxfId="122">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B578CF58-136A-41B9-800E-D75836A4CDD1}" name="LUK" dataDxfId="113">
+    <tableColumn id="9" xr3:uid="{B578CF58-136A-41B9-800E-D75836A4CDD1}" name="LUK" dataDxfId="121">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2354,7 +2382,7 @@
     <tableColumn id="7" xr3:uid="{5A405725-30A7-487F-95BF-061F71CA9C61}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{644DEF70-6EBD-403E-904B-6C30E5FBEA48}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{BA93DA54-96B9-48D1-80BB-C266771E13F1}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{3EBB17A5-47EA-458B-83A5-7056BE67D25F}" name="Total" dataDxfId="112">
+    <tableColumn id="10" xr3:uid="{3EBB17A5-47EA-458B-83A5-7056BE67D25F}" name="Total" dataDxfId="120">
       <calculatedColumnFormula>SUM(Table1682134[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2363,26 +2391,26 @@
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{A7C0F3AC-4E86-430D-AE55-8604641B493E}" name="Table192235" displayName="Table192235" ref="A15:I16" totalsRowShown="0" dataDxfId="111" tableBorderDxfId="110">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{A7C0F3AC-4E86-430D-AE55-8604641B493E}" name="Table192235" displayName="Table192235" ref="A15:I16" totalsRowShown="0" dataDxfId="119" tableBorderDxfId="118">
   <autoFilter ref="A15:I16" xr:uid="{D0DF3ED4-9A21-493B-88F4-CE5814AF31C9}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A78A876E-6C8B-4FC8-BFD4-A9BC80EA3FC2}" name="Level" dataDxfId="109"/>
-    <tableColumn id="2" xr3:uid="{4B423FFC-D037-484D-A927-2F66E15D422A}" name="HP" dataDxfId="108">
+    <tableColumn id="1" xr3:uid="{A78A876E-6C8B-4FC8-BFD4-A9BC80EA3FC2}" name="Level" dataDxfId="117"/>
+    <tableColumn id="2" xr3:uid="{4B423FFC-D037-484D-A927-2F66E15D422A}" name="HP" dataDxfId="116">
       <calculatedColumnFormula>(Table192235[Level]*75 + 500)*2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B695FEDE-EC59-44D8-AE99-CBF568DE5C93}" name="MP" dataDxfId="107">
+    <tableColumn id="3" xr3:uid="{B695FEDE-EC59-44D8-AE99-CBF568DE5C93}" name="MP" dataDxfId="115">
       <calculatedColumnFormula>Table192235[[#This Row],[Level]]*14 + 80</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{160D5D77-34E8-44F3-B51D-7CC0736DDCB1}" name="ATK" dataDxfId="106">
+    <tableColumn id="4" xr3:uid="{160D5D77-34E8-44F3-B51D-7CC0736DDCB1}" name="ATK" dataDxfId="114">
       <calculatedColumnFormula>Table192235[[#This Row],[Level]]*1.5+ 15 + 50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{559DAC37-CD6A-449F-AFF0-355ADE7CED80}" name="DEF" dataDxfId="105"/>
-    <tableColumn id="6" xr3:uid="{EEC344A5-27A5-450E-B795-04D237DD063F}" name="MAT" dataDxfId="104">
+    <tableColumn id="5" xr3:uid="{559DAC37-CD6A-449F-AFF0-355ADE7CED80}" name="DEF" dataDxfId="113"/>
+    <tableColumn id="6" xr3:uid="{EEC344A5-27A5-450E-B795-04D237DD063F}" name="MAT" dataDxfId="112">
       <calculatedColumnFormula>Table192235[Level]*1.5+15+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{54363CA4-9EE5-495F-8323-6C0C1261453C}" name="MDF" dataDxfId="103"/>
-    <tableColumn id="8" xr3:uid="{26B56E9D-2FCD-4476-A6CF-8F2EDC965246}" name="AGI" dataDxfId="102"/>
-    <tableColumn id="9" xr3:uid="{95814D66-3343-4190-9BF4-F4E45AB27D95}" name="LUK" dataDxfId="101"/>
+    <tableColumn id="7" xr3:uid="{54363CA4-9EE5-495F-8323-6C0C1261453C}" name="MDF" dataDxfId="111"/>
+    <tableColumn id="8" xr3:uid="{26B56E9D-2FCD-4476-A6CF-8F2EDC965246}" name="AGI" dataDxfId="110"/>
+    <tableColumn id="9" xr3:uid="{95814D66-3343-4190-9BF4-F4E45AB27D95}" name="LUK" dataDxfId="109"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2401,7 +2429,7 @@
     <tableColumn id="7" xr3:uid="{22216E02-260E-4471-8BB1-4E6E1250BAC9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{DC2670AC-8DF2-47F7-A3F6-EE7896309BC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{749652E2-F6CF-428C-B67C-FD0B1EFCCBBF}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="100">
+    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="108">
       <calculatedColumnFormula>SUM(Table15[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2414,28 +2442,28 @@
   <autoFilter ref="A15:I20" xr:uid="{A1CF627F-8D28-44AD-9A35-411103976FCA}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F14CC326-DE44-48D8-856F-8DCDCFC89CAD}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="99">
+    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="107">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*63-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="98">
+    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="106">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="97">
+    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="105">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="96">
+    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="104">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="95">
+    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="103">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="94">
+    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="102">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="93">
+    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="101">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="92">
+    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="100">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2448,28 +2476,28 @@
   <autoFilter ref="K11:S17" xr:uid="{EAF9FB6A-F011-40E3-AB2F-E53826722AFB}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DF3E0800-6EE4-4E1B-BA6F-0194351D6E7C}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="91">
+    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="99">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*56.25+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="90">
+    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="98">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="89">
+    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="97">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="88">
+    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="96">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="87">
+    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="95">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="86">
+    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="94">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="85">
+    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="93">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="84">
+    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="92">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2482,28 +2510,28 @@
   <autoFilter ref="K8:S14" xr:uid="{AB7E938D-7ACC-4BFB-A6B9-682B8B29CEF2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{66EB8EF1-BCF4-44F7-B8A6-3C3B425F8FF5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="238">
+    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="246">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*56.25+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="237">
+    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="245">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="236">
+    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="244">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25+ 15+30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="235">
+    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="243">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25 + 15+33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="234">
+    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="242">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="233">
+    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="241">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="232">
+    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="240">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="231">
+    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="239">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2516,28 +2544,28 @@
   <autoFilter ref="A26:I31" xr:uid="{870F76F2-5EA7-4FD7-B1F9-507D64592088}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{3C04B742-338A-4366-BF3D-C5BC13023785}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="83">
+    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="91">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*63+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="82">
+    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="90">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="81">
+    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="89">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="80">
+    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="88">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="79">
+    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="87">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="78">
+    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="86">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="77">
+    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="85">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="76">
+    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="84">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2550,28 +2578,28 @@
   <autoFilter ref="A36:I41" xr:uid="{9BD043AF-0D77-4FF4-B2F9-B4AC3C3F1F82}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{7BB908A3-05D7-4357-920B-BF4C6BC20C06}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="75">
+    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="83">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*56.5+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="74">
+    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="82">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*12.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="73">
+    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="81">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="72">
+    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="80">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1 + 15+14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="71">
+    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="79">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="70">
+    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="78">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.5+ 15+13</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="69">
+    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="77">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="68">
+    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="76">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.375 + 15+40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2592,7 +2620,7 @@
     <tableColumn id="7" xr3:uid="{09E4151E-54A0-41FF-BA5B-3B1C748DA23D}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{909575E0-EC13-4E35-A35F-2451A5741589}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2CDCF32E-D8FC-48D9-A28D-8D9C5F3EB001}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{001DA1BB-34DD-4786-BDE4-23C510900A3D}" name="Total" dataDxfId="67">
+    <tableColumn id="10" xr3:uid="{001DA1BB-34DD-4786-BDE4-23C510900A3D}" name="Total" dataDxfId="75">
       <calculatedColumnFormula>SUM(Table168213429[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2605,28 +2633,28 @@
   <autoFilter ref="A7:I12" xr:uid="{4ED64482-035D-49B9-A477-A1D5AEB4A5A4}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{141B0E2E-D4F3-4884-86FD-AAD67C363749}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{D4B50877-EF56-4EF7-8C6D-9928A6D654F6}" name="HP" dataDxfId="66">
+    <tableColumn id="2" xr3:uid="{D4B50877-EF56-4EF7-8C6D-9928A6D654F6}" name="HP" dataDxfId="74">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*125</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F4B06187-BE28-4283-9518-F773FE75C2BF}" name="MP" dataDxfId="65">
+    <tableColumn id="3" xr3:uid="{F4B06187-BE28-4283-9518-F773FE75C2BF}" name="MP" dataDxfId="73">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{91A68FC7-5F16-4880-AE82-97341814BB95}" name="ATK" dataDxfId="64">
+    <tableColumn id="4" xr3:uid="{91A68FC7-5F16-4880-AE82-97341814BB95}" name="ATK" dataDxfId="72">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*4.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{2BCD0E58-85DE-4C10-BFBC-AF77BC569C92}" name="DEF" dataDxfId="63">
+    <tableColumn id="5" xr3:uid="{2BCD0E58-85DE-4C10-BFBC-AF77BC569C92}" name="DEF" dataDxfId="71">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7C48A1FC-CE8F-4CDD-9A3D-308B46D78A48}" name="MAT" dataDxfId="62">
+    <tableColumn id="6" xr3:uid="{7C48A1FC-CE8F-4CDD-9A3D-308B46D78A48}" name="MAT" dataDxfId="70">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{474D8178-EA8C-4322-93C3-B7F6EBA88102}" name="MDF" dataDxfId="61">
+    <tableColumn id="7" xr3:uid="{474D8178-EA8C-4322-93C3-B7F6EBA88102}" name="MDF" dataDxfId="69">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{257B31D9-5838-45E0-A56E-9B1566E1A34A}" name="AGI" dataDxfId="60">
+    <tableColumn id="8" xr3:uid="{257B31D9-5838-45E0-A56E-9B1566E1A34A}" name="AGI" dataDxfId="68">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{17960EB4-4250-49DB-9A6B-455B9913B04B}" name="LUK" dataDxfId="59">
+    <tableColumn id="9" xr3:uid="{17960EB4-4250-49DB-9A6B-455B9913B04B}" name="LUK" dataDxfId="67">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1.125</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2647,7 +2675,7 @@
     <tableColumn id="7" xr3:uid="{07EA0638-8880-4944-AC9E-13E3F1B9F651}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{AA18E602-126F-4D69-9CC8-C097E8EB9C70}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{5563B0CB-2EA7-4851-8D1F-D77E0F90CBAD}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{2D960B43-0F76-4936-9508-4D501A79A83C}" name="Total" dataDxfId="58">
+    <tableColumn id="10" xr3:uid="{2D960B43-0F76-4936-9508-4D501A79A83C}" name="Total" dataDxfId="66">
       <calculatedColumnFormula>SUM(Table16821342932[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2660,28 +2688,28 @@
   <autoFilter ref="A5:I10" xr:uid="{2922C913-6AE8-4B89-BDA6-9F44D59987D8}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{3D67222C-6501-4A5D-A9FC-528EE591A288}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EE3E4CCC-C404-4B78-AAB4-3B38166E23BA}" name="HP" dataDxfId="57">
+    <tableColumn id="2" xr3:uid="{EE3E4CCC-C404-4B78-AAB4-3B38166E23BA}" name="HP" dataDxfId="65">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DE5141FB-3B4E-46D4-9E0D-AF1DEE998B4A}" name="MP" dataDxfId="56">
+    <tableColumn id="3" xr3:uid="{DE5141FB-3B4E-46D4-9E0D-AF1DEE998B4A}" name="MP" dataDxfId="64">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{404B3E88-DF62-4AA0-82D6-C21C2BCA762B}" name="ATK" dataDxfId="55">
+    <tableColumn id="4" xr3:uid="{404B3E88-DF62-4AA0-82D6-C21C2BCA762B}" name="ATK" dataDxfId="63">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*4.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{342B3F39-F7A2-45D8-9CD4-39B5ABC72D2F}" name="DEF" dataDxfId="54">
+    <tableColumn id="5" xr3:uid="{342B3F39-F7A2-45D8-9CD4-39B5ABC72D2F}" name="DEF" dataDxfId="62">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{CD819DB3-9F2E-4428-AAFC-72776ECB8EAF}" name="MAT" dataDxfId="53">
+    <tableColumn id="6" xr3:uid="{CD819DB3-9F2E-4428-AAFC-72776ECB8EAF}" name="MAT" dataDxfId="61">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{270DF964-8095-43FD-B050-DD4A2A138F32}" name="MDF" dataDxfId="52">
+    <tableColumn id="7" xr3:uid="{270DF964-8095-43FD-B050-DD4A2A138F32}" name="MDF" dataDxfId="60">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4F4D3B2A-5B86-4AB7-A97E-18E2868266B8}" name="AGI" dataDxfId="51">
+    <tableColumn id="8" xr3:uid="{4F4D3B2A-5B86-4AB7-A97E-18E2868266B8}" name="AGI" dataDxfId="59">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{0178CE2D-63C5-426A-A081-D62E62FF91AC}" name="LUK" dataDxfId="50">
+    <tableColumn id="9" xr3:uid="{0178CE2D-63C5-426A-A081-D62E62FF91AC}" name="LUK" dataDxfId="58">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*1.5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2702,7 +2730,7 @@
     <tableColumn id="7" xr3:uid="{C374A90B-690A-432C-974A-C8A7D22E367F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{05C64890-0DC2-4577-975E-95477DCED789}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{CE6AAEA9-D599-4B9B-BD40-7E602F47088C}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{30017AE7-6C23-415F-A2EA-70EA09C835E6}" name="Total" dataDxfId="49">
+    <tableColumn id="10" xr3:uid="{30017AE7-6C23-415F-A2EA-70EA09C835E6}" name="Total" dataDxfId="57">
       <calculatedColumnFormula>SUM(Table1682134293227[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2715,28 +2743,28 @@
   <autoFilter ref="A6:I11" xr:uid="{D09397F4-7631-4CD3-AF40-3B14C64478EE}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BF4E6A79-8CCF-498E-B3B0-FA782AB06519}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{37E52E57-C499-4FFB-AC3F-20E63EEA4D3A}" name="HP" dataDxfId="48">
+    <tableColumn id="2" xr3:uid="{37E52E57-C499-4FFB-AC3F-20E63EEA4D3A}" name="HP" dataDxfId="56">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*87.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D29F5CDE-1200-4C77-A4BA-0DE4F7C46627}" name="MP" dataDxfId="47">
+    <tableColumn id="3" xr3:uid="{D29F5CDE-1200-4C77-A4BA-0DE4F7C46627}" name="MP" dataDxfId="55">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{9701140A-64F9-4967-9DEE-3460411D91C1}" name="ATK" dataDxfId="46">
+    <tableColumn id="4" xr3:uid="{9701140A-64F9-4967-9DEE-3460411D91C1}" name="ATK" dataDxfId="54">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F90A425E-E031-4255-8AF9-DAD672F8DD7D}" name="DEF" dataDxfId="45">
+    <tableColumn id="5" xr3:uid="{F90A425E-E031-4255-8AF9-DAD672F8DD7D}" name="DEF" dataDxfId="53">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*4.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{255210A0-6EB8-4CFB-84DD-42C88AEAF7AA}" name="MAT" dataDxfId="44">
+    <tableColumn id="6" xr3:uid="{255210A0-6EB8-4CFB-84DD-42C88AEAF7AA}" name="MAT" dataDxfId="52">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{91177FDD-F316-4D6B-A547-FC5FA6DAC266}" name="MDF" dataDxfId="43">
+    <tableColumn id="7" xr3:uid="{91177FDD-F316-4D6B-A547-FC5FA6DAC266}" name="MDF" dataDxfId="51">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{ADA902F7-B7D7-4B1B-A144-E5252296AB61}" name="AGI" dataDxfId="42">
+    <tableColumn id="8" xr3:uid="{ADA902F7-B7D7-4B1B-A144-E5252296AB61}" name="AGI" dataDxfId="50">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{78273DA6-F2CA-4999-B4EA-F6C044BC41AB}" name="LUK" dataDxfId="41">
+    <tableColumn id="9" xr3:uid="{78273DA6-F2CA-4999-B4EA-F6C044BC41AB}" name="LUK" dataDxfId="49">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2749,28 +2777,28 @@
   <autoFilter ref="A4:I9" xr:uid="{DD778A26-93EC-4B14-A9D1-160AE03B48D3}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F0A3DB96-38E4-4CD0-BAF6-C8BB768B1256}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{07B77441-F84C-41C6-A00C-B69369FBF0F1}" name="HP" dataDxfId="40">
+    <tableColumn id="2" xr3:uid="{07B77441-F84C-41C6-A00C-B69369FBF0F1}" name="HP" dataDxfId="48">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{2DBE06DE-38E0-4433-B590-3850C554BB8E}" name="MP" dataDxfId="39">
+    <tableColumn id="3" xr3:uid="{2DBE06DE-38E0-4433-B590-3850C554BB8E}" name="MP" dataDxfId="47">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DE8CC9D0-45D8-4F85-9317-09844C8D4DD7}" name="ATK" dataDxfId="38">
+    <tableColumn id="4" xr3:uid="{DE8CC9D0-45D8-4F85-9317-09844C8D4DD7}" name="ATK" dataDxfId="46">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1.375+ 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{9D33BCF5-CDB6-4BB0-8603-810E71EE1C47}" name="DEF" dataDxfId="37">
+    <tableColumn id="5" xr3:uid="{9D33BCF5-CDB6-4BB0-8603-810E71EE1C47}" name="DEF" dataDxfId="45">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1.375 + 15 + 19</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{1693AB2F-85DB-4286-A43C-82A15CDDA173}" name="MAT" dataDxfId="36">
+    <tableColumn id="6" xr3:uid="{1693AB2F-85DB-4286-A43C-82A15CDDA173}" name="MAT" dataDxfId="44">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{DCA68233-62C9-4E66-9306-24AE49EE344C}" name="MDF" dataDxfId="35">
+    <tableColumn id="7" xr3:uid="{DCA68233-62C9-4E66-9306-24AE49EE344C}" name="MDF" dataDxfId="43">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1 + 15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{60943D8A-0008-4FFE-AE90-4DDEB0149A21}" name="AGI" dataDxfId="34">
+    <tableColumn id="8" xr3:uid="{60943D8A-0008-4FFE-AE90-4DDEB0149A21}" name="AGI" dataDxfId="42">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E7EC6C93-3486-414B-87DB-F4D38BB2A0DC}" name="LUK" dataDxfId="33">
+    <tableColumn id="9" xr3:uid="{E7EC6C93-3486-414B-87DB-F4D38BB2A0DC}" name="LUK" dataDxfId="41">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2783,28 +2811,28 @@
   <autoFilter ref="A12:I16" xr:uid="{2A794F38-5DB8-40A3-A8E2-90B5A0A4A192}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{C5A2CF3A-0965-428C-AD05-883EDB0D400F}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C8840580-F723-4CA3-A107-42FCC677D424}" name="HP" dataDxfId="32">
+    <tableColumn id="2" xr3:uid="{C8840580-F723-4CA3-A107-42FCC677D424}" name="HP" dataDxfId="40">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*62.5+ 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5D9241C6-74A5-4C1F-A8F7-69DB1BDA83FE}" name="MP" dataDxfId="31">
+    <tableColumn id="3" xr3:uid="{5D9241C6-74A5-4C1F-A8F7-69DB1BDA83FE}" name="MP" dataDxfId="39">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*12.5+60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D98F9CCD-2FEF-4FB2-B5AD-D2A6B610781B}" name="ATK" dataDxfId="30">
+    <tableColumn id="4" xr3:uid="{D98F9CCD-2FEF-4FB2-B5AD-D2A6B610781B}" name="ATK" dataDxfId="38">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CF1AF448-2207-48D1-8FE3-0A6B5DE3511C}" name="DEF" dataDxfId="29">
+    <tableColumn id="5" xr3:uid="{CF1AF448-2207-48D1-8FE3-0A6B5DE3511C}" name="DEF" dataDxfId="37">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1 + 15 + 10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A632BAA7-E71C-41F8-B5B0-90891BB5BA9B}" name="MAT" dataDxfId="28">
+    <tableColumn id="6" xr3:uid="{A632BAA7-E71C-41F8-B5B0-90891BB5BA9B}" name="MAT" dataDxfId="36">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E76132BC-BC67-4915-8112-E0B292C65C91}" name="MDF" dataDxfId="27">
+    <tableColumn id="7" xr3:uid="{E76132BC-BC67-4915-8112-E0B292C65C91}" name="MDF" dataDxfId="35">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1 + 15 + 8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B25B7E33-B3CF-4D3D-9A14-3CE5B75535E8}" name="AGI" dataDxfId="26">
+    <tableColumn id="8" xr3:uid="{B25B7E33-B3CF-4D3D-9A14-3CE5B75535E8}" name="AGI" dataDxfId="34">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{40820F61-4B4C-4B23-95CF-AD5CDE975F4A}" name="LUK" dataDxfId="25">
+    <tableColumn id="9" xr3:uid="{40820F61-4B4C-4B23-95CF-AD5CDE975F4A}" name="LUK" dataDxfId="33">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2825,7 +2853,7 @@
     <tableColumn id="7" xr3:uid="{F833922A-76F9-427C-8462-D94DE51D0477}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{203171A1-C88B-4F81-ADC2-1EE072D645F3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{34003EF6-E9A5-4584-A186-09DFF4EC11C7}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{C4602156-F897-42BE-8F3F-411E13EEB095}" name="Total" dataDxfId="230">
+    <tableColumn id="10" xr3:uid="{C4602156-F897-42BE-8F3F-411E13EEB095}" name="Total" dataDxfId="238">
       <calculatedColumnFormula>SUM(Table114[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2838,28 +2866,28 @@
   <autoFilter ref="A20:I24" xr:uid="{6015D08B-C4A1-43B9-B8BF-6F441CC08DCA}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D4205A68-390A-4750-8556-3B4847E58D16}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{D7D1DEBE-6CE0-4976-A401-D4F35A038AA9}" name="HP" dataDxfId="24">
+    <tableColumn id="2" xr3:uid="{D7D1DEBE-6CE0-4976-A401-D4F35A038AA9}" name="HP" dataDxfId="32">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{3CB0ED8A-F14B-4E5F-8474-F3034EA78A85}" name="MP" dataDxfId="23">
+    <tableColumn id="3" xr3:uid="{3CB0ED8A-F14B-4E5F-8474-F3034EA78A85}" name="MP" dataDxfId="31">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F3186E07-87BD-4E53-8F85-AB4798362B0C}" name="ATK" dataDxfId="22">
+    <tableColumn id="4" xr3:uid="{F3186E07-87BD-4E53-8F85-AB4798362B0C}" name="ATK" dataDxfId="30">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{22ED75D6-B85C-4DF9-BC39-4154BAF3990E}" name="DEF" dataDxfId="21">
+    <tableColumn id="5" xr3:uid="{22ED75D6-B85C-4DF9-BC39-4154BAF3990E}" name="DEF" dataDxfId="29">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1 + 15 + 4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B2DFC87A-2BEE-4B5A-AF53-4E18078ABC1B}" name="MAT" dataDxfId="20">
+    <tableColumn id="6" xr3:uid="{B2DFC87A-2BEE-4B5A-AF53-4E18078ABC1B}" name="MAT" dataDxfId="28">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.375 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{8FF82542-4129-4E67-AA7B-7CB38D8FB051}" name="MDF" dataDxfId="19">
+    <tableColumn id="7" xr3:uid="{8FF82542-4129-4E67-AA7B-7CB38D8FB051}" name="MDF" dataDxfId="27">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.375 + 15 + 14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{85F4097E-90A5-4A7C-B184-42B110E62300}" name="AGI" dataDxfId="18">
+    <tableColumn id="8" xr3:uid="{85F4097E-90A5-4A7C-B184-42B110E62300}" name="AGI" dataDxfId="26">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E1A21F56-D819-4CE3-9122-F47B8A4039A9}" name="LUK" dataDxfId="17">
+    <tableColumn id="9" xr3:uid="{E1A21F56-D819-4CE3-9122-F47B8A4039A9}" name="LUK" dataDxfId="25">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2872,28 +2900,28 @@
   <autoFilter ref="A27:I30" xr:uid="{4506A984-1EE8-4D0B-9AFB-6DE5576F3317}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{97BB3945-930E-41A9-B479-678FD9D8EE85}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{2197951B-D7A2-413F-8152-C8BB282E3498}" name="HP" dataDxfId="7">
+    <tableColumn id="2" xr3:uid="{2197951B-D7A2-413F-8152-C8BB282E3498}" name="HP" dataDxfId="24">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*62.5+ 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{54D89380-BDA0-4B18-8B8B-482E9AA62AD3}" name="MP" dataDxfId="6">
+    <tableColumn id="3" xr3:uid="{54D89380-BDA0-4B18-8B8B-482E9AA62AD3}" name="MP" dataDxfId="23">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*12.5+60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DCD1A325-B7AE-4283-89E4-85446F157A12}" name="ATK" dataDxfId="5">
+    <tableColumn id="4" xr3:uid="{DCD1A325-B7AE-4283-89E4-85446F157A12}" name="ATK" dataDxfId="22">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1CD051D4-B531-4706-95A8-BBF452C5188D}" name="DEF" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{1CD051D4-B531-4706-95A8-BBF452C5188D}" name="DEF" dataDxfId="21">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.25 + 15 + 19</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{E17A43F1-7669-40E6-BD8C-8623B203A60F}" name="MAT" dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{E17A43F1-7669-40E6-BD8C-8623B203A60F}" name="MAT" dataDxfId="20">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{04F7D6BA-3673-4BE0-97CA-65C8DD4612E3}" name="MDF" dataDxfId="1">
+    <tableColumn id="7" xr3:uid="{04F7D6BA-3673-4BE0-97CA-65C8DD4612E3}" name="MDF" dataDxfId="19">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.25 + 15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{7AA9AD24-2AFF-4204-AAEF-0CC3265C40FA}" name="AGI" dataDxfId="3">
+    <tableColumn id="8" xr3:uid="{7AA9AD24-2AFF-4204-AAEF-0CC3265C40FA}" name="AGI" dataDxfId="18">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{ABFCE932-20B6-4AEE-A261-B747D2EC6FA8}" name="LUK" dataDxfId="2">
+    <tableColumn id="9" xr3:uid="{ABFCE932-20B6-4AEE-A261-B747D2EC6FA8}" name="LUK" dataDxfId="17">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2902,6 +2930,40 @@
 </file>
 
 <file path=xl/tables/table42.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="42" xr:uid="{B11B1E6C-19A5-42E4-847D-0CD22EB4A103}" name="Table1318222743" displayName="Table1318222743" ref="A3:I7" totalsRowShown="0">
+  <autoFilter ref="A3:I7" xr:uid="{7F8360B3-D323-4505-8E52-764F2EEFEF08}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{2DA75379-E191-41C6-A461-F7A952576C54}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{0E110670-3AC7-427B-B6F4-6865DC721C3B}" name="HP" dataDxfId="16">
+      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*62.5+ 300</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{DD071379-690C-45AA-9EB0-1452F203E78A}" name="MP" dataDxfId="15">
+      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*12.5+60</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{16C4CC92-9435-4196-8A09-D27E77854475}" name="ATK" dataDxfId="14">
+      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{ACFF3F1F-0DEB-4962-A30C-E7A1BD1814C4}" name="DEF" dataDxfId="13">
+      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1 + 15 + 10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{AF9BE2E5-89EE-468C-B0ED-D05B0FFE3880}" name="MAT" dataDxfId="12">
+      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{BF26333D-F5E1-471D-8EB4-69106E629333}" name="MDF" dataDxfId="11">
+      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1 + 15 + 8</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{419D6271-6B9C-434E-BF38-4DE7848F9419}" name="AGI" dataDxfId="10">
+      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{CB85A19D-24B4-428F-A77F-481DA3FAACF8}" name="LUK" dataDxfId="9">
+      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table43.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="44" xr:uid="{63EFECE9-294D-4BD5-B983-D7DF0138B45B}" name="Table168213429322745" displayName="Table168213429322745" ref="A4:J6" totalsRowShown="0">
   <autoFilter ref="A4:J6" xr:uid="{9FA97447-7595-4CE0-9387-AEB91FE50244}"/>
   <tableColumns count="10">
@@ -2914,7 +2976,7 @@
     <tableColumn id="7" xr3:uid="{6B239F5E-F897-4532-B3C2-8B926BDED5BF}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{CB8FDC45-B604-4FEB-9A7B-367828FC7568}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{6C00B6B1-0959-4058-96EE-2711BA8C66BD}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{1803A62E-480C-481E-8063-2EB8C650EA1D}" name="Total" dataDxfId="16">
+    <tableColumn id="10" xr3:uid="{1803A62E-480C-481E-8063-2EB8C650EA1D}" name="Total" dataDxfId="8">
       <calculatedColumnFormula>SUM(Table168213429322745[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2922,33 +2984,33 @@
 </table>
 </file>
 
-<file path=xl/tables/table43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table44.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="46" xr:uid="{6B246BF5-6CE4-4B50-8843-8DACC434192B}" name="Table1316183336373847" displayName="Table1316183336373847" ref="A8:I13" totalsRowShown="0">
   <autoFilter ref="A8:I13" xr:uid="{F3DE48F5-A98B-4A15-8805-1948F568C45F}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2E01F6BC-B2F6-42D6-A20F-FDB9BA2D677A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{21915B10-9976-4EFE-936F-170B253E711B}" name="HP" dataDxfId="15">
+    <tableColumn id="2" xr3:uid="{21915B10-9976-4EFE-936F-170B253E711B}" name="HP" dataDxfId="7">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*168.75</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{052B9451-309F-4C84-8FC4-08AD4866120D}" name="MP" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{052B9451-309F-4C84-8FC4-08AD4866120D}" name="MP" dataDxfId="6">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{B73769F3-1F79-45AE-998C-FF1A9A557091}" name="ATK" dataDxfId="13">
+    <tableColumn id="4" xr3:uid="{B73769F3-1F79-45AE-998C-FF1A9A557091}" name="ATK" dataDxfId="5">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*3.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B5E81D1B-B382-4DF5-92BA-F92F12A23A07}" name="DEF" dataDxfId="12">
+    <tableColumn id="5" xr3:uid="{B5E81D1B-B382-4DF5-92BA-F92F12A23A07}" name="DEF" dataDxfId="4">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*4.75</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A815FA03-2618-4DC9-9734-50DCE6DA615F}" name="MAT" dataDxfId="11">
+    <tableColumn id="6" xr3:uid="{A815FA03-2618-4DC9-9734-50DCE6DA615F}" name="MAT" dataDxfId="3">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D8263081-7D11-47BB-9AEC-CE559647F35D}" name="MDF" dataDxfId="10">
+    <tableColumn id="7" xr3:uid="{D8263081-7D11-47BB-9AEC-CE559647F35D}" name="MDF" dataDxfId="2">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*4.75</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C838F145-4059-4C8C-8152-B8F66431FFE1}" name="AGI" dataDxfId="9">
+    <tableColumn id="8" xr3:uid="{C838F145-4059-4C8C-8152-B8F66431FFE1}" name="AGI" dataDxfId="1">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*3.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{431AC55C-A81C-4BB0-B544-6631F8331D55}" name="LUK" dataDxfId="8">
+    <tableColumn id="9" xr3:uid="{431AC55C-A81C-4BB0-B544-6631F8331D55}" name="LUK" dataDxfId="0">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*2.125</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2961,28 +3023,28 @@
   <autoFilter ref="A8:I14" xr:uid="{D3C3F418-ED32-4504-9D73-88545A192967}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{13E0AF4A-AA83-489A-A156-B01D4F48D2F5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{B970139F-8BB5-4CE6-92F8-79E3236AC62B}" name="HP" dataDxfId="229">
+    <tableColumn id="2" xr3:uid="{B970139F-8BB5-4CE6-92F8-79E3236AC62B}" name="HP" dataDxfId="237">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*63+300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7BCF83B8-7492-4991-A008-F212725940B9}" name="MP" dataDxfId="228">
+    <tableColumn id="3" xr3:uid="{7BCF83B8-7492-4991-A008-F212725940B9}" name="MP" dataDxfId="236">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{33220A80-38D8-4480-ACC7-DF484072C96B}" name="ATK" dataDxfId="227">
+    <tableColumn id="4" xr3:uid="{33220A80-38D8-4480-ACC7-DF484072C96B}" name="ATK" dataDxfId="235">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.5+ 15+40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{36708515-5004-4705-A558-44B59D0CE676}" name="DEF" dataDxfId="226">
+    <tableColumn id="5" xr3:uid="{36708515-5004-4705-A558-44B59D0CE676}" name="DEF" dataDxfId="234">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25 + 15+21</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{11729EA3-08C4-4E0B-B5EE-5B3C08A31A9C}" name="MAT" dataDxfId="225">
+    <tableColumn id="6" xr3:uid="{11729EA3-08C4-4E0B-B5EE-5B3C08A31A9C}" name="MAT" dataDxfId="233">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B179D090-E484-4663-937A-480D1164D655}" name="MDF" dataDxfId="224">
+    <tableColumn id="7" xr3:uid="{B179D090-E484-4663-937A-480D1164D655}" name="MDF" dataDxfId="232">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25+15 + 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{28323AD0-B3BD-401F-A237-92C8B8D70FEA}" name="AGI" dataDxfId="223">
+    <tableColumn id="8" xr3:uid="{28323AD0-B3BD-401F-A237-92C8B8D70FEA}" name="AGI" dataDxfId="231">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{657BED8B-4C8A-42DC-BECD-5EEF9D1B7F37}" name="LUK" dataDxfId="222">
+    <tableColumn id="9" xr3:uid="{657BED8B-4C8A-42DC-BECD-5EEF9D1B7F37}" name="LUK" dataDxfId="230">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3003,7 +3065,7 @@
     <tableColumn id="7" xr3:uid="{D1DFC0D2-A987-4E3F-BA23-52162FB0C0BA}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{AB6209DB-CCCB-4C37-B455-4C7652E0DAC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2CD4CD14-92FD-41A7-9CCD-1329B5A77390}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{3B2C0A10-5038-4C21-BAC5-12FB16275D2E}" name="Total" dataDxfId="221">
+    <tableColumn id="10" xr3:uid="{3B2C0A10-5038-4C21-BAC5-12FB16275D2E}" name="Total" dataDxfId="229">
       <calculatedColumnFormula>SUM(Table11412[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3016,28 +3078,28 @@
   <autoFilter ref="A8:I14" xr:uid="{43F790D1-EA7B-4BAE-8A37-7CAD791E8821}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F6E842E1-B25F-4CA1-9107-AC7179420C29}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EFB2F0D5-318D-4A65-BA2B-20ADDE071648}" name="HP" dataDxfId="220">
+    <tableColumn id="2" xr3:uid="{EFB2F0D5-318D-4A65-BA2B-20ADDE071648}" name="HP" dataDxfId="228">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0D914B89-2678-453F-BC18-571DCD45E628}" name="MP" dataDxfId="219">
+    <tableColumn id="3" xr3:uid="{0D914B89-2678-453F-BC18-571DCD45E628}" name="MP" dataDxfId="227">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*13.75 + 80</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{6FBD2F64-5B1C-4035-BB1A-AFB092DB60C3}" name="ATK" dataDxfId="218">
+    <tableColumn id="4" xr3:uid="{6FBD2F64-5B1C-4035-BB1A-AFB092DB60C3}" name="ATK" dataDxfId="226">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7E0AF3FC-CC5D-4A6A-A4A2-DE278DEC4062}" name="DEF" dataDxfId="217">
+    <tableColumn id="5" xr3:uid="{7E0AF3FC-CC5D-4A6A-A4A2-DE278DEC4062}" name="DEF" dataDxfId="225">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1 + 15 + 4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3AF4D559-893B-4D50-BCB4-A1BD1FAF2F23}" name="MAT" dataDxfId="216">
+    <tableColumn id="6" xr3:uid="{3AF4D559-893B-4D50-BCB4-A1BD1FAF2F23}" name="MAT" dataDxfId="224">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6E9418A6-75AC-4541-9029-814EC5C06E70}" name="MDF" dataDxfId="215">
+    <tableColumn id="7" xr3:uid="{6E9418A6-75AC-4541-9029-814EC5C06E70}" name="MDF" dataDxfId="223">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.375+15 + 14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD605BEE-D561-4A2C-8D06-8E9AD70C32AC}" name="AGI" dataDxfId="214">
+    <tableColumn id="8" xr3:uid="{CD605BEE-D561-4A2C-8D06-8E9AD70C32AC}" name="AGI" dataDxfId="222">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E26506B2-F488-4AA4-AC87-819A22964609}" name="LUK" dataDxfId="213">
+    <tableColumn id="9" xr3:uid="{E26506B2-F488-4AA4-AC87-819A22964609}" name="LUK" dataDxfId="221">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3058,7 +3120,7 @@
     <tableColumn id="7" xr3:uid="{E91A64A8-F750-4893-9958-7C6ABC37405F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{3832FF0E-95E5-4B1F-B122-1EAFBF719DE3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{237404A9-EB50-465E-89AF-7167C57AFB99}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{927EBD24-571F-408C-A33B-59C753D9D96D}" name="Total" dataDxfId="212">
+    <tableColumn id="10" xr3:uid="{927EBD24-571F-408C-A33B-59C753D9D96D}" name="Total" dataDxfId="220">
       <calculatedColumnFormula>SUM(Table1141219[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3071,28 +3133,28 @@
   <autoFilter ref="A7:I13" xr:uid="{2539D8EE-2982-4734-B28B-342036FEDAC6}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FEE8F081-132E-4ED3-8FFD-2CF48368B2CC}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A79BC043-DB1A-48B4-AC21-AD31632979A6}" name="HP" dataDxfId="211">
+    <tableColumn id="2" xr3:uid="{A79BC043-DB1A-48B4-AC21-AD31632979A6}" name="HP" dataDxfId="219">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*63 + 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{42935B44-C727-42B0-B48E-0369818BF78A}" name="MP" dataDxfId="210">
+    <tableColumn id="3" xr3:uid="{42935B44-C727-42B0-B48E-0369818BF78A}" name="MP" dataDxfId="218">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{FC4572C7-88EC-4981-A6ED-43397844845B}" name="ATK" dataDxfId="209">
+    <tableColumn id="4" xr3:uid="{FC4572C7-88EC-4981-A6ED-43397844845B}" name="ATK" dataDxfId="217">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C8D61CEB-FFEC-42C3-9123-5140E65C1A2C}" name="DEF" dataDxfId="208">
+    <tableColumn id="5" xr3:uid="{C8D61CEB-FFEC-42C3-9123-5140E65C1A2C}" name="DEF" dataDxfId="216">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.375 + 15 + 19</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8C971683-28D2-4474-83CA-936F352F1324}" name="MAT" dataDxfId="207">
+    <tableColumn id="6" xr3:uid="{8C971683-28D2-4474-83CA-936F352F1324}" name="MAT" dataDxfId="215">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3371862A-9CF2-47CA-A149-4921E3B33162}" name="MDF" dataDxfId="206">
+    <tableColumn id="7" xr3:uid="{3371862A-9CF2-47CA-A149-4921E3B33162}" name="MDF" dataDxfId="214">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.375+15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC6AC739-B4C9-47A6-9472-439C60B629A0}" name="AGI" dataDxfId="205">
+    <tableColumn id="8" xr3:uid="{AC6AC739-B4C9-47A6-9472-439C60B629A0}" name="AGI" dataDxfId="213">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E727A271-B479-47C0-A557-227ABD8EC0AC}" name="LUK" dataDxfId="204">
+    <tableColumn id="9" xr3:uid="{E727A271-B479-47C0-A557-227ABD8EC0AC}" name="LUK" dataDxfId="212">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7046,8 +7108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDEC26FB-B5E4-44F5-B062-22E344453193}">
   <dimension ref="A2:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7802,6 +7864,206 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F20BDF8A-A837-40AC-945B-5DCD3F792613}">
+  <dimension ref="A2:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <f>Table1318222743[[#This Row],[Level]]*62.5+ 300</f>
+        <v>362.5</v>
+      </c>
+      <c r="C4">
+        <f>Table1318222743[[#This Row],[Level]]*12.5+60</f>
+        <v>72.5</v>
+      </c>
+      <c r="D4">
+        <f>Table1318222743[[#This Row],[Level]]*1.25 + 15</f>
+        <v>16.25</v>
+      </c>
+      <c r="E4">
+        <f>Table1318222743[[#This Row],[Level]]*1 + 15 + 10</f>
+        <v>26</v>
+      </c>
+      <c r="F4">
+        <f>Table1318222743[[#This Row],[Level]]*1.25 + 15</f>
+        <v>16.25</v>
+      </c>
+      <c r="G4">
+        <f>Table1318222743[[#This Row],[Level]]*1 + 15 + 8</f>
+        <v>24</v>
+      </c>
+      <c r="H4">
+        <f>Table1318222743[[#This Row],[Level]]*1.5 + 15 + 40</f>
+        <v>56.5</v>
+      </c>
+      <c r="I4">
+        <f>Table1318222743[[#This Row],[Level]]*1.25 + 15</f>
+        <v>16.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <f>Table1318222743[[#This Row],[Level]]*62.5+ 300</f>
+        <v>1237.5</v>
+      </c>
+      <c r="C5">
+        <f>Table1318222743[[#This Row],[Level]]*12.5+60</f>
+        <v>247.5</v>
+      </c>
+      <c r="D5">
+        <f>Table1318222743[[#This Row],[Level]]*1.25 + 15</f>
+        <v>33.75</v>
+      </c>
+      <c r="E5">
+        <f>Table1318222743[[#This Row],[Level]]*1 + 15 + 10</f>
+        <v>40</v>
+      </c>
+      <c r="F5">
+        <f>Table1318222743[[#This Row],[Level]]*1.25 + 15</f>
+        <v>33.75</v>
+      </c>
+      <c r="G5">
+        <f>Table1318222743[[#This Row],[Level]]*1 + 15 + 8</f>
+        <v>38</v>
+      </c>
+      <c r="H5">
+        <f>Table1318222743[[#This Row],[Level]]*1.5 + 15 + 40</f>
+        <v>77.5</v>
+      </c>
+      <c r="I5">
+        <f>Table1318222743[[#This Row],[Level]]*1.25 + 15</f>
+        <v>33.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <f>Table1318222743[[#This Row],[Level]]*62.5+ 300</f>
+        <v>1675</v>
+      </c>
+      <c r="C6">
+        <f>Table1318222743[[#This Row],[Level]]*12.5+60</f>
+        <v>335</v>
+      </c>
+      <c r="D6">
+        <f>Table1318222743[[#This Row],[Level]]*1.25 + 15</f>
+        <v>42.5</v>
+      </c>
+      <c r="E6">
+        <f>Table1318222743[[#This Row],[Level]]*1 + 15 + 10</f>
+        <v>47</v>
+      </c>
+      <c r="F6">
+        <f>Table1318222743[[#This Row],[Level]]*1.25 + 15</f>
+        <v>42.5</v>
+      </c>
+      <c r="G6">
+        <f>Table1318222743[[#This Row],[Level]]*1 + 15 + 8</f>
+        <v>45</v>
+      </c>
+      <c r="H6">
+        <f>Table1318222743[[#This Row],[Level]]*1.5 + 15 + 40</f>
+        <v>88</v>
+      </c>
+      <c r="I6">
+        <f>Table1318222743[[#This Row],[Level]]*1.25 + 15</f>
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1">
+        <f>Table1318222743[[#This Row],[Level]]*62.5+ 300</f>
+        <v>1862.5</v>
+      </c>
+      <c r="C7" s="1">
+        <f>Table1318222743[[#This Row],[Level]]*12.5+60</f>
+        <v>372.5</v>
+      </c>
+      <c r="D7" s="1">
+        <f>Table1318222743[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+      <c r="E7" s="1">
+        <f>Table1318222743[[#This Row],[Level]]*1 + 15 + 10</f>
+        <v>50</v>
+      </c>
+      <c r="F7" s="1">
+        <f>Table1318222743[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+      <c r="G7" s="1">
+        <f>Table1318222743[[#This Row],[Level]]*1 + 15 + 8</f>
+        <v>48</v>
+      </c>
+      <c r="H7" s="1">
+        <f>Table1318222743[[#This Row],[Level]]*1.5 + 15 + 40</f>
+        <v>92.5</v>
+      </c>
+      <c r="I7" s="1">
+        <f>Table1318222743[[#This Row],[Level]]*1.25 + 15</f>
+        <v>46.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832521D1-8A9A-424A-96D4-48DD11A591EE}">
   <dimension ref="A1:J13"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added skills for Stella, working on market mapping
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="12" activeTab="17" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="14" activeTab="16" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Skeleton Soldier" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="73">
   <si>
     <t>Skeletons are the most basic undead, they have low magical attributes, agility, and luck.</t>
   </si>
@@ -256,12 +256,18 @@
   <si>
     <t>Chelsea, light phys armor, dual equipped daggers -&gt; 40, 10/8 + 8 + 8</t>
   </si>
+  <si>
+    <t>Golem</t>
+  </si>
+  <si>
+    <t>Mercenary Golem, -&gt; 40 Attack, 20 Def, 40 MDF</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,16 +275,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -317,21 +343,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="256">
+  <dxfs count="264">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1894,7 +1987,7 @@
     <tableColumn id="7" xr3:uid="{F9852B29-E77D-4E17-A56E-5F0C649FA862}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{9A914BFF-1060-46E4-B8F9-412BD9293C3D}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2F83B650-811D-4FEE-92D5-03D4DC4376E5}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="255">
+    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="263">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1915,7 +2008,7 @@
     <tableColumn id="7" xr3:uid="{3A2FD57C-060A-462E-8BB9-B06F717E9D20}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{ED9393EA-F7F9-4661-8D0B-0D9246DDABF8}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{6F56342F-5442-42CD-8B6C-D98B6D6C0C56}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="211">
+    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="219">
       <calculatedColumnFormula>SUM(Table16[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1928,28 +2021,28 @@
   <autoFilter ref="A8:I13" xr:uid="{7BE337CC-37BD-4688-B60D-A66F4420668B}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{71340E4C-6101-4C59-8ED7-689E2AD5A962}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="210">
+    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="218">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*63-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="209">
+    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="217">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="208">
+    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="216">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="207">
+    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="215">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="206">
+    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="214">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="205">
+    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="213">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="204">
+    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="212">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="203">
+    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="211">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1970,7 +2063,7 @@
     <tableColumn id="7" xr3:uid="{4899BF24-9D2A-4CC0-AE35-4F49604AAC5A}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{CB1CC6BA-1D38-4B74-9BC6-7057FB9773EE}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{C47FADF6-C526-4188-9187-383757CE17C1}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="202">
+    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="210">
       <calculatedColumnFormula>SUM(Table168[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1983,28 +2076,28 @@
   <autoFilter ref="A9:I15" xr:uid="{06A56D17-07E5-4650-8EE9-7EA8F94D4020}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A2BE27C9-9DAE-49F5-9A70-C6CF7428BF31}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="201">
+    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="209">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="200">
+    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="208">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="199">
+    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="207">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="198">
+    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="206">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="197">
+    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="205">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.375+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="196">
+    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="204">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="195">
+    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="203">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="194">
+    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="202">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2025,7 +2118,7 @@
     <tableColumn id="7" xr3:uid="{60AD88FB-4685-412B-B5FD-BF8412C6B8E2}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{6A88D48C-D864-4F16-BEF2-BA88783A3FF3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{D40BD230-6392-4A28-A29D-F13EFE35C95E}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A0E09B2B-FD41-413F-8063-62214E990751}" name="Total" dataDxfId="193">
+    <tableColumn id="10" xr3:uid="{A0E09B2B-FD41-413F-8063-62214E990751}" name="Total" dataDxfId="201">
       <calculatedColumnFormula>SUM(Table16826[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2038,28 +2131,28 @@
   <autoFilter ref="A8:I14" xr:uid="{F7062CBA-4FAA-4900-9D3A-5C6613BCB6CE}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{ADCB4852-D3A0-456B-A8BD-E5F74BDBB762}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{ED76047D-1BC2-4C1B-B9B0-58BE0ACDDA48}" name="HP" dataDxfId="192">
+    <tableColumn id="2" xr3:uid="{ED76047D-1BC2-4C1B-B9B0-58BE0ACDDA48}" name="HP" dataDxfId="200">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EC859C53-0BA5-45D1-868B-F22DC8CE7D25}" name="MP" dataDxfId="191">
+    <tableColumn id="3" xr3:uid="{EC859C53-0BA5-45D1-868B-F22DC8CE7D25}" name="MP" dataDxfId="199">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DED33AB9-A2BB-4F9E-AA6D-02F8D1D65CD1}" name="ATK" dataDxfId="190">
+    <tableColumn id="4" xr3:uid="{DED33AB9-A2BB-4F9E-AA6D-02F8D1D65CD1}" name="ATK" dataDxfId="198">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.375+ 15+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{329B716D-9CA6-4546-AB13-92D88BE40F5F}" name="DEF" dataDxfId="189">
+    <tableColumn id="5" xr3:uid="{329B716D-9CA6-4546-AB13-92D88BE40F5F}" name="DEF" dataDxfId="197">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1 + 15+12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{67F8198A-5FC2-4C6D-9558-68B3141EA756}" name="MAT" dataDxfId="188">
+    <tableColumn id="6" xr3:uid="{67F8198A-5FC2-4C6D-9558-68B3141EA756}" name="MAT" dataDxfId="196">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C70F5BF6-63B0-44C1-862D-25E3FB55320F}" name="MDF" dataDxfId="187">
+    <tableColumn id="7" xr3:uid="{C70F5BF6-63B0-44C1-862D-25E3FB55320F}" name="MDF" dataDxfId="195">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.5+15+11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AB20AF53-453C-4266-A46B-40E693C91985}" name="AGI" dataDxfId="186">
+    <tableColumn id="8" xr3:uid="{AB20AF53-453C-4266-A46B-40E693C91985}" name="AGI" dataDxfId="194">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7FC46A31-F9F1-432E-B399-0823E198FE0A}" name="LUK" dataDxfId="185">
+    <tableColumn id="9" xr3:uid="{7FC46A31-F9F1-432E-B399-0823E198FE0A}" name="LUK" dataDxfId="193">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.5+15+20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2080,7 +2173,7 @@
     <tableColumn id="7" xr3:uid="{20C5D094-BAF0-471C-ACF3-C6658991DB5F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{E08E2AF0-56DD-4A69-A536-27139D793022}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{12AD8606-1127-4E5B-BA2C-872780F22F9E}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{5E2EF778-63AE-48B7-9F49-0D2AFEBD66A1}" name="Total" dataDxfId="184">
+    <tableColumn id="10" xr3:uid="{5E2EF778-63AE-48B7-9F49-0D2AFEBD66A1}" name="Total" dataDxfId="192">
       <calculatedColumnFormula>SUM(Table1682630[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2093,28 +2186,28 @@
   <autoFilter ref="A8:I14" xr:uid="{299912CC-280B-49E1-8859-432D05893259}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4F0B657F-C9A5-4A73-AAA3-27D307385193}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{526284E7-597F-4726-AB18-230CA03461B1}" name="HP" dataDxfId="183">
+    <tableColumn id="2" xr3:uid="{526284E7-597F-4726-AB18-230CA03461B1}" name="HP" dataDxfId="191">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*63+ 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E7BA3C7A-2677-415F-BA47-A4E88679B948}" name="MP" dataDxfId="182">
+    <tableColumn id="3" xr3:uid="{E7BA3C7A-2677-415F-BA47-A4E88679B948}" name="MP" dataDxfId="190">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE7BE678-2229-44F6-8732-71214FB69DD7}" name="ATK" dataDxfId="181">
+    <tableColumn id="4" xr3:uid="{AE7BE678-2229-44F6-8732-71214FB69DD7}" name="ATK" dataDxfId="189">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+ 15+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4715E3DB-8817-43D5-9074-9FB5F0BEF5B4}" name="DEF" dataDxfId="180">
+    <tableColumn id="5" xr3:uid="{4715E3DB-8817-43D5-9074-9FB5F0BEF5B4}" name="DEF" dataDxfId="188">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1 + 15+12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9CE76933-D045-418B-A975-378EEA51D856}" name="MAT" dataDxfId="179">
+    <tableColumn id="6" xr3:uid="{9CE76933-D045-418B-A975-378EEA51D856}" name="MAT" dataDxfId="187">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244B9611-6CB0-4946-B5CD-7D42311C7D7E}" name="MDF" dataDxfId="178">
+    <tableColumn id="7" xr3:uid="{244B9611-6CB0-4946-B5CD-7D42311C7D7E}" name="MDF" dataDxfId="186">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+15+11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32550C13-49BB-41D2-BA0A-26798830A0FD}" name="AGI" dataDxfId="177">
+    <tableColumn id="8" xr3:uid="{32550C13-49BB-41D2-BA0A-26798830A0FD}" name="AGI" dataDxfId="185">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{BB22F289-8AF5-4DD6-877B-F09520710555}" name="LUK" dataDxfId="176">
+    <tableColumn id="9" xr3:uid="{BB22F289-8AF5-4DD6-877B-F09520710555}" name="LUK" dataDxfId="184">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+15+20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2127,28 +2220,28 @@
   <autoFilter ref="A4:I10" xr:uid="{A1EAC62C-C07D-464E-91B1-4A34E6604BA2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{430FD3D4-914C-4309-B2E6-6F01B5CAED94}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="175">
+    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="183">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="174">
+    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="182">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="173">
+    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="181">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="172">
+    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="180">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15 + 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="171">
+    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="179">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15 + 30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="170">
+    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="178">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15 + 21</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="169">
+    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="177">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="168">
+    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="176">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2161,28 +2254,28 @@
   <autoFilter ref="A7:I12" xr:uid="{9BE7336F-352A-4FAE-B0E4-61965FC814C7}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B8DA50BB-4379-43D1-879B-CDBE6D82C13A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="167">
+    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="175">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="166">
+    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="174">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="165">
+    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="173">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="164">
+    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="172">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="163">
+    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="171">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="162">
+    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="170">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="161">
+    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="169">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="160">
+    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="168">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2195,28 +2288,28 @@
   <autoFilter ref="A8:I13" xr:uid="{67385006-CBB9-4472-99D4-7881E042769D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FD96F8F7-CCAB-44FA-B525-A5081670706A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="254">
+    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="262">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="253">
+    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="261">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="252">
+    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="260">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="251">
+    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="259">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="250">
+    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="258">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="249">
+    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="257">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="248">
+    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="256">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="247">
+    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="255">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2237,7 +2330,7 @@
     <tableColumn id="7" xr3:uid="{AEFF5C29-BE6A-4CF8-A2BB-F6B076077DA9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{4DE9B01E-67F2-4136-ADC3-60389FB67DCC}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{F5A82F03-513C-46D4-9F91-470F0060526B}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="159">
+    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="167">
       <calculatedColumnFormula>SUM(Table16821[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2246,22 +2339,22 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="158" tableBorderDxfId="157">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="166" tableBorderDxfId="165">
   <autoFilter ref="A15:I16" xr:uid="{434CBBE2-2F8D-4EEB-895C-68FC850EF1FD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="156"/>
-    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="155">
+    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="164"/>
+    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="163">
       <calculatedColumnFormula>Table1922[Level]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="154">
+    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="162">
       <calculatedColumnFormula>Table1922[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="153"/>
-    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="152"/>
-    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="151"/>
-    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="150"/>
-    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="149"/>
-    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="148"/>
+    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="161"/>
+    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="160"/>
+    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="159"/>
+    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="158"/>
+    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="157"/>
+    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="156"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2272,28 +2365,28 @@
   <autoFilter ref="A3:I9" xr:uid="{A90D1C2A-DBF9-4EEF-ACC2-3DC17C207301}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BD3505AC-AE6D-4947-A74E-A6C2D68658F1}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="147">
+    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="155">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="146">
+    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="154">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="145">
+    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="153">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="144">
+    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="152">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="143">
+    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="151">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="142">
+    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="150">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="141">
+    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="149">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="140">
+    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="148">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2302,32 +2395,32 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="139" tableBorderDxfId="138">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="147" tableBorderDxfId="146">
   <autoFilter ref="L3:T4" xr:uid="{5D2C3EA8-1297-4C77-AF32-84E50F8232C5}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="137"/>
-    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="136">
+    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="145"/>
+    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="144">
       <calculatedColumnFormula>Table19[Level]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="135">
+    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="143">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="134">
+    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="142">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="133">
+    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="141">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1 + 15 + 6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="132">
+    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="140">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="131">
+    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="139">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="130">
+    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="138">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="129">
+    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="137">
       <calculatedColumnFormula>Table19[Level] + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2340,28 +2433,28 @@
   <autoFilter ref="A7:I12" xr:uid="{553298A4-7E43-42CF-9EEB-1F9E7E6BAD27}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2AA35C8B-719C-4BA6-9CDF-2963E1C9F233}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C087FAFA-9653-40EC-B4B9-5CB8F9D7255E}" name="HP" dataDxfId="128">
+    <tableColumn id="2" xr3:uid="{C087FAFA-9653-40EC-B4B9-5CB8F9D7255E}" name="HP" dataDxfId="136">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0004B47B-3968-4C5A-BE6C-B822A307D7C5}" name="MP" dataDxfId="127">
+    <tableColumn id="3" xr3:uid="{0004B47B-3968-4C5A-BE6C-B822A307D7C5}" name="MP" dataDxfId="135">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{67EC8D91-0122-40D7-87D0-A3AB6788CE9D}" name="ATK" dataDxfId="126">
+    <tableColumn id="4" xr3:uid="{67EC8D91-0122-40D7-87D0-A3AB6788CE9D}" name="ATK" dataDxfId="134">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E9988E54-33D6-41EB-B6BE-6E832544E18C}" name="DEF" dataDxfId="125">
+    <tableColumn id="5" xr3:uid="{E9988E54-33D6-41EB-B6BE-6E832544E18C}" name="DEF" dataDxfId="133">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{16D71A55-372C-4029-A831-ECF2325E46C4}" name="MAT" dataDxfId="124">
+    <tableColumn id="6" xr3:uid="{16D71A55-372C-4029-A831-ECF2325E46C4}" name="MAT" dataDxfId="132">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{1802FB48-B110-4DBF-A8F2-64CD4890E741}" name="MDF" dataDxfId="123">
+    <tableColumn id="7" xr3:uid="{1802FB48-B110-4DBF-A8F2-64CD4890E741}" name="MDF" dataDxfId="131">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{350CA8CC-761C-4994-9D80-14685787EF3D}" name="AGI" dataDxfId="122">
+    <tableColumn id="8" xr3:uid="{350CA8CC-761C-4994-9D80-14685787EF3D}" name="AGI" dataDxfId="130">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B578CF58-136A-41B9-800E-D75836A4CDD1}" name="LUK" dataDxfId="121">
+    <tableColumn id="9" xr3:uid="{B578CF58-136A-41B9-800E-D75836A4CDD1}" name="LUK" dataDxfId="129">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2382,7 +2475,7 @@
     <tableColumn id="7" xr3:uid="{5A405725-30A7-487F-95BF-061F71CA9C61}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{644DEF70-6EBD-403E-904B-6C30E5FBEA48}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{BA93DA54-96B9-48D1-80BB-C266771E13F1}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{3EBB17A5-47EA-458B-83A5-7056BE67D25F}" name="Total" dataDxfId="120">
+    <tableColumn id="10" xr3:uid="{3EBB17A5-47EA-458B-83A5-7056BE67D25F}" name="Total" dataDxfId="128">
       <calculatedColumnFormula>SUM(Table1682134[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2391,26 +2484,26 @@
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{A7C0F3AC-4E86-430D-AE55-8604641B493E}" name="Table192235" displayName="Table192235" ref="A15:I16" totalsRowShown="0" dataDxfId="119" tableBorderDxfId="118">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{A7C0F3AC-4E86-430D-AE55-8604641B493E}" name="Table192235" displayName="Table192235" ref="A15:I16" totalsRowShown="0" dataDxfId="127" tableBorderDxfId="126">
   <autoFilter ref="A15:I16" xr:uid="{D0DF3ED4-9A21-493B-88F4-CE5814AF31C9}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A78A876E-6C8B-4FC8-BFD4-A9BC80EA3FC2}" name="Level" dataDxfId="117"/>
-    <tableColumn id="2" xr3:uid="{4B423FFC-D037-484D-A927-2F66E15D422A}" name="HP" dataDxfId="116">
+    <tableColumn id="1" xr3:uid="{A78A876E-6C8B-4FC8-BFD4-A9BC80EA3FC2}" name="Level" dataDxfId="125"/>
+    <tableColumn id="2" xr3:uid="{4B423FFC-D037-484D-A927-2F66E15D422A}" name="HP" dataDxfId="124">
       <calculatedColumnFormula>(Table192235[Level]*75 + 500)*2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B695FEDE-EC59-44D8-AE99-CBF568DE5C93}" name="MP" dataDxfId="115">
+    <tableColumn id="3" xr3:uid="{B695FEDE-EC59-44D8-AE99-CBF568DE5C93}" name="MP" dataDxfId="123">
       <calculatedColumnFormula>Table192235[[#This Row],[Level]]*14 + 80</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{160D5D77-34E8-44F3-B51D-7CC0736DDCB1}" name="ATK" dataDxfId="114">
+    <tableColumn id="4" xr3:uid="{160D5D77-34E8-44F3-B51D-7CC0736DDCB1}" name="ATK" dataDxfId="122">
       <calculatedColumnFormula>Table192235[[#This Row],[Level]]*1.5+ 15 + 50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{559DAC37-CD6A-449F-AFF0-355ADE7CED80}" name="DEF" dataDxfId="113"/>
-    <tableColumn id="6" xr3:uid="{EEC344A5-27A5-450E-B795-04D237DD063F}" name="MAT" dataDxfId="112">
+    <tableColumn id="5" xr3:uid="{559DAC37-CD6A-449F-AFF0-355ADE7CED80}" name="DEF" dataDxfId="121"/>
+    <tableColumn id="6" xr3:uid="{EEC344A5-27A5-450E-B795-04D237DD063F}" name="MAT" dataDxfId="120">
       <calculatedColumnFormula>Table192235[Level]*1.5+15+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{54363CA4-9EE5-495F-8323-6C0C1261453C}" name="MDF" dataDxfId="111"/>
-    <tableColumn id="8" xr3:uid="{26B56E9D-2FCD-4476-A6CF-8F2EDC965246}" name="AGI" dataDxfId="110"/>
-    <tableColumn id="9" xr3:uid="{95814D66-3343-4190-9BF4-F4E45AB27D95}" name="LUK" dataDxfId="109"/>
+    <tableColumn id="7" xr3:uid="{54363CA4-9EE5-495F-8323-6C0C1261453C}" name="MDF" dataDxfId="119"/>
+    <tableColumn id="8" xr3:uid="{26B56E9D-2FCD-4476-A6CF-8F2EDC965246}" name="AGI" dataDxfId="118"/>
+    <tableColumn id="9" xr3:uid="{95814D66-3343-4190-9BF4-F4E45AB27D95}" name="LUK" dataDxfId="117"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2429,7 +2522,7 @@
     <tableColumn id="7" xr3:uid="{22216E02-260E-4471-8BB1-4E6E1250BAC9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{DC2670AC-8DF2-47F7-A3F6-EE7896309BC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{749652E2-F6CF-428C-B67C-FD0B1EFCCBBF}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="108">
+    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="116">
       <calculatedColumnFormula>SUM(Table15[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2442,28 +2535,28 @@
   <autoFilter ref="A15:I20" xr:uid="{A1CF627F-8D28-44AD-9A35-411103976FCA}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F14CC326-DE44-48D8-856F-8DCDCFC89CAD}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="107">
+    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="115">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*63-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="106">
+    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="114">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="105">
+    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="113">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="104">
+    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="112">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="103">
+    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="111">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="102">
+    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="110">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="101">
+    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="109">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="100">
+    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="108">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2476,28 +2569,28 @@
   <autoFilter ref="K11:S17" xr:uid="{EAF9FB6A-F011-40E3-AB2F-E53826722AFB}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DF3E0800-6EE4-4E1B-BA6F-0194351D6E7C}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="99">
+    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="107">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*56.25+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="98">
+    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="106">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="97">
+    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="105">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="96">
+    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="104">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="95">
+    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="103">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="94">
+    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="102">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="93">
+    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="101">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="92">
+    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="100">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2510,28 +2603,28 @@
   <autoFilter ref="K8:S14" xr:uid="{AB7E938D-7ACC-4BFB-A6B9-682B8B29CEF2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{66EB8EF1-BCF4-44F7-B8A6-3C3B425F8FF5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="246">
+    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="254">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*56.25+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="245">
+    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="253">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="244">
+    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="252">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25+ 15+30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="243">
+    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="251">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25 + 15+33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="242">
+    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="250">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="241">
+    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="249">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="240">
+    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="248">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="239">
+    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="247">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2544,28 +2637,28 @@
   <autoFilter ref="A26:I31" xr:uid="{870F76F2-5EA7-4FD7-B1F9-507D64592088}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{3C04B742-338A-4366-BF3D-C5BC13023785}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="91">
+    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="99">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*63+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="90">
+    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="98">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="89">
+    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="97">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="88">
+    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="96">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="87">
+    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="95">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="86">
+    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="94">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="85">
+    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="93">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="84">
+    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="92">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2578,28 +2671,28 @@
   <autoFilter ref="A36:I41" xr:uid="{9BD043AF-0D77-4FF4-B2F9-B4AC3C3F1F82}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{7BB908A3-05D7-4357-920B-BF4C6BC20C06}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="83">
+    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="91">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*56.5+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="82">
+    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="90">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*12.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="81">
+    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="89">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="80">
+    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="88">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1 + 15+14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="79">
+    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="87">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="78">
+    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="86">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.5+ 15+13</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="77">
+    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="85">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="76">
+    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="84">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.375 + 15+40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2620,7 +2713,7 @@
     <tableColumn id="7" xr3:uid="{09E4151E-54A0-41FF-BA5B-3B1C748DA23D}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{909575E0-EC13-4E35-A35F-2451A5741589}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2CDCF32E-D8FC-48D9-A28D-8D9C5F3EB001}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{001DA1BB-34DD-4786-BDE4-23C510900A3D}" name="Total" dataDxfId="75">
+    <tableColumn id="10" xr3:uid="{001DA1BB-34DD-4786-BDE4-23C510900A3D}" name="Total" dataDxfId="83">
       <calculatedColumnFormula>SUM(Table168213429[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2633,28 +2726,28 @@
   <autoFilter ref="A7:I12" xr:uid="{4ED64482-035D-49B9-A477-A1D5AEB4A5A4}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{141B0E2E-D4F3-4884-86FD-AAD67C363749}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{D4B50877-EF56-4EF7-8C6D-9928A6D654F6}" name="HP" dataDxfId="74">
+    <tableColumn id="2" xr3:uid="{D4B50877-EF56-4EF7-8C6D-9928A6D654F6}" name="HP" dataDxfId="82">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*125</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F4B06187-BE28-4283-9518-F773FE75C2BF}" name="MP" dataDxfId="73">
+    <tableColumn id="3" xr3:uid="{F4B06187-BE28-4283-9518-F773FE75C2BF}" name="MP" dataDxfId="81">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{91A68FC7-5F16-4880-AE82-97341814BB95}" name="ATK" dataDxfId="72">
+    <tableColumn id="4" xr3:uid="{91A68FC7-5F16-4880-AE82-97341814BB95}" name="ATK" dataDxfId="80">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*4.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{2BCD0E58-85DE-4C10-BFBC-AF77BC569C92}" name="DEF" dataDxfId="71">
+    <tableColumn id="5" xr3:uid="{2BCD0E58-85DE-4C10-BFBC-AF77BC569C92}" name="DEF" dataDxfId="79">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7C48A1FC-CE8F-4CDD-9A3D-308B46D78A48}" name="MAT" dataDxfId="70">
+    <tableColumn id="6" xr3:uid="{7C48A1FC-CE8F-4CDD-9A3D-308B46D78A48}" name="MAT" dataDxfId="78">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{474D8178-EA8C-4322-93C3-B7F6EBA88102}" name="MDF" dataDxfId="69">
+    <tableColumn id="7" xr3:uid="{474D8178-EA8C-4322-93C3-B7F6EBA88102}" name="MDF" dataDxfId="77">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{257B31D9-5838-45E0-A56E-9B1566E1A34A}" name="AGI" dataDxfId="68">
+    <tableColumn id="8" xr3:uid="{257B31D9-5838-45E0-A56E-9B1566E1A34A}" name="AGI" dataDxfId="76">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{17960EB4-4250-49DB-9A6B-455B9913B04B}" name="LUK" dataDxfId="67">
+    <tableColumn id="9" xr3:uid="{17960EB4-4250-49DB-9A6B-455B9913B04B}" name="LUK" dataDxfId="75">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1.125</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2675,7 +2768,7 @@
     <tableColumn id="7" xr3:uid="{07EA0638-8880-4944-AC9E-13E3F1B9F651}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{AA18E602-126F-4D69-9CC8-C097E8EB9C70}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{5563B0CB-2EA7-4851-8D1F-D77E0F90CBAD}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{2D960B43-0F76-4936-9508-4D501A79A83C}" name="Total" dataDxfId="66">
+    <tableColumn id="10" xr3:uid="{2D960B43-0F76-4936-9508-4D501A79A83C}" name="Total" dataDxfId="74">
       <calculatedColumnFormula>SUM(Table16821342932[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2688,28 +2781,28 @@
   <autoFilter ref="A5:I10" xr:uid="{2922C913-6AE8-4B89-BDA6-9F44D59987D8}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{3D67222C-6501-4A5D-A9FC-528EE591A288}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EE3E4CCC-C404-4B78-AAB4-3B38166E23BA}" name="HP" dataDxfId="65">
+    <tableColumn id="2" xr3:uid="{EE3E4CCC-C404-4B78-AAB4-3B38166E23BA}" name="HP" dataDxfId="73">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DE5141FB-3B4E-46D4-9E0D-AF1DEE998B4A}" name="MP" dataDxfId="64">
+    <tableColumn id="3" xr3:uid="{DE5141FB-3B4E-46D4-9E0D-AF1DEE998B4A}" name="MP" dataDxfId="72">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{404B3E88-DF62-4AA0-82D6-C21C2BCA762B}" name="ATK" dataDxfId="63">
+    <tableColumn id="4" xr3:uid="{404B3E88-DF62-4AA0-82D6-C21C2BCA762B}" name="ATK" dataDxfId="71">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*4.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{342B3F39-F7A2-45D8-9CD4-39B5ABC72D2F}" name="DEF" dataDxfId="62">
+    <tableColumn id="5" xr3:uid="{342B3F39-F7A2-45D8-9CD4-39B5ABC72D2F}" name="DEF" dataDxfId="70">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{CD819DB3-9F2E-4428-AAFC-72776ECB8EAF}" name="MAT" dataDxfId="61">
+    <tableColumn id="6" xr3:uid="{CD819DB3-9F2E-4428-AAFC-72776ECB8EAF}" name="MAT" dataDxfId="69">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{270DF964-8095-43FD-B050-DD4A2A138F32}" name="MDF" dataDxfId="60">
+    <tableColumn id="7" xr3:uid="{270DF964-8095-43FD-B050-DD4A2A138F32}" name="MDF" dataDxfId="68">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4F4D3B2A-5B86-4AB7-A97E-18E2868266B8}" name="AGI" dataDxfId="59">
+    <tableColumn id="8" xr3:uid="{4F4D3B2A-5B86-4AB7-A97E-18E2868266B8}" name="AGI" dataDxfId="67">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{0178CE2D-63C5-426A-A081-D62E62FF91AC}" name="LUK" dataDxfId="58">
+    <tableColumn id="9" xr3:uid="{0178CE2D-63C5-426A-A081-D62E62FF91AC}" name="LUK" dataDxfId="66">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*1.5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2730,7 +2823,7 @@
     <tableColumn id="7" xr3:uid="{C374A90B-690A-432C-974A-C8A7D22E367F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{05C64890-0DC2-4577-975E-95477DCED789}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{CE6AAEA9-D599-4B9B-BD40-7E602F47088C}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{30017AE7-6C23-415F-A2EA-70EA09C835E6}" name="Total" dataDxfId="57">
+    <tableColumn id="10" xr3:uid="{30017AE7-6C23-415F-A2EA-70EA09C835E6}" name="Total" dataDxfId="65">
       <calculatedColumnFormula>SUM(Table1682134293227[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2743,28 +2836,28 @@
   <autoFilter ref="A6:I11" xr:uid="{D09397F4-7631-4CD3-AF40-3B14C64478EE}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BF4E6A79-8CCF-498E-B3B0-FA782AB06519}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{37E52E57-C499-4FFB-AC3F-20E63EEA4D3A}" name="HP" dataDxfId="56">
+    <tableColumn id="2" xr3:uid="{37E52E57-C499-4FFB-AC3F-20E63EEA4D3A}" name="HP" dataDxfId="64">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*87.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D29F5CDE-1200-4C77-A4BA-0DE4F7C46627}" name="MP" dataDxfId="55">
+    <tableColumn id="3" xr3:uid="{D29F5CDE-1200-4C77-A4BA-0DE4F7C46627}" name="MP" dataDxfId="63">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{9701140A-64F9-4967-9DEE-3460411D91C1}" name="ATK" dataDxfId="54">
+    <tableColumn id="4" xr3:uid="{9701140A-64F9-4967-9DEE-3460411D91C1}" name="ATK" dataDxfId="62">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F90A425E-E031-4255-8AF9-DAD672F8DD7D}" name="DEF" dataDxfId="53">
+    <tableColumn id="5" xr3:uid="{F90A425E-E031-4255-8AF9-DAD672F8DD7D}" name="DEF" dataDxfId="61">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*4.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{255210A0-6EB8-4CFB-84DD-42C88AEAF7AA}" name="MAT" dataDxfId="52">
+    <tableColumn id="6" xr3:uid="{255210A0-6EB8-4CFB-84DD-42C88AEAF7AA}" name="MAT" dataDxfId="60">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{91177FDD-F316-4D6B-A547-FC5FA6DAC266}" name="MDF" dataDxfId="51">
+    <tableColumn id="7" xr3:uid="{91177FDD-F316-4D6B-A547-FC5FA6DAC266}" name="MDF" dataDxfId="59">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{ADA902F7-B7D7-4B1B-A144-E5252296AB61}" name="AGI" dataDxfId="50">
+    <tableColumn id="8" xr3:uid="{ADA902F7-B7D7-4B1B-A144-E5252296AB61}" name="AGI" dataDxfId="58">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{78273DA6-F2CA-4999-B4EA-F6C044BC41AB}" name="LUK" dataDxfId="49">
+    <tableColumn id="9" xr3:uid="{78273DA6-F2CA-4999-B4EA-F6C044BC41AB}" name="LUK" dataDxfId="57">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2777,28 +2870,28 @@
   <autoFilter ref="A4:I9" xr:uid="{DD778A26-93EC-4B14-A9D1-160AE03B48D3}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F0A3DB96-38E4-4CD0-BAF6-C8BB768B1256}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{07B77441-F84C-41C6-A00C-B69369FBF0F1}" name="HP" dataDxfId="48">
+    <tableColumn id="2" xr3:uid="{07B77441-F84C-41C6-A00C-B69369FBF0F1}" name="HP" dataDxfId="56">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{2DBE06DE-38E0-4433-B590-3850C554BB8E}" name="MP" dataDxfId="47">
+    <tableColumn id="3" xr3:uid="{2DBE06DE-38E0-4433-B590-3850C554BB8E}" name="MP" dataDxfId="55">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DE8CC9D0-45D8-4F85-9317-09844C8D4DD7}" name="ATK" dataDxfId="46">
+    <tableColumn id="4" xr3:uid="{DE8CC9D0-45D8-4F85-9317-09844C8D4DD7}" name="ATK" dataDxfId="54">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1.375+ 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{9D33BCF5-CDB6-4BB0-8603-810E71EE1C47}" name="DEF" dataDxfId="45">
+    <tableColumn id="5" xr3:uid="{9D33BCF5-CDB6-4BB0-8603-810E71EE1C47}" name="DEF" dataDxfId="53">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1.375 + 15 + 19</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{1693AB2F-85DB-4286-A43C-82A15CDDA173}" name="MAT" dataDxfId="44">
+    <tableColumn id="6" xr3:uid="{1693AB2F-85DB-4286-A43C-82A15CDDA173}" name="MAT" dataDxfId="52">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{DCA68233-62C9-4E66-9306-24AE49EE344C}" name="MDF" dataDxfId="43">
+    <tableColumn id="7" xr3:uid="{DCA68233-62C9-4E66-9306-24AE49EE344C}" name="MDF" dataDxfId="51">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1 + 15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{60943D8A-0008-4FFE-AE90-4DDEB0149A21}" name="AGI" dataDxfId="42">
+    <tableColumn id="8" xr3:uid="{60943D8A-0008-4FFE-AE90-4DDEB0149A21}" name="AGI" dataDxfId="50">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E7EC6C93-3486-414B-87DB-F4D38BB2A0DC}" name="LUK" dataDxfId="41">
+    <tableColumn id="9" xr3:uid="{E7EC6C93-3486-414B-87DB-F4D38BB2A0DC}" name="LUK" dataDxfId="49">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2811,28 +2904,28 @@
   <autoFilter ref="A12:I16" xr:uid="{2A794F38-5DB8-40A3-A8E2-90B5A0A4A192}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{C5A2CF3A-0965-428C-AD05-883EDB0D400F}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C8840580-F723-4CA3-A107-42FCC677D424}" name="HP" dataDxfId="40">
+    <tableColumn id="2" xr3:uid="{C8840580-F723-4CA3-A107-42FCC677D424}" name="HP" dataDxfId="48">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*62.5+ 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5D9241C6-74A5-4C1F-A8F7-69DB1BDA83FE}" name="MP" dataDxfId="39">
+    <tableColumn id="3" xr3:uid="{5D9241C6-74A5-4C1F-A8F7-69DB1BDA83FE}" name="MP" dataDxfId="47">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*12.5+60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D98F9CCD-2FEF-4FB2-B5AD-D2A6B610781B}" name="ATK" dataDxfId="38">
+    <tableColumn id="4" xr3:uid="{D98F9CCD-2FEF-4FB2-B5AD-D2A6B610781B}" name="ATK" dataDxfId="46">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CF1AF448-2207-48D1-8FE3-0A6B5DE3511C}" name="DEF" dataDxfId="37">
+    <tableColumn id="5" xr3:uid="{CF1AF448-2207-48D1-8FE3-0A6B5DE3511C}" name="DEF" dataDxfId="45">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1 + 15 + 10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A632BAA7-E71C-41F8-B5B0-90891BB5BA9B}" name="MAT" dataDxfId="36">
+    <tableColumn id="6" xr3:uid="{A632BAA7-E71C-41F8-B5B0-90891BB5BA9B}" name="MAT" dataDxfId="44">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E76132BC-BC67-4915-8112-E0B292C65C91}" name="MDF" dataDxfId="35">
+    <tableColumn id="7" xr3:uid="{E76132BC-BC67-4915-8112-E0B292C65C91}" name="MDF" dataDxfId="43">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1 + 15 + 8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B25B7E33-B3CF-4D3D-9A14-3CE5B75535E8}" name="AGI" dataDxfId="34">
+    <tableColumn id="8" xr3:uid="{B25B7E33-B3CF-4D3D-9A14-3CE5B75535E8}" name="AGI" dataDxfId="42">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{40820F61-4B4C-4B23-95CF-AD5CDE975F4A}" name="LUK" dataDxfId="33">
+    <tableColumn id="9" xr3:uid="{40820F61-4B4C-4B23-95CF-AD5CDE975F4A}" name="LUK" dataDxfId="41">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2853,7 +2946,7 @@
     <tableColumn id="7" xr3:uid="{F833922A-76F9-427C-8462-D94DE51D0477}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{203171A1-C88B-4F81-ADC2-1EE072D645F3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{34003EF6-E9A5-4584-A186-09DFF4EC11C7}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{C4602156-F897-42BE-8F3F-411E13EEB095}" name="Total" dataDxfId="238">
+    <tableColumn id="10" xr3:uid="{C4602156-F897-42BE-8F3F-411E13EEB095}" name="Total" dataDxfId="246">
       <calculatedColumnFormula>SUM(Table114[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2866,28 +2959,28 @@
   <autoFilter ref="A20:I24" xr:uid="{6015D08B-C4A1-43B9-B8BF-6F441CC08DCA}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D4205A68-390A-4750-8556-3B4847E58D16}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{D7D1DEBE-6CE0-4976-A401-D4F35A038AA9}" name="HP" dataDxfId="32">
+    <tableColumn id="2" xr3:uid="{D7D1DEBE-6CE0-4976-A401-D4F35A038AA9}" name="HP" dataDxfId="40">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{3CB0ED8A-F14B-4E5F-8474-F3034EA78A85}" name="MP" dataDxfId="31">
+    <tableColumn id="3" xr3:uid="{3CB0ED8A-F14B-4E5F-8474-F3034EA78A85}" name="MP" dataDxfId="39">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F3186E07-87BD-4E53-8F85-AB4798362B0C}" name="ATK" dataDxfId="30">
+    <tableColumn id="4" xr3:uid="{F3186E07-87BD-4E53-8F85-AB4798362B0C}" name="ATK" dataDxfId="38">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{22ED75D6-B85C-4DF9-BC39-4154BAF3990E}" name="DEF" dataDxfId="29">
+    <tableColumn id="5" xr3:uid="{22ED75D6-B85C-4DF9-BC39-4154BAF3990E}" name="DEF" dataDxfId="37">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1 + 15 + 4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B2DFC87A-2BEE-4B5A-AF53-4E18078ABC1B}" name="MAT" dataDxfId="28">
+    <tableColumn id="6" xr3:uid="{B2DFC87A-2BEE-4B5A-AF53-4E18078ABC1B}" name="MAT" dataDxfId="36">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.375 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{8FF82542-4129-4E67-AA7B-7CB38D8FB051}" name="MDF" dataDxfId="27">
+    <tableColumn id="7" xr3:uid="{8FF82542-4129-4E67-AA7B-7CB38D8FB051}" name="MDF" dataDxfId="35">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.375 + 15 + 14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{85F4097E-90A5-4A7C-B184-42B110E62300}" name="AGI" dataDxfId="26">
+    <tableColumn id="8" xr3:uid="{85F4097E-90A5-4A7C-B184-42B110E62300}" name="AGI" dataDxfId="34">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E1A21F56-D819-4CE3-9122-F47B8A4039A9}" name="LUK" dataDxfId="25">
+    <tableColumn id="9" xr3:uid="{E1A21F56-D819-4CE3-9122-F47B8A4039A9}" name="LUK" dataDxfId="33">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2900,28 +2993,28 @@
   <autoFilter ref="A27:I30" xr:uid="{4506A984-1EE8-4D0B-9AFB-6DE5576F3317}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{97BB3945-930E-41A9-B479-678FD9D8EE85}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{2197951B-D7A2-413F-8152-C8BB282E3498}" name="HP" dataDxfId="24">
+    <tableColumn id="2" xr3:uid="{2197951B-D7A2-413F-8152-C8BB282E3498}" name="HP" dataDxfId="32">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*62.5+ 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{54D89380-BDA0-4B18-8B8B-482E9AA62AD3}" name="MP" dataDxfId="23">
+    <tableColumn id="3" xr3:uid="{54D89380-BDA0-4B18-8B8B-482E9AA62AD3}" name="MP" dataDxfId="31">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*12.5+60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DCD1A325-B7AE-4283-89E4-85446F157A12}" name="ATK" dataDxfId="22">
+    <tableColumn id="4" xr3:uid="{DCD1A325-B7AE-4283-89E4-85446F157A12}" name="ATK" dataDxfId="30">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1CD051D4-B531-4706-95A8-BBF452C5188D}" name="DEF" dataDxfId="21">
+    <tableColumn id="5" xr3:uid="{1CD051D4-B531-4706-95A8-BBF452C5188D}" name="DEF" dataDxfId="29">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.25 + 15 + 19</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{E17A43F1-7669-40E6-BD8C-8623B203A60F}" name="MAT" dataDxfId="20">
+    <tableColumn id="6" xr3:uid="{E17A43F1-7669-40E6-BD8C-8623B203A60F}" name="MAT" dataDxfId="28">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{04F7D6BA-3673-4BE0-97CA-65C8DD4612E3}" name="MDF" dataDxfId="19">
+    <tableColumn id="7" xr3:uid="{04F7D6BA-3673-4BE0-97CA-65C8DD4612E3}" name="MDF" dataDxfId="27">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.25 + 15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{7AA9AD24-2AFF-4204-AAEF-0CC3265C40FA}" name="AGI" dataDxfId="18">
+    <tableColumn id="8" xr3:uid="{7AA9AD24-2AFF-4204-AAEF-0CC3265C40FA}" name="AGI" dataDxfId="26">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{ABFCE932-20B6-4AEE-A261-B747D2EC6FA8}" name="LUK" dataDxfId="17">
+    <tableColumn id="9" xr3:uid="{ABFCE932-20B6-4AEE-A261-B747D2EC6FA8}" name="LUK" dataDxfId="25">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2930,33 +3023,33 @@
 </file>
 
 <file path=xl/tables/table42.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="42" xr:uid="{B11B1E6C-19A5-42E4-847D-0CD22EB4A103}" name="Table1318222743" displayName="Table1318222743" ref="A3:I7" totalsRowShown="0">
-  <autoFilter ref="A3:I7" xr:uid="{7F8360B3-D323-4505-8E52-764F2EEFEF08}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="45" xr:uid="{B9200053-35AC-4923-AC77-58FBB0806D21}" name="Table13163946" displayName="Table13163946" ref="L4:T9" totalsRowShown="0">
+  <autoFilter ref="L4:T9" xr:uid="{7E10C2C1-D4A2-4595-8F68-D39C5EF91F11}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{2DA75379-E191-41C6-A461-F7A952576C54}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{0E110670-3AC7-427B-B6F4-6865DC721C3B}" name="HP" dataDxfId="16">
-      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*62.5+ 300</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{DD071379-690C-45AA-9EB0-1452F203E78A}" name="MP" dataDxfId="15">
-      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*12.5+60</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{16C4CC92-9435-4196-8A09-D27E77854475}" name="ATK" dataDxfId="14">
-      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{ACFF3F1F-0DEB-4962-A30C-E7A1BD1814C4}" name="DEF" dataDxfId="13">
-      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1 + 15 + 10</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{AF9BE2E5-89EE-468C-B0ED-D05B0FFE3880}" name="MAT" dataDxfId="12">
-      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{BF26333D-F5E1-471D-8EB4-69106E629333}" name="MDF" dataDxfId="11">
-      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1 + 15 + 8</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{419D6271-6B9C-434E-BF38-4DE7848F9419}" name="AGI" dataDxfId="10">
-      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{CB85A19D-24B4-428F-A77F-481DA3FAACF8}" name="LUK" dataDxfId="9">
-      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{0DA2010E-5B86-4EB0-A1CB-2F1DA2E20D55}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{18F550C2-BA99-442C-BEF0-F2A727225321}" name="HP" dataDxfId="5">
+      <calculatedColumnFormula>Table13163946[[#This Row],[Level]]*106.25 + 500</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{AF6041D8-0897-4671-9A81-6EE8816F6BBE}" name="MP" dataDxfId="7">
+      <calculatedColumnFormula>Table13163946[[#This Row],[Level]]*10+20</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{E65D65BD-05C4-4A9B-ABA0-B601294BE295}" name="ATK" dataDxfId="4">
+      <calculatedColumnFormula>Table13163946[[#This Row],[Level]]*2.125+ 15 + 40</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{778501FE-4E31-4734-A31A-EEEE7EF05B63}" name="DEF" dataDxfId="1">
+      <calculatedColumnFormula>Table13163946[[#This Row],[Level]]*2.125 + 15 + 20</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{B5B2244A-14A8-46D8-BF8F-67AC8D3241DA}" name="MAT" dataDxfId="6">
+      <calculatedColumnFormula>Table13163946[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{9A962E99-0281-41D8-9287-E65CD6E131FB}" name="MDF" dataDxfId="0">
+      <calculatedColumnFormula>Table13163946[[#This Row],[Level]]*2.125 + 15 + 40</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{1AEB996E-4494-401F-BBA6-260C80317786}" name="AGI" dataDxfId="3">
+      <calculatedColumnFormula>Table13163946[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{9670DFBA-0FF6-4756-ACBC-24B43785B711}" name="LUK" dataDxfId="2">
+      <calculatedColumnFormula>Table13163946[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2964,6 +3057,40 @@
 </file>
 
 <file path=xl/tables/table43.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="42" xr:uid="{B11B1E6C-19A5-42E4-847D-0CD22EB4A103}" name="Table1318222743" displayName="Table1318222743" ref="A3:I7" totalsRowShown="0">
+  <autoFilter ref="A3:I7" xr:uid="{7F8360B3-D323-4505-8E52-764F2EEFEF08}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{2DA75379-E191-41C6-A461-F7A952576C54}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{0E110670-3AC7-427B-B6F4-6865DC721C3B}" name="HP" dataDxfId="24">
+      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*62.5+ 300</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{DD071379-690C-45AA-9EB0-1452F203E78A}" name="MP" dataDxfId="23">
+      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*12.5+60</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{16C4CC92-9435-4196-8A09-D27E77854475}" name="ATK" dataDxfId="22">
+      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{ACFF3F1F-0DEB-4962-A30C-E7A1BD1814C4}" name="DEF" dataDxfId="21">
+      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1 + 15 + 10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{AF9BE2E5-89EE-468C-B0ED-D05B0FFE3880}" name="MAT" dataDxfId="20">
+      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{BF26333D-F5E1-471D-8EB4-69106E629333}" name="MDF" dataDxfId="19">
+      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1 + 15 + 8</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{419D6271-6B9C-434E-BF38-4DE7848F9419}" name="AGI" dataDxfId="18">
+      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{CB85A19D-24B4-428F-A77F-481DA3FAACF8}" name="LUK" dataDxfId="17">
+      <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table44.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="44" xr:uid="{63EFECE9-294D-4BD5-B983-D7DF0138B45B}" name="Table168213429322745" displayName="Table168213429322745" ref="A4:J6" totalsRowShown="0">
   <autoFilter ref="A4:J6" xr:uid="{9FA97447-7595-4CE0-9387-AEB91FE50244}"/>
   <tableColumns count="10">
@@ -2976,7 +3103,7 @@
     <tableColumn id="7" xr3:uid="{6B239F5E-F897-4532-B3C2-8B926BDED5BF}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{CB8FDC45-B604-4FEB-9A7B-367828FC7568}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{6C00B6B1-0959-4058-96EE-2711BA8C66BD}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{1803A62E-480C-481E-8063-2EB8C650EA1D}" name="Total" dataDxfId="8">
+    <tableColumn id="10" xr3:uid="{1803A62E-480C-481E-8063-2EB8C650EA1D}" name="Total" dataDxfId="16">
       <calculatedColumnFormula>SUM(Table168213429322745[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2984,33 +3111,33 @@
 </table>
 </file>
 
-<file path=xl/tables/table44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table45.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="46" xr:uid="{6B246BF5-6CE4-4B50-8843-8DACC434192B}" name="Table1316183336373847" displayName="Table1316183336373847" ref="A8:I13" totalsRowShown="0">
   <autoFilter ref="A8:I13" xr:uid="{F3DE48F5-A98B-4A15-8805-1948F568C45F}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2E01F6BC-B2F6-42D6-A20F-FDB9BA2D677A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{21915B10-9976-4EFE-936F-170B253E711B}" name="HP" dataDxfId="7">
+    <tableColumn id="2" xr3:uid="{21915B10-9976-4EFE-936F-170B253E711B}" name="HP" dataDxfId="15">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*168.75</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{052B9451-309F-4C84-8FC4-08AD4866120D}" name="MP" dataDxfId="6">
+    <tableColumn id="3" xr3:uid="{052B9451-309F-4C84-8FC4-08AD4866120D}" name="MP" dataDxfId="14">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{B73769F3-1F79-45AE-998C-FF1A9A557091}" name="ATK" dataDxfId="5">
+    <tableColumn id="4" xr3:uid="{B73769F3-1F79-45AE-998C-FF1A9A557091}" name="ATK" dataDxfId="13">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*3.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B5E81D1B-B382-4DF5-92BA-F92F12A23A07}" name="DEF" dataDxfId="4">
+    <tableColumn id="5" xr3:uid="{B5E81D1B-B382-4DF5-92BA-F92F12A23A07}" name="DEF" dataDxfId="12">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*4.75</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A815FA03-2618-4DC9-9734-50DCE6DA615F}" name="MAT" dataDxfId="3">
+    <tableColumn id="6" xr3:uid="{A815FA03-2618-4DC9-9734-50DCE6DA615F}" name="MAT" dataDxfId="11">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D8263081-7D11-47BB-9AEC-CE559647F35D}" name="MDF" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{D8263081-7D11-47BB-9AEC-CE559647F35D}" name="MDF" dataDxfId="10">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*4.75</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C838F145-4059-4C8C-8152-B8F66431FFE1}" name="AGI" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{C838F145-4059-4C8C-8152-B8F66431FFE1}" name="AGI" dataDxfId="9">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*3.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{431AC55C-A81C-4BB0-B544-6631F8331D55}" name="LUK" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{431AC55C-A81C-4BB0-B544-6631F8331D55}" name="LUK" dataDxfId="8">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*2.125</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3023,28 +3150,28 @@
   <autoFilter ref="A8:I14" xr:uid="{D3C3F418-ED32-4504-9D73-88545A192967}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{13E0AF4A-AA83-489A-A156-B01D4F48D2F5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{B970139F-8BB5-4CE6-92F8-79E3236AC62B}" name="HP" dataDxfId="237">
+    <tableColumn id="2" xr3:uid="{B970139F-8BB5-4CE6-92F8-79E3236AC62B}" name="HP" dataDxfId="245">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*63+300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7BCF83B8-7492-4991-A008-F212725940B9}" name="MP" dataDxfId="236">
+    <tableColumn id="3" xr3:uid="{7BCF83B8-7492-4991-A008-F212725940B9}" name="MP" dataDxfId="244">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{33220A80-38D8-4480-ACC7-DF484072C96B}" name="ATK" dataDxfId="235">
+    <tableColumn id="4" xr3:uid="{33220A80-38D8-4480-ACC7-DF484072C96B}" name="ATK" dataDxfId="243">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.5+ 15+40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{36708515-5004-4705-A558-44B59D0CE676}" name="DEF" dataDxfId="234">
+    <tableColumn id="5" xr3:uid="{36708515-5004-4705-A558-44B59D0CE676}" name="DEF" dataDxfId="242">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25 + 15+21</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{11729EA3-08C4-4E0B-B5EE-5B3C08A31A9C}" name="MAT" dataDxfId="233">
+    <tableColumn id="6" xr3:uid="{11729EA3-08C4-4E0B-B5EE-5B3C08A31A9C}" name="MAT" dataDxfId="241">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B179D090-E484-4663-937A-480D1164D655}" name="MDF" dataDxfId="232">
+    <tableColumn id="7" xr3:uid="{B179D090-E484-4663-937A-480D1164D655}" name="MDF" dataDxfId="240">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25+15 + 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{28323AD0-B3BD-401F-A237-92C8B8D70FEA}" name="AGI" dataDxfId="231">
+    <tableColumn id="8" xr3:uid="{28323AD0-B3BD-401F-A237-92C8B8D70FEA}" name="AGI" dataDxfId="239">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{657BED8B-4C8A-42DC-BECD-5EEF9D1B7F37}" name="LUK" dataDxfId="230">
+    <tableColumn id="9" xr3:uid="{657BED8B-4C8A-42DC-BECD-5EEF9D1B7F37}" name="LUK" dataDxfId="238">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3065,7 +3192,7 @@
     <tableColumn id="7" xr3:uid="{D1DFC0D2-A987-4E3F-BA23-52162FB0C0BA}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{AB6209DB-CCCB-4C37-B455-4C7652E0DAC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2CD4CD14-92FD-41A7-9CCD-1329B5A77390}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{3B2C0A10-5038-4C21-BAC5-12FB16275D2E}" name="Total" dataDxfId="229">
+    <tableColumn id="10" xr3:uid="{3B2C0A10-5038-4C21-BAC5-12FB16275D2E}" name="Total" dataDxfId="237">
       <calculatedColumnFormula>SUM(Table11412[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3078,28 +3205,28 @@
   <autoFilter ref="A8:I14" xr:uid="{43F790D1-EA7B-4BAE-8A37-7CAD791E8821}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F6E842E1-B25F-4CA1-9107-AC7179420C29}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EFB2F0D5-318D-4A65-BA2B-20ADDE071648}" name="HP" dataDxfId="228">
+    <tableColumn id="2" xr3:uid="{EFB2F0D5-318D-4A65-BA2B-20ADDE071648}" name="HP" dataDxfId="236">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0D914B89-2678-453F-BC18-571DCD45E628}" name="MP" dataDxfId="227">
+    <tableColumn id="3" xr3:uid="{0D914B89-2678-453F-BC18-571DCD45E628}" name="MP" dataDxfId="235">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*13.75 + 80</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{6FBD2F64-5B1C-4035-BB1A-AFB092DB60C3}" name="ATK" dataDxfId="226">
+    <tableColumn id="4" xr3:uid="{6FBD2F64-5B1C-4035-BB1A-AFB092DB60C3}" name="ATK" dataDxfId="234">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7E0AF3FC-CC5D-4A6A-A4A2-DE278DEC4062}" name="DEF" dataDxfId="225">
+    <tableColumn id="5" xr3:uid="{7E0AF3FC-CC5D-4A6A-A4A2-DE278DEC4062}" name="DEF" dataDxfId="233">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1 + 15 + 4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3AF4D559-893B-4D50-BCB4-A1BD1FAF2F23}" name="MAT" dataDxfId="224">
+    <tableColumn id="6" xr3:uid="{3AF4D559-893B-4D50-BCB4-A1BD1FAF2F23}" name="MAT" dataDxfId="232">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6E9418A6-75AC-4541-9029-814EC5C06E70}" name="MDF" dataDxfId="223">
+    <tableColumn id="7" xr3:uid="{6E9418A6-75AC-4541-9029-814EC5C06E70}" name="MDF" dataDxfId="231">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.375+15 + 14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD605BEE-D561-4A2C-8D06-8E9AD70C32AC}" name="AGI" dataDxfId="222">
+    <tableColumn id="8" xr3:uid="{CD605BEE-D561-4A2C-8D06-8E9AD70C32AC}" name="AGI" dataDxfId="230">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E26506B2-F488-4AA4-AC87-819A22964609}" name="LUK" dataDxfId="221">
+    <tableColumn id="9" xr3:uid="{E26506B2-F488-4AA4-AC87-819A22964609}" name="LUK" dataDxfId="229">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3120,7 +3247,7 @@
     <tableColumn id="7" xr3:uid="{E91A64A8-F750-4893-9958-7C6ABC37405F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{3832FF0E-95E5-4B1F-B122-1EAFBF719DE3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{237404A9-EB50-465E-89AF-7167C57AFB99}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{927EBD24-571F-408C-A33B-59C753D9D96D}" name="Total" dataDxfId="220">
+    <tableColumn id="10" xr3:uid="{927EBD24-571F-408C-A33B-59C753D9D96D}" name="Total" dataDxfId="228">
       <calculatedColumnFormula>SUM(Table1141219[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3133,28 +3260,28 @@
   <autoFilter ref="A7:I13" xr:uid="{2539D8EE-2982-4734-B28B-342036FEDAC6}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FEE8F081-132E-4ED3-8FFD-2CF48368B2CC}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A79BC043-DB1A-48B4-AC21-AD31632979A6}" name="HP" dataDxfId="219">
+    <tableColumn id="2" xr3:uid="{A79BC043-DB1A-48B4-AC21-AD31632979A6}" name="HP" dataDxfId="227">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*63 + 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{42935B44-C727-42B0-B48E-0369818BF78A}" name="MP" dataDxfId="218">
+    <tableColumn id="3" xr3:uid="{42935B44-C727-42B0-B48E-0369818BF78A}" name="MP" dataDxfId="226">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{FC4572C7-88EC-4981-A6ED-43397844845B}" name="ATK" dataDxfId="217">
+    <tableColumn id="4" xr3:uid="{FC4572C7-88EC-4981-A6ED-43397844845B}" name="ATK" dataDxfId="225">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C8D61CEB-FFEC-42C3-9123-5140E65C1A2C}" name="DEF" dataDxfId="216">
+    <tableColumn id="5" xr3:uid="{C8D61CEB-FFEC-42C3-9123-5140E65C1A2C}" name="DEF" dataDxfId="224">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.375 + 15 + 19</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8C971683-28D2-4474-83CA-936F352F1324}" name="MAT" dataDxfId="215">
+    <tableColumn id="6" xr3:uid="{8C971683-28D2-4474-83CA-936F352F1324}" name="MAT" dataDxfId="223">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3371862A-9CF2-47CA-A149-4921E3B33162}" name="MDF" dataDxfId="214">
+    <tableColumn id="7" xr3:uid="{3371862A-9CF2-47CA-A149-4921E3B33162}" name="MDF" dataDxfId="222">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.375+15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC6AC739-B4C9-47A6-9472-439C60B629A0}" name="AGI" dataDxfId="213">
+    <tableColumn id="8" xr3:uid="{AC6AC739-B4C9-47A6-9472-439C60B629A0}" name="AGI" dataDxfId="221">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E727A271-B479-47C0-A557-227ABD8EC0AC}" name="LUK" dataDxfId="212">
+    <tableColumn id="9" xr3:uid="{E727A271-B479-47C0-A557-227ABD8EC0AC}" name="LUK" dataDxfId="220">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7106,25 +7233,28 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDEC26FB-B5E4-44F5-B062-22E344453193}">
-  <dimension ref="A2:I30"/>
+  <dimension ref="A2:U30"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:I16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -7152,8 +7282,35 @@
       <c r="I4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" t="s">
+        <v>4</v>
+      </c>
+      <c r="P4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>6</v>
+      </c>
+      <c r="R4" t="s">
+        <v>7</v>
+      </c>
+      <c r="S4" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -7189,8 +7346,43 @@
         <f>Table131639[[#This Row],[Level]]*1.25 + 15</f>
         <v>16.25</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <f>Table13163946[[#This Row],[Level]]*106.25 + 500</f>
+        <v>606.25</v>
+      </c>
+      <c r="N5">
+        <f>Table13163946[[#This Row],[Level]]*10+20</f>
+        <v>30</v>
+      </c>
+      <c r="O5">
+        <f>Table13163946[[#This Row],[Level]]*2.125+ 15 + 40</f>
+        <v>57.125</v>
+      </c>
+      <c r="P5">
+        <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 20</f>
+        <v>37.125</v>
+      </c>
+      <c r="Q5">
+        <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+      <c r="R5">
+        <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 40</f>
+        <v>57.125</v>
+      </c>
+      <c r="S5">
+        <f>Table13163946[[#This Row],[Level]]*1.5 + 15</f>
+        <v>16.5</v>
+      </c>
+      <c r="T5">
+        <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
@@ -7226,8 +7418,43 @@
         <f>Table131639[[#This Row],[Level]]*1.25 + 15</f>
         <v>27.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>10</v>
+      </c>
+      <c r="M6">
+        <f>Table13163946[[#This Row],[Level]]*106.25 + 500</f>
+        <v>1562.5</v>
+      </c>
+      <c r="N6">
+        <f>Table13163946[[#This Row],[Level]]*10+20</f>
+        <v>120</v>
+      </c>
+      <c r="O6">
+        <f>Table13163946[[#This Row],[Level]]*2.125+ 15 + 40</f>
+        <v>76.25</v>
+      </c>
+      <c r="P6">
+        <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 20</f>
+        <v>56.25</v>
+      </c>
+      <c r="Q6">
+        <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
+        <v>25</v>
+      </c>
+      <c r="R6">
+        <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 40</f>
+        <v>76.25</v>
+      </c>
+      <c r="S6">
+        <f>Table13163946[[#This Row],[Level]]*1.5 + 15</f>
+        <v>30</v>
+      </c>
+      <c r="T6">
+        <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20</v>
       </c>
@@ -7263,8 +7490,43 @@
         <f>Table131639[[#This Row],[Level]]*1.25 + 15</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>20</v>
+      </c>
+      <c r="M7">
+        <f>Table13163946[[#This Row],[Level]]*106.25 + 500</f>
+        <v>2625</v>
+      </c>
+      <c r="N7">
+        <f>Table13163946[[#This Row],[Level]]*10+20</f>
+        <v>220</v>
+      </c>
+      <c r="O7">
+        <f>Table13163946[[#This Row],[Level]]*2.125+ 15 + 40</f>
+        <v>97.5</v>
+      </c>
+      <c r="P7">
+        <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 20</f>
+        <v>77.5</v>
+      </c>
+      <c r="Q7">
+        <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
+        <v>35</v>
+      </c>
+      <c r="R7">
+        <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 40</f>
+        <v>97.5</v>
+      </c>
+      <c r="S7">
+        <f>Table13163946[[#This Row],[Level]]*1.5 + 15</f>
+        <v>45</v>
+      </c>
+      <c r="T7">
+        <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>22</v>
       </c>
@@ -7300,8 +7562,43 @@
         <f>Table131639[[#This Row],[Level]]*1.25 + 15</f>
         <v>42.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>22</v>
+      </c>
+      <c r="M8" s="1">
+        <f>Table13163946[[#This Row],[Level]]*106.25 + 500</f>
+        <v>2837.5</v>
+      </c>
+      <c r="N8" s="1">
+        <f>Table13163946[[#This Row],[Level]]*10+20</f>
+        <v>240</v>
+      </c>
+      <c r="O8" s="1">
+        <f>Table13163946[[#This Row],[Level]]*2.125+ 15 + 40</f>
+        <v>101.75</v>
+      </c>
+      <c r="P8" s="1">
+        <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 20</f>
+        <v>81.75</v>
+      </c>
+      <c r="Q8" s="1">
+        <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
+        <v>37</v>
+      </c>
+      <c r="R8" s="1">
+        <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 40</f>
+        <v>101.75</v>
+      </c>
+      <c r="S8" s="1">
+        <f>Table13163946[[#This Row],[Level]]*1.5 + 15</f>
+        <v>48</v>
+      </c>
+      <c r="T8" s="1">
+        <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>25</v>
       </c>
@@ -7337,13 +7634,78 @@
         <f>Table131639[[#This Row],[Level]]*1.25 + 15</f>
         <v>46.25</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>25</v>
+      </c>
+      <c r="M9" s="1">
+        <f>Table13163946[[#This Row],[Level]]*106.25 + 500</f>
+        <v>3156.25</v>
+      </c>
+      <c r="N9" s="1">
+        <f>Table13163946[[#This Row],[Level]]*10+20</f>
+        <v>270</v>
+      </c>
+      <c r="O9" s="1">
+        <f>Table13163946[[#This Row],[Level]]*2.125+ 15 + 40</f>
+        <v>108.125</v>
+      </c>
+      <c r="P9" s="1">
+        <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 20</f>
+        <v>88.125</v>
+      </c>
+      <c r="Q9" s="1">
+        <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="R9" s="1">
+        <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 40</f>
+        <v>108.125</v>
+      </c>
+      <c r="S9" s="1">
+        <f>Table13163946[[#This Row],[Level]]*1.5 + 15</f>
+        <v>52.5</v>
+      </c>
+      <c r="T9" s="1">
+        <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="S11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="U11" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -7371,8 +7733,39 @@
       <c r="I12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L12" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="M12" s="9">
+        <v>10</v>
+      </c>
+      <c r="N12" s="9">
+        <v>1</v>
+      </c>
+      <c r="O12" s="9">
+        <v>10</v>
+      </c>
+      <c r="P12" s="9">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="9">
+        <v>1</v>
+      </c>
+      <c r="R12" s="9">
+        <v>10</v>
+      </c>
+      <c r="S12" s="9">
+        <v>5</v>
+      </c>
+      <c r="T12" s="9">
+        <v>1</v>
+      </c>
+      <c r="U12" s="10">
+        <f>SUM(M12:T12)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -7409,7 +7802,7 @@
         <v>16.25</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>15</v>
       </c>
@@ -7446,7 +7839,7 @@
         <v>33.75</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20</v>
       </c>
@@ -7483,7 +7876,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>25</v>
       </c>
@@ -7854,11 +8247,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="4">
+  <tableParts count="5">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7867,7 +8261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F20BDF8A-A837-40AC-945B-5DCD3F792613}">
   <dimension ref="A2:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -8068,7 +8462,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="A4" sqref="A4:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Mapped mine exterior. Added three fights, working on skills
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="75">
   <si>
     <t>Skeletons are the most basic undead, they have low magical attributes, agility, and luck.</t>
   </si>
@@ -224,12 +224,6 @@
     <t>An Earth type monster, may look similar to normal wolfs but since it’s a monster it is much stronger. Base Level 2</t>
   </si>
   <si>
-    <t>Lv 20 with Iron equipment, single class, single path?</t>
-  </si>
-  <si>
-    <t>Bandit Warrior, Medium Iron Armor, Two handed weapon -&gt; 40, 19/5</t>
-  </si>
-  <si>
     <t>Bandit Rogue, light phys armor, dual equipped daggers -&gt; 40, 10/8</t>
   </si>
   <si>
@@ -261,6 +255,18 @@
   </si>
   <si>
     <t>Mercenary Golem, -&gt; 40 Attack, 20 Def, 40 MDF</t>
+  </si>
+  <si>
+    <t>Lv 20 with Iron equipment, single class, single path? Bandit Warrior, Medium Iron Armor, Two handed weapon -&gt; 40, 19/5</t>
+  </si>
+  <si>
+    <t>Lv 25 with Iron equipment, single class, single path? Bandit Warrior, Medium Iron Armor, Two handed weapon -&gt; 40, 19/5</t>
+  </si>
+  <si>
+    <t>Lv 28 with Iron equipment, Swords master, Brawler</t>
+  </si>
+  <si>
+    <t>Mercenary Boss, Heavy Iron Armor, Two handed weapon, 2 Iron Ring -&gt; 40, 21/7</t>
   </si>
 </sst>
 </file>
@@ -400,7 +406,31 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="264">
+  <dxfs count="272">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1987,7 +2017,7 @@
     <tableColumn id="7" xr3:uid="{F9852B29-E77D-4E17-A56E-5F0C649FA862}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{9A914BFF-1060-46E4-B8F9-412BD9293C3D}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2F83B650-811D-4FEE-92D5-03D4DC4376E5}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="263">
+    <tableColumn id="10" xr3:uid="{A7ECC22A-E541-4FF1-905A-C7CFAFD30F4C}" name="Total" dataDxfId="271">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2008,7 +2038,7 @@
     <tableColumn id="7" xr3:uid="{3A2FD57C-060A-462E-8BB9-B06F717E9D20}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{ED9393EA-F7F9-4661-8D0B-0D9246DDABF8}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{6F56342F-5442-42CD-8B6C-D98B6D6C0C56}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="219">
+    <tableColumn id="10" xr3:uid="{8C3FB752-E74A-4FF8-9BB4-A96D072B21F5}" name="Total" dataDxfId="227">
       <calculatedColumnFormula>SUM(Table16[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2021,28 +2051,28 @@
   <autoFilter ref="A8:I13" xr:uid="{7BE337CC-37BD-4688-B60D-A66F4420668B}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{71340E4C-6101-4C59-8ED7-689E2AD5A962}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="218">
+    <tableColumn id="2" xr3:uid="{C1A3992E-1B16-49B9-BB43-D049727FD937}" name="HP" dataDxfId="226">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*63-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="217">
+    <tableColumn id="3" xr3:uid="{C682D862-74D7-4A71-B58F-60B479692D97}" name="MP" dataDxfId="225">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="216">
+    <tableColumn id="4" xr3:uid="{A92CB1B9-B5DB-4C6F-9840-9A9CF6F3908F}" name="ATK" dataDxfId="224">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="215">
+    <tableColumn id="5" xr3:uid="{524C1F64-C076-4632-9637-C2B7F145A708}" name="DEF" dataDxfId="223">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="214">
+    <tableColumn id="6" xr3:uid="{0885B50D-EAEE-4742-B39A-A6FB8EB1237E}" name="MAT" dataDxfId="222">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="213">
+    <tableColumn id="7" xr3:uid="{61AC7716-759F-498C-8E8C-B5F398D64504}" name="MDF" dataDxfId="221">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="212">
+    <tableColumn id="8" xr3:uid="{C3006388-05CF-47C5-AB9E-F1B6224F179B}" name="AGI" dataDxfId="220">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="211">
+    <tableColumn id="9" xr3:uid="{8DBB4D25-C72A-496C-9204-90CC99BD5D11}" name="LUK" dataDxfId="219">
       <calculatedColumnFormula>Table131610[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2063,7 +2093,7 @@
     <tableColumn id="7" xr3:uid="{4899BF24-9D2A-4CC0-AE35-4F49604AAC5A}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{CB1CC6BA-1D38-4B74-9BC6-7057FB9773EE}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{C47FADF6-C526-4188-9187-383757CE17C1}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="210">
+    <tableColumn id="10" xr3:uid="{88E3283E-60B0-4EF7-BD9E-33A82A31A770}" name="Total" dataDxfId="218">
       <calculatedColumnFormula>SUM(Table168[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2076,28 +2106,28 @@
   <autoFilter ref="A9:I15" xr:uid="{06A56D17-07E5-4650-8EE9-7EA8F94D4020}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A2BE27C9-9DAE-49F5-9A70-C6CF7428BF31}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="209">
+    <tableColumn id="2" xr3:uid="{4AF6F42F-E0B8-4A6F-ABB8-DB121148C5F1}" name="HP" dataDxfId="217">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="208">
+    <tableColumn id="3" xr3:uid="{0AFD181E-F6A3-4256-8D2D-5F1DAB2B2427}" name="MP" dataDxfId="216">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="207">
+    <tableColumn id="4" xr3:uid="{57DE769C-A92E-467B-97E6-0164FBEBC66A}" name="ATK" dataDxfId="215">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="206">
+    <tableColumn id="5" xr3:uid="{BF337D43-5142-431D-B5AC-7335DB8B1181}" name="DEF" dataDxfId="214">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="205">
+    <tableColumn id="6" xr3:uid="{DC999929-3C77-4EB9-B113-30A73FEEEF46}" name="MAT" dataDxfId="213">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.375+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="204">
+    <tableColumn id="7" xr3:uid="{19E03B32-9762-40A5-ABB9-71E539F12A4D}" name="MDF" dataDxfId="212">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="203">
+    <tableColumn id="8" xr3:uid="{340B798D-7289-415A-863E-5B75541B1826}" name="AGI" dataDxfId="211">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="202">
+    <tableColumn id="9" xr3:uid="{A95C61CD-FC66-44AB-B31A-915976135796}" name="LUK" dataDxfId="210">
       <calculatedColumnFormula>Table13161013[[#This Row],[Level]]*1.5+15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2118,7 +2148,7 @@
     <tableColumn id="7" xr3:uid="{60AD88FB-4685-412B-B5FD-BF8412C6B8E2}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{6A88D48C-D864-4F16-BEF2-BA88783A3FF3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{D40BD230-6392-4A28-A29D-F13EFE35C95E}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A0E09B2B-FD41-413F-8063-62214E990751}" name="Total" dataDxfId="201">
+    <tableColumn id="10" xr3:uid="{A0E09B2B-FD41-413F-8063-62214E990751}" name="Total" dataDxfId="209">
       <calculatedColumnFormula>SUM(Table16826[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2131,28 +2161,28 @@
   <autoFilter ref="A8:I14" xr:uid="{F7062CBA-4FAA-4900-9D3A-5C6613BCB6CE}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{ADCB4852-D3A0-456B-A8BD-E5F74BDBB762}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{ED76047D-1BC2-4C1B-B9B0-58BE0ACDDA48}" name="HP" dataDxfId="200">
+    <tableColumn id="2" xr3:uid="{ED76047D-1BC2-4C1B-B9B0-58BE0ACDDA48}" name="HP" dataDxfId="208">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EC859C53-0BA5-45D1-868B-F22DC8CE7D25}" name="MP" dataDxfId="199">
+    <tableColumn id="3" xr3:uid="{EC859C53-0BA5-45D1-868B-F22DC8CE7D25}" name="MP" dataDxfId="207">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DED33AB9-A2BB-4F9E-AA6D-02F8D1D65CD1}" name="ATK" dataDxfId="198">
+    <tableColumn id="4" xr3:uid="{DED33AB9-A2BB-4F9E-AA6D-02F8D1D65CD1}" name="ATK" dataDxfId="206">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.375+ 15+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{329B716D-9CA6-4546-AB13-92D88BE40F5F}" name="DEF" dataDxfId="197">
+    <tableColumn id="5" xr3:uid="{329B716D-9CA6-4546-AB13-92D88BE40F5F}" name="DEF" dataDxfId="205">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1 + 15+12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{67F8198A-5FC2-4C6D-9558-68B3141EA756}" name="MAT" dataDxfId="196">
+    <tableColumn id="6" xr3:uid="{67F8198A-5FC2-4C6D-9558-68B3141EA756}" name="MAT" dataDxfId="204">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C70F5BF6-63B0-44C1-862D-25E3FB55320F}" name="MDF" dataDxfId="195">
+    <tableColumn id="7" xr3:uid="{C70F5BF6-63B0-44C1-862D-25E3FB55320F}" name="MDF" dataDxfId="203">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.5+15+11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AB20AF53-453C-4266-A46B-40E693C91985}" name="AGI" dataDxfId="194">
+    <tableColumn id="8" xr3:uid="{AB20AF53-453C-4266-A46B-40E693C91985}" name="AGI" dataDxfId="202">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7FC46A31-F9F1-432E-B399-0823E198FE0A}" name="LUK" dataDxfId="193">
+    <tableColumn id="9" xr3:uid="{7FC46A31-F9F1-432E-B399-0823E198FE0A}" name="LUK" dataDxfId="201">
       <calculatedColumnFormula>Table1316101328[[#This Row],[Level]]*1.5+15+20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2173,7 +2203,7 @@
     <tableColumn id="7" xr3:uid="{20C5D094-BAF0-471C-ACF3-C6658991DB5F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{E08E2AF0-56DD-4A69-A536-27139D793022}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{12AD8606-1127-4E5B-BA2C-872780F22F9E}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{5E2EF778-63AE-48B7-9F49-0D2AFEBD66A1}" name="Total" dataDxfId="192">
+    <tableColumn id="10" xr3:uid="{5E2EF778-63AE-48B7-9F49-0D2AFEBD66A1}" name="Total" dataDxfId="200">
       <calculatedColumnFormula>SUM(Table1682630[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2186,28 +2216,28 @@
   <autoFilter ref="A8:I14" xr:uid="{299912CC-280B-49E1-8859-432D05893259}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4F0B657F-C9A5-4A73-AAA3-27D307385193}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{526284E7-597F-4726-AB18-230CA03461B1}" name="HP" dataDxfId="191">
+    <tableColumn id="2" xr3:uid="{526284E7-597F-4726-AB18-230CA03461B1}" name="HP" dataDxfId="199">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*63+ 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E7BA3C7A-2677-415F-BA47-A4E88679B948}" name="MP" dataDxfId="190">
+    <tableColumn id="3" xr3:uid="{E7BA3C7A-2677-415F-BA47-A4E88679B948}" name="MP" dataDxfId="198">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE7BE678-2229-44F6-8732-71214FB69DD7}" name="ATK" dataDxfId="189">
+    <tableColumn id="4" xr3:uid="{AE7BE678-2229-44F6-8732-71214FB69DD7}" name="ATK" dataDxfId="197">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+ 15+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4715E3DB-8817-43D5-9074-9FB5F0BEF5B4}" name="DEF" dataDxfId="188">
+    <tableColumn id="5" xr3:uid="{4715E3DB-8817-43D5-9074-9FB5F0BEF5B4}" name="DEF" dataDxfId="196">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1 + 15+12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9CE76933-D045-418B-A975-378EEA51D856}" name="MAT" dataDxfId="187">
+    <tableColumn id="6" xr3:uid="{9CE76933-D045-418B-A975-378EEA51D856}" name="MAT" dataDxfId="195">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244B9611-6CB0-4946-B5CD-7D42311C7D7E}" name="MDF" dataDxfId="186">
+    <tableColumn id="7" xr3:uid="{244B9611-6CB0-4946-B5CD-7D42311C7D7E}" name="MDF" dataDxfId="194">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+15+11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32550C13-49BB-41D2-BA0A-26798830A0FD}" name="AGI" dataDxfId="185">
+    <tableColumn id="8" xr3:uid="{32550C13-49BB-41D2-BA0A-26798830A0FD}" name="AGI" dataDxfId="193">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{BB22F289-8AF5-4DD6-877B-F09520710555}" name="LUK" dataDxfId="184">
+    <tableColumn id="9" xr3:uid="{BB22F289-8AF5-4DD6-877B-F09520710555}" name="LUK" dataDxfId="192">
       <calculatedColumnFormula>Table131610132831[[#This Row],[Level]]*1.5+15+20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2220,28 +2250,28 @@
   <autoFilter ref="A4:I10" xr:uid="{A1EAC62C-C07D-464E-91B1-4A34E6604BA2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{430FD3D4-914C-4309-B2E6-6F01B5CAED94}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="183">
+    <tableColumn id="2" xr3:uid="{28AF0DE0-B21C-412D-B81D-50BDA9E69080}" name="HP" dataDxfId="191">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="182">
+    <tableColumn id="3" xr3:uid="{1DE5110F-EC07-4DF5-A7D5-34F082598910}" name="MP" dataDxfId="190">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="181">
+    <tableColumn id="4" xr3:uid="{F18C8760-61ED-4B62-BAF2-B14B62B7D248}" name="ATK" dataDxfId="189">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="180">
+    <tableColumn id="5" xr3:uid="{C1595AD9-E387-4A22-BCB6-4CBFA719F9D0}" name="DEF" dataDxfId="188">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15 + 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="179">
+    <tableColumn id="6" xr3:uid="{F489FA67-46F6-43D1-B73B-47D83B34338A}" name="MAT" dataDxfId="187">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15 + 30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="178">
+    <tableColumn id="7" xr3:uid="{3F79394A-4124-4984-9D31-828E25A56C45}" name="MDF" dataDxfId="186">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.5 + 15 + 21</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="177">
+    <tableColumn id="8" xr3:uid="{C07D4BAA-1701-41F8-AFCA-9DA08523E4CB}" name="AGI" dataDxfId="185">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="176">
+    <tableColumn id="9" xr3:uid="{4A2DA70C-A82A-443D-8342-5AD49EBB4B2C}" name="LUK" dataDxfId="184">
       <calculatedColumnFormula>Table13162015[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2254,28 +2284,28 @@
   <autoFilter ref="A7:I12" xr:uid="{9BE7336F-352A-4FAE-B0E4-61965FC814C7}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B8DA50BB-4379-43D1-879B-CDBE6D82C13A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="175">
+    <tableColumn id="2" xr3:uid="{A8A85284-4B9F-4641-B524-14D05062AA7E}" name="HP" dataDxfId="183">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="174">
+    <tableColumn id="3" xr3:uid="{4AC299E1-6D4E-4976-B070-B7CE6420FFAE}" name="MP" dataDxfId="182">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="173">
+    <tableColumn id="4" xr3:uid="{BAB284EC-09DE-422F-ABFC-8F534405AF61}" name="ATK" dataDxfId="181">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="172">
+    <tableColumn id="5" xr3:uid="{769BCE66-0870-41ED-9C9B-5AD056584176}" name="DEF" dataDxfId="180">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="171">
+    <tableColumn id="6" xr3:uid="{27956CE0-AAC2-4888-96D5-4FA26667ECE7}" name="MAT" dataDxfId="179">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="170">
+    <tableColumn id="7" xr3:uid="{6C0E582B-8B24-49CA-B28B-FF3306829EEC}" name="MDF" dataDxfId="178">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="169">
+    <tableColumn id="8" xr3:uid="{B3895228-D7EB-4A37-A986-C2AC48A359C6}" name="AGI" dataDxfId="177">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="168">
+    <tableColumn id="9" xr3:uid="{9583BDED-512B-459B-98FC-273F1975BCB9}" name="LUK" dataDxfId="176">
       <calculatedColumnFormula>Table131618[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2288,28 +2318,28 @@
   <autoFilter ref="A8:I13" xr:uid="{67385006-CBB9-4472-99D4-7881E042769D}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FD96F8F7-CCAB-44FA-B525-A5081670706A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="262">
+    <tableColumn id="2" xr3:uid="{3B6C33F1-A23B-494D-9E01-1F3B92B01ACB}" name="HP" dataDxfId="270">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*56.25-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="261">
+    <tableColumn id="3" xr3:uid="{AC26381C-1E8B-4282-BA32-FAB013C92F8A}" name="MP" dataDxfId="269">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="260">
+    <tableColumn id="4" xr3:uid="{77F74EFD-F91C-4967-9511-B8BF5E4B6952}" name="ATK" dataDxfId="268">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="259">
+    <tableColumn id="5" xr3:uid="{C5099C7E-FF2C-413F-B479-06A4BBC781C4}" name="DEF" dataDxfId="267">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="258">
+    <tableColumn id="6" xr3:uid="{55F7F6C7-C6E6-49D1-9C4C-6F3D4A44FC15}" name="MAT" dataDxfId="266">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="257">
+    <tableColumn id="7" xr3:uid="{D37B7B5E-6DF3-40C9-BC2C-99DE88C4F88F}" name="MDF" dataDxfId="265">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="256">
+    <tableColumn id="8" xr3:uid="{4DAA9289-D312-4509-B000-CD43744E2CED}" name="AGI" dataDxfId="264">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="255">
+    <tableColumn id="9" xr3:uid="{D9656154-EFE0-498B-896F-CDEF92F7DC51}" name="LUK" dataDxfId="263">
       <calculatedColumnFormula>Table1316[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2330,7 +2360,7 @@
     <tableColumn id="7" xr3:uid="{AEFF5C29-BE6A-4CF8-A2BB-F6B076077DA9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{4DE9B01E-67F2-4136-ADC3-60389FB67DCC}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{F5A82F03-513C-46D4-9F91-470F0060526B}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="167">
+    <tableColumn id="10" xr3:uid="{AC99843E-773A-414F-BD46-4FF9EE83C7C8}" name="Total" dataDxfId="175">
       <calculatedColumnFormula>SUM(Table16821[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2339,22 +2369,22 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="166" tableBorderDxfId="165">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{C0D4CA08-9B25-4DAF-9E5A-DE83069C82B6}" name="Table1922" displayName="Table1922" ref="A15:I16" totalsRowShown="0" dataDxfId="174" tableBorderDxfId="173">
   <autoFilter ref="A15:I16" xr:uid="{434CBBE2-2F8D-4EEB-895C-68FC850EF1FD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="164"/>
-    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="163">
+    <tableColumn id="1" xr3:uid="{08FAD429-66B9-4C8A-8EDB-B8DA8C26C675}" name="Level" dataDxfId="172"/>
+    <tableColumn id="2" xr3:uid="{CA74597C-BA22-42F0-BB05-90DCD7E1CDDE}" name="HP" dataDxfId="171">
       <calculatedColumnFormula>Table1922[Level]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="162">
+    <tableColumn id="3" xr3:uid="{993D070B-C7B7-45D4-93E5-17EE44EED7D3}" name="MP" dataDxfId="170">
       <calculatedColumnFormula>Table1922[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="161"/>
-    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="160"/>
-    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="159"/>
-    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="158"/>
-    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="157"/>
-    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="156"/>
+    <tableColumn id="4" xr3:uid="{C4545271-63AB-4362-AFD0-75163CCB58EF}" name="ATK" dataDxfId="169"/>
+    <tableColumn id="5" xr3:uid="{86A4D6B9-AD17-49DD-8DA2-FFA5E1524EBD}" name="DEF" dataDxfId="168"/>
+    <tableColumn id="6" xr3:uid="{E7353087-15C2-4F04-A487-D3F31754ABD6}" name="MAT" dataDxfId="167"/>
+    <tableColumn id="7" xr3:uid="{ED5F6DB9-0B11-4EFF-A230-1A55AF879970}" name="MDF" dataDxfId="166"/>
+    <tableColumn id="8" xr3:uid="{58B92910-71F9-41E1-9754-359D180D0AAC}" name="AGI" dataDxfId="165"/>
+    <tableColumn id="9" xr3:uid="{75D84CD3-53A0-4336-93D8-A352C50C03CA}" name="LUK" dataDxfId="164"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2365,28 +2395,28 @@
   <autoFilter ref="A3:I9" xr:uid="{A90D1C2A-DBF9-4EEF-ACC2-3DC17C207301}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BD3505AC-AE6D-4947-A74E-A6C2D68658F1}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="155">
+    <tableColumn id="2" xr3:uid="{A1294F9F-EBC1-4296-B011-01C603344440}" name="HP" dataDxfId="163">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="154">
+    <tableColumn id="3" xr3:uid="{59EABEF7-2BEF-47B5-8F65-5CA01989879E}" name="MP" dataDxfId="162">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="153">
+    <tableColumn id="4" xr3:uid="{1126F36B-2E1E-425F-9D79-2C33533A233C}" name="ATK" dataDxfId="161">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="152">
+    <tableColumn id="5" xr3:uid="{4235BC6B-708C-4D42-BF8A-BB1DFF8F3B48}" name="DEF" dataDxfId="160">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="151">
+    <tableColumn id="6" xr3:uid="{5089908A-1F1A-4ABC-83C5-4AB9A3F6939C}" name="MAT" dataDxfId="159">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="150">
+    <tableColumn id="7" xr3:uid="{244F2331-26E8-40D3-9798-7F332C488BA2}" name="MDF" dataDxfId="158">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="149">
+    <tableColumn id="8" xr3:uid="{2AD0FECD-797E-4EEA-B5DD-FEB78C15117F}" name="AGI" dataDxfId="157">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="148">
+    <tableColumn id="9" xr3:uid="{D4231BEE-7DAE-438E-B727-BC57B8F57597}" name="LUK" dataDxfId="156">
       <calculatedColumnFormula>Table131620[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2395,32 +2425,32 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="147" tableBorderDxfId="146">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{EB5E87D9-7176-4EDF-A213-1F2F1812D046}" name="Table19" displayName="Table19" ref="L3:T4" totalsRowShown="0" dataDxfId="155" tableBorderDxfId="154">
   <autoFilter ref="L3:T4" xr:uid="{5D2C3EA8-1297-4C77-AF32-84E50F8232C5}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="145"/>
-    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="144">
+    <tableColumn id="1" xr3:uid="{0B061316-6B56-404F-BD50-AEA8EEBE29C7}" name="Level" dataDxfId="153"/>
+    <tableColumn id="2" xr3:uid="{DD7F3A71-5685-4158-906B-EF22B1AE9AF0}" name="HP" dataDxfId="152">
       <calculatedColumnFormula>Table19[Level]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="143">
+    <tableColumn id="3" xr3:uid="{370CE45A-8A0C-43B6-91A5-13ED6B69FE90}" name="MP" dataDxfId="151">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="142">
+    <tableColumn id="4" xr3:uid="{A67BA9CE-5223-45EC-A3F0-5AD854A4F789}" name="ATK" dataDxfId="150">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="141">
+    <tableColumn id="5" xr3:uid="{C7704809-03E7-437C-B85B-D24236A90152}" name="DEF" dataDxfId="149">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1 + 15 + 6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="140">
+    <tableColumn id="6" xr3:uid="{5A5291DB-ED22-43A9-9E32-0F7D8E2DF605}" name="MAT" dataDxfId="148">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="139">
+    <tableColumn id="7" xr3:uid="{F6AEAE89-9D01-4371-80C5-75F4295522CF}" name="MDF" dataDxfId="147">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.5 + 15 + 12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="138">
+    <tableColumn id="8" xr3:uid="{27FAFF51-670F-4383-AE3D-7774533FB52E}" name="AGI" dataDxfId="146">
       <calculatedColumnFormula>Table19[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="137">
+    <tableColumn id="9" xr3:uid="{1BFA026A-DC3F-4B70-9D2A-1628D758B39D}" name="LUK" dataDxfId="145">
       <calculatedColumnFormula>Table19[Level] + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2433,28 +2463,28 @@
   <autoFilter ref="A7:I12" xr:uid="{553298A4-7E43-42CF-9EEB-1F9E7E6BAD27}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2AA35C8B-719C-4BA6-9CDF-2963E1C9F233}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C087FAFA-9653-40EC-B4B9-5CB8F9D7255E}" name="HP" dataDxfId="136">
+    <tableColumn id="2" xr3:uid="{C087FAFA-9653-40EC-B4B9-5CB8F9D7255E}" name="HP" dataDxfId="144">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0004B47B-3968-4C5A-BE6C-B822A307D7C5}" name="MP" dataDxfId="135">
+    <tableColumn id="3" xr3:uid="{0004B47B-3968-4C5A-BE6C-B822A307D7C5}" name="MP" dataDxfId="143">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{67EC8D91-0122-40D7-87D0-A3AB6788CE9D}" name="ATK" dataDxfId="134">
+    <tableColumn id="4" xr3:uid="{67EC8D91-0122-40D7-87D0-A3AB6788CE9D}" name="ATK" dataDxfId="142">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E9988E54-33D6-41EB-B6BE-6E832544E18C}" name="DEF" dataDxfId="133">
+    <tableColumn id="5" xr3:uid="{E9988E54-33D6-41EB-B6BE-6E832544E18C}" name="DEF" dataDxfId="141">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{16D71A55-372C-4029-A831-ECF2325E46C4}" name="MAT" dataDxfId="132">
+    <tableColumn id="6" xr3:uid="{16D71A55-372C-4029-A831-ECF2325E46C4}" name="MAT" dataDxfId="140">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{1802FB48-B110-4DBF-A8F2-64CD4890E741}" name="MDF" dataDxfId="131">
+    <tableColumn id="7" xr3:uid="{1802FB48-B110-4DBF-A8F2-64CD4890E741}" name="MDF" dataDxfId="139">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{350CA8CC-761C-4994-9D80-14685787EF3D}" name="AGI" dataDxfId="130">
+    <tableColumn id="8" xr3:uid="{350CA8CC-761C-4994-9D80-14685787EF3D}" name="AGI" dataDxfId="138">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B578CF58-136A-41B9-800E-D75836A4CDD1}" name="LUK" dataDxfId="129">
+    <tableColumn id="9" xr3:uid="{B578CF58-136A-41B9-800E-D75836A4CDD1}" name="LUK" dataDxfId="137">
       <calculatedColumnFormula>Table13161833[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2475,7 +2505,7 @@
     <tableColumn id="7" xr3:uid="{5A405725-30A7-487F-95BF-061F71CA9C61}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{644DEF70-6EBD-403E-904B-6C30E5FBEA48}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{BA93DA54-96B9-48D1-80BB-C266771E13F1}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{3EBB17A5-47EA-458B-83A5-7056BE67D25F}" name="Total" dataDxfId="128">
+    <tableColumn id="10" xr3:uid="{3EBB17A5-47EA-458B-83A5-7056BE67D25F}" name="Total" dataDxfId="136">
       <calculatedColumnFormula>SUM(Table1682134[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2484,26 +2514,26 @@
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{A7C0F3AC-4E86-430D-AE55-8604641B493E}" name="Table192235" displayName="Table192235" ref="A15:I16" totalsRowShown="0" dataDxfId="127" tableBorderDxfId="126">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{A7C0F3AC-4E86-430D-AE55-8604641B493E}" name="Table192235" displayName="Table192235" ref="A15:I16" totalsRowShown="0" dataDxfId="135" tableBorderDxfId="134">
   <autoFilter ref="A15:I16" xr:uid="{D0DF3ED4-9A21-493B-88F4-CE5814AF31C9}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A78A876E-6C8B-4FC8-BFD4-A9BC80EA3FC2}" name="Level" dataDxfId="125"/>
-    <tableColumn id="2" xr3:uid="{4B423FFC-D037-484D-A927-2F66E15D422A}" name="HP" dataDxfId="124">
+    <tableColumn id="1" xr3:uid="{A78A876E-6C8B-4FC8-BFD4-A9BC80EA3FC2}" name="Level" dataDxfId="133"/>
+    <tableColumn id="2" xr3:uid="{4B423FFC-D037-484D-A927-2F66E15D422A}" name="HP" dataDxfId="132">
       <calculatedColumnFormula>(Table192235[Level]*75 + 500)*2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B695FEDE-EC59-44D8-AE99-CBF568DE5C93}" name="MP" dataDxfId="123">
+    <tableColumn id="3" xr3:uid="{B695FEDE-EC59-44D8-AE99-CBF568DE5C93}" name="MP" dataDxfId="131">
       <calculatedColumnFormula>Table192235[[#This Row],[Level]]*14 + 80</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{160D5D77-34E8-44F3-B51D-7CC0736DDCB1}" name="ATK" dataDxfId="122">
+    <tableColumn id="4" xr3:uid="{160D5D77-34E8-44F3-B51D-7CC0736DDCB1}" name="ATK" dataDxfId="130">
       <calculatedColumnFormula>Table192235[[#This Row],[Level]]*1.5+ 15 + 50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{559DAC37-CD6A-449F-AFF0-355ADE7CED80}" name="DEF" dataDxfId="121"/>
-    <tableColumn id="6" xr3:uid="{EEC344A5-27A5-450E-B795-04D237DD063F}" name="MAT" dataDxfId="120">
+    <tableColumn id="5" xr3:uid="{559DAC37-CD6A-449F-AFF0-355ADE7CED80}" name="DEF" dataDxfId="129"/>
+    <tableColumn id="6" xr3:uid="{EEC344A5-27A5-450E-B795-04D237DD063F}" name="MAT" dataDxfId="128">
       <calculatedColumnFormula>Table192235[Level]*1.5+15+50</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{54363CA4-9EE5-495F-8323-6C0C1261453C}" name="MDF" dataDxfId="119"/>
-    <tableColumn id="8" xr3:uid="{26B56E9D-2FCD-4476-A6CF-8F2EDC965246}" name="AGI" dataDxfId="118"/>
-    <tableColumn id="9" xr3:uid="{95814D66-3343-4190-9BF4-F4E45AB27D95}" name="LUK" dataDxfId="117"/>
+    <tableColumn id="7" xr3:uid="{54363CA4-9EE5-495F-8323-6C0C1261453C}" name="MDF" dataDxfId="127"/>
+    <tableColumn id="8" xr3:uid="{26B56E9D-2FCD-4476-A6CF-8F2EDC965246}" name="AGI" dataDxfId="126"/>
+    <tableColumn id="9" xr3:uid="{95814D66-3343-4190-9BF4-F4E45AB27D95}" name="LUK" dataDxfId="125"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2522,7 +2552,7 @@
     <tableColumn id="7" xr3:uid="{22216E02-260E-4471-8BB1-4E6E1250BAC9}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{DC2670AC-8DF2-47F7-A3F6-EE7896309BC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{749652E2-F6CF-428C-B67C-FD0B1EFCCBBF}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="116">
+    <tableColumn id="10" xr3:uid="{A073A2A7-93B1-4F9E-9D91-2F78C352794F}" name="Total" dataDxfId="124">
       <calculatedColumnFormula>SUM(Table15[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2535,28 +2565,28 @@
   <autoFilter ref="A15:I20" xr:uid="{A1CF627F-8D28-44AD-9A35-411103976FCA}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F14CC326-DE44-48D8-856F-8DCDCFC89CAD}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="115">
+    <tableColumn id="2" xr3:uid="{92BF3802-59D2-4399-9FE0-AA0C8E30CE98}" name="HP" dataDxfId="123">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*63-100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="114">
+    <tableColumn id="3" xr3:uid="{E9621569-56FF-47E7-9862-FC92FAC1C576}" name="MP" dataDxfId="122">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="113">
+    <tableColumn id="4" xr3:uid="{28BC25CB-DFDA-4486-9929-9CA07015ACEC}" name="ATK" dataDxfId="121">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="112">
+    <tableColumn id="5" xr3:uid="{4F19BC44-4A9A-447E-BCFE-EBCA7F73E27C}" name="DEF" dataDxfId="120">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="111">
+    <tableColumn id="6" xr3:uid="{585C622F-EDFD-478A-B7AC-2300F7EC40B6}" name="MAT" dataDxfId="119">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="110">
+    <tableColumn id="7" xr3:uid="{4D664A3B-F840-4064-982E-516959FFFE80}" name="MDF" dataDxfId="118">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="109">
+    <tableColumn id="8" xr3:uid="{6A83289D-4D2C-4B86-8288-8E0D88EEFF85}" name="AGI" dataDxfId="117">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="108">
+    <tableColumn id="9" xr3:uid="{4C33EB48-74C2-47D6-870F-35D2D49D3558}" name="LUK" dataDxfId="116">
       <calculatedColumnFormula>Table13167[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2569,28 +2599,28 @@
   <autoFilter ref="K11:S17" xr:uid="{EAF9FB6A-F011-40E3-AB2F-E53826722AFB}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DF3E0800-6EE4-4E1B-BA6F-0194351D6E7C}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="107">
+    <tableColumn id="2" xr3:uid="{C6F6C58B-0423-443B-ADB0-8D76D9074DCF}" name="HP" dataDxfId="115">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*56.25+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="106">
+    <tableColumn id="3" xr3:uid="{8EEC9751-28E7-41A4-A78F-6EA9934C1A52}" name="MP" dataDxfId="114">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="105">
+    <tableColumn id="4" xr3:uid="{551DBC8D-C1F9-431E-BE65-6008C6C634D8}" name="ATK" dataDxfId="113">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.375+ 15 + 25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="104">
+    <tableColumn id="5" xr3:uid="{C9773950-14BB-4E0D-A68A-C952715F9420}" name="DEF" dataDxfId="112">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25 + 15 + 10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="103">
+    <tableColumn id="6" xr3:uid="{C9030533-FE21-4603-9B7F-56E1EA202112}" name="MAT" dataDxfId="111">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="102">
+    <tableColumn id="7" xr3:uid="{9AEE6B8F-A581-4136-83A2-A40D27A19079}" name="MDF" dataDxfId="110">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.25+ 15 + 8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="101">
+    <tableColumn id="8" xr3:uid="{30C1EA69-009B-4C45-B758-5A4E2869B8E0}" name="AGI" dataDxfId="109">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.5 + 15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="100">
+    <tableColumn id="9" xr3:uid="{0C309EA8-7C68-414C-9AEF-19A3079055BC}" name="LUK" dataDxfId="108">
       <calculatedColumnFormula>Table131679[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2603,28 +2633,28 @@
   <autoFilter ref="K8:S14" xr:uid="{AB7E938D-7ACC-4BFB-A6B9-682B8B29CEF2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{66EB8EF1-BCF4-44F7-B8A6-3C3B425F8FF5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="254">
+    <tableColumn id="2" xr3:uid="{EADBE3A7-BA36-40E2-AAFD-C66683EE9BBF}" name="HP" dataDxfId="262">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*56.25+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="253">
+    <tableColumn id="3" xr3:uid="{562074CC-9FA5-4DCD-9CD7-0BF99E403D1D}" name="MP" dataDxfId="261">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="252">
+    <tableColumn id="4" xr3:uid="{CA308242-617E-4D28-8842-309A46576513}" name="ATK" dataDxfId="260">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25+ 15+30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="251">
+    <tableColumn id="5" xr3:uid="{8DEFEC48-72A2-4000-BBAC-49E6AAC4CFA7}" name="DEF" dataDxfId="259">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1.25 + 15+33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="250">
+    <tableColumn id="6" xr3:uid="{B08936F6-A9CF-4FDB-88B5-260CD2AB0EC9}" name="MAT" dataDxfId="258">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="249">
+    <tableColumn id="7" xr3:uid="{BFBA5362-FC90-4144-922B-553D2C152D05}" name="MDF" dataDxfId="257">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1+15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="248">
+    <tableColumn id="8" xr3:uid="{AC746062-EE21-4939-ACAD-9BB491959CF0}" name="AGI" dataDxfId="256">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="247">
+    <tableColumn id="9" xr3:uid="{2F766C3C-A331-48B3-8271-4C32811B2BB3}" name="LUK" dataDxfId="255">
       <calculatedColumnFormula>Table131611[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2637,28 +2667,28 @@
   <autoFilter ref="A26:I31" xr:uid="{870F76F2-5EA7-4FD7-B1F9-507D64592088}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{3C04B742-338A-4366-BF3D-C5BC13023785}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="99">
+    <tableColumn id="2" xr3:uid="{311B5B5D-94D8-4564-862A-CCEB5AFD3A6D}" name="HP" dataDxfId="107">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*63+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="98">
+    <tableColumn id="3" xr3:uid="{BAA0998C-C9BA-4131-BCFC-05790596DB78}" name="MP" dataDxfId="106">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="97">
+    <tableColumn id="4" xr3:uid="{01F6813D-3052-455F-8D17-6AAE233215C4}" name="ATK" dataDxfId="105">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="96">
+    <tableColumn id="5" xr3:uid="{B48E24B7-D7BD-4C2D-A60C-0393FF7535C3}" name="DEF" dataDxfId="104">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.375 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="95">
+    <tableColumn id="6" xr3:uid="{13BA118E-6B00-4F41-9AFE-6F1E4548C218}" name="MAT" dataDxfId="103">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="94">
+    <tableColumn id="7" xr3:uid="{2ED3B673-EB80-40C4-80C0-583E0B6370DB}" name="MDF" dataDxfId="102">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="93">
+    <tableColumn id="8" xr3:uid="{5AD00210-9BCE-4AF3-9075-1C6B934E686C}" name="AGI" dataDxfId="101">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="92">
+    <tableColumn id="9" xr3:uid="{02B9C036-A321-4EBE-90DF-CF68CB6FB35E}" name="LUK" dataDxfId="100">
       <calculatedColumnFormula>Table1316717[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2671,28 +2701,28 @@
   <autoFilter ref="A36:I41" xr:uid="{9BD043AF-0D77-4FF4-B2F9-B4AC3C3F1F82}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{7BB908A3-05D7-4357-920B-BF4C6BC20C06}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="91">
+    <tableColumn id="2" xr3:uid="{346E2BC5-B5D5-44A0-84D6-859E1B4DC76D}" name="HP" dataDxfId="99">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*56.5+200</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="90">
+    <tableColumn id="3" xr3:uid="{48184CEA-2CA3-4CEA-8AE5-71C005FA24C9}" name="MP" dataDxfId="98">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*12.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="89">
+    <tableColumn id="4" xr3:uid="{3B46ED9A-2E4B-401C-B83E-32CE8A74CB32}" name="ATK" dataDxfId="97">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="88">
+    <tableColumn id="5" xr3:uid="{E3091C6D-70B6-453C-B493-8D9CC0DD5C37}" name="DEF" dataDxfId="96">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1 + 15+14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="87">
+    <tableColumn id="6" xr3:uid="{C2E89F50-3D99-49B9-8E98-20EFA4CBA8EB}" name="MAT" dataDxfId="95">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="86">
+    <tableColumn id="7" xr3:uid="{51AF53BA-4D3D-4ABA-A3CC-2F9EF73D34CB}" name="MDF" dataDxfId="94">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.5+ 15+13</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="85">
+    <tableColumn id="8" xr3:uid="{285CB6EF-4E49-4066-90AB-68B42C1B2989}" name="AGI" dataDxfId="93">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="84">
+    <tableColumn id="9" xr3:uid="{34BE8683-723F-43E8-AE99-E2D525D32717}" name="LUK" dataDxfId="92">
       <calculatedColumnFormula>Table13167173[[#This Row],[Level]]*1.375 + 15+40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2713,7 +2743,7 @@
     <tableColumn id="7" xr3:uid="{09E4151E-54A0-41FF-BA5B-3B1C748DA23D}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{909575E0-EC13-4E35-A35F-2451A5741589}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2CDCF32E-D8FC-48D9-A28D-8D9C5F3EB001}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{001DA1BB-34DD-4786-BDE4-23C510900A3D}" name="Total" dataDxfId="83">
+    <tableColumn id="10" xr3:uid="{001DA1BB-34DD-4786-BDE4-23C510900A3D}" name="Total" dataDxfId="91">
       <calculatedColumnFormula>SUM(Table168213429[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2726,28 +2756,28 @@
   <autoFilter ref="A7:I12" xr:uid="{4ED64482-035D-49B9-A477-A1D5AEB4A5A4}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{141B0E2E-D4F3-4884-86FD-AAD67C363749}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{D4B50877-EF56-4EF7-8C6D-9928A6D654F6}" name="HP" dataDxfId="82">
+    <tableColumn id="2" xr3:uid="{D4B50877-EF56-4EF7-8C6D-9928A6D654F6}" name="HP" dataDxfId="90">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*125</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F4B06187-BE28-4283-9518-F773FE75C2BF}" name="MP" dataDxfId="81">
+    <tableColumn id="3" xr3:uid="{F4B06187-BE28-4283-9518-F773FE75C2BF}" name="MP" dataDxfId="89">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{91A68FC7-5F16-4880-AE82-97341814BB95}" name="ATK" dataDxfId="80">
+    <tableColumn id="4" xr3:uid="{91A68FC7-5F16-4880-AE82-97341814BB95}" name="ATK" dataDxfId="88">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*4.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{2BCD0E58-85DE-4C10-BFBC-AF77BC569C92}" name="DEF" dataDxfId="79">
+    <tableColumn id="5" xr3:uid="{2BCD0E58-85DE-4C10-BFBC-AF77BC569C92}" name="DEF" dataDxfId="87">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7C48A1FC-CE8F-4CDD-9A3D-308B46D78A48}" name="MAT" dataDxfId="78">
+    <tableColumn id="6" xr3:uid="{7C48A1FC-CE8F-4CDD-9A3D-308B46D78A48}" name="MAT" dataDxfId="86">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{474D8178-EA8C-4322-93C3-B7F6EBA88102}" name="MDF" dataDxfId="77">
+    <tableColumn id="7" xr3:uid="{474D8178-EA8C-4322-93C3-B7F6EBA88102}" name="MDF" dataDxfId="85">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{257B31D9-5838-45E0-A56E-9B1566E1A34A}" name="AGI" dataDxfId="76">
+    <tableColumn id="8" xr3:uid="{257B31D9-5838-45E0-A56E-9B1566E1A34A}" name="AGI" dataDxfId="84">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{17960EB4-4250-49DB-9A6B-455B9913B04B}" name="LUK" dataDxfId="75">
+    <tableColumn id="9" xr3:uid="{17960EB4-4250-49DB-9A6B-455B9913B04B}" name="LUK" dataDxfId="83">
       <calculatedColumnFormula>Table1316183336[[#This Row],[Level]]*1.125</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2768,7 +2798,7 @@
     <tableColumn id="7" xr3:uid="{07EA0638-8880-4944-AC9E-13E3F1B9F651}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{AA18E602-126F-4D69-9CC8-C097E8EB9C70}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{5563B0CB-2EA7-4851-8D1F-D77E0F90CBAD}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{2D960B43-0F76-4936-9508-4D501A79A83C}" name="Total" dataDxfId="74">
+    <tableColumn id="10" xr3:uid="{2D960B43-0F76-4936-9508-4D501A79A83C}" name="Total" dataDxfId="82">
       <calculatedColumnFormula>SUM(Table16821342932[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2781,28 +2811,28 @@
   <autoFilter ref="A5:I10" xr:uid="{2922C913-6AE8-4B89-BDA6-9F44D59987D8}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{3D67222C-6501-4A5D-A9FC-528EE591A288}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EE3E4CCC-C404-4B78-AAB4-3B38166E23BA}" name="HP" dataDxfId="73">
+    <tableColumn id="2" xr3:uid="{EE3E4CCC-C404-4B78-AAB4-3B38166E23BA}" name="HP" dataDxfId="81">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DE5141FB-3B4E-46D4-9E0D-AF1DEE998B4A}" name="MP" dataDxfId="72">
+    <tableColumn id="3" xr3:uid="{DE5141FB-3B4E-46D4-9E0D-AF1DEE998B4A}" name="MP" dataDxfId="80">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{404B3E88-DF62-4AA0-82D6-C21C2BCA762B}" name="ATK" dataDxfId="71">
+    <tableColumn id="4" xr3:uid="{404B3E88-DF62-4AA0-82D6-C21C2BCA762B}" name="ATK" dataDxfId="79">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*4.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{342B3F39-F7A2-45D8-9CD4-39B5ABC72D2F}" name="DEF" dataDxfId="70">
+    <tableColumn id="5" xr3:uid="{342B3F39-F7A2-45D8-9CD4-39B5ABC72D2F}" name="DEF" dataDxfId="78">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{CD819DB3-9F2E-4428-AAFC-72776ECB8EAF}" name="MAT" dataDxfId="69">
+    <tableColumn id="6" xr3:uid="{CD819DB3-9F2E-4428-AAFC-72776ECB8EAF}" name="MAT" dataDxfId="77">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{270DF964-8095-43FD-B050-DD4A2A138F32}" name="MDF" dataDxfId="68">
+    <tableColumn id="7" xr3:uid="{270DF964-8095-43FD-B050-DD4A2A138F32}" name="MDF" dataDxfId="76">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4F4D3B2A-5B86-4AB7-A97E-18E2868266B8}" name="AGI" dataDxfId="67">
+    <tableColumn id="8" xr3:uid="{4F4D3B2A-5B86-4AB7-A97E-18E2868266B8}" name="AGI" dataDxfId="75">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{0178CE2D-63C5-426A-A081-D62E62FF91AC}" name="LUK" dataDxfId="66">
+    <tableColumn id="9" xr3:uid="{0178CE2D-63C5-426A-A081-D62E62FF91AC}" name="LUK" dataDxfId="74">
       <calculatedColumnFormula>Table131618333637[[#This Row],[Level]]*1.5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2823,7 +2853,7 @@
     <tableColumn id="7" xr3:uid="{C374A90B-690A-432C-974A-C8A7D22E367F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{05C64890-0DC2-4577-975E-95477DCED789}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{CE6AAEA9-D599-4B9B-BD40-7E602F47088C}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{30017AE7-6C23-415F-A2EA-70EA09C835E6}" name="Total" dataDxfId="65">
+    <tableColumn id="10" xr3:uid="{30017AE7-6C23-415F-A2EA-70EA09C835E6}" name="Total" dataDxfId="73">
       <calculatedColumnFormula>SUM(Table1682134293227[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2836,28 +2866,28 @@
   <autoFilter ref="A6:I11" xr:uid="{D09397F4-7631-4CD3-AF40-3B14C64478EE}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BF4E6A79-8CCF-498E-B3B0-FA782AB06519}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{37E52E57-C499-4FFB-AC3F-20E63EEA4D3A}" name="HP" dataDxfId="64">
+    <tableColumn id="2" xr3:uid="{37E52E57-C499-4FFB-AC3F-20E63EEA4D3A}" name="HP" dataDxfId="72">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*87.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D29F5CDE-1200-4C77-A4BA-0DE4F7C46627}" name="MP" dataDxfId="63">
+    <tableColumn id="3" xr3:uid="{D29F5CDE-1200-4C77-A4BA-0DE4F7C46627}" name="MP" dataDxfId="71">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{9701140A-64F9-4967-9DEE-3460411D91C1}" name="ATK" dataDxfId="62">
+    <tableColumn id="4" xr3:uid="{9701140A-64F9-4967-9DEE-3460411D91C1}" name="ATK" dataDxfId="70">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F90A425E-E031-4255-8AF9-DAD672F8DD7D}" name="DEF" dataDxfId="61">
+    <tableColumn id="5" xr3:uid="{F90A425E-E031-4255-8AF9-DAD672F8DD7D}" name="DEF" dataDxfId="69">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*4.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{255210A0-6EB8-4CFB-84DD-42C88AEAF7AA}" name="MAT" dataDxfId="60">
+    <tableColumn id="6" xr3:uid="{255210A0-6EB8-4CFB-84DD-42C88AEAF7AA}" name="MAT" dataDxfId="68">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{91177FDD-F316-4D6B-A547-FC5FA6DAC266}" name="MDF" dataDxfId="59">
+    <tableColumn id="7" xr3:uid="{91177FDD-F316-4D6B-A547-FC5FA6DAC266}" name="MDF" dataDxfId="67">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{ADA902F7-B7D7-4B1B-A144-E5252296AB61}" name="AGI" dataDxfId="58">
+    <tableColumn id="8" xr3:uid="{ADA902F7-B7D7-4B1B-A144-E5252296AB61}" name="AGI" dataDxfId="66">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{78273DA6-F2CA-4999-B4EA-F6C044BC41AB}" name="LUK" dataDxfId="57">
+    <tableColumn id="9" xr3:uid="{78273DA6-F2CA-4999-B4EA-F6C044BC41AB}" name="LUK" dataDxfId="65">
       <calculatedColumnFormula>Table13161833363738[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2870,28 +2900,28 @@
   <autoFilter ref="A4:I9" xr:uid="{DD778A26-93EC-4B14-A9D1-160AE03B48D3}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F0A3DB96-38E4-4CD0-BAF6-C8BB768B1256}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{07B77441-F84C-41C6-A00C-B69369FBF0F1}" name="HP" dataDxfId="56">
+    <tableColumn id="2" xr3:uid="{07B77441-F84C-41C6-A00C-B69369FBF0F1}" name="HP" dataDxfId="64">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*75 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{2DBE06DE-38E0-4433-B590-3850C554BB8E}" name="MP" dataDxfId="55">
+    <tableColumn id="3" xr3:uid="{2DBE06DE-38E0-4433-B590-3850C554BB8E}" name="MP" dataDxfId="63">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DE8CC9D0-45D8-4F85-9317-09844C8D4DD7}" name="ATK" dataDxfId="54">
+    <tableColumn id="4" xr3:uid="{DE8CC9D0-45D8-4F85-9317-09844C8D4DD7}" name="ATK" dataDxfId="62">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1.375+ 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{9D33BCF5-CDB6-4BB0-8603-810E71EE1C47}" name="DEF" dataDxfId="53">
+    <tableColumn id="5" xr3:uid="{9D33BCF5-CDB6-4BB0-8603-810E71EE1C47}" name="DEF" dataDxfId="61">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1.375 + 15 + 19</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{1693AB2F-85DB-4286-A43C-82A15CDDA173}" name="MAT" dataDxfId="52">
+    <tableColumn id="6" xr3:uid="{1693AB2F-85DB-4286-A43C-82A15CDDA173}" name="MAT" dataDxfId="60">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{DCA68233-62C9-4E66-9306-24AE49EE344C}" name="MDF" dataDxfId="51">
+    <tableColumn id="7" xr3:uid="{DCA68233-62C9-4E66-9306-24AE49EE344C}" name="MDF" dataDxfId="59">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1 + 15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{60943D8A-0008-4FFE-AE90-4DDEB0149A21}" name="AGI" dataDxfId="50">
+    <tableColumn id="8" xr3:uid="{60943D8A-0008-4FFE-AE90-4DDEB0149A21}" name="AGI" dataDxfId="58">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E7EC6C93-3486-414B-87DB-F4D38BB2A0DC}" name="LUK" dataDxfId="49">
+    <tableColumn id="9" xr3:uid="{E7EC6C93-3486-414B-87DB-F4D38BB2A0DC}" name="LUK" dataDxfId="57">
       <calculatedColumnFormula>Table131639[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2904,28 +2934,28 @@
   <autoFilter ref="A12:I16" xr:uid="{2A794F38-5DB8-40A3-A8E2-90B5A0A4A192}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{C5A2CF3A-0965-428C-AD05-883EDB0D400F}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{C8840580-F723-4CA3-A107-42FCC677D424}" name="HP" dataDxfId="48">
+    <tableColumn id="2" xr3:uid="{C8840580-F723-4CA3-A107-42FCC677D424}" name="HP" dataDxfId="56">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*62.5+ 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5D9241C6-74A5-4C1F-A8F7-69DB1BDA83FE}" name="MP" dataDxfId="47">
+    <tableColumn id="3" xr3:uid="{5D9241C6-74A5-4C1F-A8F7-69DB1BDA83FE}" name="MP" dataDxfId="55">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*12.5+60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D98F9CCD-2FEF-4FB2-B5AD-D2A6B610781B}" name="ATK" dataDxfId="46">
+    <tableColumn id="4" xr3:uid="{D98F9CCD-2FEF-4FB2-B5AD-D2A6B610781B}" name="ATK" dataDxfId="54">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CF1AF448-2207-48D1-8FE3-0A6B5DE3511C}" name="DEF" dataDxfId="45">
+    <tableColumn id="5" xr3:uid="{CF1AF448-2207-48D1-8FE3-0A6B5DE3511C}" name="DEF" dataDxfId="53">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1 + 15 + 10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A632BAA7-E71C-41F8-B5B0-90891BB5BA9B}" name="MAT" dataDxfId="44">
+    <tableColumn id="6" xr3:uid="{A632BAA7-E71C-41F8-B5B0-90891BB5BA9B}" name="MAT" dataDxfId="52">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E76132BC-BC67-4915-8112-E0B292C65C91}" name="MDF" dataDxfId="43">
+    <tableColumn id="7" xr3:uid="{E76132BC-BC67-4915-8112-E0B292C65C91}" name="MDF" dataDxfId="51">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1 + 15 + 8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B25B7E33-B3CF-4D3D-9A14-3CE5B75535E8}" name="AGI" dataDxfId="42">
+    <tableColumn id="8" xr3:uid="{B25B7E33-B3CF-4D3D-9A14-3CE5B75535E8}" name="AGI" dataDxfId="50">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{40820F61-4B4C-4B23-95CF-AD5CDE975F4A}" name="LUK" dataDxfId="41">
+    <tableColumn id="9" xr3:uid="{40820F61-4B4C-4B23-95CF-AD5CDE975F4A}" name="LUK" dataDxfId="49">
       <calculatedColumnFormula>Table13182227[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2946,7 +2976,7 @@
     <tableColumn id="7" xr3:uid="{F833922A-76F9-427C-8462-D94DE51D0477}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{203171A1-C88B-4F81-ADC2-1EE072D645F3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{34003EF6-E9A5-4584-A186-09DFF4EC11C7}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{C4602156-F897-42BE-8F3F-411E13EEB095}" name="Total" dataDxfId="246">
+    <tableColumn id="10" xr3:uid="{C4602156-F897-42BE-8F3F-411E13EEB095}" name="Total" dataDxfId="254">
       <calculatedColumnFormula>SUM(Table114[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2959,28 +2989,28 @@
   <autoFilter ref="A20:I24" xr:uid="{6015D08B-C4A1-43B9-B8BF-6F441CC08DCA}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D4205A68-390A-4750-8556-3B4847E58D16}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{D7D1DEBE-6CE0-4976-A401-D4F35A038AA9}" name="HP" dataDxfId="40">
+    <tableColumn id="2" xr3:uid="{D7D1DEBE-6CE0-4976-A401-D4F35A038AA9}" name="HP" dataDxfId="48">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{3CB0ED8A-F14B-4E5F-8474-F3034EA78A85}" name="MP" dataDxfId="39">
+    <tableColumn id="3" xr3:uid="{3CB0ED8A-F14B-4E5F-8474-F3034EA78A85}" name="MP" dataDxfId="47">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*15+100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F3186E07-87BD-4E53-8F85-AB4798362B0C}" name="ATK" dataDxfId="38">
+    <tableColumn id="4" xr3:uid="{F3186E07-87BD-4E53-8F85-AB4798362B0C}" name="ATK" dataDxfId="46">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1+ 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{22ED75D6-B85C-4DF9-BC39-4154BAF3990E}" name="DEF" dataDxfId="37">
+    <tableColumn id="5" xr3:uid="{22ED75D6-B85C-4DF9-BC39-4154BAF3990E}" name="DEF" dataDxfId="45">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1 + 15 + 4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B2DFC87A-2BEE-4B5A-AF53-4E18078ABC1B}" name="MAT" dataDxfId="36">
+    <tableColumn id="6" xr3:uid="{B2DFC87A-2BEE-4B5A-AF53-4E18078ABC1B}" name="MAT" dataDxfId="44">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.375 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{8FF82542-4129-4E67-AA7B-7CB38D8FB051}" name="MDF" dataDxfId="35">
+    <tableColumn id="7" xr3:uid="{8FF82542-4129-4E67-AA7B-7CB38D8FB051}" name="MDF" dataDxfId="43">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.375 + 15 + 14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{85F4097E-90A5-4A7C-B184-42B110E62300}" name="AGI" dataDxfId="34">
+    <tableColumn id="8" xr3:uid="{85F4097E-90A5-4A7C-B184-42B110E62300}" name="AGI" dataDxfId="42">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E1A21F56-D819-4CE3-9122-F47B8A4039A9}" name="LUK" dataDxfId="33">
+    <tableColumn id="9" xr3:uid="{E1A21F56-D819-4CE3-9122-F47B8A4039A9}" name="LUK" dataDxfId="41">
       <calculatedColumnFormula>Table13162044[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2993,28 +3023,28 @@
   <autoFilter ref="A27:I30" xr:uid="{4506A984-1EE8-4D0B-9AFB-6DE5576F3317}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{97BB3945-930E-41A9-B479-678FD9D8EE85}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{2197951B-D7A2-413F-8152-C8BB282E3498}" name="HP" dataDxfId="32">
+    <tableColumn id="2" xr3:uid="{2197951B-D7A2-413F-8152-C8BB282E3498}" name="HP" dataDxfId="40">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*62.5+ 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{54D89380-BDA0-4B18-8B8B-482E9AA62AD3}" name="MP" dataDxfId="31">
+    <tableColumn id="3" xr3:uid="{54D89380-BDA0-4B18-8B8B-482E9AA62AD3}" name="MP" dataDxfId="39">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*12.5+60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DCD1A325-B7AE-4283-89E4-85446F157A12}" name="ATK" dataDxfId="30">
+    <tableColumn id="4" xr3:uid="{DCD1A325-B7AE-4283-89E4-85446F157A12}" name="ATK" dataDxfId="38">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1CD051D4-B531-4706-95A8-BBF452C5188D}" name="DEF" dataDxfId="29">
+    <tableColumn id="5" xr3:uid="{1CD051D4-B531-4706-95A8-BBF452C5188D}" name="DEF" dataDxfId="37">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.25 + 15 + 19</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{E17A43F1-7669-40E6-BD8C-8623B203A60F}" name="MAT" dataDxfId="28">
+    <tableColumn id="6" xr3:uid="{E17A43F1-7669-40E6-BD8C-8623B203A60F}" name="MAT" dataDxfId="36">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.125 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{04F7D6BA-3673-4BE0-97CA-65C8DD4612E3}" name="MDF" dataDxfId="27">
+    <tableColumn id="7" xr3:uid="{04F7D6BA-3673-4BE0-97CA-65C8DD4612E3}" name="MDF" dataDxfId="35">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.25 + 15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{7AA9AD24-2AFF-4204-AAEF-0CC3265C40FA}" name="AGI" dataDxfId="26">
+    <tableColumn id="8" xr3:uid="{7AA9AD24-2AFF-4204-AAEF-0CC3265C40FA}" name="AGI" dataDxfId="34">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{ABFCE932-20B6-4AEE-A261-B747D2EC6FA8}" name="LUK" dataDxfId="25">
+    <tableColumn id="9" xr3:uid="{ABFCE932-20B6-4AEE-A261-B747D2EC6FA8}" name="LUK" dataDxfId="33">
       <calculatedColumnFormula>Table131822[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3023,32 +3053,32 @@
 </file>
 
 <file path=xl/tables/table42.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="45" xr:uid="{B9200053-35AC-4923-AC77-58FBB0806D21}" name="Table13163946" displayName="Table13163946" ref="L4:T9" totalsRowShown="0">
-  <autoFilter ref="L4:T9" xr:uid="{7E10C2C1-D4A2-4595-8F68-D39C5EF91F11}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="45" xr:uid="{B9200053-35AC-4923-AC77-58FBB0806D21}" name="Table13163946" displayName="Table13163946" ref="P4:X9" totalsRowShown="0">
+  <autoFilter ref="P4:X9" xr:uid="{7E10C2C1-D4A2-4595-8F68-D39C5EF91F11}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0DA2010E-5B86-4EB0-A1CB-2F1DA2E20D55}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{18F550C2-BA99-442C-BEF0-F2A727225321}" name="HP" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{18F550C2-BA99-442C-BEF0-F2A727225321}" name="HP" dataDxfId="32">
       <calculatedColumnFormula>Table13163946[[#This Row],[Level]]*106.25 + 500</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{AF6041D8-0897-4671-9A81-6EE8816F6BBE}" name="MP" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{AF6041D8-0897-4671-9A81-6EE8816F6BBE}" name="MP" dataDxfId="31">
       <calculatedColumnFormula>Table13163946[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E65D65BD-05C4-4A9B-ABA0-B601294BE295}" name="ATK" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{E65D65BD-05C4-4A9B-ABA0-B601294BE295}" name="ATK" dataDxfId="30">
       <calculatedColumnFormula>Table13163946[[#This Row],[Level]]*2.125+ 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{778501FE-4E31-4734-A31A-EEEE7EF05B63}" name="DEF" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{778501FE-4E31-4734-A31A-EEEE7EF05B63}" name="DEF" dataDxfId="29">
       <calculatedColumnFormula>Table13163946[[#This Row],[Level]]*2.125 + 15 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B5B2244A-14A8-46D8-BF8F-67AC8D3241DA}" name="MAT" dataDxfId="6">
+    <tableColumn id="6" xr3:uid="{B5B2244A-14A8-46D8-BF8F-67AC8D3241DA}" name="MAT" dataDxfId="28">
       <calculatedColumnFormula>Table13163946[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9A962E99-0281-41D8-9287-E65CD6E131FB}" name="MDF" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{9A962E99-0281-41D8-9287-E65CD6E131FB}" name="MDF" dataDxfId="27">
       <calculatedColumnFormula>Table13163946[[#This Row],[Level]]*2.125 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{1AEB996E-4494-401F-BBA6-260C80317786}" name="AGI" dataDxfId="3">
+    <tableColumn id="8" xr3:uid="{1AEB996E-4494-401F-BBA6-260C80317786}" name="AGI" dataDxfId="26">
       <calculatedColumnFormula>Table13163946[[#This Row],[Level]]*1.5 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9670DFBA-0FF6-4756-ACBC-24B43785B711}" name="LUK" dataDxfId="2">
+    <tableColumn id="9" xr3:uid="{9670DFBA-0FF6-4756-ACBC-24B43785B711}" name="LUK" dataDxfId="25">
       <calculatedColumnFormula>Table13163946[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3057,6 +3087,40 @@
 </file>
 
 <file path=xl/tables/table43.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="47" xr:uid="{C94EF299-00E0-43B9-883C-EE42B8F651D8}" name="Table13163948" displayName="Table13163948" ref="P17:X22" totalsRowShown="0">
+  <autoFilter ref="P17:X22" xr:uid="{34DCA2BD-7E90-4BA9-882D-4A0B5CA055A2}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{2AC3EA1B-ED8B-468F-B2A6-478A7888C995}" name="Level"/>
+    <tableColumn id="2" xr3:uid="{11C9D480-A783-4641-BBCD-983BB72FDE5E}" name="HP" dataDxfId="0">
+      <calculatedColumnFormula>Table13163948[[#This Row],[Level]]*75 + 500 + 800</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{03905492-344D-488D-BA0A-796528D82C7E}" name="MP" dataDxfId="7">
+      <calculatedColumnFormula>Table13163948[[#This Row],[Level]]*10+20</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{F7DA4593-8DF4-45AC-B00B-B64FDCC5B736}" name="ATK" dataDxfId="6">
+      <calculatedColumnFormula>Table13163948[[#This Row],[Level]]*1.375+ 15 + 40</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{53D3990A-7FA7-46A4-830F-4FB19D3D6B6B}" name="DEF" dataDxfId="2">
+      <calculatedColumnFormula>Table13163948[[#This Row],[Level]]*1.375 + 15 + 21</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{6DF255D1-55F9-4368-A244-C7F30A95F80B}" name="MAT" dataDxfId="5">
+      <calculatedColumnFormula>Table13163948[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{3FCEFA1B-B764-42CB-BA1A-3C45F9507B46}" name="MDF" dataDxfId="1">
+      <calculatedColumnFormula>Table13163948[[#This Row],[Level]]*1 + 15 + 7</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{3774B5F6-1896-4C00-9EB2-5E37E70AFBEA}" name="AGI" dataDxfId="4">
+      <calculatedColumnFormula>Table13163948[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{8F366B0D-3C62-4955-826F-672B2C04A72E}" name="LUK" dataDxfId="3">
+      <calculatedColumnFormula>Table13163948[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table44.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="42" xr:uid="{B11B1E6C-19A5-42E4-847D-0CD22EB4A103}" name="Table1318222743" displayName="Table1318222743" ref="A3:I7" totalsRowShown="0">
   <autoFilter ref="A3:I7" xr:uid="{7F8360B3-D323-4505-8E52-764F2EEFEF08}"/>
   <tableColumns count="9">
@@ -3090,7 +3154,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table45.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="44" xr:uid="{63EFECE9-294D-4BD5-B983-D7DF0138B45B}" name="Table168213429322745" displayName="Table168213429322745" ref="A4:J6" totalsRowShown="0">
   <autoFilter ref="A4:J6" xr:uid="{9FA97447-7595-4CE0-9387-AEB91FE50244}"/>
   <tableColumns count="10">
@@ -3111,7 +3175,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table46.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="46" xr:uid="{6B246BF5-6CE4-4B50-8843-8DACC434192B}" name="Table1316183336373847" displayName="Table1316183336373847" ref="A8:I13" totalsRowShown="0">
   <autoFilter ref="A8:I13" xr:uid="{F3DE48F5-A98B-4A15-8805-1948F568C45F}"/>
   <tableColumns count="9">
@@ -3150,28 +3214,28 @@
   <autoFilter ref="A8:I14" xr:uid="{D3C3F418-ED32-4504-9D73-88545A192967}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{13E0AF4A-AA83-489A-A156-B01D4F48D2F5}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{B970139F-8BB5-4CE6-92F8-79E3236AC62B}" name="HP" dataDxfId="245">
+    <tableColumn id="2" xr3:uid="{B970139F-8BB5-4CE6-92F8-79E3236AC62B}" name="HP" dataDxfId="253">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*63+300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7BCF83B8-7492-4991-A008-F212725940B9}" name="MP" dataDxfId="244">
+    <tableColumn id="3" xr3:uid="{7BCF83B8-7492-4991-A008-F212725940B9}" name="MP" dataDxfId="252">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{33220A80-38D8-4480-ACC7-DF484072C96B}" name="ATK" dataDxfId="243">
+    <tableColumn id="4" xr3:uid="{33220A80-38D8-4480-ACC7-DF484072C96B}" name="ATK" dataDxfId="251">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.5+ 15+40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{36708515-5004-4705-A558-44B59D0CE676}" name="DEF" dataDxfId="242">
+    <tableColumn id="5" xr3:uid="{36708515-5004-4705-A558-44B59D0CE676}" name="DEF" dataDxfId="250">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25 + 15+21</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{11729EA3-08C4-4E0B-B5EE-5B3C08A31A9C}" name="MAT" dataDxfId="241">
+    <tableColumn id="6" xr3:uid="{11729EA3-08C4-4E0B-B5EE-5B3C08A31A9C}" name="MAT" dataDxfId="249">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B179D090-E484-4663-937A-480D1164D655}" name="MDF" dataDxfId="240">
+    <tableColumn id="7" xr3:uid="{B179D090-E484-4663-937A-480D1164D655}" name="MDF" dataDxfId="248">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25+15 + 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{28323AD0-B3BD-401F-A237-92C8B8D70FEA}" name="AGI" dataDxfId="239">
+    <tableColumn id="8" xr3:uid="{28323AD0-B3BD-401F-A237-92C8B8D70FEA}" name="AGI" dataDxfId="247">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{657BED8B-4C8A-42DC-BECD-5EEF9D1B7F37}" name="LUK" dataDxfId="238">
+    <tableColumn id="9" xr3:uid="{657BED8B-4C8A-42DC-BECD-5EEF9D1B7F37}" name="LUK" dataDxfId="246">
       <calculatedColumnFormula>Table13161123[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3192,7 +3256,7 @@
     <tableColumn id="7" xr3:uid="{D1DFC0D2-A987-4E3F-BA23-52162FB0C0BA}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{AB6209DB-CCCB-4C37-B455-4C7652E0DAC9}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{2CD4CD14-92FD-41A7-9CCD-1329B5A77390}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{3B2C0A10-5038-4C21-BAC5-12FB16275D2E}" name="Total" dataDxfId="237">
+    <tableColumn id="10" xr3:uid="{3B2C0A10-5038-4C21-BAC5-12FB16275D2E}" name="Total" dataDxfId="245">
       <calculatedColumnFormula>SUM(Table11412[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3205,28 +3269,28 @@
   <autoFilter ref="A8:I14" xr:uid="{43F790D1-EA7B-4BAE-8A37-7CAD791E8821}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F6E842E1-B25F-4CA1-9107-AC7179420C29}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{EFB2F0D5-318D-4A65-BA2B-20ADDE071648}" name="HP" dataDxfId="236">
+    <tableColumn id="2" xr3:uid="{EFB2F0D5-318D-4A65-BA2B-20ADDE071648}" name="HP" dataDxfId="244">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*50 + 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{0D914B89-2678-453F-BC18-571DCD45E628}" name="MP" dataDxfId="235">
+    <tableColumn id="3" xr3:uid="{0D914B89-2678-453F-BC18-571DCD45E628}" name="MP" dataDxfId="243">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*13.75 + 80</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{6FBD2F64-5B1C-4035-BB1A-AFB092DB60C3}" name="ATK" dataDxfId="234">
+    <tableColumn id="4" xr3:uid="{6FBD2F64-5B1C-4035-BB1A-AFB092DB60C3}" name="ATK" dataDxfId="242">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7E0AF3FC-CC5D-4A6A-A4A2-DE278DEC4062}" name="DEF" dataDxfId="233">
+    <tableColumn id="5" xr3:uid="{7E0AF3FC-CC5D-4A6A-A4A2-DE278DEC4062}" name="DEF" dataDxfId="241">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1 + 15 + 4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3AF4D559-893B-4D50-BCB4-A1BD1FAF2F23}" name="MAT" dataDxfId="232">
+    <tableColumn id="6" xr3:uid="{3AF4D559-893B-4D50-BCB4-A1BD1FAF2F23}" name="MAT" dataDxfId="240">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6E9418A6-75AC-4541-9029-814EC5C06E70}" name="MDF" dataDxfId="231">
+    <tableColumn id="7" xr3:uid="{6E9418A6-75AC-4541-9029-814EC5C06E70}" name="MDF" dataDxfId="239">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.375+15 + 14</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD605BEE-D561-4A2C-8D06-8E9AD70C32AC}" name="AGI" dataDxfId="230">
+    <tableColumn id="8" xr3:uid="{CD605BEE-D561-4A2C-8D06-8E9AD70C32AC}" name="AGI" dataDxfId="238">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E26506B2-F488-4AA4-AC87-819A22964609}" name="LUK" dataDxfId="229">
+    <tableColumn id="9" xr3:uid="{E26506B2-F488-4AA4-AC87-819A22964609}" name="LUK" dataDxfId="237">
       <calculatedColumnFormula>Table1316112324[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3247,7 +3311,7 @@
     <tableColumn id="7" xr3:uid="{E91A64A8-F750-4893-9958-7C6ABC37405F}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{3832FF0E-95E5-4B1F-B122-1EAFBF719DE3}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{237404A9-EB50-465E-89AF-7167C57AFB99}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{927EBD24-571F-408C-A33B-59C753D9D96D}" name="Total" dataDxfId="228">
+    <tableColumn id="10" xr3:uid="{927EBD24-571F-408C-A33B-59C753D9D96D}" name="Total" dataDxfId="236">
       <calculatedColumnFormula>SUM(Table1141219[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3260,28 +3324,28 @@
   <autoFilter ref="A7:I13" xr:uid="{2539D8EE-2982-4734-B28B-342036FEDAC6}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FEE8F081-132E-4ED3-8FFD-2CF48368B2CC}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{A79BC043-DB1A-48B4-AC21-AD31632979A6}" name="HP" dataDxfId="227">
+    <tableColumn id="2" xr3:uid="{A79BC043-DB1A-48B4-AC21-AD31632979A6}" name="HP" dataDxfId="235">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*63 + 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{42935B44-C727-42B0-B48E-0369818BF78A}" name="MP" dataDxfId="226">
+    <tableColumn id="3" xr3:uid="{42935B44-C727-42B0-B48E-0369818BF78A}" name="MP" dataDxfId="234">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*10 + 20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{FC4572C7-88EC-4981-A6ED-43397844845B}" name="ATK" dataDxfId="225">
+    <tableColumn id="4" xr3:uid="{FC4572C7-88EC-4981-A6ED-43397844845B}" name="ATK" dataDxfId="233">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C8D61CEB-FFEC-42C3-9123-5140E65C1A2C}" name="DEF" dataDxfId="224">
+    <tableColumn id="5" xr3:uid="{C8D61CEB-FFEC-42C3-9123-5140E65C1A2C}" name="DEF" dataDxfId="232">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.375 + 15 + 19</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8C971683-28D2-4474-83CA-936F352F1324}" name="MAT" dataDxfId="223">
+    <tableColumn id="6" xr3:uid="{8C971683-28D2-4474-83CA-936F352F1324}" name="MAT" dataDxfId="231">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3371862A-9CF2-47CA-A149-4921E3B33162}" name="MDF" dataDxfId="222">
+    <tableColumn id="7" xr3:uid="{3371862A-9CF2-47CA-A149-4921E3B33162}" name="MDF" dataDxfId="230">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.375+15 + 5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AC6AC739-B4C9-47A6-9472-439C60B629A0}" name="AGI" dataDxfId="221">
+    <tableColumn id="8" xr3:uid="{AC6AC739-B4C9-47A6-9472-439C60B629A0}" name="AGI" dataDxfId="229">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{E727A271-B479-47C0-A557-227ABD8EC0AC}" name="LUK" dataDxfId="220">
+    <tableColumn id="9" xr3:uid="{E727A271-B479-47C0-A557-227ABD8EC0AC}" name="LUK" dataDxfId="228">
       <calculatedColumnFormula>Table131611232425[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7233,28 +7297,28 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDEC26FB-B5E4-44F5-B062-22E344453193}">
-  <dimension ref="A2:U30"/>
+  <dimension ref="A2:Y30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" topLeftCell="F6" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
-      </c>
-      <c r="L3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -7282,35 +7346,35 @@
       <c r="I4" t="s">
         <v>9</v>
       </c>
-      <c r="L4" t="s">
+      <c r="P4" t="s">
         <v>12</v>
       </c>
-      <c r="M4" t="s">
+      <c r="Q4" t="s">
         <v>2</v>
       </c>
-      <c r="N4" t="s">
+      <c r="R4" t="s">
         <v>3</v>
       </c>
-      <c r="O4" t="s">
+      <c r="S4" t="s">
         <v>4</v>
       </c>
-      <c r="P4" t="s">
+      <c r="T4" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="U4" t="s">
         <v>6</v>
       </c>
-      <c r="R4" t="s">
+      <c r="V4" t="s">
         <v>7</v>
       </c>
-      <c r="S4" t="s">
+      <c r="W4" t="s">
         <v>8</v>
       </c>
-      <c r="T4" t="s">
+      <c r="X4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -7346,43 +7410,43 @@
         <f>Table131639[[#This Row],[Level]]*1.25 + 15</f>
         <v>16.25</v>
       </c>
-      <c r="L5">
+      <c r="P5">
         <v>1</v>
       </c>
-      <c r="M5">
+      <c r="Q5">
         <f>Table13163946[[#This Row],[Level]]*106.25 + 500</f>
         <v>606.25</v>
       </c>
-      <c r="N5">
+      <c r="R5">
         <f>Table13163946[[#This Row],[Level]]*10+20</f>
         <v>30</v>
       </c>
-      <c r="O5">
+      <c r="S5">
         <f>Table13163946[[#This Row],[Level]]*2.125+ 15 + 40</f>
         <v>57.125</v>
       </c>
-      <c r="P5">
+      <c r="T5">
         <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 20</f>
         <v>37.125</v>
       </c>
-      <c r="Q5">
+      <c r="U5">
         <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
         <v>16</v>
       </c>
-      <c r="R5">
+      <c r="V5">
         <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 40</f>
         <v>57.125</v>
       </c>
-      <c r="S5">
+      <c r="W5">
         <f>Table13163946[[#This Row],[Level]]*1.5 + 15</f>
         <v>16.5</v>
       </c>
-      <c r="T5">
+      <c r="X5">
         <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
@@ -7418,43 +7482,43 @@
         <f>Table131639[[#This Row],[Level]]*1.25 + 15</f>
         <v>27.5</v>
       </c>
-      <c r="L6">
+      <c r="P6">
         <v>10</v>
       </c>
-      <c r="M6">
+      <c r="Q6">
         <f>Table13163946[[#This Row],[Level]]*106.25 + 500</f>
         <v>1562.5</v>
       </c>
-      <c r="N6">
+      <c r="R6">
         <f>Table13163946[[#This Row],[Level]]*10+20</f>
         <v>120</v>
       </c>
-      <c r="O6">
+      <c r="S6">
         <f>Table13163946[[#This Row],[Level]]*2.125+ 15 + 40</f>
         <v>76.25</v>
       </c>
-      <c r="P6">
+      <c r="T6">
         <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 20</f>
         <v>56.25</v>
       </c>
-      <c r="Q6">
+      <c r="U6">
         <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
         <v>25</v>
       </c>
-      <c r="R6">
+      <c r="V6">
         <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 40</f>
         <v>76.25</v>
       </c>
-      <c r="S6">
+      <c r="W6">
         <f>Table13163946[[#This Row],[Level]]*1.5 + 15</f>
         <v>30</v>
       </c>
-      <c r="T6">
+      <c r="X6">
         <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20</v>
       </c>
@@ -7490,43 +7554,43 @@
         <f>Table131639[[#This Row],[Level]]*1.25 + 15</f>
         <v>40</v>
       </c>
-      <c r="L7">
+      <c r="P7">
         <v>20</v>
       </c>
-      <c r="M7">
+      <c r="Q7">
         <f>Table13163946[[#This Row],[Level]]*106.25 + 500</f>
         <v>2625</v>
       </c>
-      <c r="N7">
+      <c r="R7">
         <f>Table13163946[[#This Row],[Level]]*10+20</f>
         <v>220</v>
       </c>
-      <c r="O7">
+      <c r="S7">
         <f>Table13163946[[#This Row],[Level]]*2.125+ 15 + 40</f>
         <v>97.5</v>
       </c>
-      <c r="P7">
+      <c r="T7">
         <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 20</f>
         <v>77.5</v>
       </c>
-      <c r="Q7">
+      <c r="U7">
         <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
         <v>35</v>
       </c>
-      <c r="R7">
+      <c r="V7">
         <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 40</f>
         <v>97.5</v>
       </c>
-      <c r="S7">
+      <c r="W7">
         <f>Table13163946[[#This Row],[Level]]*1.5 + 15</f>
         <v>45</v>
       </c>
-      <c r="T7">
+      <c r="X7">
         <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>22</v>
       </c>
@@ -7562,43 +7626,43 @@
         <f>Table131639[[#This Row],[Level]]*1.25 + 15</f>
         <v>42.5</v>
       </c>
-      <c r="L8">
+      <c r="P8">
         <v>22</v>
       </c>
-      <c r="M8" s="1">
+      <c r="Q8" s="1">
         <f>Table13163946[[#This Row],[Level]]*106.25 + 500</f>
         <v>2837.5</v>
       </c>
-      <c r="N8" s="1">
+      <c r="R8" s="1">
         <f>Table13163946[[#This Row],[Level]]*10+20</f>
         <v>240</v>
       </c>
-      <c r="O8" s="1">
+      <c r="S8" s="1">
         <f>Table13163946[[#This Row],[Level]]*2.125+ 15 + 40</f>
         <v>101.75</v>
       </c>
-      <c r="P8" s="1">
+      <c r="T8" s="1">
         <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 20</f>
         <v>81.75</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="U8" s="1">
         <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
         <v>37</v>
       </c>
-      <c r="R8" s="1">
+      <c r="V8" s="1">
         <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 40</f>
         <v>101.75</v>
       </c>
-      <c r="S8" s="1">
+      <c r="W8" s="1">
         <f>Table13163946[[#This Row],[Level]]*1.5 + 15</f>
         <v>48</v>
       </c>
-      <c r="T8" s="1">
+      <c r="X8" s="1">
         <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>25</v>
       </c>
@@ -7634,78 +7698,78 @@
         <f>Table131639[[#This Row],[Level]]*1.25 + 15</f>
         <v>46.25</v>
       </c>
-      <c r="L9">
+      <c r="P9">
         <v>25</v>
       </c>
-      <c r="M9" s="1">
+      <c r="Q9" s="1">
         <f>Table13163946[[#This Row],[Level]]*106.25 + 500</f>
         <v>3156.25</v>
       </c>
-      <c r="N9" s="1">
+      <c r="R9" s="1">
         <f>Table13163946[[#This Row],[Level]]*10+20</f>
         <v>270</v>
       </c>
-      <c r="O9" s="1">
+      <c r="S9" s="1">
         <f>Table13163946[[#This Row],[Level]]*2.125+ 15 + 40</f>
         <v>108.125</v>
       </c>
-      <c r="P9" s="1">
+      <c r="T9" s="1">
         <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 20</f>
         <v>88.125</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="U9" s="1">
         <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
         <v>40</v>
       </c>
-      <c r="R9" s="1">
+      <c r="V9" s="1">
         <f>Table13163946[[#This Row],[Level]]*2.125 + 15 + 40</f>
         <v>108.125</v>
       </c>
-      <c r="S9" s="1">
+      <c r="W9" s="1">
         <f>Table13163946[[#This Row],[Level]]*1.5 + 15</f>
         <v>52.5</v>
       </c>
-      <c r="T9" s="1">
+      <c r="X9" s="1">
         <f>Table13163946[[#This Row],[Level]]*1 + 15</f>
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
-      </c>
-      <c r="L11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="P11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="M11" s="6" t="s">
+      <c r="Q11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="N11" s="6" t="s">
+      <c r="R11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="O11" s="6" t="s">
+      <c r="S11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="P11" s="6" t="s">
+      <c r="T11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Q11" s="6" t="s">
+      <c r="U11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="R11" s="6" t="s">
+      <c r="V11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="S11" s="6" t="s">
+      <c r="W11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="T11" s="6" t="s">
+      <c r="X11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="U11" s="7" t="s">
+      <c r="Y11" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -7733,39 +7797,39 @@
       <c r="I12" t="s">
         <v>9</v>
       </c>
-      <c r="L12" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="M12" s="9">
+      <c r="P12" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q12" s="9">
         <v>10</v>
       </c>
-      <c r="N12" s="9">
+      <c r="R12" s="9">
         <v>1</v>
       </c>
-      <c r="O12" s="9">
+      <c r="S12" s="9">
         <v>10</v>
       </c>
-      <c r="P12" s="9">
+      <c r="T12" s="9">
         <v>10</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="U12" s="9">
         <v>1</v>
       </c>
-      <c r="R12" s="9">
+      <c r="V12" s="9">
         <v>10</v>
       </c>
-      <c r="S12" s="9">
+      <c r="W12" s="9">
         <v>5</v>
       </c>
-      <c r="T12" s="9">
+      <c r="X12" s="9">
         <v>1</v>
       </c>
-      <c r="U12" s="10">
-        <f>SUM(M12:T12)</f>
+      <c r="Y12" s="10">
+        <f>SUM(Q12:X12)</f>
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -7802,7 +7866,7 @@
         <v>16.25</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>15</v>
       </c>
@@ -7839,7 +7903,7 @@
         <v>33.75</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20</v>
       </c>
@@ -7875,8 +7939,11 @@
         <f>Table13182227[[#This Row],[Level]]*1.25 + 15</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>25</v>
       </c>
@@ -7912,18 +7979,120 @@
         <f>Table13182227[[#This Row],[Level]]*1.25 + 15</f>
         <v>46.25</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="P16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P17" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>2</v>
+      </c>
+      <c r="R17" t="s">
+        <v>3</v>
+      </c>
+      <c r="S17" t="s">
+        <v>4</v>
+      </c>
+      <c r="T17" t="s">
+        <v>5</v>
+      </c>
+      <c r="U17" t="s">
+        <v>6</v>
+      </c>
+      <c r="V17" t="s">
+        <v>7</v>
+      </c>
+      <c r="W17" t="s">
+        <v>8</v>
+      </c>
+      <c r="X17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <f>Table13163948[[#This Row],[Level]]*75 + 500 + 800</f>
+        <v>1375</v>
+      </c>
+      <c r="R18">
+        <f>Table13163948[[#This Row],[Level]]*10+20</f>
+        <v>30</v>
+      </c>
+      <c r="S18">
+        <f>Table13163948[[#This Row],[Level]]*1.375+ 15 + 40</f>
+        <v>56.375</v>
+      </c>
+      <c r="T18">
+        <f>Table13163948[[#This Row],[Level]]*1.375 + 15 + 21</f>
+        <v>37.375</v>
+      </c>
+      <c r="U18">
+        <f>Table13163948[[#This Row],[Level]]*1 + 15</f>
+        <v>16</v>
+      </c>
+      <c r="V18">
+        <f>Table13163948[[#This Row],[Level]]*1 + 15 + 7</f>
+        <v>23</v>
+      </c>
+      <c r="W18">
+        <f>Table13163948[[#This Row],[Level]]*1.25 + 15</f>
+        <v>16.25</v>
+      </c>
+      <c r="X18">
+        <f>Table13163948[[#This Row],[Level]]*1.25 + 15</f>
+        <v>16.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="P19">
+        <v>10</v>
+      </c>
+      <c r="Q19">
+        <f>Table13163948[[#This Row],[Level]]*75 + 500 + 800</f>
+        <v>2050</v>
+      </c>
+      <c r="R19">
+        <f>Table13163948[[#This Row],[Level]]*10+20</f>
+        <v>120</v>
+      </c>
+      <c r="S19">
+        <f>Table13163948[[#This Row],[Level]]*1.375+ 15 + 40</f>
+        <v>68.75</v>
+      </c>
+      <c r="T19">
+        <f>Table13163948[[#This Row],[Level]]*1.375 + 15 + 21</f>
+        <v>49.75</v>
+      </c>
+      <c r="U19">
+        <f>Table13163948[[#This Row],[Level]]*1 + 15</f>
+        <v>25</v>
+      </c>
+      <c r="V19">
+        <f>Table13163948[[#This Row],[Level]]*1 + 15 + 7</f>
+        <v>32</v>
+      </c>
+      <c r="W19">
+        <f>Table13163948[[#This Row],[Level]]*1.25 + 15</f>
+        <v>27.5</v>
+      </c>
+      <c r="X19">
+        <f>Table13163948[[#This Row],[Level]]*1.25 + 15</f>
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -7951,8 +8120,43 @@
       <c r="I20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="P20">
+        <v>20</v>
+      </c>
+      <c r="Q20">
+        <f>Table13163948[[#This Row],[Level]]*75 + 500 + 800</f>
+        <v>2800</v>
+      </c>
+      <c r="R20">
+        <f>Table13163948[[#This Row],[Level]]*10+20</f>
+        <v>220</v>
+      </c>
+      <c r="S20">
+        <f>Table13163948[[#This Row],[Level]]*1.375+ 15 + 40</f>
+        <v>82.5</v>
+      </c>
+      <c r="T20">
+        <f>Table13163948[[#This Row],[Level]]*1.375 + 15 + 21</f>
+        <v>63.5</v>
+      </c>
+      <c r="U20">
+        <f>Table13163948[[#This Row],[Level]]*1 + 15</f>
+        <v>35</v>
+      </c>
+      <c r="V20">
+        <f>Table13163948[[#This Row],[Level]]*1 + 15 + 7</f>
+        <v>42</v>
+      </c>
+      <c r="W20">
+        <f>Table13163948[[#This Row],[Level]]*1.25 + 15</f>
+        <v>40</v>
+      </c>
+      <c r="X20">
+        <f>Table13163948[[#This Row],[Level]]*1.25 + 15</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -7988,8 +8192,43 @@
         <f>Table13162044[[#This Row],[Level]]*1.25 + 15</f>
         <v>16.25</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="P21">
+        <v>22</v>
+      </c>
+      <c r="Q21" s="1">
+        <f>Table13163948[[#This Row],[Level]]*75 + 500 + 800</f>
+        <v>2950</v>
+      </c>
+      <c r="R21" s="1">
+        <f>Table13163948[[#This Row],[Level]]*10+20</f>
+        <v>240</v>
+      </c>
+      <c r="S21" s="1">
+        <f>Table13163948[[#This Row],[Level]]*1.375+ 15 + 40</f>
+        <v>85.25</v>
+      </c>
+      <c r="T21" s="1">
+        <f>Table13163948[[#This Row],[Level]]*1.375 + 15 + 21</f>
+        <v>66.25</v>
+      </c>
+      <c r="U21" s="1">
+        <f>Table13163948[[#This Row],[Level]]*1 + 15</f>
+        <v>37</v>
+      </c>
+      <c r="V21" s="1">
+        <f>Table13163948[[#This Row],[Level]]*1 + 15 + 7</f>
+        <v>44</v>
+      </c>
+      <c r="W21" s="1">
+        <f>Table13163948[[#This Row],[Level]]*1.25 + 15</f>
+        <v>42.5</v>
+      </c>
+      <c r="X21" s="1">
+        <f>Table13163948[[#This Row],[Level]]*1.25 + 15</f>
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10</v>
       </c>
@@ -8025,8 +8264,43 @@
         <f>Table13162044[[#This Row],[Level]]*1.25 + 15</f>
         <v>27.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="P22">
+        <v>28</v>
+      </c>
+      <c r="Q22" s="1">
+        <f>Table13163948[[#This Row],[Level]]*75 + 500 + 800</f>
+        <v>3400</v>
+      </c>
+      <c r="R22" s="1">
+        <f>Table13163948[[#This Row],[Level]]*10+20</f>
+        <v>300</v>
+      </c>
+      <c r="S22" s="1">
+        <f>Table13163948[[#This Row],[Level]]*1.375+ 15 + 40</f>
+        <v>93.5</v>
+      </c>
+      <c r="T22" s="1">
+        <f>Table13163948[[#This Row],[Level]]*1.375 + 15 + 21</f>
+        <v>74.5</v>
+      </c>
+      <c r="U22" s="1">
+        <f>Table13163948[[#This Row],[Level]]*1 + 15</f>
+        <v>43</v>
+      </c>
+      <c r="V22" s="1">
+        <f>Table13163948[[#This Row],[Level]]*1 + 15 + 7</f>
+        <v>50</v>
+      </c>
+      <c r="W22" s="1">
+        <f>Table13163948[[#This Row],[Level]]*1.25 + 15</f>
+        <v>50</v>
+      </c>
+      <c r="X22" s="1">
+        <f>Table13163948[[#This Row],[Level]]*1.25 + 15</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -8063,7 +8337,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>25</v>
       </c>
@@ -8100,12 +8374,12 @@
         <v>46.25</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -8134,7 +8408,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -8171,7 +8445,7 @@
         <v>56.5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>20</v>
       </c>
@@ -8208,7 +8482,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>25</v>
       </c>
@@ -8247,12 +8521,13 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="5">
+  <tableParts count="6">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
@@ -8269,7 +8544,7 @@
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -8472,12 +8747,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -8514,7 +8789,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B5">
         <v>20</v>
@@ -8547,7 +8822,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J6" s="1">
         <f>SUM(Table168213429322745[[#This Row],[HP]:[LUK]])</f>

</xml_diff>

<commit_message>
Added fights to Wynisa forest, working on trying to make Behemoth battle interesting. It's just a slow slog right now...
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="14" activeTab="16" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="14" activeTab="18" xr2:uid="{D5030FAB-5119-49EA-A44B-FED5D2E13C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Skeleton Soldier" sheetId="1" r:id="rId1"/>
@@ -3091,28 +3091,28 @@
   <autoFilter ref="P17:X22" xr:uid="{34DCA2BD-7E90-4BA9-882D-4A0B5CA055A2}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2AC3EA1B-ED8B-468F-B2A6-478A7888C995}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{11C9D480-A783-4641-BBCD-983BB72FDE5E}" name="HP" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{11C9D480-A783-4641-BBCD-983BB72FDE5E}" name="HP" dataDxfId="24">
       <calculatedColumnFormula>Table13163948[[#This Row],[Level]]*75 + 500 + 800</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{03905492-344D-488D-BA0A-796528D82C7E}" name="MP" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{03905492-344D-488D-BA0A-796528D82C7E}" name="MP" dataDxfId="23">
       <calculatedColumnFormula>Table13163948[[#This Row],[Level]]*10+20</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F7DA4593-8DF4-45AC-B00B-B64FDCC5B736}" name="ATK" dataDxfId="6">
+    <tableColumn id="4" xr3:uid="{F7DA4593-8DF4-45AC-B00B-B64FDCC5B736}" name="ATK" dataDxfId="22">
       <calculatedColumnFormula>Table13163948[[#This Row],[Level]]*1.375+ 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{53D3990A-7FA7-46A4-830F-4FB19D3D6B6B}" name="DEF" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{53D3990A-7FA7-46A4-830F-4FB19D3D6B6B}" name="DEF" dataDxfId="21">
       <calculatedColumnFormula>Table13163948[[#This Row],[Level]]*1.375 + 15 + 21</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{6DF255D1-55F9-4368-A244-C7F30A95F80B}" name="MAT" dataDxfId="5">
+    <tableColumn id="6" xr3:uid="{6DF255D1-55F9-4368-A244-C7F30A95F80B}" name="MAT" dataDxfId="20">
       <calculatedColumnFormula>Table13163948[[#This Row],[Level]]*1 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3FCEFA1B-B764-42CB-BA1A-3C45F9507B46}" name="MDF" dataDxfId="1">
+    <tableColumn id="7" xr3:uid="{3FCEFA1B-B764-42CB-BA1A-3C45F9507B46}" name="MDF" dataDxfId="19">
       <calculatedColumnFormula>Table13163948[[#This Row],[Level]]*1 + 15 + 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{3774B5F6-1896-4C00-9EB2-5E37E70AFBEA}" name="AGI" dataDxfId="4">
+    <tableColumn id="8" xr3:uid="{3774B5F6-1896-4C00-9EB2-5E37E70AFBEA}" name="AGI" dataDxfId="18">
       <calculatedColumnFormula>Table13163948[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{8F366B0D-3C62-4955-826F-672B2C04A72E}" name="LUK" dataDxfId="3">
+    <tableColumn id="9" xr3:uid="{8F366B0D-3C62-4955-826F-672B2C04A72E}" name="LUK" dataDxfId="17">
       <calculatedColumnFormula>Table13163948[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3125,28 +3125,28 @@
   <autoFilter ref="A3:I7" xr:uid="{7F8360B3-D323-4505-8E52-764F2EEFEF08}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2DA75379-E191-41C6-A461-F7A952576C54}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{0E110670-3AC7-427B-B6F4-6865DC721C3B}" name="HP" dataDxfId="24">
+    <tableColumn id="2" xr3:uid="{0E110670-3AC7-427B-B6F4-6865DC721C3B}" name="HP" dataDxfId="16">
       <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*62.5+ 300</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DD071379-690C-45AA-9EB0-1452F203E78A}" name="MP" dataDxfId="23">
+    <tableColumn id="3" xr3:uid="{DD071379-690C-45AA-9EB0-1452F203E78A}" name="MP" dataDxfId="15">
       <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*12.5+60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{16C4CC92-9435-4196-8A09-D27E77854475}" name="ATK" dataDxfId="22">
+    <tableColumn id="4" xr3:uid="{16C4CC92-9435-4196-8A09-D27E77854475}" name="ATK" dataDxfId="14">
       <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{ACFF3F1F-0DEB-4962-A30C-E7A1BD1814C4}" name="DEF" dataDxfId="21">
+    <tableColumn id="5" xr3:uid="{ACFF3F1F-0DEB-4962-A30C-E7A1BD1814C4}" name="DEF" dataDxfId="13">
       <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1 + 15 + 10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{AF9BE2E5-89EE-468C-B0ED-D05B0FFE3880}" name="MAT" dataDxfId="20">
+    <tableColumn id="6" xr3:uid="{AF9BE2E5-89EE-468C-B0ED-D05B0FFE3880}" name="MAT" dataDxfId="12">
       <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{BF26333D-F5E1-471D-8EB4-69106E629333}" name="MDF" dataDxfId="19">
+    <tableColumn id="7" xr3:uid="{BF26333D-F5E1-471D-8EB4-69106E629333}" name="MDF" dataDxfId="11">
       <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1 + 15 + 8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{419D6271-6B9C-434E-BF38-4DE7848F9419}" name="AGI" dataDxfId="18">
+    <tableColumn id="8" xr3:uid="{419D6271-6B9C-434E-BF38-4DE7848F9419}" name="AGI" dataDxfId="10">
       <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1.5 + 15 + 40</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{CB85A19D-24B4-428F-A77F-481DA3FAACF8}" name="LUK" dataDxfId="17">
+    <tableColumn id="9" xr3:uid="{CB85A19D-24B4-428F-A77F-481DA3FAACF8}" name="LUK" dataDxfId="9">
       <calculatedColumnFormula>Table1318222743[[#This Row],[Level]]*1.25 + 15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3167,7 +3167,7 @@
     <tableColumn id="7" xr3:uid="{6B239F5E-F897-4532-B3C2-8B926BDED5BF}" name="MDF"/>
     <tableColumn id="8" xr3:uid="{CB8FDC45-B604-4FEB-9A7B-367828FC7568}" name="AGI"/>
     <tableColumn id="9" xr3:uid="{6C00B6B1-0959-4058-96EE-2711BA8C66BD}" name="LUK"/>
-    <tableColumn id="10" xr3:uid="{1803A62E-480C-481E-8063-2EB8C650EA1D}" name="Total" dataDxfId="16">
+    <tableColumn id="10" xr3:uid="{1803A62E-480C-481E-8063-2EB8C650EA1D}" name="Total" dataDxfId="8">
       <calculatedColumnFormula>SUM(Table168213429322745[[#This Row],[HP]:[LUK]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3180,28 +3180,28 @@
   <autoFilter ref="A8:I13" xr:uid="{F3DE48F5-A98B-4A15-8805-1948F568C45F}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2E01F6BC-B2F6-42D6-A20F-FDB9BA2D677A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{21915B10-9976-4EFE-936F-170B253E711B}" name="HP" dataDxfId="15">
+    <tableColumn id="2" xr3:uid="{21915B10-9976-4EFE-936F-170B253E711B}" name="HP" dataDxfId="7">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*168.75</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{052B9451-309F-4C84-8FC4-08AD4866120D}" name="MP" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{052B9451-309F-4C84-8FC4-08AD4866120D}" name="MP" dataDxfId="6">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{B73769F3-1F79-45AE-998C-FF1A9A557091}" name="ATK" dataDxfId="13">
+    <tableColumn id="4" xr3:uid="{B73769F3-1F79-45AE-998C-FF1A9A557091}" name="ATK" dataDxfId="5">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*3.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B5E81D1B-B382-4DF5-92BA-F92F12A23A07}" name="DEF" dataDxfId="12">
+    <tableColumn id="5" xr3:uid="{B5E81D1B-B382-4DF5-92BA-F92F12A23A07}" name="DEF" dataDxfId="4">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*4.75</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A815FA03-2618-4DC9-9734-50DCE6DA615F}" name="MAT" dataDxfId="11">
+    <tableColumn id="6" xr3:uid="{A815FA03-2618-4DC9-9734-50DCE6DA615F}" name="MAT" dataDxfId="3">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D8263081-7D11-47BB-9AEC-CE559647F35D}" name="MDF" dataDxfId="10">
+    <tableColumn id="7" xr3:uid="{D8263081-7D11-47BB-9AEC-CE559647F35D}" name="MDF" dataDxfId="2">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*4.75</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C838F145-4059-4C8C-8152-B8F66431FFE1}" name="AGI" dataDxfId="9">
+    <tableColumn id="8" xr3:uid="{C838F145-4059-4C8C-8152-B8F66431FFE1}" name="AGI" dataDxfId="1">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*3.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{431AC55C-A81C-4BB0-B544-6631F8331D55}" name="LUK" dataDxfId="8">
+    <tableColumn id="9" xr3:uid="{431AC55C-A81C-4BB0-B544-6631F8331D55}" name="LUK" dataDxfId="0">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*2.125</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7299,7 +7299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDEC26FB-B5E4-44F5-B062-22E344453193}">
   <dimension ref="A2:Y30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F6" workbookViewId="0">
+    <sheetView topLeftCell="F6" workbookViewId="0">
       <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
@@ -8736,8 +8736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832521D1-8A9A-424A-96D4-48DD11A591EE}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8824,9 +8824,33 @@
       <c r="A6" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="1">
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>30</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
         <f>SUM(Table168213429322745[[#This Row],[HP]:[LUK]])</f>
-        <v>0</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added quest turning for Z6 Sidequest. Made Behemoth fight more challenging and less of a snoozefest
</commit_message>
<xml_diff>
--- a/enemies.xlsx
+++ b/enemies.xlsx
@@ -3186,22 +3186,22 @@
     <tableColumn id="3" xr3:uid="{052B9451-309F-4C84-8FC4-08AD4866120D}" name="MP" dataDxfId="6">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{B73769F3-1F79-45AE-998C-FF1A9A557091}" name="ATK" dataDxfId="5">
+    <tableColumn id="4" xr3:uid="{B73769F3-1F79-45AE-998C-FF1A9A557091}" name="ATK" dataDxfId="0">
+      <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*4.5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{B5E81D1B-B382-4DF5-92BA-F92F12A23A07}" name="DEF" dataDxfId="5">
+      <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*4.75</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{A815FA03-2618-4DC9-9734-50DCE6DA615F}" name="MAT" dataDxfId="4">
+      <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{D8263081-7D11-47BB-9AEC-CE559647F35D}" name="MDF" dataDxfId="3">
+      <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*4.75</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{C838F145-4059-4C8C-8152-B8F66431FFE1}" name="AGI" dataDxfId="2">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*3.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B5E81D1B-B382-4DF5-92BA-F92F12A23A07}" name="DEF" dataDxfId="4">
-      <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*4.75</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{A815FA03-2618-4DC9-9734-50DCE6DA615F}" name="MAT" dataDxfId="3">
-      <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*1</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{D8263081-7D11-47BB-9AEC-CE559647F35D}" name="MDF" dataDxfId="2">
-      <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*4.75</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{C838F145-4059-4C8C-8152-B8F66431FFE1}" name="AGI" dataDxfId="1">
-      <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*3.5</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{431AC55C-A81C-4BB0-B544-6631F8331D55}" name="LUK" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{431AC55C-A81C-4BB0-B544-6631F8331D55}" name="LUK" dataDxfId="1">
       <calculatedColumnFormula>Table1316183336373847[[#This Row],[Level]]*2.125</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8737,7 +8737,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8798,7 +8798,7 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E5">
         <v>30</v>
@@ -8817,7 +8817,7 @@
       </c>
       <c r="J5">
         <f>SUM(Table168213429322745[[#This Row],[HP]:[LUK]])</f>
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -8831,7 +8831,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E6">
         <v>30</v>
@@ -8850,7 +8850,7 @@
       </c>
       <c r="J6">
         <f>SUM(Table168213429322745[[#This Row],[HP]:[LUK]])</f>
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -8895,8 +8895,8 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <f>Table1316183336373847[[#This Row],[Level]]*3.5</f>
-        <v>3.5</v>
+        <f>Table1316183336373847[[#This Row],[Level]]*4.5</f>
+        <v>4.5</v>
       </c>
       <c r="E9">
         <f>Table1316183336373847[[#This Row],[Level]]*4.75</f>
@@ -8932,8 +8932,8 @@
         <v>150</v>
       </c>
       <c r="D10">
-        <f>Table1316183336373847[[#This Row],[Level]]*3.5</f>
-        <v>52.5</v>
+        <f>Table1316183336373847[[#This Row],[Level]]*4.5</f>
+        <v>67.5</v>
       </c>
       <c r="E10">
         <f>Table1316183336373847[[#This Row],[Level]]*4.75</f>
@@ -8969,8 +8969,8 @@
         <v>250</v>
       </c>
       <c r="D11">
-        <f>Table1316183336373847[[#This Row],[Level]]*3.5</f>
-        <v>87.5</v>
+        <f>Table1316183336373847[[#This Row],[Level]]*4.5</f>
+        <v>112.5</v>
       </c>
       <c r="E11">
         <f>Table1316183336373847[[#This Row],[Level]]*4.75</f>
@@ -9006,8 +9006,8 @@
         <v>300</v>
       </c>
       <c r="D12">
-        <f>Table1316183336373847[[#This Row],[Level]]*3.5</f>
-        <v>105</v>
+        <f>Table1316183336373847[[#This Row],[Level]]*4.5</f>
+        <v>135</v>
       </c>
       <c r="E12">
         <f>Table1316183336373847[[#This Row],[Level]]*4.75</f>
@@ -9043,8 +9043,8 @@
         <v>200</v>
       </c>
       <c r="D13">
-        <f>Table1316183336373847[[#This Row],[Level]]*3.5</f>
-        <v>70</v>
+        <f>Table1316183336373847[[#This Row],[Level]]*4.5</f>
+        <v>90</v>
       </c>
       <c r="E13">
         <f>Table1316183336373847[[#This Row],[Level]]*4.75</f>

</xml_diff>